<commit_message>
3.1.0: telegramType plain is implemented.
</commit_message>
<xml_diff>
--- a/meta/plainApi/BlancoApiPlainSample.xlsx
+++ b/meta/plainApi/BlancoApiPlainSample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10611"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorKt/meta/plainApi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorTs/meta/plainApi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F64AFF-70D0-8B45-9675-30E890E033E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E6D3F9-E84F-6A4D-8C53-50C57BECDB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2440" yWindow="1280" windowWidth="29440" windowHeight="21600" tabRatio="860" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2440" yWindow="500" windowWidth="29440" windowHeight="20500" tabRatio="860" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="process" sheetId="19" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="244">
   <si>
     <t>項目名</t>
     <rPh sb="0" eb="3">
@@ -2476,6 +2476,22 @@
   </si>
   <si>
     <t>ArrayList</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>""</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>[]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>new ObjectSample()</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>{}</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -3632,10 +3648,88 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="49" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3647,9 +3741,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3658,12 +3749,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3695,12 +3780,6 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3710,80 +3789,14 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3792,10 +3805,13 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3807,10 +3823,10 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4403,152 +4419,152 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="162" t="s">
+      <c r="A5" s="129" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="162"/>
-      <c r="C5" s="162"/>
-      <c r="D5" s="162"/>
-      <c r="E5" s="162"/>
+      <c r="B5" s="129"/>
+      <c r="C5" s="129"/>
+      <c r="D5" s="129"/>
+      <c r="E5" s="129"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="173" t="s">
+      <c r="A6" s="135" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="174"/>
-      <c r="C6" s="175"/>
-      <c r="D6" s="171" t="s">
+      <c r="B6" s="136"/>
+      <c r="C6" s="137"/>
+      <c r="D6" s="130" t="s">
         <v>234</v>
       </c>
-      <c r="E6" s="171"/>
+      <c r="E6" s="130"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="162" t="s">
+      <c r="A7" s="129" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="162"/>
-      <c r="C7" s="162"/>
-      <c r="D7" s="171" t="s">
+      <c r="B7" s="129"/>
+      <c r="C7" s="129"/>
+      <c r="D7" s="130" t="s">
         <v>160</v>
       </c>
-      <c r="E7" s="171"/>
+      <c r="E7" s="130"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="162" t="s">
+      <c r="A8" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="162"/>
-      <c r="C8" s="162"/>
-      <c r="D8" s="171" t="s">
+      <c r="B8" s="129"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="130" t="s">
         <v>234</v>
       </c>
-      <c r="E8" s="171"/>
+      <c r="E8" s="130"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="162" t="s">
+      <c r="A9" s="129" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="162"/>
-      <c r="C9" s="162"/>
-      <c r="D9" s="171" t="s">
+      <c r="B9" s="129"/>
+      <c r="C9" s="129"/>
+      <c r="D9" s="130" t="s">
         <v>98</v>
       </c>
-      <c r="E9" s="171"/>
+      <c r="E9" s="130"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="162" t="s">
+      <c r="A10" s="129" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="162"/>
-      <c r="C10" s="162"/>
-      <c r="D10" s="171"/>
-      <c r="E10" s="171"/>
+      <c r="B10" s="129"/>
+      <c r="C10" s="129"/>
+      <c r="D10" s="130"/>
+      <c r="E10" s="130"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="162" t="s">
+      <c r="A11" s="129" t="s">
         <v>97</v>
       </c>
-      <c r="B11" s="162"/>
-      <c r="C11" s="162"/>
-      <c r="D11" s="171" t="s">
+      <c r="B11" s="129"/>
+      <c r="C11" s="129"/>
+      <c r="D11" s="130" t="s">
         <v>157</v>
       </c>
-      <c r="E11" s="171"/>
+      <c r="E11" s="130"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="134" t="s">
+      <c r="A12" s="131" t="s">
         <v>168</v>
       </c>
-      <c r="B12" s="134"/>
-      <c r="C12" s="134"/>
-      <c r="D12" s="151" t="s">
+      <c r="B12" s="131"/>
+      <c r="C12" s="131"/>
+      <c r="D12" s="133" t="s">
         <v>169</v>
       </c>
-      <c r="E12" s="151"/>
+      <c r="E12" s="133"/>
       <c r="F12" s="1" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="134" t="s">
+      <c r="A13" s="131" t="s">
         <v>171</v>
       </c>
-      <c r="B13" s="134"/>
-      <c r="C13" s="134"/>
-      <c r="D13" s="150" t="s">
+      <c r="B13" s="131"/>
+      <c r="C13" s="131"/>
+      <c r="D13" s="132" t="s">
         <v>209</v>
       </c>
-      <c r="E13" s="151"/>
+      <c r="E13" s="133"/>
     </row>
     <row r="14" spans="1:6" ht="55" customHeight="1">
-      <c r="A14" s="134" t="s">
+      <c r="A14" s="131" t="s">
         <v>208</v>
       </c>
-      <c r="B14" s="134"/>
-      <c r="C14" s="134"/>
-      <c r="D14" s="172" t="s">
+      <c r="B14" s="131"/>
+      <c r="C14" s="131"/>
+      <c r="D14" s="134" t="s">
         <v>233</v>
       </c>
-      <c r="E14" s="151"/>
+      <c r="E14" s="133"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="134" t="s">
+      <c r="A15" s="131" t="s">
         <v>192</v>
       </c>
-      <c r="B15" s="134"/>
-      <c r="C15" s="134"/>
-      <c r="D15" s="150"/>
-      <c r="E15" s="151"/>
+      <c r="B15" s="131"/>
+      <c r="C15" s="131"/>
+      <c r="D15" s="132"/>
+      <c r="E15" s="133"/>
       <c r="F15" s="1" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="134" t="s">
+      <c r="A16" s="131" t="s">
         <v>193</v>
       </c>
-      <c r="B16" s="134"/>
-      <c r="C16" s="134"/>
-      <c r="D16" s="150"/>
-      <c r="E16" s="151"/>
+      <c r="B16" s="131"/>
+      <c r="C16" s="131"/>
+      <c r="D16" s="132"/>
+      <c r="E16" s="133"/>
       <c r="F16" s="1" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="152" t="s">
+      <c r="A17" s="173" t="s">
         <v>139</v>
       </c>
-      <c r="B17" s="153"/>
-      <c r="C17" s="154"/>
+      <c r="B17" s="174"/>
+      <c r="C17" s="175"/>
       <c r="D17" s="104"/>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="135" t="s">
+      <c r="A18" s="160" t="s">
         <v>173</v>
       </c>
-      <c r="B18" s="136"/>
-      <c r="C18" s="137"/>
+      <c r="B18" s="161"/>
+      <c r="C18" s="162"/>
       <c r="D18" s="90" t="s">
         <v>137</v>
       </c>
@@ -4568,15 +4584,15 @@
       <c r="B19" s="6"/>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="147" t="s">
+      <c r="A20" s="170" t="s">
         <v>182</v>
       </c>
-      <c r="B20" s="148"/>
-      <c r="C20" s="148"/>
-      <c r="D20" s="148"/>
-      <c r="E20" s="148"/>
-      <c r="F20" s="148"/>
-      <c r="G20" s="149"/>
+      <c r="B20" s="171"/>
+      <c r="C20" s="171"/>
+      <c r="D20" s="171"/>
+      <c r="E20" s="171"/>
+      <c r="F20" s="171"/>
+      <c r="G20" s="172"/>
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="91" t="s">
@@ -4620,28 +4636,28 @@
       <c r="C24"/>
     </row>
     <row r="25" spans="1:15">
-      <c r="A25" s="146" t="s">
+      <c r="A25" s="169" t="s">
         <v>183</v>
       </c>
-      <c r="B25" s="146"/>
-      <c r="C25" s="146"/>
-      <c r="D25" s="146"/>
-      <c r="E25" s="146"/>
-      <c r="F25" s="146"/>
-      <c r="G25" s="146"/>
+      <c r="B25" s="169"/>
+      <c r="C25" s="169"/>
+      <c r="D25" s="169"/>
+      <c r="E25" s="169"/>
+      <c r="F25" s="169"/>
+      <c r="G25" s="169"/>
     </row>
     <row r="26" spans="1:15">
       <c r="A26" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="140" t="s">
+      <c r="B26" s="163" t="s">
         <v>177</v>
       </c>
-      <c r="C26" s="141"/>
-      <c r="D26" s="141"/>
-      <c r="E26" s="141"/>
-      <c r="F26" s="141"/>
-      <c r="G26" s="142"/>
+      <c r="C26" s="164"/>
+      <c r="D26" s="164"/>
+      <c r="E26" s="164"/>
+      <c r="F26" s="164"/>
+      <c r="G26" s="165"/>
       <c r="H26" s="95"/>
       <c r="I26" s="95"/>
       <c r="J26" s="95"/>
@@ -4652,12 +4668,12 @@
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="106"/>
-      <c r="B27" s="157"/>
-      <c r="C27" s="157"/>
-      <c r="D27" s="157"/>
-      <c r="E27" s="157"/>
-      <c r="F27" s="157"/>
-      <c r="G27" s="157"/>
+      <c r="B27" s="148"/>
+      <c r="C27" s="148"/>
+      <c r="D27" s="148"/>
+      <c r="E27" s="148"/>
+      <c r="F27" s="148"/>
+      <c r="G27" s="148"/>
       <c r="H27" s="102"/>
       <c r="I27" s="102"/>
       <c r="J27" s="102"/>
@@ -4668,12 +4684,12 @@
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="107"/>
-      <c r="B28" s="158"/>
-      <c r="C28" s="158"/>
-      <c r="D28" s="158"/>
-      <c r="E28" s="158"/>
-      <c r="F28" s="158"/>
-      <c r="G28" s="158"/>
+      <c r="B28" s="150"/>
+      <c r="C28" s="150"/>
+      <c r="D28" s="150"/>
+      <c r="E28" s="150"/>
+      <c r="F28" s="150"/>
+      <c r="G28" s="150"/>
       <c r="H28" s="102"/>
       <c r="I28" s="102"/>
       <c r="J28" s="102"/>
@@ -4684,12 +4700,12 @@
     </row>
     <row r="29" spans="1:15">
       <c r="A29" s="108"/>
-      <c r="B29" s="159"/>
-      <c r="C29" s="159"/>
-      <c r="D29" s="159"/>
-      <c r="E29" s="159"/>
-      <c r="F29" s="159"/>
-      <c r="G29" s="159"/>
+      <c r="B29" s="152"/>
+      <c r="C29" s="152"/>
+      <c r="D29" s="152"/>
+      <c r="E29" s="152"/>
+      <c r="F29" s="152"/>
+      <c r="G29" s="152"/>
       <c r="H29" s="102"/>
       <c r="I29" s="102"/>
       <c r="J29" s="102"/>
@@ -4702,28 +4718,28 @@
       <c r="C30"/>
     </row>
     <row r="31" spans="1:15">
-      <c r="A31" s="143" t="s">
+      <c r="A31" s="166" t="s">
         <v>184</v>
       </c>
-      <c r="B31" s="144"/>
-      <c r="C31" s="144"/>
-      <c r="D31" s="144"/>
-      <c r="E31" s="144"/>
-      <c r="F31" s="144"/>
-      <c r="G31" s="145"/>
+      <c r="B31" s="167"/>
+      <c r="C31" s="167"/>
+      <c r="D31" s="167"/>
+      <c r="E31" s="167"/>
+      <c r="F31" s="167"/>
+      <c r="G31" s="168"/>
     </row>
     <row r="32" spans="1:15">
       <c r="A32" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="164" t="s">
+      <c r="B32" s="144" t="s">
         <v>178</v>
       </c>
-      <c r="C32" s="164"/>
-      <c r="D32" s="164"/>
-      <c r="E32" s="164"/>
-      <c r="F32" s="164"/>
-      <c r="G32" s="164"/>
+      <c r="C32" s="144"/>
+      <c r="D32" s="144"/>
+      <c r="E32" s="144"/>
+      <c r="F32" s="144"/>
+      <c r="G32" s="144"/>
       <c r="H32" s="95"/>
       <c r="I32" s="95"/>
       <c r="J32" s="95"/>
@@ -4736,14 +4752,14 @@
       <c r="A33" s="106">
         <v>1</v>
       </c>
-      <c r="B33" s="165" t="s">
+      <c r="B33" s="145" t="s">
         <v>179</v>
       </c>
-      <c r="C33" s="165"/>
-      <c r="D33" s="165"/>
-      <c r="E33" s="165"/>
-      <c r="F33" s="165"/>
-      <c r="G33" s="165"/>
+      <c r="C33" s="145"/>
+      <c r="D33" s="145"/>
+      <c r="E33" s="145"/>
+      <c r="F33" s="145"/>
+      <c r="G33" s="145"/>
       <c r="H33" s="102"/>
       <c r="I33" s="102"/>
       <c r="J33" s="102"/>
@@ -4754,12 +4770,12 @@
     </row>
     <row r="34" spans="1:15">
       <c r="A34" s="107"/>
-      <c r="B34" s="166"/>
-      <c r="C34" s="166"/>
-      <c r="D34" s="166"/>
-      <c r="E34" s="166"/>
-      <c r="F34" s="166"/>
-      <c r="G34" s="166"/>
+      <c r="B34" s="146"/>
+      <c r="C34" s="146"/>
+      <c r="D34" s="146"/>
+      <c r="E34" s="146"/>
+      <c r="F34" s="146"/>
+      <c r="G34" s="146"/>
       <c r="H34" s="102"/>
       <c r="I34" s="102"/>
       <c r="J34" s="102"/>
@@ -4770,12 +4786,12 @@
     </row>
     <row r="35" spans="1:15">
       <c r="A35" s="108"/>
-      <c r="B35" s="167"/>
-      <c r="C35" s="167"/>
-      <c r="D35" s="167"/>
-      <c r="E35" s="167"/>
-      <c r="F35" s="167"/>
-      <c r="G35" s="167"/>
+      <c r="B35" s="147"/>
+      <c r="C35" s="147"/>
+      <c r="D35" s="147"/>
+      <c r="E35" s="147"/>
+      <c r="F35" s="147"/>
+      <c r="G35" s="147"/>
       <c r="H35" s="102"/>
       <c r="I35" s="102"/>
       <c r="J35" s="102"/>
@@ -4800,28 +4816,28 @@
       <c r="M36"/>
     </row>
     <row r="37" spans="1:15">
-      <c r="A37" s="143" t="s">
+      <c r="A37" s="166" t="s">
         <v>185</v>
       </c>
-      <c r="B37" s="144"/>
-      <c r="C37" s="144"/>
-      <c r="D37" s="144"/>
-      <c r="E37" s="144"/>
-      <c r="F37" s="144"/>
-      <c r="G37" s="145"/>
+      <c r="B37" s="167"/>
+      <c r="C37" s="167"/>
+      <c r="D37" s="167"/>
+      <c r="E37" s="167"/>
+      <c r="F37" s="167"/>
+      <c r="G37" s="168"/>
     </row>
     <row r="38" spans="1:15">
       <c r="A38" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B38" s="164" t="s">
+      <c r="B38" s="144" t="s">
         <v>180</v>
       </c>
-      <c r="C38" s="164"/>
-      <c r="D38" s="164"/>
-      <c r="E38" s="164"/>
-      <c r="F38" s="164"/>
-      <c r="G38" s="164"/>
+      <c r="C38" s="144"/>
+      <c r="D38" s="144"/>
+      <c r="E38" s="144"/>
+      <c r="F38" s="144"/>
+      <c r="G38" s="144"/>
       <c r="H38" s="95"/>
       <c r="I38" s="95"/>
       <c r="J38" s="95"/>
@@ -4832,12 +4848,12 @@
     </row>
     <row r="39" spans="1:15">
       <c r="A39" s="106"/>
-      <c r="B39" s="157"/>
-      <c r="C39" s="157"/>
-      <c r="D39" s="157"/>
-      <c r="E39" s="157"/>
-      <c r="F39" s="157"/>
-      <c r="G39" s="168"/>
+      <c r="B39" s="148"/>
+      <c r="C39" s="148"/>
+      <c r="D39" s="148"/>
+      <c r="E39" s="148"/>
+      <c r="F39" s="148"/>
+      <c r="G39" s="149"/>
       <c r="H39" s="102"/>
       <c r="I39" s="102"/>
       <c r="J39" s="102"/>
@@ -4848,12 +4864,12 @@
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="107"/>
-      <c r="B40" s="158"/>
-      <c r="C40" s="158"/>
-      <c r="D40" s="158"/>
-      <c r="E40" s="158"/>
-      <c r="F40" s="158"/>
-      <c r="G40" s="169"/>
+      <c r="B40" s="150"/>
+      <c r="C40" s="150"/>
+      <c r="D40" s="150"/>
+      <c r="E40" s="150"/>
+      <c r="F40" s="150"/>
+      <c r="G40" s="151"/>
       <c r="H40" s="102"/>
       <c r="I40" s="102"/>
       <c r="J40" s="102"/>
@@ -4864,12 +4880,12 @@
     </row>
     <row r="41" spans="1:15">
       <c r="A41" s="108"/>
-      <c r="B41" s="159"/>
-      <c r="C41" s="159"/>
-      <c r="D41" s="159"/>
-      <c r="E41" s="159"/>
-      <c r="F41" s="159"/>
-      <c r="G41" s="170"/>
+      <c r="B41" s="152"/>
+      <c r="C41" s="152"/>
+      <c r="D41" s="152"/>
+      <c r="E41" s="152"/>
+      <c r="F41" s="152"/>
+      <c r="G41" s="153"/>
       <c r="H41" s="102"/>
       <c r="I41" s="102"/>
       <c r="J41" s="102"/>
@@ -4895,15 +4911,15 @@
       <c r="O42"/>
     </row>
     <row r="43" spans="1:15">
-      <c r="A43" s="146" t="s">
+      <c r="A43" s="169" t="s">
         <v>205</v>
       </c>
-      <c r="B43" s="146"/>
-      <c r="C43" s="146"/>
-      <c r="D43" s="146"/>
-      <c r="E43" s="146"/>
-      <c r="F43" s="146"/>
-      <c r="G43" s="146"/>
+      <c r="B43" s="169"/>
+      <c r="C43" s="169"/>
+      <c r="D43" s="169"/>
+      <c r="E43" s="169"/>
+      <c r="F43" s="169"/>
+      <c r="G43" s="169"/>
     </row>
     <row r="44" spans="1:15">
       <c r="A44" s="105" t="s">
@@ -5019,221 +5035,299 @@
       <c r="F49" s="5"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="131" t="s">
+      <c r="A50" s="157" t="s">
         <v>64</v>
       </c>
-      <c r="B50" s="133"/>
-      <c r="C50" s="131" t="s">
+      <c r="B50" s="159"/>
+      <c r="C50" s="157" t="s">
         <v>65</v>
       </c>
-      <c r="D50" s="132"/>
-      <c r="E50" s="133"/>
+      <c r="D50" s="158"/>
+      <c r="E50" s="159"/>
       <c r="F50" s="27" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="138"/>
-      <c r="B51" s="139"/>
-      <c r="C51" s="138"/>
-      <c r="D51" s="160"/>
-      <c r="E51" s="139"/>
+      <c r="A51" s="154"/>
+      <c r="B51" s="156"/>
+      <c r="C51" s="154"/>
+      <c r="D51" s="155"/>
+      <c r="E51" s="156"/>
       <c r="F51" s="43"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="129"/>
-      <c r="B52" s="130"/>
-      <c r="C52" s="129"/>
-      <c r="D52" s="161"/>
-      <c r="E52" s="130"/>
+      <c r="A52" s="138"/>
+      <c r="B52" s="140"/>
+      <c r="C52" s="138"/>
+      <c r="D52" s="139"/>
+      <c r="E52" s="140"/>
       <c r="F52" s="43"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="129"/>
-      <c r="B53" s="130"/>
-      <c r="C53" s="129"/>
-      <c r="D53" s="161"/>
-      <c r="E53" s="130"/>
+      <c r="A53" s="138"/>
+      <c r="B53" s="140"/>
+      <c r="C53" s="138"/>
+      <c r="D53" s="139"/>
+      <c r="E53" s="140"/>
       <c r="F53" s="43"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="129"/>
-      <c r="B54" s="130"/>
-      <c r="C54" s="129"/>
-      <c r="D54" s="161"/>
-      <c r="E54" s="130"/>
+      <c r="A54" s="138"/>
+      <c r="B54" s="140"/>
+      <c r="C54" s="138"/>
+      <c r="D54" s="139"/>
+      <c r="E54" s="140"/>
       <c r="F54" s="43"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="129"/>
-      <c r="B55" s="130"/>
-      <c r="C55" s="129"/>
-      <c r="D55" s="161"/>
-      <c r="E55" s="130"/>
+      <c r="A55" s="138"/>
+      <c r="B55" s="140"/>
+      <c r="C55" s="138"/>
+      <c r="D55" s="139"/>
+      <c r="E55" s="140"/>
       <c r="F55" s="43"/>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="129"/>
-      <c r="B56" s="130"/>
-      <c r="C56" s="129"/>
-      <c r="D56" s="161"/>
-      <c r="E56" s="130"/>
+      <c r="A56" s="138"/>
+      <c r="B56" s="140"/>
+      <c r="C56" s="138"/>
+      <c r="D56" s="139"/>
+      <c r="E56" s="140"/>
       <c r="F56" s="43"/>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="129"/>
-      <c r="B57" s="130"/>
-      <c r="C57" s="129"/>
-      <c r="D57" s="161"/>
-      <c r="E57" s="130"/>
+      <c r="A57" s="138"/>
+      <c r="B57" s="140"/>
+      <c r="C57" s="138"/>
+      <c r="D57" s="139"/>
+      <c r="E57" s="140"/>
       <c r="F57" s="43"/>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="129"/>
-      <c r="B58" s="130"/>
-      <c r="C58" s="129"/>
-      <c r="D58" s="161"/>
-      <c r="E58" s="130"/>
+      <c r="A58" s="138"/>
+      <c r="B58" s="140"/>
+      <c r="C58" s="138"/>
+      <c r="D58" s="139"/>
+      <c r="E58" s="140"/>
       <c r="F58" s="43"/>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="129"/>
-      <c r="B59" s="130"/>
-      <c r="C59" s="129"/>
-      <c r="D59" s="161"/>
-      <c r="E59" s="130"/>
+      <c r="A59" s="138"/>
+      <c r="B59" s="140"/>
+      <c r="C59" s="138"/>
+      <c r="D59" s="139"/>
+      <c r="E59" s="140"/>
       <c r="F59" s="43"/>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="129"/>
-      <c r="B60" s="130"/>
-      <c r="C60" s="129"/>
-      <c r="D60" s="161"/>
-      <c r="E60" s="130"/>
+      <c r="A60" s="138"/>
+      <c r="B60" s="140"/>
+      <c r="C60" s="138"/>
+      <c r="D60" s="139"/>
+      <c r="E60" s="140"/>
       <c r="F60" s="43"/>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="129"/>
-      <c r="B61" s="130"/>
-      <c r="C61" s="129"/>
-      <c r="D61" s="161"/>
-      <c r="E61" s="130"/>
+      <c r="A61" s="138"/>
+      <c r="B61" s="140"/>
+      <c r="C61" s="138"/>
+      <c r="D61" s="139"/>
+      <c r="E61" s="140"/>
       <c r="F61" s="43"/>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="129"/>
-      <c r="B62" s="130"/>
-      <c r="C62" s="129"/>
-      <c r="D62" s="161"/>
-      <c r="E62" s="130"/>
+      <c r="A62" s="138"/>
+      <c r="B62" s="140"/>
+      <c r="C62" s="138"/>
+      <c r="D62" s="139"/>
+      <c r="E62" s="140"/>
       <c r="F62" s="43"/>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="129"/>
-      <c r="B63" s="130"/>
-      <c r="C63" s="129"/>
-      <c r="D63" s="161"/>
-      <c r="E63" s="130"/>
+      <c r="A63" s="138"/>
+      <c r="B63" s="140"/>
+      <c r="C63" s="138"/>
+      <c r="D63" s="139"/>
+      <c r="E63" s="140"/>
       <c r="F63" s="43"/>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="129"/>
-      <c r="B64" s="130"/>
-      <c r="C64" s="129"/>
-      <c r="D64" s="161"/>
-      <c r="E64" s="130"/>
+      <c r="A64" s="138"/>
+      <c r="B64" s="140"/>
+      <c r="C64" s="138"/>
+      <c r="D64" s="139"/>
+      <c r="E64" s="140"/>
       <c r="F64" s="43"/>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="129"/>
-      <c r="B65" s="130"/>
-      <c r="C65" s="129"/>
-      <c r="D65" s="161"/>
-      <c r="E65" s="130"/>
+      <c r="A65" s="138"/>
+      <c r="B65" s="140"/>
+      <c r="C65" s="138"/>
+      <c r="D65" s="139"/>
+      <c r="E65" s="140"/>
       <c r="F65" s="43"/>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="129"/>
-      <c r="B66" s="130"/>
-      <c r="C66" s="129"/>
-      <c r="D66" s="161"/>
-      <c r="E66" s="130"/>
+      <c r="A66" s="138"/>
+      <c r="B66" s="140"/>
+      <c r="C66" s="138"/>
+      <c r="D66" s="139"/>
+      <c r="E66" s="140"/>
       <c r="F66" s="43"/>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="129"/>
-      <c r="B67" s="130"/>
-      <c r="C67" s="129"/>
-      <c r="D67" s="161"/>
-      <c r="E67" s="130"/>
+      <c r="A67" s="138"/>
+      <c r="B67" s="140"/>
+      <c r="C67" s="138"/>
+      <c r="D67" s="139"/>
+      <c r="E67" s="140"/>
       <c r="F67" s="43"/>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="129"/>
-      <c r="B68" s="130"/>
-      <c r="C68" s="129"/>
-      <c r="D68" s="161"/>
-      <c r="E68" s="130"/>
+      <c r="A68" s="138"/>
+      <c r="B68" s="140"/>
+      <c r="C68" s="138"/>
+      <c r="D68" s="139"/>
+      <c r="E68" s="140"/>
       <c r="F68" s="43"/>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="129"/>
-      <c r="B69" s="130"/>
-      <c r="C69" s="129"/>
-      <c r="D69" s="161"/>
-      <c r="E69" s="130"/>
+      <c r="A69" s="138"/>
+      <c r="B69" s="140"/>
+      <c r="C69" s="138"/>
+      <c r="D69" s="139"/>
+      <c r="E69" s="140"/>
       <c r="F69" s="43"/>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="129"/>
-      <c r="B70" s="130"/>
-      <c r="C70" s="129"/>
-      <c r="D70" s="161"/>
-      <c r="E70" s="130"/>
+      <c r="A70" s="138"/>
+      <c r="B70" s="140"/>
+      <c r="C70" s="138"/>
+      <c r="D70" s="139"/>
+      <c r="E70" s="140"/>
       <c r="F70" s="43"/>
     </row>
     <row r="71" spans="1:6">
-      <c r="A71" s="129"/>
-      <c r="B71" s="130"/>
-      <c r="C71" s="129"/>
-      <c r="D71" s="161"/>
-      <c r="E71" s="130"/>
+      <c r="A71" s="138"/>
+      <c r="B71" s="140"/>
+      <c r="C71" s="138"/>
+      <c r="D71" s="139"/>
+      <c r="E71" s="140"/>
       <c r="F71" s="43"/>
     </row>
     <row r="72" spans="1:6">
-      <c r="A72" s="129"/>
-      <c r="B72" s="130"/>
-      <c r="C72" s="129"/>
-      <c r="D72" s="161"/>
-      <c r="E72" s="130"/>
+      <c r="A72" s="138"/>
+      <c r="B72" s="140"/>
+      <c r="C72" s="138"/>
+      <c r="D72" s="139"/>
+      <c r="E72" s="140"/>
       <c r="F72" s="43"/>
     </row>
     <row r="73" spans="1:6">
-      <c r="A73" s="129"/>
-      <c r="B73" s="130"/>
-      <c r="C73" s="129"/>
-      <c r="D73" s="161"/>
-      <c r="E73" s="130"/>
+      <c r="A73" s="138"/>
+      <c r="B73" s="140"/>
+      <c r="C73" s="138"/>
+      <c r="D73" s="139"/>
+      <c r="E73" s="140"/>
       <c r="F73" s="43"/>
     </row>
     <row r="74" spans="1:6">
-      <c r="A74" s="129"/>
-      <c r="B74" s="130"/>
-      <c r="C74" s="129"/>
-      <c r="D74" s="161"/>
-      <c r="E74" s="130"/>
+      <c r="A74" s="138"/>
+      <c r="B74" s="140"/>
+      <c r="C74" s="138"/>
+      <c r="D74" s="139"/>
+      <c r="E74" s="140"/>
       <c r="F74" s="43"/>
     </row>
     <row r="75" spans="1:6">
-      <c r="A75" s="155"/>
-      <c r="B75" s="156"/>
-      <c r="C75" s="155"/>
-      <c r="D75" s="163"/>
-      <c r="E75" s="156"/>
+      <c r="A75" s="141"/>
+      <c r="B75" s="143"/>
+      <c r="C75" s="141"/>
+      <c r="D75" s="142"/>
+      <c r="E75" s="143"/>
       <c r="F75" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="94">
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A43:G43"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C73:E73"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C75:E75"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="C72:E72"/>
     <mergeCell ref="A5:E5"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D7:E7"/>
@@ -5250,84 +5344,6 @@
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="C75:E75"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C73:E73"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="A37:G37"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="A20:G20"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A43:G43"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="2">
@@ -5365,8 +5381,8 @@
   </sheetPr>
   <dimension ref="A1:V67"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K47" sqref="K47"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -5526,10 +5542,10 @@
         <v>168</v>
       </c>
       <c r="B16" s="111"/>
-      <c r="C16" s="151" t="s">
+      <c r="C16" s="133" t="s">
         <v>169</v>
       </c>
-      <c r="D16" s="151"/>
+      <c r="D16" s="133"/>
       <c r="E16" s="1" t="s">
         <v>170</v>
       </c>
@@ -5539,20 +5555,20 @@
         <v>171</v>
       </c>
       <c r="B17" s="111"/>
-      <c r="C17" s="151" t="s">
+      <c r="C17" s="133" t="s">
         <v>172</v>
       </c>
-      <c r="D17" s="151"/>
+      <c r="D17" s="133"/>
     </row>
     <row r="18" spans="1:22">
       <c r="A18" s="111" t="s">
         <v>208</v>
       </c>
       <c r="B18" s="111"/>
-      <c r="C18" s="150" t="s">
+      <c r="C18" s="132" t="s">
         <v>210</v>
       </c>
-      <c r="D18" s="151"/>
+      <c r="D18" s="133"/>
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="112" t="s">
@@ -5610,28 +5626,28 @@
       <c r="A21" s="6"/>
     </row>
     <row r="22" spans="1:22">
-      <c r="A22" s="146" t="s">
+      <c r="A22" s="169" t="s">
         <v>186</v>
       </c>
-      <c r="B22" s="146"/>
-      <c r="C22" s="146"/>
-      <c r="D22" s="146"/>
-      <c r="E22" s="146"/>
-      <c r="F22" s="146"/>
-      <c r="G22" s="146"/>
+      <c r="B22" s="169"/>
+      <c r="C22" s="169"/>
+      <c r="D22" s="169"/>
+      <c r="E22" s="169"/>
+      <c r="F22" s="169"/>
+      <c r="G22" s="169"/>
     </row>
     <row r="23" spans="1:22">
       <c r="A23" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="140" t="s">
+      <c r="B23" s="163" t="s">
         <v>177</v>
       </c>
-      <c r="C23" s="141"/>
-      <c r="D23" s="141"/>
-      <c r="E23" s="141"/>
-      <c r="F23" s="141"/>
-      <c r="G23" s="142"/>
+      <c r="C23" s="164"/>
+      <c r="D23" s="164"/>
+      <c r="E23" s="164"/>
+      <c r="F23" s="164"/>
+      <c r="G23" s="165"/>
       <c r="H23" s="95"/>
       <c r="I23" s="95"/>
       <c r="J23" s="95"/>
@@ -5649,12 +5665,12 @@
     </row>
     <row r="24" spans="1:22">
       <c r="A24" s="106"/>
-      <c r="B24" s="157"/>
-      <c r="C24" s="157"/>
-      <c r="D24" s="157"/>
-      <c r="E24" s="157"/>
-      <c r="F24" s="157"/>
-      <c r="G24" s="157"/>
+      <c r="B24" s="148"/>
+      <c r="C24" s="148"/>
+      <c r="D24" s="148"/>
+      <c r="E24" s="148"/>
+      <c r="F24" s="148"/>
+      <c r="G24" s="148"/>
       <c r="H24" s="102"/>
       <c r="I24" s="102"/>
       <c r="J24" s="102"/>
@@ -5672,12 +5688,12 @@
     </row>
     <row r="25" spans="1:22">
       <c r="A25" s="107"/>
-      <c r="B25" s="158"/>
-      <c r="C25" s="158"/>
-      <c r="D25" s="158"/>
-      <c r="E25" s="158"/>
-      <c r="F25" s="158"/>
-      <c r="G25" s="158"/>
+      <c r="B25" s="150"/>
+      <c r="C25" s="150"/>
+      <c r="D25" s="150"/>
+      <c r="E25" s="150"/>
+      <c r="F25" s="150"/>
+      <c r="G25" s="150"/>
       <c r="H25" s="102"/>
       <c r="I25" s="102"/>
       <c r="J25" s="102"/>
@@ -5695,12 +5711,12 @@
     </row>
     <row r="26" spans="1:22">
       <c r="A26" s="108"/>
-      <c r="B26" s="159"/>
-      <c r="C26" s="159"/>
-      <c r="D26" s="159"/>
-      <c r="E26" s="159"/>
-      <c r="F26" s="159"/>
-      <c r="G26" s="159"/>
+      <c r="B26" s="152"/>
+      <c r="C26" s="152"/>
+      <c r="D26" s="152"/>
+      <c r="E26" s="152"/>
+      <c r="F26" s="152"/>
+      <c r="G26" s="152"/>
       <c r="H26" s="102"/>
       <c r="I26" s="102"/>
       <c r="J26" s="102"/>
@@ -5720,28 +5736,28 @@
       <c r="C27"/>
     </row>
     <row r="28" spans="1:22">
-      <c r="A28" s="143" t="s">
+      <c r="A28" s="166" t="s">
         <v>187</v>
       </c>
-      <c r="B28" s="144"/>
-      <c r="C28" s="144"/>
-      <c r="D28" s="144"/>
-      <c r="E28" s="144"/>
-      <c r="F28" s="144"/>
-      <c r="G28" s="145"/>
+      <c r="B28" s="167"/>
+      <c r="C28" s="167"/>
+      <c r="D28" s="167"/>
+      <c r="E28" s="167"/>
+      <c r="F28" s="167"/>
+      <c r="G28" s="168"/>
     </row>
     <row r="29" spans="1:22">
       <c r="A29" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="164" t="s">
+      <c r="B29" s="144" t="s">
         <v>178</v>
       </c>
-      <c r="C29" s="164"/>
-      <c r="D29" s="164"/>
-      <c r="E29" s="164"/>
-      <c r="F29" s="164"/>
-      <c r="G29" s="164"/>
+      <c r="C29" s="144"/>
+      <c r="D29" s="144"/>
+      <c r="E29" s="144"/>
+      <c r="F29" s="144"/>
+      <c r="G29" s="144"/>
       <c r="H29" s="95"/>
       <c r="I29" s="95"/>
       <c r="J29" s="95"/>
@@ -5761,14 +5777,14 @@
       <c r="A30" s="106">
         <v>1</v>
       </c>
-      <c r="B30" s="165" t="s">
+      <c r="B30" s="145" t="s">
         <v>179</v>
       </c>
-      <c r="C30" s="165"/>
-      <c r="D30" s="165"/>
-      <c r="E30" s="165"/>
-      <c r="F30" s="165"/>
-      <c r="G30" s="165"/>
+      <c r="C30" s="145"/>
+      <c r="D30" s="145"/>
+      <c r="E30" s="145"/>
+      <c r="F30" s="145"/>
+      <c r="G30" s="145"/>
       <c r="H30" s="102"/>
       <c r="I30" s="102"/>
       <c r="J30" s="102"/>
@@ -5786,12 +5802,12 @@
     </row>
     <row r="31" spans="1:22">
       <c r="A31" s="107"/>
-      <c r="B31" s="166"/>
-      <c r="C31" s="166"/>
-      <c r="D31" s="166"/>
-      <c r="E31" s="166"/>
-      <c r="F31" s="166"/>
-      <c r="G31" s="166"/>
+      <c r="B31" s="146"/>
+      <c r="C31" s="146"/>
+      <c r="D31" s="146"/>
+      <c r="E31" s="146"/>
+      <c r="F31" s="146"/>
+      <c r="G31" s="146"/>
       <c r="H31" s="102"/>
       <c r="I31" s="102"/>
       <c r="J31" s="102"/>
@@ -5809,12 +5825,12 @@
     </row>
     <row r="32" spans="1:22">
       <c r="A32" s="108"/>
-      <c r="B32" s="167"/>
-      <c r="C32" s="167"/>
-      <c r="D32" s="167"/>
-      <c r="E32" s="167"/>
-      <c r="F32" s="167"/>
-      <c r="G32" s="167"/>
+      <c r="B32" s="147"/>
+      <c r="C32" s="147"/>
+      <c r="D32" s="147"/>
+      <c r="E32" s="147"/>
+      <c r="F32" s="147"/>
+      <c r="G32" s="147"/>
       <c r="H32" s="102"/>
       <c r="I32" s="102"/>
       <c r="J32" s="102"/>
@@ -5853,28 +5869,28 @@
       <c r="T33"/>
     </row>
     <row r="34" spans="1:22">
-      <c r="A34" s="143" t="s">
+      <c r="A34" s="166" t="s">
         <v>188</v>
       </c>
-      <c r="B34" s="144"/>
-      <c r="C34" s="144"/>
-      <c r="D34" s="144"/>
-      <c r="E34" s="144"/>
-      <c r="F34" s="144"/>
-      <c r="G34" s="145"/>
+      <c r="B34" s="167"/>
+      <c r="C34" s="167"/>
+      <c r="D34" s="167"/>
+      <c r="E34" s="167"/>
+      <c r="F34" s="167"/>
+      <c r="G34" s="168"/>
     </row>
     <row r="35" spans="1:22">
       <c r="A35" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="164" t="s">
+      <c r="B35" s="144" t="s">
         <v>180</v>
       </c>
-      <c r="C35" s="164"/>
-      <c r="D35" s="164"/>
-      <c r="E35" s="164"/>
-      <c r="F35" s="164"/>
-      <c r="G35" s="164"/>
+      <c r="C35" s="144"/>
+      <c r="D35" s="144"/>
+      <c r="E35" s="144"/>
+      <c r="F35" s="144"/>
+      <c r="G35" s="144"/>
       <c r="H35" s="95"/>
       <c r="I35" s="95"/>
       <c r="J35" s="95"/>
@@ -5892,12 +5908,12 @@
     </row>
     <row r="36" spans="1:22">
       <c r="A36" s="106"/>
-      <c r="B36" s="157"/>
-      <c r="C36" s="157"/>
-      <c r="D36" s="157"/>
-      <c r="E36" s="157"/>
-      <c r="F36" s="157"/>
-      <c r="G36" s="168"/>
+      <c r="B36" s="148"/>
+      <c r="C36" s="148"/>
+      <c r="D36" s="148"/>
+      <c r="E36" s="148"/>
+      <c r="F36" s="148"/>
+      <c r="G36" s="149"/>
       <c r="H36" s="102"/>
       <c r="I36" s="102"/>
       <c r="J36" s="102"/>
@@ -5915,12 +5931,12 @@
     </row>
     <row r="37" spans="1:22">
       <c r="A37" s="107"/>
-      <c r="B37" s="158"/>
-      <c r="C37" s="158"/>
-      <c r="D37" s="158"/>
-      <c r="E37" s="158"/>
-      <c r="F37" s="158"/>
-      <c r="G37" s="169"/>
+      <c r="B37" s="150"/>
+      <c r="C37" s="150"/>
+      <c r="D37" s="150"/>
+      <c r="E37" s="150"/>
+      <c r="F37" s="150"/>
+      <c r="G37" s="151"/>
       <c r="H37" s="102"/>
       <c r="I37" s="102"/>
       <c r="J37" s="102"/>
@@ -5938,12 +5954,12 @@
     </row>
     <row r="38" spans="1:22">
       <c r="A38" s="108"/>
-      <c r="B38" s="159"/>
-      <c r="C38" s="159"/>
-      <c r="D38" s="159"/>
-      <c r="E38" s="159"/>
-      <c r="F38" s="159"/>
-      <c r="G38" s="170"/>
+      <c r="B38" s="152"/>
+      <c r="C38" s="152"/>
+      <c r="D38" s="152"/>
+      <c r="E38" s="152"/>
+      <c r="F38" s="152"/>
+      <c r="G38" s="153"/>
       <c r="H38" s="102"/>
       <c r="I38" s="102"/>
       <c r="J38" s="102"/>
@@ -6019,16 +6035,16 @@
       <c r="B42" s="176" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="178" t="s">
+      <c r="C42" s="182" t="s">
         <v>1</v>
       </c>
       <c r="D42" s="176" t="s">
         <v>2</v>
       </c>
-      <c r="E42" s="181" t="s">
+      <c r="E42" s="180" t="s">
         <v>156</v>
       </c>
-      <c r="F42" s="181" t="s">
+      <c r="F42" s="180" t="s">
         <v>171</v>
       </c>
       <c r="G42" s="176" t="s">
@@ -6040,13 +6056,13 @@
       <c r="I42" s="176" t="s">
         <v>237</v>
       </c>
-      <c r="J42" s="181" t="s">
+      <c r="J42" s="180" t="s">
         <v>238</v>
       </c>
-      <c r="K42" s="181" t="s">
+      <c r="K42" s="180" t="s">
         <v>208</v>
       </c>
-      <c r="L42" s="189" t="s">
+      <c r="L42" s="179" t="s">
         <v>225</v>
       </c>
       <c r="M42" s="176" t="s">
@@ -6058,14 +6074,14 @@
       <c r="O42" s="176" t="s">
         <v>190</v>
       </c>
-      <c r="P42" s="179" t="s">
+      <c r="P42" s="183" t="s">
         <v>70</v>
       </c>
-      <c r="Q42" s="180"/>
-      <c r="R42" s="179" t="s">
+      <c r="Q42" s="184"/>
+      <c r="R42" s="183" t="s">
         <v>16</v>
       </c>
-      <c r="S42" s="180"/>
+      <c r="S42" s="184"/>
       <c r="T42" s="32" t="s">
         <v>69</v>
       </c>
@@ -6074,21 +6090,21 @@
       </c>
     </row>
     <row r="43" spans="1:22">
-      <c r="A43" s="177"/>
-      <c r="B43" s="177"/>
-      <c r="C43" s="177"/>
-      <c r="D43" s="177"/>
-      <c r="E43" s="182"/>
-      <c r="F43" s="182"/>
-      <c r="G43" s="177"/>
-      <c r="H43" s="177"/>
-      <c r="I43" s="177"/>
-      <c r="J43" s="182"/>
-      <c r="K43" s="182"/>
-      <c r="L43" s="183"/>
-      <c r="M43" s="177"/>
-      <c r="N43" s="177"/>
-      <c r="O43" s="183"/>
+      <c r="A43" s="178"/>
+      <c r="B43" s="178"/>
+      <c r="C43" s="178"/>
+      <c r="D43" s="178"/>
+      <c r="E43" s="181"/>
+      <c r="F43" s="181"/>
+      <c r="G43" s="178"/>
+      <c r="H43" s="178"/>
+      <c r="I43" s="178"/>
+      <c r="J43" s="181"/>
+      <c r="K43" s="181"/>
+      <c r="L43" s="177"/>
+      <c r="M43" s="178"/>
+      <c r="N43" s="178"/>
+      <c r="O43" s="177"/>
       <c r="P43" s="27" t="s">
         <v>74</v>
       </c>
@@ -6104,7 +6120,7 @@
       <c r="T43" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="U43" s="177"/>
+      <c r="U43" s="178"/>
     </row>
     <row r="44" spans="1:22">
       <c r="A44" s="7">
@@ -6124,7 +6140,9 @@
       <c r="G44" s="75" t="s">
         <v>137</v>
       </c>
-      <c r="H44" s="23"/>
+      <c r="H44" s="23" t="s">
+        <v>240</v>
+      </c>
       <c r="I44" s="23"/>
       <c r="J44" s="23"/>
       <c r="K44" s="23"/>
@@ -6166,7 +6184,9 @@
       <c r="E45" s="24"/>
       <c r="F45" s="24"/>
       <c r="G45" s="76"/>
-      <c r="H45" s="24"/>
+      <c r="H45" s="24">
+        <v>0</v>
+      </c>
       <c r="I45" s="24"/>
       <c r="J45" s="24"/>
       <c r="K45" s="24"/>
@@ -6240,7 +6260,9 @@
       </c>
       <c r="F47" s="73"/>
       <c r="G47" s="78"/>
-      <c r="H47" s="73"/>
+      <c r="H47" s="73" t="s">
+        <v>241</v>
+      </c>
       <c r="I47" s="23" t="s">
         <v>239</v>
       </c>
@@ -6278,7 +6300,9 @@
       </c>
       <c r="F48" s="25"/>
       <c r="G48" s="77"/>
-      <c r="H48" s="25"/>
+      <c r="H48" s="25" t="s">
+        <v>241</v>
+      </c>
       <c r="I48" s="25"/>
       <c r="J48" s="25"/>
       <c r="K48" s="25"/>
@@ -6310,7 +6334,9 @@
       <c r="E49" s="25"/>
       <c r="F49" s="25"/>
       <c r="G49" s="77"/>
-      <c r="H49" s="25"/>
+      <c r="H49" s="25" t="s">
+        <v>243</v>
+      </c>
       <c r="I49" s="25"/>
       <c r="J49" s="25"/>
       <c r="K49" s="25"/>
@@ -6340,7 +6366,9 @@
       <c r="E50" s="25"/>
       <c r="F50" s="25"/>
       <c r="G50" s="77"/>
-      <c r="H50" s="25"/>
+      <c r="H50" s="25" t="s">
+        <v>242</v>
+      </c>
       <c r="I50" s="25"/>
       <c r="J50" s="25"/>
       <c r="K50" s="25"/>
@@ -6748,26 +6776,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="O42:O43"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="A34:G34"/>
-    <mergeCell ref="M42:M43"/>
-    <mergeCell ref="H42:H43"/>
-    <mergeCell ref="L42:L43"/>
-    <mergeCell ref="K42:K43"/>
-    <mergeCell ref="I42:I43"/>
-    <mergeCell ref="J42:J43"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="A22:G22"/>
@@ -6784,6 +6792,26 @@
     <mergeCell ref="F42:F43"/>
     <mergeCell ref="B23:G23"/>
     <mergeCell ref="B24:G24"/>
+    <mergeCell ref="O42:O43"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="M42:M43"/>
+    <mergeCell ref="H42:H43"/>
+    <mergeCell ref="L42:L43"/>
+    <mergeCell ref="K42:K43"/>
+    <mergeCell ref="I42:I43"/>
+    <mergeCell ref="J42:J43"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="B35:G35"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="4">
@@ -6976,10 +7004,10 @@
         <v>168</v>
       </c>
       <c r="B13" s="111"/>
-      <c r="C13" s="151" t="s">
+      <c r="C13" s="133" t="s">
         <v>169</v>
       </c>
-      <c r="D13" s="151"/>
+      <c r="D13" s="133"/>
       <c r="E13" s="1" t="s">
         <v>170</v>
       </c>
@@ -6989,10 +7017,10 @@
         <v>171</v>
       </c>
       <c r="B14" s="111"/>
-      <c r="C14" s="151" t="s">
+      <c r="C14" s="133" t="s">
         <v>172</v>
       </c>
-      <c r="D14" s="151"/>
+      <c r="D14" s="133"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="112" t="s">
@@ -7018,28 +7046,28 @@
       <c r="A16" s="6"/>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="146" t="s">
+      <c r="A17" s="169" t="s">
         <v>186</v>
       </c>
-      <c r="B17" s="146"/>
-      <c r="C17" s="146"/>
-      <c r="D17" s="146"/>
-      <c r="E17" s="146"/>
-      <c r="F17" s="146"/>
-      <c r="G17" s="146"/>
+      <c r="B17" s="169"/>
+      <c r="C17" s="169"/>
+      <c r="D17" s="169"/>
+      <c r="E17" s="169"/>
+      <c r="F17" s="169"/>
+      <c r="G17" s="169"/>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="140" t="s">
+      <c r="B18" s="163" t="s">
         <v>177</v>
       </c>
-      <c r="C18" s="141"/>
-      <c r="D18" s="141"/>
-      <c r="E18" s="141"/>
-      <c r="F18" s="141"/>
-      <c r="G18" s="142"/>
+      <c r="C18" s="164"/>
+      <c r="D18" s="164"/>
+      <c r="E18" s="164"/>
+      <c r="F18" s="164"/>
+      <c r="G18" s="165"/>
       <c r="H18" s="95"/>
       <c r="I18" s="95"/>
       <c r="K18" s="95"/>
@@ -7051,12 +7079,12 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="106"/>
-      <c r="B19" s="157"/>
-      <c r="C19" s="157"/>
-      <c r="D19" s="157"/>
-      <c r="E19" s="157"/>
-      <c r="F19" s="157"/>
-      <c r="G19" s="157"/>
+      <c r="B19" s="148"/>
+      <c r="C19" s="148"/>
+      <c r="D19" s="148"/>
+      <c r="E19" s="148"/>
+      <c r="F19" s="148"/>
+      <c r="G19" s="148"/>
       <c r="H19" s="102"/>
       <c r="I19" s="102"/>
       <c r="K19" s="102"/>
@@ -7068,12 +7096,12 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="107"/>
-      <c r="B20" s="158"/>
-      <c r="C20" s="158"/>
-      <c r="D20" s="158"/>
-      <c r="E20" s="158"/>
-      <c r="F20" s="158"/>
-      <c r="G20" s="158"/>
+      <c r="B20" s="150"/>
+      <c r="C20" s="150"/>
+      <c r="D20" s="150"/>
+      <c r="E20" s="150"/>
+      <c r="F20" s="150"/>
+      <c r="G20" s="150"/>
       <c r="H20" s="102"/>
       <c r="I20" s="102"/>
       <c r="K20" s="102"/>
@@ -7085,12 +7113,12 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="108"/>
-      <c r="B21" s="159"/>
-      <c r="C21" s="159"/>
-      <c r="D21" s="159"/>
-      <c r="E21" s="159"/>
-      <c r="F21" s="159"/>
-      <c r="G21" s="159"/>
+      <c r="B21" s="152"/>
+      <c r="C21" s="152"/>
+      <c r="D21" s="152"/>
+      <c r="E21" s="152"/>
+      <c r="F21" s="152"/>
+      <c r="G21" s="152"/>
       <c r="H21" s="102"/>
       <c r="I21" s="102"/>
       <c r="J21" s="95"/>
@@ -7106,29 +7134,29 @@
       <c r="J22" s="102"/>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="143" t="s">
+      <c r="A23" s="166" t="s">
         <v>187</v>
       </c>
-      <c r="B23" s="144"/>
-      <c r="C23" s="144"/>
-      <c r="D23" s="144"/>
-      <c r="E23" s="144"/>
-      <c r="F23" s="144"/>
-      <c r="G23" s="145"/>
+      <c r="B23" s="167"/>
+      <c r="C23" s="167"/>
+      <c r="D23" s="167"/>
+      <c r="E23" s="167"/>
+      <c r="F23" s="167"/>
+      <c r="G23" s="168"/>
       <c r="J23" s="102"/>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="164" t="s">
+      <c r="B24" s="144" t="s">
         <v>178</v>
       </c>
-      <c r="C24" s="164"/>
-      <c r="D24" s="164"/>
-      <c r="E24" s="164"/>
-      <c r="F24" s="164"/>
-      <c r="G24" s="164"/>
+      <c r="C24" s="144"/>
+      <c r="D24" s="144"/>
+      <c r="E24" s="144"/>
+      <c r="F24" s="144"/>
+      <c r="G24" s="144"/>
       <c r="H24" s="95"/>
       <c r="I24" s="95"/>
       <c r="J24" s="102"/>
@@ -7143,14 +7171,14 @@
       <c r="A25" s="106">
         <v>1</v>
       </c>
-      <c r="B25" s="165" t="s">
+      <c r="B25" s="145" t="s">
         <v>179</v>
       </c>
-      <c r="C25" s="165"/>
-      <c r="D25" s="165"/>
-      <c r="E25" s="165"/>
-      <c r="F25" s="165"/>
-      <c r="G25" s="165"/>
+      <c r="C25" s="145"/>
+      <c r="D25" s="145"/>
+      <c r="E25" s="145"/>
+      <c r="F25" s="145"/>
+      <c r="G25" s="145"/>
       <c r="H25" s="102"/>
       <c r="I25" s="102"/>
       <c r="K25" s="102"/>
@@ -7162,12 +7190,12 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="107"/>
-      <c r="B26" s="166"/>
-      <c r="C26" s="166"/>
-      <c r="D26" s="166"/>
-      <c r="E26" s="166"/>
-      <c r="F26" s="166"/>
-      <c r="G26" s="166"/>
+      <c r="B26" s="146"/>
+      <c r="C26" s="146"/>
+      <c r="D26" s="146"/>
+      <c r="E26" s="146"/>
+      <c r="F26" s="146"/>
+      <c r="G26" s="146"/>
       <c r="H26" s="102"/>
       <c r="I26" s="102"/>
       <c r="K26" s="102"/>
@@ -7179,12 +7207,12 @@
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="108"/>
-      <c r="B27" s="167"/>
-      <c r="C27" s="167"/>
-      <c r="D27" s="167"/>
-      <c r="E27" s="167"/>
-      <c r="F27" s="167"/>
-      <c r="G27" s="167"/>
+      <c r="B27" s="147"/>
+      <c r="C27" s="147"/>
+      <c r="D27" s="147"/>
+      <c r="E27" s="147"/>
+      <c r="F27" s="147"/>
+      <c r="G27" s="147"/>
       <c r="H27" s="102"/>
       <c r="I27" s="102"/>
       <c r="J27" s="95"/>
@@ -7213,29 +7241,29 @@
       <c r="O28"/>
     </row>
     <row r="29" spans="1:17">
-      <c r="A29" s="143" t="s">
+      <c r="A29" s="166" t="s">
         <v>188</v>
       </c>
-      <c r="B29" s="144"/>
-      <c r="C29" s="144"/>
-      <c r="D29" s="144"/>
-      <c r="E29" s="144"/>
-      <c r="F29" s="144"/>
-      <c r="G29" s="145"/>
+      <c r="B29" s="167"/>
+      <c r="C29" s="167"/>
+      <c r="D29" s="167"/>
+      <c r="E29" s="167"/>
+      <c r="F29" s="167"/>
+      <c r="G29" s="168"/>
       <c r="J29" s="102"/>
     </row>
     <row r="30" spans="1:17">
       <c r="A30" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B30" s="164" t="s">
+      <c r="B30" s="144" t="s">
         <v>180</v>
       </c>
-      <c r="C30" s="164"/>
-      <c r="D30" s="164"/>
-      <c r="E30" s="164"/>
-      <c r="F30" s="164"/>
-      <c r="G30" s="164"/>
+      <c r="C30" s="144"/>
+      <c r="D30" s="144"/>
+      <c r="E30" s="144"/>
+      <c r="F30" s="144"/>
+      <c r="G30" s="144"/>
       <c r="H30" s="95"/>
       <c r="I30" s="95"/>
       <c r="J30" s="102"/>
@@ -7248,12 +7276,12 @@
     </row>
     <row r="31" spans="1:17">
       <c r="A31" s="106"/>
-      <c r="B31" s="157"/>
-      <c r="C31" s="157"/>
-      <c r="D31" s="157"/>
-      <c r="E31" s="157"/>
-      <c r="F31" s="157"/>
-      <c r="G31" s="168"/>
+      <c r="B31" s="148"/>
+      <c r="C31" s="148"/>
+      <c r="D31" s="148"/>
+      <c r="E31" s="148"/>
+      <c r="F31" s="148"/>
+      <c r="G31" s="149"/>
       <c r="H31" s="102"/>
       <c r="I31" s="102"/>
       <c r="J31"/>
@@ -7266,12 +7294,12 @@
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="107"/>
-      <c r="B32" s="158"/>
-      <c r="C32" s="158"/>
-      <c r="D32" s="158"/>
-      <c r="E32" s="158"/>
-      <c r="F32" s="158"/>
-      <c r="G32" s="169"/>
+      <c r="B32" s="150"/>
+      <c r="C32" s="150"/>
+      <c r="D32" s="150"/>
+      <c r="E32" s="150"/>
+      <c r="F32" s="150"/>
+      <c r="G32" s="151"/>
       <c r="H32" s="102"/>
       <c r="I32" s="102"/>
       <c r="K32" s="102"/>
@@ -7283,12 +7311,12 @@
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="108"/>
-      <c r="B33" s="159"/>
-      <c r="C33" s="159"/>
-      <c r="D33" s="159"/>
-      <c r="E33" s="159"/>
-      <c r="F33" s="159"/>
-      <c r="G33" s="170"/>
+      <c r="B33" s="152"/>
+      <c r="C33" s="152"/>
+      <c r="D33" s="152"/>
+      <c r="E33" s="152"/>
+      <c r="F33" s="152"/>
+      <c r="G33" s="153"/>
       <c r="H33" s="102"/>
       <c r="I33" s="102"/>
       <c r="J33" s="95"/>
@@ -7341,31 +7369,31 @@
       <c r="P36" s="49"/>
     </row>
     <row r="37" spans="1:17" ht="15">
-      <c r="A37" s="181" t="s">
+      <c r="A37" s="180" t="s">
         <v>115</v>
       </c>
-      <c r="B37" s="181" t="s">
+      <c r="B37" s="180" t="s">
         <v>116</v>
       </c>
       <c r="C37" s="51" t="s">
         <v>117</v>
       </c>
-      <c r="D37" s="181" t="s">
+      <c r="D37" s="180" t="s">
         <v>99</v>
       </c>
-      <c r="E37" s="181" t="s">
+      <c r="E37" s="180" t="s">
         <v>156</v>
       </c>
-      <c r="F37" s="181" t="s">
+      <c r="F37" s="180" t="s">
         <v>171</v>
       </c>
-      <c r="G37" s="181" t="s">
+      <c r="G37" s="180" t="s">
         <v>136</v>
       </c>
-      <c r="H37" s="181" t="s">
+      <c r="H37" s="180" t="s">
         <v>113</v>
       </c>
-      <c r="I37" s="181" t="s">
+      <c r="I37" s="180" t="s">
         <v>230</v>
       </c>
       <c r="J37" s="176" t="s">
@@ -7382,23 +7410,23 @@
       <c r="O37" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="P37" s="181" t="s">
+      <c r="P37" s="180" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="15">
-      <c r="A38" s="184"/>
-      <c r="B38" s="184"/>
+      <c r="A38" s="188"/>
+      <c r="B38" s="188"/>
       <c r="C38" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="D38" s="184"/>
-      <c r="E38" s="182"/>
-      <c r="F38" s="182"/>
-      <c r="G38" s="184"/>
-      <c r="H38" s="184"/>
-      <c r="I38" s="184"/>
-      <c r="J38" s="183"/>
+      <c r="D38" s="188"/>
+      <c r="E38" s="181"/>
+      <c r="F38" s="181"/>
+      <c r="G38" s="188"/>
+      <c r="H38" s="188"/>
+      <c r="I38" s="188"/>
+      <c r="J38" s="177"/>
       <c r="K38" s="53" t="s">
         <v>123</v>
       </c>
@@ -7414,7 +7442,7 @@
       <c r="O38" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="P38" s="184"/>
+      <c r="P38" s="188"/>
     </row>
     <row r="39" spans="1:17">
       <c r="A39" s="55">
@@ -7912,6 +7940,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="P37:P38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="H37:H38"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="J37:J38"/>
@@ -7928,19 +7969,6 @@
     <mergeCell ref="A17:G17"/>
     <mergeCell ref="B18:G18"/>
     <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="P37:P38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">
@@ -8150,10 +8178,10 @@
         <v>168</v>
       </c>
       <c r="B15" s="111"/>
-      <c r="C15" s="151" t="s">
+      <c r="C15" s="133" t="s">
         <v>169</v>
       </c>
-      <c r="D15" s="151"/>
+      <c r="D15" s="133"/>
       <c r="E15" s="1" t="s">
         <v>170</v>
       </c>
@@ -8163,10 +8191,10 @@
         <v>171</v>
       </c>
       <c r="B16" s="111"/>
-      <c r="C16" s="151" t="s">
+      <c r="C16" s="133" t="s">
         <v>172</v>
       </c>
-      <c r="D16" s="151"/>
+      <c r="D16" s="133"/>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="112" t="s">
@@ -8192,28 +8220,28 @@
       <c r="A18" s="6"/>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="146" t="s">
+      <c r="A19" s="169" t="s">
         <v>186</v>
       </c>
-      <c r="B19" s="146"/>
-      <c r="C19" s="146"/>
-      <c r="D19" s="146"/>
-      <c r="E19" s="146"/>
-      <c r="F19" s="146"/>
-      <c r="G19" s="146"/>
+      <c r="B19" s="169"/>
+      <c r="C19" s="169"/>
+      <c r="D19" s="169"/>
+      <c r="E19" s="169"/>
+      <c r="F19" s="169"/>
+      <c r="G19" s="169"/>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B20" s="140" t="s">
+      <c r="B20" s="163" t="s">
         <v>177</v>
       </c>
-      <c r="C20" s="141"/>
-      <c r="D20" s="141"/>
-      <c r="E20" s="141"/>
-      <c r="F20" s="141"/>
-      <c r="G20" s="142"/>
+      <c r="C20" s="164"/>
+      <c r="D20" s="164"/>
+      <c r="E20" s="164"/>
+      <c r="F20" s="164"/>
+      <c r="G20" s="165"/>
       <c r="H20" s="95"/>
       <c r="I20" s="95"/>
       <c r="K20" s="95"/>
@@ -8225,12 +8253,12 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="106"/>
-      <c r="B21" s="157"/>
-      <c r="C21" s="157"/>
-      <c r="D21" s="157"/>
-      <c r="E21" s="157"/>
-      <c r="F21" s="157"/>
-      <c r="G21" s="157"/>
+      <c r="B21" s="148"/>
+      <c r="C21" s="148"/>
+      <c r="D21" s="148"/>
+      <c r="E21" s="148"/>
+      <c r="F21" s="148"/>
+      <c r="G21" s="148"/>
       <c r="H21" s="102"/>
       <c r="I21" s="102"/>
       <c r="K21" s="102"/>
@@ -8242,12 +8270,12 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="107"/>
-      <c r="B22" s="158"/>
-      <c r="C22" s="158"/>
-      <c r="D22" s="158"/>
-      <c r="E22" s="158"/>
-      <c r="F22" s="158"/>
-      <c r="G22" s="158"/>
+      <c r="B22" s="150"/>
+      <c r="C22" s="150"/>
+      <c r="D22" s="150"/>
+      <c r="E22" s="150"/>
+      <c r="F22" s="150"/>
+      <c r="G22" s="150"/>
       <c r="H22" s="102"/>
       <c r="I22" s="102"/>
       <c r="K22" s="102"/>
@@ -8259,12 +8287,12 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="108"/>
-      <c r="B23" s="159"/>
-      <c r="C23" s="159"/>
-      <c r="D23" s="159"/>
-      <c r="E23" s="159"/>
-      <c r="F23" s="159"/>
-      <c r="G23" s="159"/>
+      <c r="B23" s="152"/>
+      <c r="C23" s="152"/>
+      <c r="D23" s="152"/>
+      <c r="E23" s="152"/>
+      <c r="F23" s="152"/>
+      <c r="G23" s="152"/>
       <c r="H23" s="102"/>
       <c r="I23" s="102"/>
       <c r="J23" s="95"/>
@@ -8280,29 +8308,29 @@
       <c r="J24" s="102"/>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" s="143" t="s">
+      <c r="A25" s="166" t="s">
         <v>187</v>
       </c>
-      <c r="B25" s="144"/>
-      <c r="C25" s="144"/>
-      <c r="D25" s="144"/>
-      <c r="E25" s="144"/>
-      <c r="F25" s="144"/>
-      <c r="G25" s="145"/>
+      <c r="B25" s="167"/>
+      <c r="C25" s="167"/>
+      <c r="D25" s="167"/>
+      <c r="E25" s="167"/>
+      <c r="F25" s="167"/>
+      <c r="G25" s="168"/>
       <c r="J25" s="102"/>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="164" t="s">
+      <c r="B26" s="144" t="s">
         <v>178</v>
       </c>
-      <c r="C26" s="164"/>
-      <c r="D26" s="164"/>
-      <c r="E26" s="164"/>
-      <c r="F26" s="164"/>
-      <c r="G26" s="164"/>
+      <c r="C26" s="144"/>
+      <c r="D26" s="144"/>
+      <c r="E26" s="144"/>
+      <c r="F26" s="144"/>
+      <c r="G26" s="144"/>
       <c r="H26" s="95"/>
       <c r="I26" s="95"/>
       <c r="J26" s="102"/>
@@ -8317,14 +8345,14 @@
       <c r="A27" s="106">
         <v>1</v>
       </c>
-      <c r="B27" s="165" t="s">
+      <c r="B27" s="145" t="s">
         <v>179</v>
       </c>
-      <c r="C27" s="165"/>
-      <c r="D27" s="165"/>
-      <c r="E27" s="165"/>
-      <c r="F27" s="165"/>
-      <c r="G27" s="165"/>
+      <c r="C27" s="145"/>
+      <c r="D27" s="145"/>
+      <c r="E27" s="145"/>
+      <c r="F27" s="145"/>
+      <c r="G27" s="145"/>
       <c r="H27" s="102"/>
       <c r="I27" s="102"/>
       <c r="K27" s="102"/>
@@ -8336,12 +8364,12 @@
     </row>
     <row r="28" spans="1:17">
       <c r="A28" s="107"/>
-      <c r="B28" s="166"/>
-      <c r="C28" s="166"/>
-      <c r="D28" s="166"/>
-      <c r="E28" s="166"/>
-      <c r="F28" s="166"/>
-      <c r="G28" s="166"/>
+      <c r="B28" s="146"/>
+      <c r="C28" s="146"/>
+      <c r="D28" s="146"/>
+      <c r="E28" s="146"/>
+      <c r="F28" s="146"/>
+      <c r="G28" s="146"/>
       <c r="H28" s="102"/>
       <c r="I28" s="102"/>
       <c r="K28" s="102"/>
@@ -8353,12 +8381,12 @@
     </row>
     <row r="29" spans="1:17">
       <c r="A29" s="108"/>
-      <c r="B29" s="167"/>
-      <c r="C29" s="167"/>
-      <c r="D29" s="167"/>
-      <c r="E29" s="167"/>
-      <c r="F29" s="167"/>
-      <c r="G29" s="167"/>
+      <c r="B29" s="147"/>
+      <c r="C29" s="147"/>
+      <c r="D29" s="147"/>
+      <c r="E29" s="147"/>
+      <c r="F29" s="147"/>
+      <c r="G29" s="147"/>
       <c r="H29" s="102"/>
       <c r="I29" s="102"/>
       <c r="J29" s="95"/>
@@ -8387,29 +8415,29 @@
       <c r="O30"/>
     </row>
     <row r="31" spans="1:17">
-      <c r="A31" s="143" t="s">
+      <c r="A31" s="166" t="s">
         <v>188</v>
       </c>
-      <c r="B31" s="144"/>
-      <c r="C31" s="144"/>
-      <c r="D31" s="144"/>
-      <c r="E31" s="144"/>
-      <c r="F31" s="144"/>
-      <c r="G31" s="145"/>
+      <c r="B31" s="167"/>
+      <c r="C31" s="167"/>
+      <c r="D31" s="167"/>
+      <c r="E31" s="167"/>
+      <c r="F31" s="167"/>
+      <c r="G31" s="168"/>
       <c r="J31" s="102"/>
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="164" t="s">
+      <c r="B32" s="144" t="s">
         <v>180</v>
       </c>
-      <c r="C32" s="164"/>
-      <c r="D32" s="164"/>
-      <c r="E32" s="164"/>
-      <c r="F32" s="164"/>
-      <c r="G32" s="164"/>
+      <c r="C32" s="144"/>
+      <c r="D32" s="144"/>
+      <c r="E32" s="144"/>
+      <c r="F32" s="144"/>
+      <c r="G32" s="144"/>
       <c r="H32" s="95"/>
       <c r="I32" s="95"/>
       <c r="J32" s="102"/>
@@ -8422,12 +8450,12 @@
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="106"/>
-      <c r="B33" s="157"/>
-      <c r="C33" s="157"/>
-      <c r="D33" s="157"/>
-      <c r="E33" s="157"/>
-      <c r="F33" s="157"/>
-      <c r="G33" s="168"/>
+      <c r="B33" s="148"/>
+      <c r="C33" s="148"/>
+      <c r="D33" s="148"/>
+      <c r="E33" s="148"/>
+      <c r="F33" s="148"/>
+      <c r="G33" s="149"/>
       <c r="H33" s="102"/>
       <c r="I33" s="102"/>
       <c r="J33"/>
@@ -8440,12 +8468,12 @@
     </row>
     <row r="34" spans="1:17">
       <c r="A34" s="107"/>
-      <c r="B34" s="158"/>
-      <c r="C34" s="158"/>
-      <c r="D34" s="158"/>
-      <c r="E34" s="158"/>
-      <c r="F34" s="158"/>
-      <c r="G34" s="169"/>
+      <c r="B34" s="150"/>
+      <c r="C34" s="150"/>
+      <c r="D34" s="150"/>
+      <c r="E34" s="150"/>
+      <c r="F34" s="150"/>
+      <c r="G34" s="151"/>
       <c r="H34" s="102"/>
       <c r="I34" s="102"/>
       <c r="K34" s="102"/>
@@ -8457,12 +8485,12 @@
     </row>
     <row r="35" spans="1:17">
       <c r="A35" s="108"/>
-      <c r="B35" s="159"/>
-      <c r="C35" s="159"/>
-      <c r="D35" s="159"/>
-      <c r="E35" s="159"/>
-      <c r="F35" s="159"/>
-      <c r="G35" s="170"/>
+      <c r="B35" s="152"/>
+      <c r="C35" s="152"/>
+      <c r="D35" s="152"/>
+      <c r="E35" s="152"/>
+      <c r="F35" s="152"/>
+      <c r="G35" s="153"/>
       <c r="H35" s="102"/>
       <c r="I35" s="102"/>
       <c r="J35" s="95"/>
@@ -8515,31 +8543,31 @@
       <c r="P38" s="49"/>
     </row>
     <row r="39" spans="1:17" ht="15">
-      <c r="A39" s="181" t="s">
+      <c r="A39" s="180" t="s">
         <v>115</v>
       </c>
-      <c r="B39" s="181" t="s">
+      <c r="B39" s="180" t="s">
         <v>116</v>
       </c>
       <c r="C39" s="51" t="s">
         <v>117</v>
       </c>
-      <c r="D39" s="181" t="s">
+      <c r="D39" s="180" t="s">
         <v>99</v>
       </c>
-      <c r="E39" s="181" t="s">
+      <c r="E39" s="180" t="s">
         <v>156</v>
       </c>
-      <c r="F39" s="181" t="s">
+      <c r="F39" s="180" t="s">
         <v>171</v>
       </c>
-      <c r="G39" s="181" t="s">
+      <c r="G39" s="180" t="s">
         <v>136</v>
       </c>
-      <c r="H39" s="188" t="s">
+      <c r="H39" s="189" t="s">
         <v>113</v>
       </c>
-      <c r="I39" s="188" t="s">
+      <c r="I39" s="189" t="s">
         <v>225</v>
       </c>
       <c r="J39" s="176" t="s">
@@ -8556,23 +8584,23 @@
       <c r="O39" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="P39" s="181" t="s">
+      <c r="P39" s="180" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="15">
-      <c r="A40" s="184"/>
-      <c r="B40" s="184"/>
+      <c r="A40" s="188"/>
+      <c r="B40" s="188"/>
       <c r="C40" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="D40" s="184"/>
-      <c r="E40" s="182"/>
-      <c r="F40" s="182"/>
-      <c r="G40" s="184"/>
-      <c r="H40" s="184"/>
-      <c r="I40" s="184"/>
-      <c r="J40" s="183"/>
+      <c r="D40" s="188"/>
+      <c r="E40" s="181"/>
+      <c r="F40" s="181"/>
+      <c r="G40" s="188"/>
+      <c r="H40" s="188"/>
+      <c r="I40" s="188"/>
+      <c r="J40" s="177"/>
       <c r="K40" s="53" t="s">
         <v>123</v>
       </c>
@@ -8588,7 +8616,7 @@
       <c r="O40" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="P40" s="184"/>
+      <c r="P40" s="188"/>
     </row>
     <row r="41" spans="1:17">
       <c r="A41" s="55">
@@ -9044,19 +9072,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
     <mergeCell ref="P39:P40"/>
     <mergeCell ref="A31:G31"/>
     <mergeCell ref="B32:G32"/>
@@ -9073,6 +9088,19 @@
     <mergeCell ref="J39:J40"/>
     <mergeCell ref="K39:L39"/>
     <mergeCell ref="M39:N39"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">
@@ -9120,8 +9148,8 @@
   </sheetPr>
   <dimension ref="A1:V67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -9281,10 +9309,10 @@
         <v>168</v>
       </c>
       <c r="B16" s="111"/>
-      <c r="C16" s="151" t="s">
+      <c r="C16" s="133" t="s">
         <v>169</v>
       </c>
-      <c r="D16" s="151"/>
+      <c r="D16" s="133"/>
       <c r="E16" s="1" t="s">
         <v>170</v>
       </c>
@@ -9294,20 +9322,20 @@
         <v>171</v>
       </c>
       <c r="B17" s="111"/>
-      <c r="C17" s="151" t="s">
+      <c r="C17" s="133" t="s">
         <v>172</v>
       </c>
-      <c r="D17" s="151"/>
+      <c r="D17" s="133"/>
     </row>
     <row r="18" spans="1:22">
       <c r="A18" s="111" t="s">
         <v>208</v>
       </c>
       <c r="B18" s="111"/>
-      <c r="C18" s="150" t="s">
+      <c r="C18" s="132" t="s">
         <v>210</v>
       </c>
-      <c r="D18" s="151"/>
+      <c r="D18" s="133"/>
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="112" t="s">
@@ -9365,28 +9393,28 @@
       <c r="A21" s="6"/>
     </row>
     <row r="22" spans="1:22">
-      <c r="A22" s="146" t="s">
+      <c r="A22" s="169" t="s">
         <v>186</v>
       </c>
-      <c r="B22" s="146"/>
-      <c r="C22" s="146"/>
-      <c r="D22" s="146"/>
-      <c r="E22" s="146"/>
-      <c r="F22" s="146"/>
-      <c r="G22" s="146"/>
+      <c r="B22" s="169"/>
+      <c r="C22" s="169"/>
+      <c r="D22" s="169"/>
+      <c r="E22" s="169"/>
+      <c r="F22" s="169"/>
+      <c r="G22" s="169"/>
     </row>
     <row r="23" spans="1:22">
       <c r="A23" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="140" t="s">
+      <c r="B23" s="163" t="s">
         <v>177</v>
       </c>
-      <c r="C23" s="141"/>
-      <c r="D23" s="141"/>
-      <c r="E23" s="141"/>
-      <c r="F23" s="141"/>
-      <c r="G23" s="142"/>
+      <c r="C23" s="164"/>
+      <c r="D23" s="164"/>
+      <c r="E23" s="164"/>
+      <c r="F23" s="164"/>
+      <c r="G23" s="165"/>
       <c r="H23" s="95"/>
       <c r="I23" s="95"/>
       <c r="J23" s="95"/>
@@ -9404,12 +9432,12 @@
     </row>
     <row r="24" spans="1:22">
       <c r="A24" s="106"/>
-      <c r="B24" s="157"/>
-      <c r="C24" s="157"/>
-      <c r="D24" s="157"/>
-      <c r="E24" s="157"/>
-      <c r="F24" s="157"/>
-      <c r="G24" s="157"/>
+      <c r="B24" s="148"/>
+      <c r="C24" s="148"/>
+      <c r="D24" s="148"/>
+      <c r="E24" s="148"/>
+      <c r="F24" s="148"/>
+      <c r="G24" s="148"/>
       <c r="H24" s="102"/>
       <c r="I24" s="102"/>
       <c r="J24" s="102"/>
@@ -9427,12 +9455,12 @@
     </row>
     <row r="25" spans="1:22">
       <c r="A25" s="107"/>
-      <c r="B25" s="158"/>
-      <c r="C25" s="158"/>
-      <c r="D25" s="158"/>
-      <c r="E25" s="158"/>
-      <c r="F25" s="158"/>
-      <c r="G25" s="158"/>
+      <c r="B25" s="150"/>
+      <c r="C25" s="150"/>
+      <c r="D25" s="150"/>
+      <c r="E25" s="150"/>
+      <c r="F25" s="150"/>
+      <c r="G25" s="150"/>
       <c r="H25" s="102"/>
       <c r="I25" s="102"/>
       <c r="J25" s="102"/>
@@ -9450,12 +9478,12 @@
     </row>
     <row r="26" spans="1:22">
       <c r="A26" s="108"/>
-      <c r="B26" s="159"/>
-      <c r="C26" s="159"/>
-      <c r="D26" s="159"/>
-      <c r="E26" s="159"/>
-      <c r="F26" s="159"/>
-      <c r="G26" s="159"/>
+      <c r="B26" s="152"/>
+      <c r="C26" s="152"/>
+      <c r="D26" s="152"/>
+      <c r="E26" s="152"/>
+      <c r="F26" s="152"/>
+      <c r="G26" s="152"/>
       <c r="H26" s="102"/>
       <c r="I26" s="102"/>
       <c r="J26" s="102"/>
@@ -9475,28 +9503,28 @@
       <c r="C27"/>
     </row>
     <row r="28" spans="1:22">
-      <c r="A28" s="143" t="s">
+      <c r="A28" s="166" t="s">
         <v>187</v>
       </c>
-      <c r="B28" s="144"/>
-      <c r="C28" s="144"/>
-      <c r="D28" s="144"/>
-      <c r="E28" s="144"/>
-      <c r="F28" s="144"/>
-      <c r="G28" s="145"/>
+      <c r="B28" s="167"/>
+      <c r="C28" s="167"/>
+      <c r="D28" s="167"/>
+      <c r="E28" s="167"/>
+      <c r="F28" s="167"/>
+      <c r="G28" s="168"/>
     </row>
     <row r="29" spans="1:22">
       <c r="A29" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="164" t="s">
+      <c r="B29" s="144" t="s">
         <v>178</v>
       </c>
-      <c r="C29" s="164"/>
-      <c r="D29" s="164"/>
-      <c r="E29" s="164"/>
-      <c r="F29" s="164"/>
-      <c r="G29" s="164"/>
+      <c r="C29" s="144"/>
+      <c r="D29" s="144"/>
+      <c r="E29" s="144"/>
+      <c r="F29" s="144"/>
+      <c r="G29" s="144"/>
       <c r="H29" s="95"/>
       <c r="I29" s="95"/>
       <c r="J29" s="95"/>
@@ -9516,14 +9544,14 @@
       <c r="A30" s="106">
         <v>1</v>
       </c>
-      <c r="B30" s="165" t="s">
+      <c r="B30" s="145" t="s">
         <v>179</v>
       </c>
-      <c r="C30" s="165"/>
-      <c r="D30" s="165"/>
-      <c r="E30" s="165"/>
-      <c r="F30" s="165"/>
-      <c r="G30" s="165"/>
+      <c r="C30" s="145"/>
+      <c r="D30" s="145"/>
+      <c r="E30" s="145"/>
+      <c r="F30" s="145"/>
+      <c r="G30" s="145"/>
       <c r="H30" s="102"/>
       <c r="I30" s="102"/>
       <c r="J30" s="102"/>
@@ -9541,12 +9569,12 @@
     </row>
     <row r="31" spans="1:22">
       <c r="A31" s="107"/>
-      <c r="B31" s="166"/>
-      <c r="C31" s="166"/>
-      <c r="D31" s="166"/>
-      <c r="E31" s="166"/>
-      <c r="F31" s="166"/>
-      <c r="G31" s="166"/>
+      <c r="B31" s="146"/>
+      <c r="C31" s="146"/>
+      <c r="D31" s="146"/>
+      <c r="E31" s="146"/>
+      <c r="F31" s="146"/>
+      <c r="G31" s="146"/>
       <c r="H31" s="102"/>
       <c r="I31" s="102"/>
       <c r="J31" s="102"/>
@@ -9564,12 +9592,12 @@
     </row>
     <row r="32" spans="1:22">
       <c r="A32" s="108"/>
-      <c r="B32" s="167"/>
-      <c r="C32" s="167"/>
-      <c r="D32" s="167"/>
-      <c r="E32" s="167"/>
-      <c r="F32" s="167"/>
-      <c r="G32" s="167"/>
+      <c r="B32" s="147"/>
+      <c r="C32" s="147"/>
+      <c r="D32" s="147"/>
+      <c r="E32" s="147"/>
+      <c r="F32" s="147"/>
+      <c r="G32" s="147"/>
       <c r="H32" s="102"/>
       <c r="I32" s="102"/>
       <c r="J32" s="102"/>
@@ -9608,28 +9636,28 @@
       <c r="T33"/>
     </row>
     <row r="34" spans="1:22">
-      <c r="A34" s="143" t="s">
+      <c r="A34" s="166" t="s">
         <v>188</v>
       </c>
-      <c r="B34" s="144"/>
-      <c r="C34" s="144"/>
-      <c r="D34" s="144"/>
-      <c r="E34" s="144"/>
-      <c r="F34" s="144"/>
-      <c r="G34" s="145"/>
+      <c r="B34" s="167"/>
+      <c r="C34" s="167"/>
+      <c r="D34" s="167"/>
+      <c r="E34" s="167"/>
+      <c r="F34" s="167"/>
+      <c r="G34" s="168"/>
     </row>
     <row r="35" spans="1:22">
       <c r="A35" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="164" t="s">
+      <c r="B35" s="144" t="s">
         <v>180</v>
       </c>
-      <c r="C35" s="164"/>
-      <c r="D35" s="164"/>
-      <c r="E35" s="164"/>
-      <c r="F35" s="164"/>
-      <c r="G35" s="164"/>
+      <c r="C35" s="144"/>
+      <c r="D35" s="144"/>
+      <c r="E35" s="144"/>
+      <c r="F35" s="144"/>
+      <c r="G35" s="144"/>
       <c r="H35" s="95"/>
       <c r="I35" s="95"/>
       <c r="J35" s="95"/>
@@ -9647,12 +9675,12 @@
     </row>
     <row r="36" spans="1:22">
       <c r="A36" s="106"/>
-      <c r="B36" s="157"/>
-      <c r="C36" s="157"/>
-      <c r="D36" s="157"/>
-      <c r="E36" s="157"/>
-      <c r="F36" s="157"/>
-      <c r="G36" s="168"/>
+      <c r="B36" s="148"/>
+      <c r="C36" s="148"/>
+      <c r="D36" s="148"/>
+      <c r="E36" s="148"/>
+      <c r="F36" s="148"/>
+      <c r="G36" s="149"/>
       <c r="H36" s="102"/>
       <c r="I36" s="102"/>
       <c r="J36" s="102"/>
@@ -9670,12 +9698,12 @@
     </row>
     <row r="37" spans="1:22">
       <c r="A37" s="107"/>
-      <c r="B37" s="158"/>
-      <c r="C37" s="158"/>
-      <c r="D37" s="158"/>
-      <c r="E37" s="158"/>
-      <c r="F37" s="158"/>
-      <c r="G37" s="169"/>
+      <c r="B37" s="150"/>
+      <c r="C37" s="150"/>
+      <c r="D37" s="150"/>
+      <c r="E37" s="150"/>
+      <c r="F37" s="150"/>
+      <c r="G37" s="151"/>
       <c r="H37" s="102"/>
       <c r="I37" s="102"/>
       <c r="J37" s="102"/>
@@ -9693,12 +9721,12 @@
     </row>
     <row r="38" spans="1:22">
       <c r="A38" s="108"/>
-      <c r="B38" s="159"/>
-      <c r="C38" s="159"/>
-      <c r="D38" s="159"/>
-      <c r="E38" s="159"/>
-      <c r="F38" s="159"/>
-      <c r="G38" s="170"/>
+      <c r="B38" s="152"/>
+      <c r="C38" s="152"/>
+      <c r="D38" s="152"/>
+      <c r="E38" s="152"/>
+      <c r="F38" s="152"/>
+      <c r="G38" s="153"/>
       <c r="H38" s="102"/>
       <c r="I38" s="102"/>
       <c r="J38" s="102"/>
@@ -9774,16 +9802,16 @@
       <c r="B42" s="176" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="178" t="s">
+      <c r="C42" s="182" t="s">
         <v>1</v>
       </c>
       <c r="D42" s="176" t="s">
         <v>2</v>
       </c>
-      <c r="E42" s="181" t="s">
+      <c r="E42" s="180" t="s">
         <v>156</v>
       </c>
-      <c r="F42" s="181" t="s">
+      <c r="F42" s="180" t="s">
         <v>171</v>
       </c>
       <c r="G42" s="176" t="s">
@@ -9795,13 +9823,13 @@
       <c r="I42" s="176" t="s">
         <v>237</v>
       </c>
-      <c r="J42" s="181" t="s">
+      <c r="J42" s="180" t="s">
         <v>238</v>
       </c>
-      <c r="K42" s="181" t="s">
+      <c r="K42" s="180" t="s">
         <v>208</v>
       </c>
-      <c r="L42" s="189" t="s">
+      <c r="L42" s="179" t="s">
         <v>225</v>
       </c>
       <c r="M42" s="176" t="s">
@@ -9813,14 +9841,14 @@
       <c r="O42" s="176" t="s">
         <v>190</v>
       </c>
-      <c r="P42" s="179" t="s">
+      <c r="P42" s="183" t="s">
         <v>70</v>
       </c>
-      <c r="Q42" s="180"/>
-      <c r="R42" s="179" t="s">
+      <c r="Q42" s="184"/>
+      <c r="R42" s="183" t="s">
         <v>16</v>
       </c>
-      <c r="S42" s="180"/>
+      <c r="S42" s="184"/>
       <c r="T42" s="32" t="s">
         <v>69</v>
       </c>
@@ -9829,21 +9857,21 @@
       </c>
     </row>
     <row r="43" spans="1:22">
-      <c r="A43" s="177"/>
-      <c r="B43" s="177"/>
-      <c r="C43" s="177"/>
-      <c r="D43" s="177"/>
-      <c r="E43" s="182"/>
-      <c r="F43" s="182"/>
-      <c r="G43" s="177"/>
-      <c r="H43" s="177"/>
-      <c r="I43" s="177"/>
-      <c r="J43" s="182"/>
-      <c r="K43" s="182"/>
-      <c r="L43" s="183"/>
-      <c r="M43" s="177"/>
-      <c r="N43" s="177"/>
-      <c r="O43" s="183"/>
+      <c r="A43" s="178"/>
+      <c r="B43" s="178"/>
+      <c r="C43" s="178"/>
+      <c r="D43" s="178"/>
+      <c r="E43" s="181"/>
+      <c r="F43" s="181"/>
+      <c r="G43" s="178"/>
+      <c r="H43" s="178"/>
+      <c r="I43" s="178"/>
+      <c r="J43" s="181"/>
+      <c r="K43" s="181"/>
+      <c r="L43" s="177"/>
+      <c r="M43" s="178"/>
+      <c r="N43" s="178"/>
+      <c r="O43" s="177"/>
       <c r="P43" s="27" t="s">
         <v>74</v>
       </c>
@@ -9859,7 +9887,7 @@
       <c r="T43" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="U43" s="177"/>
+      <c r="U43" s="178"/>
     </row>
     <row r="44" spans="1:22">
       <c r="A44" s="7">
@@ -9879,7 +9907,9 @@
       <c r="G44" s="75" t="s">
         <v>137</v>
       </c>
-      <c r="H44" s="23"/>
+      <c r="H44" s="23" t="s">
+        <v>240</v>
+      </c>
       <c r="I44" s="23"/>
       <c r="J44" s="23"/>
       <c r="K44" s="23"/>
@@ -9921,7 +9951,9 @@
       <c r="E45" s="24"/>
       <c r="F45" s="24"/>
       <c r="G45" s="76"/>
-      <c r="H45" s="24"/>
+      <c r="H45" s="24">
+        <v>0</v>
+      </c>
       <c r="I45" s="24"/>
       <c r="J45" s="24"/>
       <c r="K45" s="24"/>
@@ -9961,7 +9993,9 @@
       </c>
       <c r="F46" s="25"/>
       <c r="G46" s="77"/>
-      <c r="H46" s="25"/>
+      <c r="H46" s="25" t="s">
+        <v>241</v>
+      </c>
       <c r="I46" s="25"/>
       <c r="J46" s="25"/>
       <c r="K46" s="25"/>
@@ -9995,7 +10029,9 @@
       </c>
       <c r="F47" s="73"/>
       <c r="G47" s="78"/>
-      <c r="H47" s="73"/>
+      <c r="H47" s="73" t="s">
+        <v>241</v>
+      </c>
       <c r="I47" s="23" t="s">
         <v>239</v>
       </c>
@@ -10031,7 +10067,9 @@
       </c>
       <c r="F48" s="25"/>
       <c r="G48" s="77"/>
-      <c r="H48" s="25"/>
+      <c r="H48" s="25" t="s">
+        <v>241</v>
+      </c>
       <c r="I48" s="25"/>
       <c r="J48" s="25"/>
       <c r="K48" s="25"/>
@@ -10063,7 +10101,9 @@
       <c r="E49" s="25"/>
       <c r="F49" s="25"/>
       <c r="G49" s="77"/>
-      <c r="H49" s="25"/>
+      <c r="H49" s="25" t="s">
+        <v>243</v>
+      </c>
       <c r="I49" s="25"/>
       <c r="J49" s="25"/>
       <c r="K49" s="25"/>
@@ -10093,7 +10133,9 @@
       <c r="E50" s="25"/>
       <c r="F50" s="25"/>
       <c r="G50" s="77"/>
-      <c r="H50" s="25"/>
+      <c r="H50" s="25" t="s">
+        <v>242</v>
+      </c>
       <c r="I50" s="25"/>
       <c r="J50" s="25"/>
       <c r="K50" s="25"/>
@@ -10501,11 +10543,30 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="M42:M43"/>
-    <mergeCell ref="N42:N43"/>
-    <mergeCell ref="O42:O43"/>
-    <mergeCell ref="P42:Q42"/>
-    <mergeCell ref="R42:S42"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
     <mergeCell ref="U42:U43"/>
     <mergeCell ref="G42:G43"/>
     <mergeCell ref="H42:H43"/>
@@ -10513,30 +10574,11 @@
     <mergeCell ref="J42:J43"/>
     <mergeCell ref="K42:K43"/>
     <mergeCell ref="L42:L43"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="A34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="M42:M43"/>
+    <mergeCell ref="N42:N43"/>
+    <mergeCell ref="O42:O43"/>
+    <mergeCell ref="P42:Q42"/>
+    <mergeCell ref="R42:S42"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="4">
@@ -10729,10 +10771,10 @@
         <v>168</v>
       </c>
       <c r="B13" s="111"/>
-      <c r="C13" s="151" t="s">
+      <c r="C13" s="133" t="s">
         <v>169</v>
       </c>
-      <c r="D13" s="151"/>
+      <c r="D13" s="133"/>
       <c r="E13" s="1" t="s">
         <v>170</v>
       </c>
@@ -10742,10 +10784,10 @@
         <v>171</v>
       </c>
       <c r="B14" s="111"/>
-      <c r="C14" s="151" t="s">
+      <c r="C14" s="133" t="s">
         <v>172</v>
       </c>
-      <c r="D14" s="151"/>
+      <c r="D14" s="133"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="112" t="s">
@@ -10771,28 +10813,28 @@
       <c r="A16" s="6"/>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="146" t="s">
+      <c r="A17" s="169" t="s">
         <v>186</v>
       </c>
-      <c r="B17" s="146"/>
-      <c r="C17" s="146"/>
-      <c r="D17" s="146"/>
-      <c r="E17" s="146"/>
-      <c r="F17" s="146"/>
-      <c r="G17" s="146"/>
+      <c r="B17" s="169"/>
+      <c r="C17" s="169"/>
+      <c r="D17" s="169"/>
+      <c r="E17" s="169"/>
+      <c r="F17" s="169"/>
+      <c r="G17" s="169"/>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="140" t="s">
+      <c r="B18" s="163" t="s">
         <v>177</v>
       </c>
-      <c r="C18" s="141"/>
-      <c r="D18" s="141"/>
-      <c r="E18" s="141"/>
-      <c r="F18" s="141"/>
-      <c r="G18" s="142"/>
+      <c r="C18" s="164"/>
+      <c r="D18" s="164"/>
+      <c r="E18" s="164"/>
+      <c r="F18" s="164"/>
+      <c r="G18" s="165"/>
       <c r="H18" s="95"/>
       <c r="I18" s="95"/>
       <c r="K18" s="95"/>
@@ -10804,12 +10846,12 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="106"/>
-      <c r="B19" s="157"/>
-      <c r="C19" s="157"/>
-      <c r="D19" s="157"/>
-      <c r="E19" s="157"/>
-      <c r="F19" s="157"/>
-      <c r="G19" s="157"/>
+      <c r="B19" s="148"/>
+      <c r="C19" s="148"/>
+      <c r="D19" s="148"/>
+      <c r="E19" s="148"/>
+      <c r="F19" s="148"/>
+      <c r="G19" s="148"/>
       <c r="H19" s="102"/>
       <c r="I19" s="102"/>
       <c r="K19" s="102"/>
@@ -10821,12 +10863,12 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="107"/>
-      <c r="B20" s="158"/>
-      <c r="C20" s="158"/>
-      <c r="D20" s="158"/>
-      <c r="E20" s="158"/>
-      <c r="F20" s="158"/>
-      <c r="G20" s="158"/>
+      <c r="B20" s="150"/>
+      <c r="C20" s="150"/>
+      <c r="D20" s="150"/>
+      <c r="E20" s="150"/>
+      <c r="F20" s="150"/>
+      <c r="G20" s="150"/>
       <c r="H20" s="102"/>
       <c r="I20" s="102"/>
       <c r="K20" s="102"/>
@@ -10838,12 +10880,12 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="108"/>
-      <c r="B21" s="159"/>
-      <c r="C21" s="159"/>
-      <c r="D21" s="159"/>
-      <c r="E21" s="159"/>
-      <c r="F21" s="159"/>
-      <c r="G21" s="159"/>
+      <c r="B21" s="152"/>
+      <c r="C21" s="152"/>
+      <c r="D21" s="152"/>
+      <c r="E21" s="152"/>
+      <c r="F21" s="152"/>
+      <c r="G21" s="152"/>
       <c r="H21" s="102"/>
       <c r="I21" s="102"/>
       <c r="J21" s="95"/>
@@ -10859,29 +10901,29 @@
       <c r="J22" s="102"/>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="143" t="s">
+      <c r="A23" s="166" t="s">
         <v>187</v>
       </c>
-      <c r="B23" s="144"/>
-      <c r="C23" s="144"/>
-      <c r="D23" s="144"/>
-      <c r="E23" s="144"/>
-      <c r="F23" s="144"/>
-      <c r="G23" s="145"/>
+      <c r="B23" s="167"/>
+      <c r="C23" s="167"/>
+      <c r="D23" s="167"/>
+      <c r="E23" s="167"/>
+      <c r="F23" s="167"/>
+      <c r="G23" s="168"/>
       <c r="J23" s="102"/>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="164" t="s">
+      <c r="B24" s="144" t="s">
         <v>178</v>
       </c>
-      <c r="C24" s="164"/>
-      <c r="D24" s="164"/>
-      <c r="E24" s="164"/>
-      <c r="F24" s="164"/>
-      <c r="G24" s="164"/>
+      <c r="C24" s="144"/>
+      <c r="D24" s="144"/>
+      <c r="E24" s="144"/>
+      <c r="F24" s="144"/>
+      <c r="G24" s="144"/>
       <c r="H24" s="95"/>
       <c r="I24" s="95"/>
       <c r="J24" s="102"/>
@@ -10896,14 +10938,14 @@
       <c r="A25" s="106">
         <v>1</v>
       </c>
-      <c r="B25" s="165" t="s">
+      <c r="B25" s="145" t="s">
         <v>179</v>
       </c>
-      <c r="C25" s="165"/>
-      <c r="D25" s="165"/>
-      <c r="E25" s="165"/>
-      <c r="F25" s="165"/>
-      <c r="G25" s="165"/>
+      <c r="C25" s="145"/>
+      <c r="D25" s="145"/>
+      <c r="E25" s="145"/>
+      <c r="F25" s="145"/>
+      <c r="G25" s="145"/>
       <c r="H25" s="102"/>
       <c r="I25" s="102"/>
       <c r="K25" s="102"/>
@@ -10915,12 +10957,12 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="107"/>
-      <c r="B26" s="166"/>
-      <c r="C26" s="166"/>
-      <c r="D26" s="166"/>
-      <c r="E26" s="166"/>
-      <c r="F26" s="166"/>
-      <c r="G26" s="166"/>
+      <c r="B26" s="146"/>
+      <c r="C26" s="146"/>
+      <c r="D26" s="146"/>
+      <c r="E26" s="146"/>
+      <c r="F26" s="146"/>
+      <c r="G26" s="146"/>
       <c r="H26" s="102"/>
       <c r="I26" s="102"/>
       <c r="K26" s="102"/>
@@ -10932,12 +10974,12 @@
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="108"/>
-      <c r="B27" s="167"/>
-      <c r="C27" s="167"/>
-      <c r="D27" s="167"/>
-      <c r="E27" s="167"/>
-      <c r="F27" s="167"/>
-      <c r="G27" s="167"/>
+      <c r="B27" s="147"/>
+      <c r="C27" s="147"/>
+      <c r="D27" s="147"/>
+      <c r="E27" s="147"/>
+      <c r="F27" s="147"/>
+      <c r="G27" s="147"/>
       <c r="H27" s="102"/>
       <c r="I27" s="102"/>
       <c r="J27" s="95"/>
@@ -10966,29 +11008,29 @@
       <c r="O28"/>
     </row>
     <row r="29" spans="1:17">
-      <c r="A29" s="143" t="s">
+      <c r="A29" s="166" t="s">
         <v>188</v>
       </c>
-      <c r="B29" s="144"/>
-      <c r="C29" s="144"/>
-      <c r="D29" s="144"/>
-      <c r="E29" s="144"/>
-      <c r="F29" s="144"/>
-      <c r="G29" s="145"/>
+      <c r="B29" s="167"/>
+      <c r="C29" s="167"/>
+      <c r="D29" s="167"/>
+      <c r="E29" s="167"/>
+      <c r="F29" s="167"/>
+      <c r="G29" s="168"/>
       <c r="J29" s="102"/>
     </row>
     <row r="30" spans="1:17">
       <c r="A30" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B30" s="164" t="s">
+      <c r="B30" s="144" t="s">
         <v>180</v>
       </c>
-      <c r="C30" s="164"/>
-      <c r="D30" s="164"/>
-      <c r="E30" s="164"/>
-      <c r="F30" s="164"/>
-      <c r="G30" s="164"/>
+      <c r="C30" s="144"/>
+      <c r="D30" s="144"/>
+      <c r="E30" s="144"/>
+      <c r="F30" s="144"/>
+      <c r="G30" s="144"/>
       <c r="H30" s="95"/>
       <c r="I30" s="95"/>
       <c r="J30" s="102"/>
@@ -11001,12 +11043,12 @@
     </row>
     <row r="31" spans="1:17">
       <c r="A31" s="106"/>
-      <c r="B31" s="157"/>
-      <c r="C31" s="157"/>
-      <c r="D31" s="157"/>
-      <c r="E31" s="157"/>
-      <c r="F31" s="157"/>
-      <c r="G31" s="168"/>
+      <c r="B31" s="148"/>
+      <c r="C31" s="148"/>
+      <c r="D31" s="148"/>
+      <c r="E31" s="148"/>
+      <c r="F31" s="148"/>
+      <c r="G31" s="149"/>
       <c r="H31" s="102"/>
       <c r="I31" s="102"/>
       <c r="J31"/>
@@ -11019,12 +11061,12 @@
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="107"/>
-      <c r="B32" s="158"/>
-      <c r="C32" s="158"/>
-      <c r="D32" s="158"/>
-      <c r="E32" s="158"/>
-      <c r="F32" s="158"/>
-      <c r="G32" s="169"/>
+      <c r="B32" s="150"/>
+      <c r="C32" s="150"/>
+      <c r="D32" s="150"/>
+      <c r="E32" s="150"/>
+      <c r="F32" s="150"/>
+      <c r="G32" s="151"/>
       <c r="H32" s="102"/>
       <c r="I32" s="102"/>
       <c r="K32" s="102"/>
@@ -11036,12 +11078,12 @@
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="108"/>
-      <c r="B33" s="159"/>
-      <c r="C33" s="159"/>
-      <c r="D33" s="159"/>
-      <c r="E33" s="159"/>
-      <c r="F33" s="159"/>
-      <c r="G33" s="170"/>
+      <c r="B33" s="152"/>
+      <c r="C33" s="152"/>
+      <c r="D33" s="152"/>
+      <c r="E33" s="152"/>
+      <c r="F33" s="152"/>
+      <c r="G33" s="153"/>
       <c r="H33" s="102"/>
       <c r="I33" s="102"/>
       <c r="J33" s="95"/>
@@ -11094,31 +11136,31 @@
       <c r="P36" s="49"/>
     </row>
     <row r="37" spans="1:17" ht="15">
-      <c r="A37" s="181" t="s">
+      <c r="A37" s="180" t="s">
         <v>115</v>
       </c>
-      <c r="B37" s="181" t="s">
+      <c r="B37" s="180" t="s">
         <v>116</v>
       </c>
       <c r="C37" s="51" t="s">
         <v>117</v>
       </c>
-      <c r="D37" s="181" t="s">
+      <c r="D37" s="180" t="s">
         <v>99</v>
       </c>
-      <c r="E37" s="181" t="s">
+      <c r="E37" s="180" t="s">
         <v>156</v>
       </c>
-      <c r="F37" s="181" t="s">
+      <c r="F37" s="180" t="s">
         <v>171</v>
       </c>
-      <c r="G37" s="181" t="s">
+      <c r="G37" s="180" t="s">
         <v>136</v>
       </c>
-      <c r="H37" s="181" t="s">
+      <c r="H37" s="180" t="s">
         <v>113</v>
       </c>
-      <c r="I37" s="181" t="s">
+      <c r="I37" s="180" t="s">
         <v>230</v>
       </c>
       <c r="J37" s="176" t="s">
@@ -11135,23 +11177,23 @@
       <c r="O37" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="P37" s="181" t="s">
+      <c r="P37" s="180" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="15">
-      <c r="A38" s="184"/>
-      <c r="B38" s="184"/>
+      <c r="A38" s="188"/>
+      <c r="B38" s="188"/>
       <c r="C38" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="D38" s="184"/>
-      <c r="E38" s="182"/>
-      <c r="F38" s="182"/>
-      <c r="G38" s="184"/>
-      <c r="H38" s="184"/>
-      <c r="I38" s="184"/>
-      <c r="J38" s="183"/>
+      <c r="D38" s="188"/>
+      <c r="E38" s="181"/>
+      <c r="F38" s="181"/>
+      <c r="G38" s="188"/>
+      <c r="H38" s="188"/>
+      <c r="I38" s="188"/>
+      <c r="J38" s="177"/>
       <c r="K38" s="53" t="s">
         <v>123</v>
       </c>
@@ -11167,7 +11209,7 @@
       <c r="O38" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="P38" s="184"/>
+      <c r="P38" s="188"/>
     </row>
     <row r="39" spans="1:17">
       <c r="A39" s="55">
@@ -11665,6 +11707,28 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="A23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B33:G33"/>
     <mergeCell ref="P37:P38"/>
     <mergeCell ref="G37:G38"/>
     <mergeCell ref="H37:H38"/>
@@ -11672,28 +11736,6 @@
     <mergeCell ref="J37:J38"/>
     <mergeCell ref="K37:L37"/>
     <mergeCell ref="M37:N37"/>
-    <mergeCell ref="A29:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="A23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">
@@ -11903,10 +11945,10 @@
         <v>168</v>
       </c>
       <c r="B15" s="111"/>
-      <c r="C15" s="151" t="s">
+      <c r="C15" s="133" t="s">
         <v>169</v>
       </c>
-      <c r="D15" s="151"/>
+      <c r="D15" s="133"/>
       <c r="E15" s="1" t="s">
         <v>170</v>
       </c>
@@ -11916,10 +11958,10 @@
         <v>171</v>
       </c>
       <c r="B16" s="111"/>
-      <c r="C16" s="151" t="s">
+      <c r="C16" s="133" t="s">
         <v>172</v>
       </c>
-      <c r="D16" s="151"/>
+      <c r="D16" s="133"/>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="112" t="s">
@@ -11945,28 +11987,28 @@
       <c r="A18" s="6"/>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="146" t="s">
+      <c r="A19" s="169" t="s">
         <v>186</v>
       </c>
-      <c r="B19" s="146"/>
-      <c r="C19" s="146"/>
-      <c r="D19" s="146"/>
-      <c r="E19" s="146"/>
-      <c r="F19" s="146"/>
-      <c r="G19" s="146"/>
+      <c r="B19" s="169"/>
+      <c r="C19" s="169"/>
+      <c r="D19" s="169"/>
+      <c r="E19" s="169"/>
+      <c r="F19" s="169"/>
+      <c r="G19" s="169"/>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B20" s="140" t="s">
+      <c r="B20" s="163" t="s">
         <v>177</v>
       </c>
-      <c r="C20" s="141"/>
-      <c r="D20" s="141"/>
-      <c r="E20" s="141"/>
-      <c r="F20" s="141"/>
-      <c r="G20" s="142"/>
+      <c r="C20" s="164"/>
+      <c r="D20" s="164"/>
+      <c r="E20" s="164"/>
+      <c r="F20" s="164"/>
+      <c r="G20" s="165"/>
       <c r="H20" s="95"/>
       <c r="I20" s="95"/>
       <c r="K20" s="95"/>
@@ -11978,12 +12020,12 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="106"/>
-      <c r="B21" s="157"/>
-      <c r="C21" s="157"/>
-      <c r="D21" s="157"/>
-      <c r="E21" s="157"/>
-      <c r="F21" s="157"/>
-      <c r="G21" s="157"/>
+      <c r="B21" s="148"/>
+      <c r="C21" s="148"/>
+      <c r="D21" s="148"/>
+      <c r="E21" s="148"/>
+      <c r="F21" s="148"/>
+      <c r="G21" s="148"/>
       <c r="H21" s="102"/>
       <c r="I21" s="102"/>
       <c r="K21" s="102"/>
@@ -11995,12 +12037,12 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="107"/>
-      <c r="B22" s="158"/>
-      <c r="C22" s="158"/>
-      <c r="D22" s="158"/>
-      <c r="E22" s="158"/>
-      <c r="F22" s="158"/>
-      <c r="G22" s="158"/>
+      <c r="B22" s="150"/>
+      <c r="C22" s="150"/>
+      <c r="D22" s="150"/>
+      <c r="E22" s="150"/>
+      <c r="F22" s="150"/>
+      <c r="G22" s="150"/>
       <c r="H22" s="102"/>
       <c r="I22" s="102"/>
       <c r="K22" s="102"/>
@@ -12012,12 +12054,12 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="108"/>
-      <c r="B23" s="159"/>
-      <c r="C23" s="159"/>
-      <c r="D23" s="159"/>
-      <c r="E23" s="159"/>
-      <c r="F23" s="159"/>
-      <c r="G23" s="159"/>
+      <c r="B23" s="152"/>
+      <c r="C23" s="152"/>
+      <c r="D23" s="152"/>
+      <c r="E23" s="152"/>
+      <c r="F23" s="152"/>
+      <c r="G23" s="152"/>
       <c r="H23" s="102"/>
       <c r="I23" s="102"/>
       <c r="J23" s="95"/>
@@ -12033,29 +12075,29 @@
       <c r="J24" s="102"/>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" s="143" t="s">
+      <c r="A25" s="166" t="s">
         <v>187</v>
       </c>
-      <c r="B25" s="144"/>
-      <c r="C25" s="144"/>
-      <c r="D25" s="144"/>
-      <c r="E25" s="144"/>
-      <c r="F25" s="144"/>
-      <c r="G25" s="145"/>
+      <c r="B25" s="167"/>
+      <c r="C25" s="167"/>
+      <c r="D25" s="167"/>
+      <c r="E25" s="167"/>
+      <c r="F25" s="167"/>
+      <c r="G25" s="168"/>
       <c r="J25" s="102"/>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="164" t="s">
+      <c r="B26" s="144" t="s">
         <v>178</v>
       </c>
-      <c r="C26" s="164"/>
-      <c r="D26" s="164"/>
-      <c r="E26" s="164"/>
-      <c r="F26" s="164"/>
-      <c r="G26" s="164"/>
+      <c r="C26" s="144"/>
+      <c r="D26" s="144"/>
+      <c r="E26" s="144"/>
+      <c r="F26" s="144"/>
+      <c r="G26" s="144"/>
       <c r="H26" s="95"/>
       <c r="I26" s="95"/>
       <c r="J26" s="102"/>
@@ -12070,14 +12112,14 @@
       <c r="A27" s="106">
         <v>1</v>
       </c>
-      <c r="B27" s="165" t="s">
+      <c r="B27" s="145" t="s">
         <v>179</v>
       </c>
-      <c r="C27" s="165"/>
-      <c r="D27" s="165"/>
-      <c r="E27" s="165"/>
-      <c r="F27" s="165"/>
-      <c r="G27" s="165"/>
+      <c r="C27" s="145"/>
+      <c r="D27" s="145"/>
+      <c r="E27" s="145"/>
+      <c r="F27" s="145"/>
+      <c r="G27" s="145"/>
       <c r="H27" s="102"/>
       <c r="I27" s="102"/>
       <c r="K27" s="102"/>
@@ -12089,12 +12131,12 @@
     </row>
     <row r="28" spans="1:17">
       <c r="A28" s="107"/>
-      <c r="B28" s="166"/>
-      <c r="C28" s="166"/>
-      <c r="D28" s="166"/>
-      <c r="E28" s="166"/>
-      <c r="F28" s="166"/>
-      <c r="G28" s="166"/>
+      <c r="B28" s="146"/>
+      <c r="C28" s="146"/>
+      <c r="D28" s="146"/>
+      <c r="E28" s="146"/>
+      <c r="F28" s="146"/>
+      <c r="G28" s="146"/>
       <c r="H28" s="102"/>
       <c r="I28" s="102"/>
       <c r="K28" s="102"/>
@@ -12106,12 +12148,12 @@
     </row>
     <row r="29" spans="1:17">
       <c r="A29" s="108"/>
-      <c r="B29" s="167"/>
-      <c r="C29" s="167"/>
-      <c r="D29" s="167"/>
-      <c r="E29" s="167"/>
-      <c r="F29" s="167"/>
-      <c r="G29" s="167"/>
+      <c r="B29" s="147"/>
+      <c r="C29" s="147"/>
+      <c r="D29" s="147"/>
+      <c r="E29" s="147"/>
+      <c r="F29" s="147"/>
+      <c r="G29" s="147"/>
       <c r="H29" s="102"/>
       <c r="I29" s="102"/>
       <c r="J29" s="95"/>
@@ -12140,29 +12182,29 @@
       <c r="O30"/>
     </row>
     <row r="31" spans="1:17">
-      <c r="A31" s="143" t="s">
+      <c r="A31" s="166" t="s">
         <v>188</v>
       </c>
-      <c r="B31" s="144"/>
-      <c r="C31" s="144"/>
-      <c r="D31" s="144"/>
-      <c r="E31" s="144"/>
-      <c r="F31" s="144"/>
-      <c r="G31" s="145"/>
+      <c r="B31" s="167"/>
+      <c r="C31" s="167"/>
+      <c r="D31" s="167"/>
+      <c r="E31" s="167"/>
+      <c r="F31" s="167"/>
+      <c r="G31" s="168"/>
       <c r="J31" s="102"/>
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="164" t="s">
+      <c r="B32" s="144" t="s">
         <v>180</v>
       </c>
-      <c r="C32" s="164"/>
-      <c r="D32" s="164"/>
-      <c r="E32" s="164"/>
-      <c r="F32" s="164"/>
-      <c r="G32" s="164"/>
+      <c r="C32" s="144"/>
+      <c r="D32" s="144"/>
+      <c r="E32" s="144"/>
+      <c r="F32" s="144"/>
+      <c r="G32" s="144"/>
       <c r="H32" s="95"/>
       <c r="I32" s="95"/>
       <c r="J32" s="102"/>
@@ -12175,12 +12217,12 @@
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="106"/>
-      <c r="B33" s="157"/>
-      <c r="C33" s="157"/>
-      <c r="D33" s="157"/>
-      <c r="E33" s="157"/>
-      <c r="F33" s="157"/>
-      <c r="G33" s="168"/>
+      <c r="B33" s="148"/>
+      <c r="C33" s="148"/>
+      <c r="D33" s="148"/>
+      <c r="E33" s="148"/>
+      <c r="F33" s="148"/>
+      <c r="G33" s="149"/>
       <c r="H33" s="102"/>
       <c r="I33" s="102"/>
       <c r="J33"/>
@@ -12193,12 +12235,12 @@
     </row>
     <row r="34" spans="1:17">
       <c r="A34" s="107"/>
-      <c r="B34" s="158"/>
-      <c r="C34" s="158"/>
-      <c r="D34" s="158"/>
-      <c r="E34" s="158"/>
-      <c r="F34" s="158"/>
-      <c r="G34" s="169"/>
+      <c r="B34" s="150"/>
+      <c r="C34" s="150"/>
+      <c r="D34" s="150"/>
+      <c r="E34" s="150"/>
+      <c r="F34" s="150"/>
+      <c r="G34" s="151"/>
       <c r="H34" s="102"/>
       <c r="I34" s="102"/>
       <c r="K34" s="102"/>
@@ -12210,12 +12252,12 @@
     </row>
     <row r="35" spans="1:17">
       <c r="A35" s="108"/>
-      <c r="B35" s="159"/>
-      <c r="C35" s="159"/>
-      <c r="D35" s="159"/>
-      <c r="E35" s="159"/>
-      <c r="F35" s="159"/>
-      <c r="G35" s="170"/>
+      <c r="B35" s="152"/>
+      <c r="C35" s="152"/>
+      <c r="D35" s="152"/>
+      <c r="E35" s="152"/>
+      <c r="F35" s="152"/>
+      <c r="G35" s="153"/>
       <c r="H35" s="102"/>
       <c r="I35" s="102"/>
       <c r="J35" s="95"/>
@@ -12268,31 +12310,31 @@
       <c r="P38" s="49"/>
     </row>
     <row r="39" spans="1:17" ht="15">
-      <c r="A39" s="181" t="s">
+      <c r="A39" s="180" t="s">
         <v>115</v>
       </c>
-      <c r="B39" s="181" t="s">
+      <c r="B39" s="180" t="s">
         <v>116</v>
       </c>
       <c r="C39" s="51" t="s">
         <v>117</v>
       </c>
-      <c r="D39" s="181" t="s">
+      <c r="D39" s="180" t="s">
         <v>99</v>
       </c>
-      <c r="E39" s="181" t="s">
+      <c r="E39" s="180" t="s">
         <v>156</v>
       </c>
-      <c r="F39" s="181" t="s">
+      <c r="F39" s="180" t="s">
         <v>171</v>
       </c>
-      <c r="G39" s="181" t="s">
+      <c r="G39" s="180" t="s">
         <v>136</v>
       </c>
-      <c r="H39" s="188" t="s">
+      <c r="H39" s="189" t="s">
         <v>113</v>
       </c>
-      <c r="I39" s="188" t="s">
+      <c r="I39" s="189" t="s">
         <v>225</v>
       </c>
       <c r="J39" s="176" t="s">
@@ -12309,23 +12351,23 @@
       <c r="O39" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="P39" s="181" t="s">
+      <c r="P39" s="180" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="15">
-      <c r="A40" s="184"/>
-      <c r="B40" s="184"/>
+      <c r="A40" s="188"/>
+      <c r="B40" s="188"/>
       <c r="C40" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="D40" s="184"/>
-      <c r="E40" s="182"/>
-      <c r="F40" s="182"/>
-      <c r="G40" s="184"/>
-      <c r="H40" s="184"/>
-      <c r="I40" s="184"/>
-      <c r="J40" s="183"/>
+      <c r="D40" s="188"/>
+      <c r="E40" s="181"/>
+      <c r="F40" s="181"/>
+      <c r="G40" s="188"/>
+      <c r="H40" s="188"/>
+      <c r="I40" s="188"/>
+      <c r="J40" s="177"/>
       <c r="K40" s="53" t="s">
         <v>123</v>
       </c>
@@ -12341,7 +12383,7 @@
       <c r="O40" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="P40" s="184"/>
+      <c r="P40" s="188"/>
     </row>
     <row r="41" spans="1:17">
       <c r="A41" s="55">
@@ -12797,6 +12839,28 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B35:G35"/>
     <mergeCell ref="P39:P40"/>
     <mergeCell ref="G39:G40"/>
     <mergeCell ref="H39:H40"/>
@@ -12804,28 +12868,6 @@
     <mergeCell ref="J39:J40"/>
     <mergeCell ref="K39:L39"/>
     <mergeCell ref="M39:N39"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">

</xml_diff>

<commit_message>
3.1.1: additionalPath is added to telegrams.
</commit_message>
<xml_diff>
--- a/meta/plainApi/BlancoApiPlainSample.xlsx
+++ b/meta/plainApi/BlancoApiPlainSample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorTs/meta/plainApi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E6D3F9-E84F-6A4D-8C53-50C57BECDB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78906414-04E9-B34B-A873-74C3755B5F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2440" yWindow="500" windowWidth="29440" windowHeight="20500" tabRatio="860" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2440" yWindow="500" windowWidth="29440" windowHeight="20500" tabRatio="860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="process" sheetId="19" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="245">
   <si>
     <t>項目名</t>
     <rPh sb="0" eb="3">
@@ -2492,6 +2492,10 @@
   </si>
   <si>
     <t>{}</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/get_addition</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -3648,88 +3652,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="49" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3741,6 +3667,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3749,6 +3678,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3780,6 +3715,12 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3789,22 +3730,73 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3814,6 +3806,21 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3821,9 +3828,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4375,7 +4379,7 @@
   </sheetPr>
   <dimension ref="A1:O75"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -4419,152 +4423,152 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="129" t="s">
+      <c r="A5" s="162" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="129"/>
-      <c r="C5" s="129"/>
-      <c r="D5" s="129"/>
-      <c r="E5" s="129"/>
+      <c r="B5" s="162"/>
+      <c r="C5" s="162"/>
+      <c r="D5" s="162"/>
+      <c r="E5" s="162"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="135" t="s">
+      <c r="A6" s="173" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="136"/>
-      <c r="C6" s="137"/>
-      <c r="D6" s="130" t="s">
+      <c r="B6" s="174"/>
+      <c r="C6" s="175"/>
+      <c r="D6" s="171" t="s">
         <v>234</v>
       </c>
-      <c r="E6" s="130"/>
+      <c r="E6" s="171"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="129" t="s">
+      <c r="A7" s="162" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="129"/>
-      <c r="C7" s="129"/>
-      <c r="D7" s="130" t="s">
+      <c r="B7" s="162"/>
+      <c r="C7" s="162"/>
+      <c r="D7" s="171" t="s">
         <v>160</v>
       </c>
-      <c r="E7" s="130"/>
+      <c r="E7" s="171"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="129" t="s">
+      <c r="A8" s="162" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="129"/>
-      <c r="C8" s="129"/>
-      <c r="D8" s="130" t="s">
+      <c r="B8" s="162"/>
+      <c r="C8" s="162"/>
+      <c r="D8" s="171" t="s">
         <v>234</v>
       </c>
-      <c r="E8" s="130"/>
+      <c r="E8" s="171"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="129" t="s">
+      <c r="A9" s="162" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="129"/>
-      <c r="C9" s="129"/>
-      <c r="D9" s="130" t="s">
+      <c r="B9" s="162"/>
+      <c r="C9" s="162"/>
+      <c r="D9" s="171" t="s">
         <v>98</v>
       </c>
-      <c r="E9" s="130"/>
+      <c r="E9" s="171"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="129" t="s">
+      <c r="A10" s="162" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="129"/>
-      <c r="C10" s="129"/>
-      <c r="D10" s="130"/>
-      <c r="E10" s="130"/>
+      <c r="B10" s="162"/>
+      <c r="C10" s="162"/>
+      <c r="D10" s="171"/>
+      <c r="E10" s="171"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="129" t="s">
+      <c r="A11" s="162" t="s">
         <v>97</v>
       </c>
-      <c r="B11" s="129"/>
-      <c r="C11" s="129"/>
-      <c r="D11" s="130" t="s">
+      <c r="B11" s="162"/>
+      <c r="C11" s="162"/>
+      <c r="D11" s="171" t="s">
         <v>157</v>
       </c>
-      <c r="E11" s="130"/>
+      <c r="E11" s="171"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="131" t="s">
+      <c r="A12" s="134" t="s">
         <v>168</v>
       </c>
-      <c r="B12" s="131"/>
-      <c r="C12" s="131"/>
-      <c r="D12" s="133" t="s">
+      <c r="B12" s="134"/>
+      <c r="C12" s="134"/>
+      <c r="D12" s="151" t="s">
         <v>169</v>
       </c>
-      <c r="E12" s="133"/>
+      <c r="E12" s="151"/>
       <c r="F12" s="1" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="131" t="s">
+      <c r="A13" s="134" t="s">
         <v>171</v>
       </c>
-      <c r="B13" s="131"/>
-      <c r="C13" s="131"/>
-      <c r="D13" s="132" t="s">
+      <c r="B13" s="134"/>
+      <c r="C13" s="134"/>
+      <c r="D13" s="150" t="s">
         <v>209</v>
       </c>
-      <c r="E13" s="133"/>
+      <c r="E13" s="151"/>
     </row>
     <row r="14" spans="1:6" ht="55" customHeight="1">
-      <c r="A14" s="131" t="s">
+      <c r="A14" s="134" t="s">
         <v>208</v>
       </c>
-      <c r="B14" s="131"/>
-      <c r="C14" s="131"/>
-      <c r="D14" s="134" t="s">
+      <c r="B14" s="134"/>
+      <c r="C14" s="134"/>
+      <c r="D14" s="172" t="s">
         <v>233</v>
       </c>
-      <c r="E14" s="133"/>
+      <c r="E14" s="151"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="131" t="s">
+      <c r="A15" s="134" t="s">
         <v>192</v>
       </c>
-      <c r="B15" s="131"/>
-      <c r="C15" s="131"/>
-      <c r="D15" s="132"/>
-      <c r="E15" s="133"/>
+      <c r="B15" s="134"/>
+      <c r="C15" s="134"/>
+      <c r="D15" s="150"/>
+      <c r="E15" s="151"/>
       <c r="F15" s="1" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="131" t="s">
+      <c r="A16" s="134" t="s">
         <v>193</v>
       </c>
-      <c r="B16" s="131"/>
-      <c r="C16" s="131"/>
-      <c r="D16" s="132"/>
-      <c r="E16" s="133"/>
+      <c r="B16" s="134"/>
+      <c r="C16" s="134"/>
+      <c r="D16" s="150"/>
+      <c r="E16" s="151"/>
       <c r="F16" s="1" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="173" t="s">
+      <c r="A17" s="152" t="s">
         <v>139</v>
       </c>
-      <c r="B17" s="174"/>
-      <c r="C17" s="175"/>
+      <c r="B17" s="153"/>
+      <c r="C17" s="154"/>
       <c r="D17" s="104"/>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="160" t="s">
+      <c r="A18" s="135" t="s">
         <v>173</v>
       </c>
-      <c r="B18" s="161"/>
-      <c r="C18" s="162"/>
+      <c r="B18" s="136"/>
+      <c r="C18" s="137"/>
       <c r="D18" s="90" t="s">
         <v>137</v>
       </c>
@@ -4584,15 +4588,15 @@
       <c r="B19" s="6"/>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="170" t="s">
+      <c r="A20" s="147" t="s">
         <v>182</v>
       </c>
-      <c r="B20" s="171"/>
-      <c r="C20" s="171"/>
-      <c r="D20" s="171"/>
-      <c r="E20" s="171"/>
-      <c r="F20" s="171"/>
-      <c r="G20" s="172"/>
+      <c r="B20" s="148"/>
+      <c r="C20" s="148"/>
+      <c r="D20" s="148"/>
+      <c r="E20" s="148"/>
+      <c r="F20" s="148"/>
+      <c r="G20" s="149"/>
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="91" t="s">
@@ -4636,28 +4640,28 @@
       <c r="C24"/>
     </row>
     <row r="25" spans="1:15">
-      <c r="A25" s="169" t="s">
+      <c r="A25" s="146" t="s">
         <v>183</v>
       </c>
-      <c r="B25" s="169"/>
-      <c r="C25" s="169"/>
-      <c r="D25" s="169"/>
-      <c r="E25" s="169"/>
-      <c r="F25" s="169"/>
-      <c r="G25" s="169"/>
+      <c r="B25" s="146"/>
+      <c r="C25" s="146"/>
+      <c r="D25" s="146"/>
+      <c r="E25" s="146"/>
+      <c r="F25" s="146"/>
+      <c r="G25" s="146"/>
     </row>
     <row r="26" spans="1:15">
       <c r="A26" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="163" t="s">
+      <c r="B26" s="140" t="s">
         <v>177</v>
       </c>
-      <c r="C26" s="164"/>
-      <c r="D26" s="164"/>
-      <c r="E26" s="164"/>
-      <c r="F26" s="164"/>
-      <c r="G26" s="165"/>
+      <c r="C26" s="141"/>
+      <c r="D26" s="141"/>
+      <c r="E26" s="141"/>
+      <c r="F26" s="141"/>
+      <c r="G26" s="142"/>
       <c r="H26" s="95"/>
       <c r="I26" s="95"/>
       <c r="J26" s="95"/>
@@ -4668,12 +4672,12 @@
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="106"/>
-      <c r="B27" s="148"/>
-      <c r="C27" s="148"/>
-      <c r="D27" s="148"/>
-      <c r="E27" s="148"/>
-      <c r="F27" s="148"/>
-      <c r="G27" s="148"/>
+      <c r="B27" s="157"/>
+      <c r="C27" s="157"/>
+      <c r="D27" s="157"/>
+      <c r="E27" s="157"/>
+      <c r="F27" s="157"/>
+      <c r="G27" s="157"/>
       <c r="H27" s="102"/>
       <c r="I27" s="102"/>
       <c r="J27" s="102"/>
@@ -4684,12 +4688,12 @@
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="107"/>
-      <c r="B28" s="150"/>
-      <c r="C28" s="150"/>
-      <c r="D28" s="150"/>
-      <c r="E28" s="150"/>
-      <c r="F28" s="150"/>
-      <c r="G28" s="150"/>
+      <c r="B28" s="158"/>
+      <c r="C28" s="158"/>
+      <c r="D28" s="158"/>
+      <c r="E28" s="158"/>
+      <c r="F28" s="158"/>
+      <c r="G28" s="158"/>
       <c r="H28" s="102"/>
       <c r="I28" s="102"/>
       <c r="J28" s="102"/>
@@ -4700,12 +4704,12 @@
     </row>
     <row r="29" spans="1:15">
       <c r="A29" s="108"/>
-      <c r="B29" s="152"/>
-      <c r="C29" s="152"/>
-      <c r="D29" s="152"/>
-      <c r="E29" s="152"/>
-      <c r="F29" s="152"/>
-      <c r="G29" s="152"/>
+      <c r="B29" s="159"/>
+      <c r="C29" s="159"/>
+      <c r="D29" s="159"/>
+      <c r="E29" s="159"/>
+      <c r="F29" s="159"/>
+      <c r="G29" s="159"/>
       <c r="H29" s="102"/>
       <c r="I29" s="102"/>
       <c r="J29" s="102"/>
@@ -4718,28 +4722,28 @@
       <c r="C30"/>
     </row>
     <row r="31" spans="1:15">
-      <c r="A31" s="166" t="s">
+      <c r="A31" s="143" t="s">
         <v>184</v>
       </c>
-      <c r="B31" s="167"/>
-      <c r="C31" s="167"/>
-      <c r="D31" s="167"/>
-      <c r="E31" s="167"/>
-      <c r="F31" s="167"/>
-      <c r="G31" s="168"/>
+      <c r="B31" s="144"/>
+      <c r="C31" s="144"/>
+      <c r="D31" s="144"/>
+      <c r="E31" s="144"/>
+      <c r="F31" s="144"/>
+      <c r="G31" s="145"/>
     </row>
     <row r="32" spans="1:15">
       <c r="A32" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="144" t="s">
+      <c r="B32" s="164" t="s">
         <v>178</v>
       </c>
-      <c r="C32" s="144"/>
-      <c r="D32" s="144"/>
-      <c r="E32" s="144"/>
-      <c r="F32" s="144"/>
-      <c r="G32" s="144"/>
+      <c r="C32" s="164"/>
+      <c r="D32" s="164"/>
+      <c r="E32" s="164"/>
+      <c r="F32" s="164"/>
+      <c r="G32" s="164"/>
       <c r="H32" s="95"/>
       <c r="I32" s="95"/>
       <c r="J32" s="95"/>
@@ -4752,14 +4756,14 @@
       <c r="A33" s="106">
         <v>1</v>
       </c>
-      <c r="B33" s="145" t="s">
+      <c r="B33" s="165" t="s">
         <v>179</v>
       </c>
-      <c r="C33" s="145"/>
-      <c r="D33" s="145"/>
-      <c r="E33" s="145"/>
-      <c r="F33" s="145"/>
-      <c r="G33" s="145"/>
+      <c r="C33" s="165"/>
+      <c r="D33" s="165"/>
+      <c r="E33" s="165"/>
+      <c r="F33" s="165"/>
+      <c r="G33" s="165"/>
       <c r="H33" s="102"/>
       <c r="I33" s="102"/>
       <c r="J33" s="102"/>
@@ -4770,12 +4774,12 @@
     </row>
     <row r="34" spans="1:15">
       <c r="A34" s="107"/>
-      <c r="B34" s="146"/>
-      <c r="C34" s="146"/>
-      <c r="D34" s="146"/>
-      <c r="E34" s="146"/>
-      <c r="F34" s="146"/>
-      <c r="G34" s="146"/>
+      <c r="B34" s="166"/>
+      <c r="C34" s="166"/>
+      <c r="D34" s="166"/>
+      <c r="E34" s="166"/>
+      <c r="F34" s="166"/>
+      <c r="G34" s="166"/>
       <c r="H34" s="102"/>
       <c r="I34" s="102"/>
       <c r="J34" s="102"/>
@@ -4786,12 +4790,12 @@
     </row>
     <row r="35" spans="1:15">
       <c r="A35" s="108"/>
-      <c r="B35" s="147"/>
-      <c r="C35" s="147"/>
-      <c r="D35" s="147"/>
-      <c r="E35" s="147"/>
-      <c r="F35" s="147"/>
-      <c r="G35" s="147"/>
+      <c r="B35" s="167"/>
+      <c r="C35" s="167"/>
+      <c r="D35" s="167"/>
+      <c r="E35" s="167"/>
+      <c r="F35" s="167"/>
+      <c r="G35" s="167"/>
       <c r="H35" s="102"/>
       <c r="I35" s="102"/>
       <c r="J35" s="102"/>
@@ -4816,28 +4820,28 @@
       <c r="M36"/>
     </row>
     <row r="37" spans="1:15">
-      <c r="A37" s="166" t="s">
+      <c r="A37" s="143" t="s">
         <v>185</v>
       </c>
-      <c r="B37" s="167"/>
-      <c r="C37" s="167"/>
-      <c r="D37" s="167"/>
-      <c r="E37" s="167"/>
-      <c r="F37" s="167"/>
-      <c r="G37" s="168"/>
+      <c r="B37" s="144"/>
+      <c r="C37" s="144"/>
+      <c r="D37" s="144"/>
+      <c r="E37" s="144"/>
+      <c r="F37" s="144"/>
+      <c r="G37" s="145"/>
     </row>
     <row r="38" spans="1:15">
       <c r="A38" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B38" s="144" t="s">
+      <c r="B38" s="164" t="s">
         <v>180</v>
       </c>
-      <c r="C38" s="144"/>
-      <c r="D38" s="144"/>
-      <c r="E38" s="144"/>
-      <c r="F38" s="144"/>
-      <c r="G38" s="144"/>
+      <c r="C38" s="164"/>
+      <c r="D38" s="164"/>
+      <c r="E38" s="164"/>
+      <c r="F38" s="164"/>
+      <c r="G38" s="164"/>
       <c r="H38" s="95"/>
       <c r="I38" s="95"/>
       <c r="J38" s="95"/>
@@ -4848,12 +4852,12 @@
     </row>
     <row r="39" spans="1:15">
       <c r="A39" s="106"/>
-      <c r="B39" s="148"/>
-      <c r="C39" s="148"/>
-      <c r="D39" s="148"/>
-      <c r="E39" s="148"/>
-      <c r="F39" s="148"/>
-      <c r="G39" s="149"/>
+      <c r="B39" s="157"/>
+      <c r="C39" s="157"/>
+      <c r="D39" s="157"/>
+      <c r="E39" s="157"/>
+      <c r="F39" s="157"/>
+      <c r="G39" s="168"/>
       <c r="H39" s="102"/>
       <c r="I39" s="102"/>
       <c r="J39" s="102"/>
@@ -4864,12 +4868,12 @@
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="107"/>
-      <c r="B40" s="150"/>
-      <c r="C40" s="150"/>
-      <c r="D40" s="150"/>
-      <c r="E40" s="150"/>
-      <c r="F40" s="150"/>
-      <c r="G40" s="151"/>
+      <c r="B40" s="158"/>
+      <c r="C40" s="158"/>
+      <c r="D40" s="158"/>
+      <c r="E40" s="158"/>
+      <c r="F40" s="158"/>
+      <c r="G40" s="169"/>
       <c r="H40" s="102"/>
       <c r="I40" s="102"/>
       <c r="J40" s="102"/>
@@ -4880,12 +4884,12 @@
     </row>
     <row r="41" spans="1:15">
       <c r="A41" s="108"/>
-      <c r="B41" s="152"/>
-      <c r="C41" s="152"/>
-      <c r="D41" s="152"/>
-      <c r="E41" s="152"/>
-      <c r="F41" s="152"/>
-      <c r="G41" s="153"/>
+      <c r="B41" s="159"/>
+      <c r="C41" s="159"/>
+      <c r="D41" s="159"/>
+      <c r="E41" s="159"/>
+      <c r="F41" s="159"/>
+      <c r="G41" s="170"/>
       <c r="H41" s="102"/>
       <c r="I41" s="102"/>
       <c r="J41" s="102"/>
@@ -4911,15 +4915,15 @@
       <c r="O42"/>
     </row>
     <row r="43" spans="1:15">
-      <c r="A43" s="169" t="s">
+      <c r="A43" s="146" t="s">
         <v>205</v>
       </c>
-      <c r="B43" s="169"/>
-      <c r="C43" s="169"/>
-      <c r="D43" s="169"/>
-      <c r="E43" s="169"/>
-      <c r="F43" s="169"/>
-      <c r="G43" s="169"/>
+      <c r="B43" s="146"/>
+      <c r="C43" s="146"/>
+      <c r="D43" s="146"/>
+      <c r="E43" s="146"/>
+      <c r="F43" s="146"/>
+      <c r="G43" s="146"/>
     </row>
     <row r="44" spans="1:15">
       <c r="A44" s="105" t="s">
@@ -5035,231 +5039,289 @@
       <c r="F49" s="5"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="157" t="s">
+      <c r="A50" s="131" t="s">
         <v>64</v>
       </c>
-      <c r="B50" s="159"/>
-      <c r="C50" s="157" t="s">
+      <c r="B50" s="133"/>
+      <c r="C50" s="131" t="s">
         <v>65</v>
       </c>
-      <c r="D50" s="158"/>
-      <c r="E50" s="159"/>
+      <c r="D50" s="132"/>
+      <c r="E50" s="133"/>
       <c r="F50" s="27" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="154"/>
-      <c r="B51" s="156"/>
-      <c r="C51" s="154"/>
-      <c r="D51" s="155"/>
-      <c r="E51" s="156"/>
+      <c r="A51" s="138"/>
+      <c r="B51" s="139"/>
+      <c r="C51" s="138"/>
+      <c r="D51" s="160"/>
+      <c r="E51" s="139"/>
       <c r="F51" s="43"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="138"/>
-      <c r="B52" s="140"/>
-      <c r="C52" s="138"/>
-      <c r="D52" s="139"/>
-      <c r="E52" s="140"/>
+      <c r="A52" s="129"/>
+      <c r="B52" s="130"/>
+      <c r="C52" s="129"/>
+      <c r="D52" s="161"/>
+      <c r="E52" s="130"/>
       <c r="F52" s="43"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="138"/>
-      <c r="B53" s="140"/>
-      <c r="C53" s="138"/>
-      <c r="D53" s="139"/>
-      <c r="E53" s="140"/>
+      <c r="A53" s="129"/>
+      <c r="B53" s="130"/>
+      <c r="C53" s="129"/>
+      <c r="D53" s="161"/>
+      <c r="E53" s="130"/>
       <c r="F53" s="43"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="138"/>
-      <c r="B54" s="140"/>
-      <c r="C54" s="138"/>
-      <c r="D54" s="139"/>
-      <c r="E54" s="140"/>
+      <c r="A54" s="129"/>
+      <c r="B54" s="130"/>
+      <c r="C54" s="129"/>
+      <c r="D54" s="161"/>
+      <c r="E54" s="130"/>
       <c r="F54" s="43"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="138"/>
-      <c r="B55" s="140"/>
-      <c r="C55" s="138"/>
-      <c r="D55" s="139"/>
-      <c r="E55" s="140"/>
+      <c r="A55" s="129"/>
+      <c r="B55" s="130"/>
+      <c r="C55" s="129"/>
+      <c r="D55" s="161"/>
+      <c r="E55" s="130"/>
       <c r="F55" s="43"/>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="138"/>
-      <c r="B56" s="140"/>
-      <c r="C56" s="138"/>
-      <c r="D56" s="139"/>
-      <c r="E56" s="140"/>
+      <c r="A56" s="129"/>
+      <c r="B56" s="130"/>
+      <c r="C56" s="129"/>
+      <c r="D56" s="161"/>
+      <c r="E56" s="130"/>
       <c r="F56" s="43"/>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="138"/>
-      <c r="B57" s="140"/>
-      <c r="C57" s="138"/>
-      <c r="D57" s="139"/>
-      <c r="E57" s="140"/>
+      <c r="A57" s="129"/>
+      <c r="B57" s="130"/>
+      <c r="C57" s="129"/>
+      <c r="D57" s="161"/>
+      <c r="E57" s="130"/>
       <c r="F57" s="43"/>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="138"/>
-      <c r="B58" s="140"/>
-      <c r="C58" s="138"/>
-      <c r="D58" s="139"/>
-      <c r="E58" s="140"/>
+      <c r="A58" s="129"/>
+      <c r="B58" s="130"/>
+      <c r="C58" s="129"/>
+      <c r="D58" s="161"/>
+      <c r="E58" s="130"/>
       <c r="F58" s="43"/>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="138"/>
-      <c r="B59" s="140"/>
-      <c r="C59" s="138"/>
-      <c r="D59" s="139"/>
-      <c r="E59" s="140"/>
+      <c r="A59" s="129"/>
+      <c r="B59" s="130"/>
+      <c r="C59" s="129"/>
+      <c r="D59" s="161"/>
+      <c r="E59" s="130"/>
       <c r="F59" s="43"/>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="138"/>
-      <c r="B60" s="140"/>
-      <c r="C60" s="138"/>
-      <c r="D60" s="139"/>
-      <c r="E60" s="140"/>
+      <c r="A60" s="129"/>
+      <c r="B60" s="130"/>
+      <c r="C60" s="129"/>
+      <c r="D60" s="161"/>
+      <c r="E60" s="130"/>
       <c r="F60" s="43"/>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="138"/>
-      <c r="B61" s="140"/>
-      <c r="C61" s="138"/>
-      <c r="D61" s="139"/>
-      <c r="E61" s="140"/>
+      <c r="A61" s="129"/>
+      <c r="B61" s="130"/>
+      <c r="C61" s="129"/>
+      <c r="D61" s="161"/>
+      <c r="E61" s="130"/>
       <c r="F61" s="43"/>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="138"/>
-      <c r="B62" s="140"/>
-      <c r="C62" s="138"/>
-      <c r="D62" s="139"/>
-      <c r="E62" s="140"/>
+      <c r="A62" s="129"/>
+      <c r="B62" s="130"/>
+      <c r="C62" s="129"/>
+      <c r="D62" s="161"/>
+      <c r="E62" s="130"/>
       <c r="F62" s="43"/>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="138"/>
-      <c r="B63" s="140"/>
-      <c r="C63" s="138"/>
-      <c r="D63" s="139"/>
-      <c r="E63" s="140"/>
+      <c r="A63" s="129"/>
+      <c r="B63" s="130"/>
+      <c r="C63" s="129"/>
+      <c r="D63" s="161"/>
+      <c r="E63" s="130"/>
       <c r="F63" s="43"/>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="138"/>
-      <c r="B64" s="140"/>
-      <c r="C64" s="138"/>
-      <c r="D64" s="139"/>
-      <c r="E64" s="140"/>
+      <c r="A64" s="129"/>
+      <c r="B64" s="130"/>
+      <c r="C64" s="129"/>
+      <c r="D64" s="161"/>
+      <c r="E64" s="130"/>
       <c r="F64" s="43"/>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="138"/>
-      <c r="B65" s="140"/>
-      <c r="C65" s="138"/>
-      <c r="D65" s="139"/>
-      <c r="E65" s="140"/>
+      <c r="A65" s="129"/>
+      <c r="B65" s="130"/>
+      <c r="C65" s="129"/>
+      <c r="D65" s="161"/>
+      <c r="E65" s="130"/>
       <c r="F65" s="43"/>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="138"/>
-      <c r="B66" s="140"/>
-      <c r="C66" s="138"/>
-      <c r="D66" s="139"/>
-      <c r="E66" s="140"/>
+      <c r="A66" s="129"/>
+      <c r="B66" s="130"/>
+      <c r="C66" s="129"/>
+      <c r="D66" s="161"/>
+      <c r="E66" s="130"/>
       <c r="F66" s="43"/>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="138"/>
-      <c r="B67" s="140"/>
-      <c r="C67" s="138"/>
-      <c r="D67" s="139"/>
-      <c r="E67" s="140"/>
+      <c r="A67" s="129"/>
+      <c r="B67" s="130"/>
+      <c r="C67" s="129"/>
+      <c r="D67" s="161"/>
+      <c r="E67" s="130"/>
       <c r="F67" s="43"/>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="138"/>
-      <c r="B68" s="140"/>
-      <c r="C68" s="138"/>
-      <c r="D68" s="139"/>
-      <c r="E68" s="140"/>
+      <c r="A68" s="129"/>
+      <c r="B68" s="130"/>
+      <c r="C68" s="129"/>
+      <c r="D68" s="161"/>
+      <c r="E68" s="130"/>
       <c r="F68" s="43"/>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="138"/>
-      <c r="B69" s="140"/>
-      <c r="C69" s="138"/>
-      <c r="D69" s="139"/>
-      <c r="E69" s="140"/>
+      <c r="A69" s="129"/>
+      <c r="B69" s="130"/>
+      <c r="C69" s="129"/>
+      <c r="D69" s="161"/>
+      <c r="E69" s="130"/>
       <c r="F69" s="43"/>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="138"/>
-      <c r="B70" s="140"/>
-      <c r="C70" s="138"/>
-      <c r="D70" s="139"/>
-      <c r="E70" s="140"/>
+      <c r="A70" s="129"/>
+      <c r="B70" s="130"/>
+      <c r="C70" s="129"/>
+      <c r="D70" s="161"/>
+      <c r="E70" s="130"/>
       <c r="F70" s="43"/>
     </row>
     <row r="71" spans="1:6">
-      <c r="A71" s="138"/>
-      <c r="B71" s="140"/>
-      <c r="C71" s="138"/>
-      <c r="D71" s="139"/>
-      <c r="E71" s="140"/>
+      <c r="A71" s="129"/>
+      <c r="B71" s="130"/>
+      <c r="C71" s="129"/>
+      <c r="D71" s="161"/>
+      <c r="E71" s="130"/>
       <c r="F71" s="43"/>
     </row>
     <row r="72" spans="1:6">
-      <c r="A72" s="138"/>
-      <c r="B72" s="140"/>
-      <c r="C72" s="138"/>
-      <c r="D72" s="139"/>
-      <c r="E72" s="140"/>
+      <c r="A72" s="129"/>
+      <c r="B72" s="130"/>
+      <c r="C72" s="129"/>
+      <c r="D72" s="161"/>
+      <c r="E72" s="130"/>
       <c r="F72" s="43"/>
     </row>
     <row r="73" spans="1:6">
-      <c r="A73" s="138"/>
-      <c r="B73" s="140"/>
-      <c r="C73" s="138"/>
-      <c r="D73" s="139"/>
-      <c r="E73" s="140"/>
+      <c r="A73" s="129"/>
+      <c r="B73" s="130"/>
+      <c r="C73" s="129"/>
+      <c r="D73" s="161"/>
+      <c r="E73" s="130"/>
       <c r="F73" s="43"/>
     </row>
     <row r="74" spans="1:6">
-      <c r="A74" s="138"/>
-      <c r="B74" s="140"/>
-      <c r="C74" s="138"/>
-      <c r="D74" s="139"/>
-      <c r="E74" s="140"/>
+      <c r="A74" s="129"/>
+      <c r="B74" s="130"/>
+      <c r="C74" s="129"/>
+      <c r="D74" s="161"/>
+      <c r="E74" s="130"/>
       <c r="F74" s="43"/>
     </row>
     <row r="75" spans="1:6">
-      <c r="A75" s="141"/>
-      <c r="B75" s="143"/>
-      <c r="C75" s="141"/>
-      <c r="D75" s="142"/>
-      <c r="E75" s="143"/>
+      <c r="A75" s="155"/>
+      <c r="B75" s="156"/>
+      <c r="C75" s="155"/>
+      <c r="D75" s="163"/>
+      <c r="E75" s="156"/>
       <c r="F75" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="94">
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C75:E75"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C73:E73"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
     <mergeCell ref="C50:E50"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A18:C18"/>
@@ -5276,74 +5338,16 @@
     <mergeCell ref="A43:G43"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="D13:E13"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C73:E73"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="C75:E75"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="2">
@@ -5381,8 +5385,8 @@
   </sheetPr>
   <dimension ref="A1:V67"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" activeCellId="1" sqref="C14 C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -5513,7 +5517,9 @@
         <v>232</v>
       </c>
       <c r="B13" s="5"/>
-      <c r="C13" s="46"/>
+      <c r="C13" s="46" t="s">
+        <v>244</v>
+      </c>
       <c r="D13" s="33"/>
       <c r="E13" s="1" t="s">
         <v>231</v>
@@ -5542,10 +5548,10 @@
         <v>168</v>
       </c>
       <c r="B16" s="111"/>
-      <c r="C16" s="133" t="s">
+      <c r="C16" s="151" t="s">
         <v>169</v>
       </c>
-      <c r="D16" s="133"/>
+      <c r="D16" s="151"/>
       <c r="E16" s="1" t="s">
         <v>170</v>
       </c>
@@ -5555,20 +5561,20 @@
         <v>171</v>
       </c>
       <c r="B17" s="111"/>
-      <c r="C17" s="133" t="s">
+      <c r="C17" s="151" t="s">
         <v>172</v>
       </c>
-      <c r="D17" s="133"/>
+      <c r="D17" s="151"/>
     </row>
     <row r="18" spans="1:22">
       <c r="A18" s="111" t="s">
         <v>208</v>
       </c>
       <c r="B18" s="111"/>
-      <c r="C18" s="132" t="s">
+      <c r="C18" s="150" t="s">
         <v>210</v>
       </c>
-      <c r="D18" s="133"/>
+      <c r="D18" s="151"/>
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="112" t="s">
@@ -5626,28 +5632,28 @@
       <c r="A21" s="6"/>
     </row>
     <row r="22" spans="1:22">
-      <c r="A22" s="169" t="s">
+      <c r="A22" s="146" t="s">
         <v>186</v>
       </c>
-      <c r="B22" s="169"/>
-      <c r="C22" s="169"/>
-      <c r="D22" s="169"/>
-      <c r="E22" s="169"/>
-      <c r="F22" s="169"/>
-      <c r="G22" s="169"/>
+      <c r="B22" s="146"/>
+      <c r="C22" s="146"/>
+      <c r="D22" s="146"/>
+      <c r="E22" s="146"/>
+      <c r="F22" s="146"/>
+      <c r="G22" s="146"/>
     </row>
     <row r="23" spans="1:22">
       <c r="A23" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="163" t="s">
+      <c r="B23" s="140" t="s">
         <v>177</v>
       </c>
-      <c r="C23" s="164"/>
-      <c r="D23" s="164"/>
-      <c r="E23" s="164"/>
-      <c r="F23" s="164"/>
-      <c r="G23" s="165"/>
+      <c r="C23" s="141"/>
+      <c r="D23" s="141"/>
+      <c r="E23" s="141"/>
+      <c r="F23" s="141"/>
+      <c r="G23" s="142"/>
       <c r="H23" s="95"/>
       <c r="I23" s="95"/>
       <c r="J23" s="95"/>
@@ -5665,12 +5671,12 @@
     </row>
     <row r="24" spans="1:22">
       <c r="A24" s="106"/>
-      <c r="B24" s="148"/>
-      <c r="C24" s="148"/>
-      <c r="D24" s="148"/>
-      <c r="E24" s="148"/>
-      <c r="F24" s="148"/>
-      <c r="G24" s="148"/>
+      <c r="B24" s="157"/>
+      <c r="C24" s="157"/>
+      <c r="D24" s="157"/>
+      <c r="E24" s="157"/>
+      <c r="F24" s="157"/>
+      <c r="G24" s="157"/>
       <c r="H24" s="102"/>
       <c r="I24" s="102"/>
       <c r="J24" s="102"/>
@@ -5688,12 +5694,12 @@
     </row>
     <row r="25" spans="1:22">
       <c r="A25" s="107"/>
-      <c r="B25" s="150"/>
-      <c r="C25" s="150"/>
-      <c r="D25" s="150"/>
-      <c r="E25" s="150"/>
-      <c r="F25" s="150"/>
-      <c r="G25" s="150"/>
+      <c r="B25" s="158"/>
+      <c r="C25" s="158"/>
+      <c r="D25" s="158"/>
+      <c r="E25" s="158"/>
+      <c r="F25" s="158"/>
+      <c r="G25" s="158"/>
       <c r="H25" s="102"/>
       <c r="I25" s="102"/>
       <c r="J25" s="102"/>
@@ -5711,12 +5717,12 @@
     </row>
     <row r="26" spans="1:22">
       <c r="A26" s="108"/>
-      <c r="B26" s="152"/>
-      <c r="C26" s="152"/>
-      <c r="D26" s="152"/>
-      <c r="E26" s="152"/>
-      <c r="F26" s="152"/>
-      <c r="G26" s="152"/>
+      <c r="B26" s="159"/>
+      <c r="C26" s="159"/>
+      <c r="D26" s="159"/>
+      <c r="E26" s="159"/>
+      <c r="F26" s="159"/>
+      <c r="G26" s="159"/>
       <c r="H26" s="102"/>
       <c r="I26" s="102"/>
       <c r="J26" s="102"/>
@@ -5736,28 +5742,28 @@
       <c r="C27"/>
     </row>
     <row r="28" spans="1:22">
-      <c r="A28" s="166" t="s">
+      <c r="A28" s="143" t="s">
         <v>187</v>
       </c>
-      <c r="B28" s="167"/>
-      <c r="C28" s="167"/>
-      <c r="D28" s="167"/>
-      <c r="E28" s="167"/>
-      <c r="F28" s="167"/>
-      <c r="G28" s="168"/>
+      <c r="B28" s="144"/>
+      <c r="C28" s="144"/>
+      <c r="D28" s="144"/>
+      <c r="E28" s="144"/>
+      <c r="F28" s="144"/>
+      <c r="G28" s="145"/>
     </row>
     <row r="29" spans="1:22">
       <c r="A29" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="144" t="s">
+      <c r="B29" s="164" t="s">
         <v>178</v>
       </c>
-      <c r="C29" s="144"/>
-      <c r="D29" s="144"/>
-      <c r="E29" s="144"/>
-      <c r="F29" s="144"/>
-      <c r="G29" s="144"/>
+      <c r="C29" s="164"/>
+      <c r="D29" s="164"/>
+      <c r="E29" s="164"/>
+      <c r="F29" s="164"/>
+      <c r="G29" s="164"/>
       <c r="H29" s="95"/>
       <c r="I29" s="95"/>
       <c r="J29" s="95"/>
@@ -5777,14 +5783,14 @@
       <c r="A30" s="106">
         <v>1</v>
       </c>
-      <c r="B30" s="145" t="s">
+      <c r="B30" s="165" t="s">
         <v>179</v>
       </c>
-      <c r="C30" s="145"/>
-      <c r="D30" s="145"/>
-      <c r="E30" s="145"/>
-      <c r="F30" s="145"/>
-      <c r="G30" s="145"/>
+      <c r="C30" s="165"/>
+      <c r="D30" s="165"/>
+      <c r="E30" s="165"/>
+      <c r="F30" s="165"/>
+      <c r="G30" s="165"/>
       <c r="H30" s="102"/>
       <c r="I30" s="102"/>
       <c r="J30" s="102"/>
@@ -5802,12 +5808,12 @@
     </row>
     <row r="31" spans="1:22">
       <c r="A31" s="107"/>
-      <c r="B31" s="146"/>
-      <c r="C31" s="146"/>
-      <c r="D31" s="146"/>
-      <c r="E31" s="146"/>
-      <c r="F31" s="146"/>
-      <c r="G31" s="146"/>
+      <c r="B31" s="166"/>
+      <c r="C31" s="166"/>
+      <c r="D31" s="166"/>
+      <c r="E31" s="166"/>
+      <c r="F31" s="166"/>
+      <c r="G31" s="166"/>
       <c r="H31" s="102"/>
       <c r="I31" s="102"/>
       <c r="J31" s="102"/>
@@ -5825,12 +5831,12 @@
     </row>
     <row r="32" spans="1:22">
       <c r="A32" s="108"/>
-      <c r="B32" s="147"/>
-      <c r="C32" s="147"/>
-      <c r="D32" s="147"/>
-      <c r="E32" s="147"/>
-      <c r="F32" s="147"/>
-      <c r="G32" s="147"/>
+      <c r="B32" s="167"/>
+      <c r="C32" s="167"/>
+      <c r="D32" s="167"/>
+      <c r="E32" s="167"/>
+      <c r="F32" s="167"/>
+      <c r="G32" s="167"/>
       <c r="H32" s="102"/>
       <c r="I32" s="102"/>
       <c r="J32" s="102"/>
@@ -5869,28 +5875,28 @@
       <c r="T33"/>
     </row>
     <row r="34" spans="1:22">
-      <c r="A34" s="166" t="s">
+      <c r="A34" s="143" t="s">
         <v>188</v>
       </c>
-      <c r="B34" s="167"/>
-      <c r="C34" s="167"/>
-      <c r="D34" s="167"/>
-      <c r="E34" s="167"/>
-      <c r="F34" s="167"/>
-      <c r="G34" s="168"/>
+      <c r="B34" s="144"/>
+      <c r="C34" s="144"/>
+      <c r="D34" s="144"/>
+      <c r="E34" s="144"/>
+      <c r="F34" s="144"/>
+      <c r="G34" s="145"/>
     </row>
     <row r="35" spans="1:22">
       <c r="A35" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="144" t="s">
+      <c r="B35" s="164" t="s">
         <v>180</v>
       </c>
-      <c r="C35" s="144"/>
-      <c r="D35" s="144"/>
-      <c r="E35" s="144"/>
-      <c r="F35" s="144"/>
-      <c r="G35" s="144"/>
+      <c r="C35" s="164"/>
+      <c r="D35" s="164"/>
+      <c r="E35" s="164"/>
+      <c r="F35" s="164"/>
+      <c r="G35" s="164"/>
       <c r="H35" s="95"/>
       <c r="I35" s="95"/>
       <c r="J35" s="95"/>
@@ -5908,12 +5914,12 @@
     </row>
     <row r="36" spans="1:22">
       <c r="A36" s="106"/>
-      <c r="B36" s="148"/>
-      <c r="C36" s="148"/>
-      <c r="D36" s="148"/>
-      <c r="E36" s="148"/>
-      <c r="F36" s="148"/>
-      <c r="G36" s="149"/>
+      <c r="B36" s="157"/>
+      <c r="C36" s="157"/>
+      <c r="D36" s="157"/>
+      <c r="E36" s="157"/>
+      <c r="F36" s="157"/>
+      <c r="G36" s="168"/>
       <c r="H36" s="102"/>
       <c r="I36" s="102"/>
       <c r="J36" s="102"/>
@@ -5931,12 +5937,12 @@
     </row>
     <row r="37" spans="1:22">
       <c r="A37" s="107"/>
-      <c r="B37" s="150"/>
-      <c r="C37" s="150"/>
-      <c r="D37" s="150"/>
-      <c r="E37" s="150"/>
-      <c r="F37" s="150"/>
-      <c r="G37" s="151"/>
+      <c r="B37" s="158"/>
+      <c r="C37" s="158"/>
+      <c r="D37" s="158"/>
+      <c r="E37" s="158"/>
+      <c r="F37" s="158"/>
+      <c r="G37" s="169"/>
       <c r="H37" s="102"/>
       <c r="I37" s="102"/>
       <c r="J37" s="102"/>
@@ -5954,12 +5960,12 @@
     </row>
     <row r="38" spans="1:22">
       <c r="A38" s="108"/>
-      <c r="B38" s="152"/>
-      <c r="C38" s="152"/>
-      <c r="D38" s="152"/>
-      <c r="E38" s="152"/>
-      <c r="F38" s="152"/>
-      <c r="G38" s="153"/>
+      <c r="B38" s="159"/>
+      <c r="C38" s="159"/>
+      <c r="D38" s="159"/>
+      <c r="E38" s="159"/>
+      <c r="F38" s="159"/>
+      <c r="G38" s="170"/>
       <c r="H38" s="102"/>
       <c r="I38" s="102"/>
       <c r="J38" s="102"/>
@@ -6035,16 +6041,16 @@
       <c r="B42" s="176" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="182" t="s">
+      <c r="C42" s="178" t="s">
         <v>1</v>
       </c>
       <c r="D42" s="176" t="s">
         <v>2</v>
       </c>
-      <c r="E42" s="180" t="s">
+      <c r="E42" s="181" t="s">
         <v>156</v>
       </c>
-      <c r="F42" s="180" t="s">
+      <c r="F42" s="181" t="s">
         <v>171</v>
       </c>
       <c r="G42" s="176" t="s">
@@ -6056,13 +6062,13 @@
       <c r="I42" s="176" t="s">
         <v>237</v>
       </c>
-      <c r="J42" s="180" t="s">
+      <c r="J42" s="181" t="s">
         <v>238</v>
       </c>
-      <c r="K42" s="180" t="s">
+      <c r="K42" s="181" t="s">
         <v>208</v>
       </c>
-      <c r="L42" s="179" t="s">
+      <c r="L42" s="184" t="s">
         <v>225</v>
       </c>
       <c r="M42" s="176" t="s">
@@ -6074,14 +6080,14 @@
       <c r="O42" s="176" t="s">
         <v>190</v>
       </c>
-      <c r="P42" s="183" t="s">
+      <c r="P42" s="179" t="s">
         <v>70</v>
       </c>
-      <c r="Q42" s="184"/>
-      <c r="R42" s="183" t="s">
+      <c r="Q42" s="180"/>
+      <c r="R42" s="179" t="s">
         <v>16</v>
       </c>
-      <c r="S42" s="184"/>
+      <c r="S42" s="180"/>
       <c r="T42" s="32" t="s">
         <v>69</v>
       </c>
@@ -6090,21 +6096,21 @@
       </c>
     </row>
     <row r="43" spans="1:22">
-      <c r="A43" s="178"/>
-      <c r="B43" s="178"/>
-      <c r="C43" s="178"/>
-      <c r="D43" s="178"/>
-      <c r="E43" s="181"/>
-      <c r="F43" s="181"/>
-      <c r="G43" s="178"/>
-      <c r="H43" s="178"/>
-      <c r="I43" s="178"/>
-      <c r="J43" s="181"/>
-      <c r="K43" s="181"/>
-      <c r="L43" s="177"/>
-      <c r="M43" s="178"/>
-      <c r="N43" s="178"/>
-      <c r="O43" s="177"/>
+      <c r="A43" s="177"/>
+      <c r="B43" s="177"/>
+      <c r="C43" s="177"/>
+      <c r="D43" s="177"/>
+      <c r="E43" s="182"/>
+      <c r="F43" s="182"/>
+      <c r="G43" s="177"/>
+      <c r="H43" s="177"/>
+      <c r="I43" s="177"/>
+      <c r="J43" s="182"/>
+      <c r="K43" s="182"/>
+      <c r="L43" s="183"/>
+      <c r="M43" s="177"/>
+      <c r="N43" s="177"/>
+      <c r="O43" s="183"/>
       <c r="P43" s="27" t="s">
         <v>74</v>
       </c>
@@ -6120,7 +6126,7 @@
       <c r="T43" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="U43" s="178"/>
+      <c r="U43" s="177"/>
     </row>
     <row r="44" spans="1:22">
       <c r="A44" s="7">
@@ -6776,6 +6782,26 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="O42:O43"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="M42:M43"/>
+    <mergeCell ref="H42:H43"/>
+    <mergeCell ref="L42:L43"/>
+    <mergeCell ref="K42:K43"/>
+    <mergeCell ref="I42:I43"/>
+    <mergeCell ref="J42:J43"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="A22:G22"/>
@@ -6792,26 +6818,6 @@
     <mergeCell ref="F42:F43"/>
     <mergeCell ref="B23:G23"/>
     <mergeCell ref="B24:G24"/>
-    <mergeCell ref="O42:O43"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="A34:G34"/>
-    <mergeCell ref="M42:M43"/>
-    <mergeCell ref="H42:H43"/>
-    <mergeCell ref="L42:L43"/>
-    <mergeCell ref="K42:K43"/>
-    <mergeCell ref="I42:I43"/>
-    <mergeCell ref="J42:J43"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="B35:G35"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="4">
@@ -7004,10 +7010,10 @@
         <v>168</v>
       </c>
       <c r="B13" s="111"/>
-      <c r="C13" s="133" t="s">
+      <c r="C13" s="151" t="s">
         <v>169</v>
       </c>
-      <c r="D13" s="133"/>
+      <c r="D13" s="151"/>
       <c r="E13" s="1" t="s">
         <v>170</v>
       </c>
@@ -7017,10 +7023,10 @@
         <v>171</v>
       </c>
       <c r="B14" s="111"/>
-      <c r="C14" s="133" t="s">
+      <c r="C14" s="151" t="s">
         <v>172</v>
       </c>
-      <c r="D14" s="133"/>
+      <c r="D14" s="151"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="112" t="s">
@@ -7046,28 +7052,28 @@
       <c r="A16" s="6"/>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="169" t="s">
+      <c r="A17" s="146" t="s">
         <v>186</v>
       </c>
-      <c r="B17" s="169"/>
-      <c r="C17" s="169"/>
-      <c r="D17" s="169"/>
-      <c r="E17" s="169"/>
-      <c r="F17" s="169"/>
-      <c r="G17" s="169"/>
+      <c r="B17" s="146"/>
+      <c r="C17" s="146"/>
+      <c r="D17" s="146"/>
+      <c r="E17" s="146"/>
+      <c r="F17" s="146"/>
+      <c r="G17" s="146"/>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="163" t="s">
+      <c r="B18" s="140" t="s">
         <v>177</v>
       </c>
-      <c r="C18" s="164"/>
-      <c r="D18" s="164"/>
-      <c r="E18" s="164"/>
-      <c r="F18" s="164"/>
-      <c r="G18" s="165"/>
+      <c r="C18" s="141"/>
+      <c r="D18" s="141"/>
+      <c r="E18" s="141"/>
+      <c r="F18" s="141"/>
+      <c r="G18" s="142"/>
       <c r="H18" s="95"/>
       <c r="I18" s="95"/>
       <c r="K18" s="95"/>
@@ -7079,12 +7085,12 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="106"/>
-      <c r="B19" s="148"/>
-      <c r="C19" s="148"/>
-      <c r="D19" s="148"/>
-      <c r="E19" s="148"/>
-      <c r="F19" s="148"/>
-      <c r="G19" s="148"/>
+      <c r="B19" s="157"/>
+      <c r="C19" s="157"/>
+      <c r="D19" s="157"/>
+      <c r="E19" s="157"/>
+      <c r="F19" s="157"/>
+      <c r="G19" s="157"/>
       <c r="H19" s="102"/>
       <c r="I19" s="102"/>
       <c r="K19" s="102"/>
@@ -7096,12 +7102,12 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="107"/>
-      <c r="B20" s="150"/>
-      <c r="C20" s="150"/>
-      <c r="D20" s="150"/>
-      <c r="E20" s="150"/>
-      <c r="F20" s="150"/>
-      <c r="G20" s="150"/>
+      <c r="B20" s="158"/>
+      <c r="C20" s="158"/>
+      <c r="D20" s="158"/>
+      <c r="E20" s="158"/>
+      <c r="F20" s="158"/>
+      <c r="G20" s="158"/>
       <c r="H20" s="102"/>
       <c r="I20" s="102"/>
       <c r="K20" s="102"/>
@@ -7113,12 +7119,12 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="108"/>
-      <c r="B21" s="152"/>
-      <c r="C21" s="152"/>
-      <c r="D21" s="152"/>
-      <c r="E21" s="152"/>
-      <c r="F21" s="152"/>
-      <c r="G21" s="152"/>
+      <c r="B21" s="159"/>
+      <c r="C21" s="159"/>
+      <c r="D21" s="159"/>
+      <c r="E21" s="159"/>
+      <c r="F21" s="159"/>
+      <c r="G21" s="159"/>
       <c r="H21" s="102"/>
       <c r="I21" s="102"/>
       <c r="J21" s="95"/>
@@ -7134,29 +7140,29 @@
       <c r="J22" s="102"/>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="166" t="s">
+      <c r="A23" s="143" t="s">
         <v>187</v>
       </c>
-      <c r="B23" s="167"/>
-      <c r="C23" s="167"/>
-      <c r="D23" s="167"/>
-      <c r="E23" s="167"/>
-      <c r="F23" s="167"/>
-      <c r="G23" s="168"/>
+      <c r="B23" s="144"/>
+      <c r="C23" s="144"/>
+      <c r="D23" s="144"/>
+      <c r="E23" s="144"/>
+      <c r="F23" s="144"/>
+      <c r="G23" s="145"/>
       <c r="J23" s="102"/>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="144" t="s">
+      <c r="B24" s="164" t="s">
         <v>178</v>
       </c>
-      <c r="C24" s="144"/>
-      <c r="D24" s="144"/>
-      <c r="E24" s="144"/>
-      <c r="F24" s="144"/>
-      <c r="G24" s="144"/>
+      <c r="C24" s="164"/>
+      <c r="D24" s="164"/>
+      <c r="E24" s="164"/>
+      <c r="F24" s="164"/>
+      <c r="G24" s="164"/>
       <c r="H24" s="95"/>
       <c r="I24" s="95"/>
       <c r="J24" s="102"/>
@@ -7171,14 +7177,14 @@
       <c r="A25" s="106">
         <v>1</v>
       </c>
-      <c r="B25" s="145" t="s">
+      <c r="B25" s="165" t="s">
         <v>179</v>
       </c>
-      <c r="C25" s="145"/>
-      <c r="D25" s="145"/>
-      <c r="E25" s="145"/>
-      <c r="F25" s="145"/>
-      <c r="G25" s="145"/>
+      <c r="C25" s="165"/>
+      <c r="D25" s="165"/>
+      <c r="E25" s="165"/>
+      <c r="F25" s="165"/>
+      <c r="G25" s="165"/>
       <c r="H25" s="102"/>
       <c r="I25" s="102"/>
       <c r="K25" s="102"/>
@@ -7190,12 +7196,12 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="107"/>
-      <c r="B26" s="146"/>
-      <c r="C26" s="146"/>
-      <c r="D26" s="146"/>
-      <c r="E26" s="146"/>
-      <c r="F26" s="146"/>
-      <c r="G26" s="146"/>
+      <c r="B26" s="166"/>
+      <c r="C26" s="166"/>
+      <c r="D26" s="166"/>
+      <c r="E26" s="166"/>
+      <c r="F26" s="166"/>
+      <c r="G26" s="166"/>
       <c r="H26" s="102"/>
       <c r="I26" s="102"/>
       <c r="K26" s="102"/>
@@ -7207,12 +7213,12 @@
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="108"/>
-      <c r="B27" s="147"/>
-      <c r="C27" s="147"/>
-      <c r="D27" s="147"/>
-      <c r="E27" s="147"/>
-      <c r="F27" s="147"/>
-      <c r="G27" s="147"/>
+      <c r="B27" s="167"/>
+      <c r="C27" s="167"/>
+      <c r="D27" s="167"/>
+      <c r="E27" s="167"/>
+      <c r="F27" s="167"/>
+      <c r="G27" s="167"/>
       <c r="H27" s="102"/>
       <c r="I27" s="102"/>
       <c r="J27" s="95"/>
@@ -7241,29 +7247,29 @@
       <c r="O28"/>
     </row>
     <row r="29" spans="1:17">
-      <c r="A29" s="166" t="s">
+      <c r="A29" s="143" t="s">
         <v>188</v>
       </c>
-      <c r="B29" s="167"/>
-      <c r="C29" s="167"/>
-      <c r="D29" s="167"/>
-      <c r="E29" s="167"/>
-      <c r="F29" s="167"/>
-      <c r="G29" s="168"/>
+      <c r="B29" s="144"/>
+      <c r="C29" s="144"/>
+      <c r="D29" s="144"/>
+      <c r="E29" s="144"/>
+      <c r="F29" s="144"/>
+      <c r="G29" s="145"/>
       <c r="J29" s="102"/>
     </row>
     <row r="30" spans="1:17">
       <c r="A30" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B30" s="144" t="s">
+      <c r="B30" s="164" t="s">
         <v>180</v>
       </c>
-      <c r="C30" s="144"/>
-      <c r="D30" s="144"/>
-      <c r="E30" s="144"/>
-      <c r="F30" s="144"/>
-      <c r="G30" s="144"/>
+      <c r="C30" s="164"/>
+      <c r="D30" s="164"/>
+      <c r="E30" s="164"/>
+      <c r="F30" s="164"/>
+      <c r="G30" s="164"/>
       <c r="H30" s="95"/>
       <c r="I30" s="95"/>
       <c r="J30" s="102"/>
@@ -7276,12 +7282,12 @@
     </row>
     <row r="31" spans="1:17">
       <c r="A31" s="106"/>
-      <c r="B31" s="148"/>
-      <c r="C31" s="148"/>
-      <c r="D31" s="148"/>
-      <c r="E31" s="148"/>
-      <c r="F31" s="148"/>
-      <c r="G31" s="149"/>
+      <c r="B31" s="157"/>
+      <c r="C31" s="157"/>
+      <c r="D31" s="157"/>
+      <c r="E31" s="157"/>
+      <c r="F31" s="157"/>
+      <c r="G31" s="168"/>
       <c r="H31" s="102"/>
       <c r="I31" s="102"/>
       <c r="J31"/>
@@ -7294,12 +7300,12 @@
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="107"/>
-      <c r="B32" s="150"/>
-      <c r="C32" s="150"/>
-      <c r="D32" s="150"/>
-      <c r="E32" s="150"/>
-      <c r="F32" s="150"/>
-      <c r="G32" s="151"/>
+      <c r="B32" s="158"/>
+      <c r="C32" s="158"/>
+      <c r="D32" s="158"/>
+      <c r="E32" s="158"/>
+      <c r="F32" s="158"/>
+      <c r="G32" s="169"/>
       <c r="H32" s="102"/>
       <c r="I32" s="102"/>
       <c r="K32" s="102"/>
@@ -7311,12 +7317,12 @@
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="108"/>
-      <c r="B33" s="152"/>
-      <c r="C33" s="152"/>
-      <c r="D33" s="152"/>
-      <c r="E33" s="152"/>
-      <c r="F33" s="152"/>
-      <c r="G33" s="153"/>
+      <c r="B33" s="159"/>
+      <c r="C33" s="159"/>
+      <c r="D33" s="159"/>
+      <c r="E33" s="159"/>
+      <c r="F33" s="159"/>
+      <c r="G33" s="170"/>
       <c r="H33" s="102"/>
       <c r="I33" s="102"/>
       <c r="J33" s="95"/>
@@ -7369,64 +7375,64 @@
       <c r="P36" s="49"/>
     </row>
     <row r="37" spans="1:17" ht="15">
-      <c r="A37" s="180" t="s">
+      <c r="A37" s="181" t="s">
         <v>115</v>
       </c>
-      <c r="B37" s="180" t="s">
+      <c r="B37" s="181" t="s">
         <v>116</v>
       </c>
       <c r="C37" s="51" t="s">
         <v>117</v>
       </c>
-      <c r="D37" s="180" t="s">
+      <c r="D37" s="181" t="s">
         <v>99</v>
       </c>
-      <c r="E37" s="180" t="s">
+      <c r="E37" s="181" t="s">
         <v>156</v>
       </c>
-      <c r="F37" s="180" t="s">
+      <c r="F37" s="181" t="s">
         <v>171</v>
       </c>
-      <c r="G37" s="180" t="s">
+      <c r="G37" s="181" t="s">
         <v>136</v>
       </c>
-      <c r="H37" s="180" t="s">
+      <c r="H37" s="181" t="s">
         <v>113</v>
       </c>
-      <c r="I37" s="180" t="s">
+      <c r="I37" s="181" t="s">
         <v>230</v>
       </c>
       <c r="J37" s="176" t="s">
         <v>190</v>
       </c>
-      <c r="K37" s="185" t="s">
+      <c r="K37" s="186" t="s">
         <v>119</v>
       </c>
-      <c r="L37" s="186"/>
-      <c r="M37" s="187" t="s">
+      <c r="L37" s="187"/>
+      <c r="M37" s="188" t="s">
         <v>120</v>
       </c>
-      <c r="N37" s="186"/>
+      <c r="N37" s="187"/>
       <c r="O37" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="P37" s="180" t="s">
+      <c r="P37" s="181" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="15">
-      <c r="A38" s="188"/>
-      <c r="B38" s="188"/>
+      <c r="A38" s="185"/>
+      <c r="B38" s="185"/>
       <c r="C38" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="D38" s="188"/>
-      <c r="E38" s="181"/>
-      <c r="F38" s="181"/>
-      <c r="G38" s="188"/>
-      <c r="H38" s="188"/>
-      <c r="I38" s="188"/>
-      <c r="J38" s="177"/>
+      <c r="D38" s="185"/>
+      <c r="E38" s="182"/>
+      <c r="F38" s="182"/>
+      <c r="G38" s="185"/>
+      <c r="H38" s="185"/>
+      <c r="I38" s="185"/>
+      <c r="J38" s="183"/>
       <c r="K38" s="53" t="s">
         <v>123</v>
       </c>
@@ -7442,7 +7448,7 @@
       <c r="O38" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="P38" s="188"/>
+      <c r="P38" s="185"/>
     </row>
     <row r="39" spans="1:17">
       <c r="A39" s="55">
@@ -7940,19 +7946,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="P37:P38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="H37:H38"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="J37:J38"/>
@@ -7969,6 +7962,19 @@
     <mergeCell ref="A17:G17"/>
     <mergeCell ref="B18:G18"/>
     <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="P37:P38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">
@@ -8178,10 +8184,10 @@
         <v>168</v>
       </c>
       <c r="B15" s="111"/>
-      <c r="C15" s="133" t="s">
+      <c r="C15" s="151" t="s">
         <v>169</v>
       </c>
-      <c r="D15" s="133"/>
+      <c r="D15" s="151"/>
       <c r="E15" s="1" t="s">
         <v>170</v>
       </c>
@@ -8191,10 +8197,10 @@
         <v>171</v>
       </c>
       <c r="B16" s="111"/>
-      <c r="C16" s="133" t="s">
+      <c r="C16" s="151" t="s">
         <v>172</v>
       </c>
-      <c r="D16" s="133"/>
+      <c r="D16" s="151"/>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="112" t="s">
@@ -8220,28 +8226,28 @@
       <c r="A18" s="6"/>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="169" t="s">
+      <c r="A19" s="146" t="s">
         <v>186</v>
       </c>
-      <c r="B19" s="169"/>
-      <c r="C19" s="169"/>
-      <c r="D19" s="169"/>
-      <c r="E19" s="169"/>
-      <c r="F19" s="169"/>
-      <c r="G19" s="169"/>
+      <c r="B19" s="146"/>
+      <c r="C19" s="146"/>
+      <c r="D19" s="146"/>
+      <c r="E19" s="146"/>
+      <c r="F19" s="146"/>
+      <c r="G19" s="146"/>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B20" s="163" t="s">
+      <c r="B20" s="140" t="s">
         <v>177</v>
       </c>
-      <c r="C20" s="164"/>
-      <c r="D20" s="164"/>
-      <c r="E20" s="164"/>
-      <c r="F20" s="164"/>
-      <c r="G20" s="165"/>
+      <c r="C20" s="141"/>
+      <c r="D20" s="141"/>
+      <c r="E20" s="141"/>
+      <c r="F20" s="141"/>
+      <c r="G20" s="142"/>
       <c r="H20" s="95"/>
       <c r="I20" s="95"/>
       <c r="K20" s="95"/>
@@ -8253,12 +8259,12 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="106"/>
-      <c r="B21" s="148"/>
-      <c r="C21" s="148"/>
-      <c r="D21" s="148"/>
-      <c r="E21" s="148"/>
-      <c r="F21" s="148"/>
-      <c r="G21" s="148"/>
+      <c r="B21" s="157"/>
+      <c r="C21" s="157"/>
+      <c r="D21" s="157"/>
+      <c r="E21" s="157"/>
+      <c r="F21" s="157"/>
+      <c r="G21" s="157"/>
       <c r="H21" s="102"/>
       <c r="I21" s="102"/>
       <c r="K21" s="102"/>
@@ -8270,12 +8276,12 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="107"/>
-      <c r="B22" s="150"/>
-      <c r="C22" s="150"/>
-      <c r="D22" s="150"/>
-      <c r="E22" s="150"/>
-      <c r="F22" s="150"/>
-      <c r="G22" s="150"/>
+      <c r="B22" s="158"/>
+      <c r="C22" s="158"/>
+      <c r="D22" s="158"/>
+      <c r="E22" s="158"/>
+      <c r="F22" s="158"/>
+      <c r="G22" s="158"/>
       <c r="H22" s="102"/>
       <c r="I22" s="102"/>
       <c r="K22" s="102"/>
@@ -8287,12 +8293,12 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="108"/>
-      <c r="B23" s="152"/>
-      <c r="C23" s="152"/>
-      <c r="D23" s="152"/>
-      <c r="E23" s="152"/>
-      <c r="F23" s="152"/>
-      <c r="G23" s="152"/>
+      <c r="B23" s="159"/>
+      <c r="C23" s="159"/>
+      <c r="D23" s="159"/>
+      <c r="E23" s="159"/>
+      <c r="F23" s="159"/>
+      <c r="G23" s="159"/>
       <c r="H23" s="102"/>
       <c r="I23" s="102"/>
       <c r="J23" s="95"/>
@@ -8308,29 +8314,29 @@
       <c r="J24" s="102"/>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" s="166" t="s">
+      <c r="A25" s="143" t="s">
         <v>187</v>
       </c>
-      <c r="B25" s="167"/>
-      <c r="C25" s="167"/>
-      <c r="D25" s="167"/>
-      <c r="E25" s="167"/>
-      <c r="F25" s="167"/>
-      <c r="G25" s="168"/>
+      <c r="B25" s="144"/>
+      <c r="C25" s="144"/>
+      <c r="D25" s="144"/>
+      <c r="E25" s="144"/>
+      <c r="F25" s="144"/>
+      <c r="G25" s="145"/>
       <c r="J25" s="102"/>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="144" t="s">
+      <c r="B26" s="164" t="s">
         <v>178</v>
       </c>
-      <c r="C26" s="144"/>
-      <c r="D26" s="144"/>
-      <c r="E26" s="144"/>
-      <c r="F26" s="144"/>
-      <c r="G26" s="144"/>
+      <c r="C26" s="164"/>
+      <c r="D26" s="164"/>
+      <c r="E26" s="164"/>
+      <c r="F26" s="164"/>
+      <c r="G26" s="164"/>
       <c r="H26" s="95"/>
       <c r="I26" s="95"/>
       <c r="J26" s="102"/>
@@ -8345,14 +8351,14 @@
       <c r="A27" s="106">
         <v>1</v>
       </c>
-      <c r="B27" s="145" t="s">
+      <c r="B27" s="165" t="s">
         <v>179</v>
       </c>
-      <c r="C27" s="145"/>
-      <c r="D27" s="145"/>
-      <c r="E27" s="145"/>
-      <c r="F27" s="145"/>
-      <c r="G27" s="145"/>
+      <c r="C27" s="165"/>
+      <c r="D27" s="165"/>
+      <c r="E27" s="165"/>
+      <c r="F27" s="165"/>
+      <c r="G27" s="165"/>
       <c r="H27" s="102"/>
       <c r="I27" s="102"/>
       <c r="K27" s="102"/>
@@ -8364,12 +8370,12 @@
     </row>
     <row r="28" spans="1:17">
       <c r="A28" s="107"/>
-      <c r="B28" s="146"/>
-      <c r="C28" s="146"/>
-      <c r="D28" s="146"/>
-      <c r="E28" s="146"/>
-      <c r="F28" s="146"/>
-      <c r="G28" s="146"/>
+      <c r="B28" s="166"/>
+      <c r="C28" s="166"/>
+      <c r="D28" s="166"/>
+      <c r="E28" s="166"/>
+      <c r="F28" s="166"/>
+      <c r="G28" s="166"/>
       <c r="H28" s="102"/>
       <c r="I28" s="102"/>
       <c r="K28" s="102"/>
@@ -8381,12 +8387,12 @@
     </row>
     <row r="29" spans="1:17">
       <c r="A29" s="108"/>
-      <c r="B29" s="147"/>
-      <c r="C29" s="147"/>
-      <c r="D29" s="147"/>
-      <c r="E29" s="147"/>
-      <c r="F29" s="147"/>
-      <c r="G29" s="147"/>
+      <c r="B29" s="167"/>
+      <c r="C29" s="167"/>
+      <c r="D29" s="167"/>
+      <c r="E29" s="167"/>
+      <c r="F29" s="167"/>
+      <c r="G29" s="167"/>
       <c r="H29" s="102"/>
       <c r="I29" s="102"/>
       <c r="J29" s="95"/>
@@ -8415,29 +8421,29 @@
       <c r="O30"/>
     </row>
     <row r="31" spans="1:17">
-      <c r="A31" s="166" t="s">
+      <c r="A31" s="143" t="s">
         <v>188</v>
       </c>
-      <c r="B31" s="167"/>
-      <c r="C31" s="167"/>
-      <c r="D31" s="167"/>
-      <c r="E31" s="167"/>
-      <c r="F31" s="167"/>
-      <c r="G31" s="168"/>
+      <c r="B31" s="144"/>
+      <c r="C31" s="144"/>
+      <c r="D31" s="144"/>
+      <c r="E31" s="144"/>
+      <c r="F31" s="144"/>
+      <c r="G31" s="145"/>
       <c r="J31" s="102"/>
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="144" t="s">
+      <c r="B32" s="164" t="s">
         <v>180</v>
       </c>
-      <c r="C32" s="144"/>
-      <c r="D32" s="144"/>
-      <c r="E32" s="144"/>
-      <c r="F32" s="144"/>
-      <c r="G32" s="144"/>
+      <c r="C32" s="164"/>
+      <c r="D32" s="164"/>
+      <c r="E32" s="164"/>
+      <c r="F32" s="164"/>
+      <c r="G32" s="164"/>
       <c r="H32" s="95"/>
       <c r="I32" s="95"/>
       <c r="J32" s="102"/>
@@ -8450,12 +8456,12 @@
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="106"/>
-      <c r="B33" s="148"/>
-      <c r="C33" s="148"/>
-      <c r="D33" s="148"/>
-      <c r="E33" s="148"/>
-      <c r="F33" s="148"/>
-      <c r="G33" s="149"/>
+      <c r="B33" s="157"/>
+      <c r="C33" s="157"/>
+      <c r="D33" s="157"/>
+      <c r="E33" s="157"/>
+      <c r="F33" s="157"/>
+      <c r="G33" s="168"/>
       <c r="H33" s="102"/>
       <c r="I33" s="102"/>
       <c r="J33"/>
@@ -8468,12 +8474,12 @@
     </row>
     <row r="34" spans="1:17">
       <c r="A34" s="107"/>
-      <c r="B34" s="150"/>
-      <c r="C34" s="150"/>
-      <c r="D34" s="150"/>
-      <c r="E34" s="150"/>
-      <c r="F34" s="150"/>
-      <c r="G34" s="151"/>
+      <c r="B34" s="158"/>
+      <c r="C34" s="158"/>
+      <c r="D34" s="158"/>
+      <c r="E34" s="158"/>
+      <c r="F34" s="158"/>
+      <c r="G34" s="169"/>
       <c r="H34" s="102"/>
       <c r="I34" s="102"/>
       <c r="K34" s="102"/>
@@ -8485,12 +8491,12 @@
     </row>
     <row r="35" spans="1:17">
       <c r="A35" s="108"/>
-      <c r="B35" s="152"/>
-      <c r="C35" s="152"/>
-      <c r="D35" s="152"/>
-      <c r="E35" s="152"/>
-      <c r="F35" s="152"/>
-      <c r="G35" s="153"/>
+      <c r="B35" s="159"/>
+      <c r="C35" s="159"/>
+      <c r="D35" s="159"/>
+      <c r="E35" s="159"/>
+      <c r="F35" s="159"/>
+      <c r="G35" s="170"/>
       <c r="H35" s="102"/>
       <c r="I35" s="102"/>
       <c r="J35" s="95"/>
@@ -8543,25 +8549,25 @@
       <c r="P38" s="49"/>
     </row>
     <row r="39" spans="1:17" ht="15">
-      <c r="A39" s="180" t="s">
+      <c r="A39" s="181" t="s">
         <v>115</v>
       </c>
-      <c r="B39" s="180" t="s">
+      <c r="B39" s="181" t="s">
         <v>116</v>
       </c>
       <c r="C39" s="51" t="s">
         <v>117</v>
       </c>
-      <c r="D39" s="180" t="s">
+      <c r="D39" s="181" t="s">
         <v>99</v>
       </c>
-      <c r="E39" s="180" t="s">
+      <c r="E39" s="181" t="s">
         <v>156</v>
       </c>
-      <c r="F39" s="180" t="s">
+      <c r="F39" s="181" t="s">
         <v>171</v>
       </c>
-      <c r="G39" s="180" t="s">
+      <c r="G39" s="181" t="s">
         <v>136</v>
       </c>
       <c r="H39" s="189" t="s">
@@ -8573,34 +8579,34 @@
       <c r="J39" s="176" t="s">
         <v>190</v>
       </c>
-      <c r="K39" s="185" t="s">
+      <c r="K39" s="186" t="s">
         <v>119</v>
       </c>
-      <c r="L39" s="186"/>
-      <c r="M39" s="187" t="s">
+      <c r="L39" s="187"/>
+      <c r="M39" s="188" t="s">
         <v>120</v>
       </c>
-      <c r="N39" s="186"/>
+      <c r="N39" s="187"/>
       <c r="O39" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="P39" s="180" t="s">
+      <c r="P39" s="181" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="15">
-      <c r="A40" s="188"/>
-      <c r="B40" s="188"/>
+      <c r="A40" s="185"/>
+      <c r="B40" s="185"/>
       <c r="C40" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="D40" s="188"/>
-      <c r="E40" s="181"/>
-      <c r="F40" s="181"/>
-      <c r="G40" s="188"/>
-      <c r="H40" s="188"/>
-      <c r="I40" s="188"/>
-      <c r="J40" s="177"/>
+      <c r="D40" s="185"/>
+      <c r="E40" s="182"/>
+      <c r="F40" s="182"/>
+      <c r="G40" s="185"/>
+      <c r="H40" s="185"/>
+      <c r="I40" s="185"/>
+      <c r="J40" s="183"/>
       <c r="K40" s="53" t="s">
         <v>123</v>
       </c>
@@ -8616,7 +8622,7 @@
       <c r="O40" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="P40" s="188"/>
+      <c r="P40" s="185"/>
     </row>
     <row r="41" spans="1:17">
       <c r="A41" s="55">
@@ -9072,6 +9078,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
     <mergeCell ref="P39:P40"/>
     <mergeCell ref="A31:G31"/>
     <mergeCell ref="B32:G32"/>
@@ -9088,19 +9107,6 @@
     <mergeCell ref="J39:J40"/>
     <mergeCell ref="K39:L39"/>
     <mergeCell ref="M39:N39"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">
@@ -9148,8 +9154,8 @@
   </sheetPr>
   <dimension ref="A1:V67"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I49" sqref="I49"/>
+    <sheetView topLeftCell="F3" workbookViewId="0">
+      <selection activeCell="M3" sqref="M1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -9309,10 +9315,10 @@
         <v>168</v>
       </c>
       <c r="B16" s="111"/>
-      <c r="C16" s="133" t="s">
+      <c r="C16" s="151" t="s">
         <v>169</v>
       </c>
-      <c r="D16" s="133"/>
+      <c r="D16" s="151"/>
       <c r="E16" s="1" t="s">
         <v>170</v>
       </c>
@@ -9322,20 +9328,20 @@
         <v>171</v>
       </c>
       <c r="B17" s="111"/>
-      <c r="C17" s="133" t="s">
+      <c r="C17" s="151" t="s">
         <v>172</v>
       </c>
-      <c r="D17" s="133"/>
+      <c r="D17" s="151"/>
     </row>
     <row r="18" spans="1:22">
       <c r="A18" s="111" t="s">
         <v>208</v>
       </c>
       <c r="B18" s="111"/>
-      <c r="C18" s="132" t="s">
+      <c r="C18" s="150" t="s">
         <v>210</v>
       </c>
-      <c r="D18" s="133"/>
+      <c r="D18" s="151"/>
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="112" t="s">
@@ -9393,28 +9399,28 @@
       <c r="A21" s="6"/>
     </row>
     <row r="22" spans="1:22">
-      <c r="A22" s="169" t="s">
+      <c r="A22" s="146" t="s">
         <v>186</v>
       </c>
-      <c r="B22" s="169"/>
-      <c r="C22" s="169"/>
-      <c r="D22" s="169"/>
-      <c r="E22" s="169"/>
-      <c r="F22" s="169"/>
-      <c r="G22" s="169"/>
+      <c r="B22" s="146"/>
+      <c r="C22" s="146"/>
+      <c r="D22" s="146"/>
+      <c r="E22" s="146"/>
+      <c r="F22" s="146"/>
+      <c r="G22" s="146"/>
     </row>
     <row r="23" spans="1:22">
       <c r="A23" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="163" t="s">
+      <c r="B23" s="140" t="s">
         <v>177</v>
       </c>
-      <c r="C23" s="164"/>
-      <c r="D23" s="164"/>
-      <c r="E23" s="164"/>
-      <c r="F23" s="164"/>
-      <c r="G23" s="165"/>
+      <c r="C23" s="141"/>
+      <c r="D23" s="141"/>
+      <c r="E23" s="141"/>
+      <c r="F23" s="141"/>
+      <c r="G23" s="142"/>
       <c r="H23" s="95"/>
       <c r="I23" s="95"/>
       <c r="J23" s="95"/>
@@ -9432,12 +9438,12 @@
     </row>
     <row r="24" spans="1:22">
       <c r="A24" s="106"/>
-      <c r="B24" s="148"/>
-      <c r="C24" s="148"/>
-      <c r="D24" s="148"/>
-      <c r="E24" s="148"/>
-      <c r="F24" s="148"/>
-      <c r="G24" s="148"/>
+      <c r="B24" s="157"/>
+      <c r="C24" s="157"/>
+      <c r="D24" s="157"/>
+      <c r="E24" s="157"/>
+      <c r="F24" s="157"/>
+      <c r="G24" s="157"/>
       <c r="H24" s="102"/>
       <c r="I24" s="102"/>
       <c r="J24" s="102"/>
@@ -9455,12 +9461,12 @@
     </row>
     <row r="25" spans="1:22">
       <c r="A25" s="107"/>
-      <c r="B25" s="150"/>
-      <c r="C25" s="150"/>
-      <c r="D25" s="150"/>
-      <c r="E25" s="150"/>
-      <c r="F25" s="150"/>
-      <c r="G25" s="150"/>
+      <c r="B25" s="158"/>
+      <c r="C25" s="158"/>
+      <c r="D25" s="158"/>
+      <c r="E25" s="158"/>
+      <c r="F25" s="158"/>
+      <c r="G25" s="158"/>
       <c r="H25" s="102"/>
       <c r="I25" s="102"/>
       <c r="J25" s="102"/>
@@ -9478,12 +9484,12 @@
     </row>
     <row r="26" spans="1:22">
       <c r="A26" s="108"/>
-      <c r="B26" s="152"/>
-      <c r="C26" s="152"/>
-      <c r="D26" s="152"/>
-      <c r="E26" s="152"/>
-      <c r="F26" s="152"/>
-      <c r="G26" s="152"/>
+      <c r="B26" s="159"/>
+      <c r="C26" s="159"/>
+      <c r="D26" s="159"/>
+      <c r="E26" s="159"/>
+      <c r="F26" s="159"/>
+      <c r="G26" s="159"/>
       <c r="H26" s="102"/>
       <c r="I26" s="102"/>
       <c r="J26" s="102"/>
@@ -9503,28 +9509,28 @@
       <c r="C27"/>
     </row>
     <row r="28" spans="1:22">
-      <c r="A28" s="166" t="s">
+      <c r="A28" s="143" t="s">
         <v>187</v>
       </c>
-      <c r="B28" s="167"/>
-      <c r="C28" s="167"/>
-      <c r="D28" s="167"/>
-      <c r="E28" s="167"/>
-      <c r="F28" s="167"/>
-      <c r="G28" s="168"/>
+      <c r="B28" s="144"/>
+      <c r="C28" s="144"/>
+      <c r="D28" s="144"/>
+      <c r="E28" s="144"/>
+      <c r="F28" s="144"/>
+      <c r="G28" s="145"/>
     </row>
     <row r="29" spans="1:22">
       <c r="A29" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="144" t="s">
+      <c r="B29" s="164" t="s">
         <v>178</v>
       </c>
-      <c r="C29" s="144"/>
-      <c r="D29" s="144"/>
-      <c r="E29" s="144"/>
-      <c r="F29" s="144"/>
-      <c r="G29" s="144"/>
+      <c r="C29" s="164"/>
+      <c r="D29" s="164"/>
+      <c r="E29" s="164"/>
+      <c r="F29" s="164"/>
+      <c r="G29" s="164"/>
       <c r="H29" s="95"/>
       <c r="I29" s="95"/>
       <c r="J29" s="95"/>
@@ -9544,14 +9550,14 @@
       <c r="A30" s="106">
         <v>1</v>
       </c>
-      <c r="B30" s="145" t="s">
+      <c r="B30" s="165" t="s">
         <v>179</v>
       </c>
-      <c r="C30" s="145"/>
-      <c r="D30" s="145"/>
-      <c r="E30" s="145"/>
-      <c r="F30" s="145"/>
-      <c r="G30" s="145"/>
+      <c r="C30" s="165"/>
+      <c r="D30" s="165"/>
+      <c r="E30" s="165"/>
+      <c r="F30" s="165"/>
+      <c r="G30" s="165"/>
       <c r="H30" s="102"/>
       <c r="I30" s="102"/>
       <c r="J30" s="102"/>
@@ -9569,12 +9575,12 @@
     </row>
     <row r="31" spans="1:22">
       <c r="A31" s="107"/>
-      <c r="B31" s="146"/>
-      <c r="C31" s="146"/>
-      <c r="D31" s="146"/>
-      <c r="E31" s="146"/>
-      <c r="F31" s="146"/>
-      <c r="G31" s="146"/>
+      <c r="B31" s="166"/>
+      <c r="C31" s="166"/>
+      <c r="D31" s="166"/>
+      <c r="E31" s="166"/>
+      <c r="F31" s="166"/>
+      <c r="G31" s="166"/>
       <c r="H31" s="102"/>
       <c r="I31" s="102"/>
       <c r="J31" s="102"/>
@@ -9592,12 +9598,12 @@
     </row>
     <row r="32" spans="1:22">
       <c r="A32" s="108"/>
-      <c r="B32" s="147"/>
-      <c r="C32" s="147"/>
-      <c r="D32" s="147"/>
-      <c r="E32" s="147"/>
-      <c r="F32" s="147"/>
-      <c r="G32" s="147"/>
+      <c r="B32" s="167"/>
+      <c r="C32" s="167"/>
+      <c r="D32" s="167"/>
+      <c r="E32" s="167"/>
+      <c r="F32" s="167"/>
+      <c r="G32" s="167"/>
       <c r="H32" s="102"/>
       <c r="I32" s="102"/>
       <c r="J32" s="102"/>
@@ -9636,28 +9642,28 @@
       <c r="T33"/>
     </row>
     <row r="34" spans="1:22">
-      <c r="A34" s="166" t="s">
+      <c r="A34" s="143" t="s">
         <v>188</v>
       </c>
-      <c r="B34" s="167"/>
-      <c r="C34" s="167"/>
-      <c r="D34" s="167"/>
-      <c r="E34" s="167"/>
-      <c r="F34" s="167"/>
-      <c r="G34" s="168"/>
+      <c r="B34" s="144"/>
+      <c r="C34" s="144"/>
+      <c r="D34" s="144"/>
+      <c r="E34" s="144"/>
+      <c r="F34" s="144"/>
+      <c r="G34" s="145"/>
     </row>
     <row r="35" spans="1:22">
       <c r="A35" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="144" t="s">
+      <c r="B35" s="164" t="s">
         <v>180</v>
       </c>
-      <c r="C35" s="144"/>
-      <c r="D35" s="144"/>
-      <c r="E35" s="144"/>
-      <c r="F35" s="144"/>
-      <c r="G35" s="144"/>
+      <c r="C35" s="164"/>
+      <c r="D35" s="164"/>
+      <c r="E35" s="164"/>
+      <c r="F35" s="164"/>
+      <c r="G35" s="164"/>
       <c r="H35" s="95"/>
       <c r="I35" s="95"/>
       <c r="J35" s="95"/>
@@ -9675,12 +9681,12 @@
     </row>
     <row r="36" spans="1:22">
       <c r="A36" s="106"/>
-      <c r="B36" s="148"/>
-      <c r="C36" s="148"/>
-      <c r="D36" s="148"/>
-      <c r="E36" s="148"/>
-      <c r="F36" s="148"/>
-      <c r="G36" s="149"/>
+      <c r="B36" s="157"/>
+      <c r="C36" s="157"/>
+      <c r="D36" s="157"/>
+      <c r="E36" s="157"/>
+      <c r="F36" s="157"/>
+      <c r="G36" s="168"/>
       <c r="H36" s="102"/>
       <c r="I36" s="102"/>
       <c r="J36" s="102"/>
@@ -9698,12 +9704,12 @@
     </row>
     <row r="37" spans="1:22">
       <c r="A37" s="107"/>
-      <c r="B37" s="150"/>
-      <c r="C37" s="150"/>
-      <c r="D37" s="150"/>
-      <c r="E37" s="150"/>
-      <c r="F37" s="150"/>
-      <c r="G37" s="151"/>
+      <c r="B37" s="158"/>
+      <c r="C37" s="158"/>
+      <c r="D37" s="158"/>
+      <c r="E37" s="158"/>
+      <c r="F37" s="158"/>
+      <c r="G37" s="169"/>
       <c r="H37" s="102"/>
       <c r="I37" s="102"/>
       <c r="J37" s="102"/>
@@ -9721,12 +9727,12 @@
     </row>
     <row r="38" spans="1:22">
       <c r="A38" s="108"/>
-      <c r="B38" s="152"/>
-      <c r="C38" s="152"/>
-      <c r="D38" s="152"/>
-      <c r="E38" s="152"/>
-      <c r="F38" s="152"/>
-      <c r="G38" s="153"/>
+      <c r="B38" s="159"/>
+      <c r="C38" s="159"/>
+      <c r="D38" s="159"/>
+      <c r="E38" s="159"/>
+      <c r="F38" s="159"/>
+      <c r="G38" s="170"/>
       <c r="H38" s="102"/>
       <c r="I38" s="102"/>
       <c r="J38" s="102"/>
@@ -9802,16 +9808,16 @@
       <c r="B42" s="176" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="182" t="s">
+      <c r="C42" s="178" t="s">
         <v>1</v>
       </c>
       <c r="D42" s="176" t="s">
         <v>2</v>
       </c>
-      <c r="E42" s="180" t="s">
+      <c r="E42" s="181" t="s">
         <v>156</v>
       </c>
-      <c r="F42" s="180" t="s">
+      <c r="F42" s="181" t="s">
         <v>171</v>
       </c>
       <c r="G42" s="176" t="s">
@@ -9823,13 +9829,13 @@
       <c r="I42" s="176" t="s">
         <v>237</v>
       </c>
-      <c r="J42" s="180" t="s">
+      <c r="J42" s="181" t="s">
         <v>238</v>
       </c>
-      <c r="K42" s="180" t="s">
+      <c r="K42" s="181" t="s">
         <v>208</v>
       </c>
-      <c r="L42" s="179" t="s">
+      <c r="L42" s="184" t="s">
         <v>225</v>
       </c>
       <c r="M42" s="176" t="s">
@@ -9841,14 +9847,14 @@
       <c r="O42" s="176" t="s">
         <v>190</v>
       </c>
-      <c r="P42" s="183" t="s">
+      <c r="P42" s="179" t="s">
         <v>70</v>
       </c>
-      <c r="Q42" s="184"/>
-      <c r="R42" s="183" t="s">
+      <c r="Q42" s="180"/>
+      <c r="R42" s="179" t="s">
         <v>16</v>
       </c>
-      <c r="S42" s="184"/>
+      <c r="S42" s="180"/>
       <c r="T42" s="32" t="s">
         <v>69</v>
       </c>
@@ -9857,21 +9863,21 @@
       </c>
     </row>
     <row r="43" spans="1:22">
-      <c r="A43" s="178"/>
-      <c r="B43" s="178"/>
-      <c r="C43" s="178"/>
-      <c r="D43" s="178"/>
-      <c r="E43" s="181"/>
-      <c r="F43" s="181"/>
-      <c r="G43" s="178"/>
-      <c r="H43" s="178"/>
-      <c r="I43" s="178"/>
-      <c r="J43" s="181"/>
-      <c r="K43" s="181"/>
-      <c r="L43" s="177"/>
-      <c r="M43" s="178"/>
-      <c r="N43" s="178"/>
-      <c r="O43" s="177"/>
+      <c r="A43" s="177"/>
+      <c r="B43" s="177"/>
+      <c r="C43" s="177"/>
+      <c r="D43" s="177"/>
+      <c r="E43" s="182"/>
+      <c r="F43" s="182"/>
+      <c r="G43" s="177"/>
+      <c r="H43" s="177"/>
+      <c r="I43" s="177"/>
+      <c r="J43" s="182"/>
+      <c r="K43" s="182"/>
+      <c r="L43" s="183"/>
+      <c r="M43" s="177"/>
+      <c r="N43" s="177"/>
+      <c r="O43" s="183"/>
       <c r="P43" s="27" t="s">
         <v>74</v>
       </c>
@@ -9887,7 +9893,7 @@
       <c r="T43" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="U43" s="178"/>
+      <c r="U43" s="177"/>
     </row>
     <row r="44" spans="1:22">
       <c r="A44" s="7">
@@ -10543,6 +10549,30 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="U42:U43"/>
+    <mergeCell ref="G42:G43"/>
+    <mergeCell ref="H42:H43"/>
+    <mergeCell ref="I42:I43"/>
+    <mergeCell ref="J42:J43"/>
+    <mergeCell ref="K42:K43"/>
+    <mergeCell ref="L42:L43"/>
+    <mergeCell ref="M42:M43"/>
+    <mergeCell ref="N42:N43"/>
+    <mergeCell ref="O42:O43"/>
+    <mergeCell ref="P42:Q42"/>
+    <mergeCell ref="R42:S42"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
     <mergeCell ref="B31:G31"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
@@ -10555,30 +10585,6 @@
     <mergeCell ref="A28:G28"/>
     <mergeCell ref="B29:G29"/>
     <mergeCell ref="B30:G30"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="A34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="U42:U43"/>
-    <mergeCell ref="G42:G43"/>
-    <mergeCell ref="H42:H43"/>
-    <mergeCell ref="I42:I43"/>
-    <mergeCell ref="J42:J43"/>
-    <mergeCell ref="K42:K43"/>
-    <mergeCell ref="L42:L43"/>
-    <mergeCell ref="M42:M43"/>
-    <mergeCell ref="N42:N43"/>
-    <mergeCell ref="O42:O43"/>
-    <mergeCell ref="P42:Q42"/>
-    <mergeCell ref="R42:S42"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="4">
@@ -10636,7 +10642,7 @@
   <dimension ref="A1:Q62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -10701,7 +10707,7 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="119" t="str">
-        <f>process!D6&amp;PROPER(C9)&amp;IF(C8="要求電文(C→S)", "Request", "Response")</f>
+        <f>process!D6&amp;PROPER(C9)&amp;IF(C8="要求電文(C→S)","Request",IF(C8="応答電文(S→C)","Response","Error"&amp;C10))</f>
         <v>BlancoApiPlainSamplePostResponse</v>
       </c>
       <c r="D6" s="118"/>
@@ -10771,10 +10777,10 @@
         <v>168</v>
       </c>
       <c r="B13" s="111"/>
-      <c r="C13" s="133" t="s">
+      <c r="C13" s="151" t="s">
         <v>169</v>
       </c>
-      <c r="D13" s="133"/>
+      <c r="D13" s="151"/>
       <c r="E13" s="1" t="s">
         <v>170</v>
       </c>
@@ -10784,10 +10790,10 @@
         <v>171</v>
       </c>
       <c r="B14" s="111"/>
-      <c r="C14" s="133" t="s">
+      <c r="C14" s="151" t="s">
         <v>172</v>
       </c>
-      <c r="D14" s="133"/>
+      <c r="D14" s="151"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="112" t="s">
@@ -10813,28 +10819,28 @@
       <c r="A16" s="6"/>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="169" t="s">
+      <c r="A17" s="146" t="s">
         <v>186</v>
       </c>
-      <c r="B17" s="169"/>
-      <c r="C17" s="169"/>
-      <c r="D17" s="169"/>
-      <c r="E17" s="169"/>
-      <c r="F17" s="169"/>
-      <c r="G17" s="169"/>
+      <c r="B17" s="146"/>
+      <c r="C17" s="146"/>
+      <c r="D17" s="146"/>
+      <c r="E17" s="146"/>
+      <c r="F17" s="146"/>
+      <c r="G17" s="146"/>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="163" t="s">
+      <c r="B18" s="140" t="s">
         <v>177</v>
       </c>
-      <c r="C18" s="164"/>
-      <c r="D18" s="164"/>
-      <c r="E18" s="164"/>
-      <c r="F18" s="164"/>
-      <c r="G18" s="165"/>
+      <c r="C18" s="141"/>
+      <c r="D18" s="141"/>
+      <c r="E18" s="141"/>
+      <c r="F18" s="141"/>
+      <c r="G18" s="142"/>
       <c r="H18" s="95"/>
       <c r="I18" s="95"/>
       <c r="K18" s="95"/>
@@ -10846,12 +10852,12 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="106"/>
-      <c r="B19" s="148"/>
-      <c r="C19" s="148"/>
-      <c r="D19" s="148"/>
-      <c r="E19" s="148"/>
-      <c r="F19" s="148"/>
-      <c r="G19" s="148"/>
+      <c r="B19" s="157"/>
+      <c r="C19" s="157"/>
+      <c r="D19" s="157"/>
+      <c r="E19" s="157"/>
+      <c r="F19" s="157"/>
+      <c r="G19" s="157"/>
       <c r="H19" s="102"/>
       <c r="I19" s="102"/>
       <c r="K19" s="102"/>
@@ -10863,12 +10869,12 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="107"/>
-      <c r="B20" s="150"/>
-      <c r="C20" s="150"/>
-      <c r="D20" s="150"/>
-      <c r="E20" s="150"/>
-      <c r="F20" s="150"/>
-      <c r="G20" s="150"/>
+      <c r="B20" s="158"/>
+      <c r="C20" s="158"/>
+      <c r="D20" s="158"/>
+      <c r="E20" s="158"/>
+      <c r="F20" s="158"/>
+      <c r="G20" s="158"/>
       <c r="H20" s="102"/>
       <c r="I20" s="102"/>
       <c r="K20" s="102"/>
@@ -10880,12 +10886,12 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="108"/>
-      <c r="B21" s="152"/>
-      <c r="C21" s="152"/>
-      <c r="D21" s="152"/>
-      <c r="E21" s="152"/>
-      <c r="F21" s="152"/>
-      <c r="G21" s="152"/>
+      <c r="B21" s="159"/>
+      <c r="C21" s="159"/>
+      <c r="D21" s="159"/>
+      <c r="E21" s="159"/>
+      <c r="F21" s="159"/>
+      <c r="G21" s="159"/>
       <c r="H21" s="102"/>
       <c r="I21" s="102"/>
       <c r="J21" s="95"/>
@@ -10901,29 +10907,29 @@
       <c r="J22" s="102"/>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="166" t="s">
+      <c r="A23" s="143" t="s">
         <v>187</v>
       </c>
-      <c r="B23" s="167"/>
-      <c r="C23" s="167"/>
-      <c r="D23" s="167"/>
-      <c r="E23" s="167"/>
-      <c r="F23" s="167"/>
-      <c r="G23" s="168"/>
+      <c r="B23" s="144"/>
+      <c r="C23" s="144"/>
+      <c r="D23" s="144"/>
+      <c r="E23" s="144"/>
+      <c r="F23" s="144"/>
+      <c r="G23" s="145"/>
       <c r="J23" s="102"/>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="144" t="s">
+      <c r="B24" s="164" t="s">
         <v>178</v>
       </c>
-      <c r="C24" s="144"/>
-      <c r="D24" s="144"/>
-      <c r="E24" s="144"/>
-      <c r="F24" s="144"/>
-      <c r="G24" s="144"/>
+      <c r="C24" s="164"/>
+      <c r="D24" s="164"/>
+      <c r="E24" s="164"/>
+      <c r="F24" s="164"/>
+      <c r="G24" s="164"/>
       <c r="H24" s="95"/>
       <c r="I24" s="95"/>
       <c r="J24" s="102"/>
@@ -10938,14 +10944,14 @@
       <c r="A25" s="106">
         <v>1</v>
       </c>
-      <c r="B25" s="145" t="s">
+      <c r="B25" s="165" t="s">
         <v>179</v>
       </c>
-      <c r="C25" s="145"/>
-      <c r="D25" s="145"/>
-      <c r="E25" s="145"/>
-      <c r="F25" s="145"/>
-      <c r="G25" s="145"/>
+      <c r="C25" s="165"/>
+      <c r="D25" s="165"/>
+      <c r="E25" s="165"/>
+      <c r="F25" s="165"/>
+      <c r="G25" s="165"/>
       <c r="H25" s="102"/>
       <c r="I25" s="102"/>
       <c r="K25" s="102"/>
@@ -10957,12 +10963,12 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="107"/>
-      <c r="B26" s="146"/>
-      <c r="C26" s="146"/>
-      <c r="D26" s="146"/>
-      <c r="E26" s="146"/>
-      <c r="F26" s="146"/>
-      <c r="G26" s="146"/>
+      <c r="B26" s="166"/>
+      <c r="C26" s="166"/>
+      <c r="D26" s="166"/>
+      <c r="E26" s="166"/>
+      <c r="F26" s="166"/>
+      <c r="G26" s="166"/>
       <c r="H26" s="102"/>
       <c r="I26" s="102"/>
       <c r="K26" s="102"/>
@@ -10974,12 +10980,12 @@
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="108"/>
-      <c r="B27" s="147"/>
-      <c r="C27" s="147"/>
-      <c r="D27" s="147"/>
-      <c r="E27" s="147"/>
-      <c r="F27" s="147"/>
-      <c r="G27" s="147"/>
+      <c r="B27" s="167"/>
+      <c r="C27" s="167"/>
+      <c r="D27" s="167"/>
+      <c r="E27" s="167"/>
+      <c r="F27" s="167"/>
+      <c r="G27" s="167"/>
       <c r="H27" s="102"/>
       <c r="I27" s="102"/>
       <c r="J27" s="95"/>
@@ -11008,29 +11014,29 @@
       <c r="O28"/>
     </row>
     <row r="29" spans="1:17">
-      <c r="A29" s="166" t="s">
+      <c r="A29" s="143" t="s">
         <v>188</v>
       </c>
-      <c r="B29" s="167"/>
-      <c r="C29" s="167"/>
-      <c r="D29" s="167"/>
-      <c r="E29" s="167"/>
-      <c r="F29" s="167"/>
-      <c r="G29" s="168"/>
+      <c r="B29" s="144"/>
+      <c r="C29" s="144"/>
+      <c r="D29" s="144"/>
+      <c r="E29" s="144"/>
+      <c r="F29" s="144"/>
+      <c r="G29" s="145"/>
       <c r="J29" s="102"/>
     </row>
     <row r="30" spans="1:17">
       <c r="A30" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B30" s="144" t="s">
+      <c r="B30" s="164" t="s">
         <v>180</v>
       </c>
-      <c r="C30" s="144"/>
-      <c r="D30" s="144"/>
-      <c r="E30" s="144"/>
-      <c r="F30" s="144"/>
-      <c r="G30" s="144"/>
+      <c r="C30" s="164"/>
+      <c r="D30" s="164"/>
+      <c r="E30" s="164"/>
+      <c r="F30" s="164"/>
+      <c r="G30" s="164"/>
       <c r="H30" s="95"/>
       <c r="I30" s="95"/>
       <c r="J30" s="102"/>
@@ -11043,12 +11049,12 @@
     </row>
     <row r="31" spans="1:17">
       <c r="A31" s="106"/>
-      <c r="B31" s="148"/>
-      <c r="C31" s="148"/>
-      <c r="D31" s="148"/>
-      <c r="E31" s="148"/>
-      <c r="F31" s="148"/>
-      <c r="G31" s="149"/>
+      <c r="B31" s="157"/>
+      <c r="C31" s="157"/>
+      <c r="D31" s="157"/>
+      <c r="E31" s="157"/>
+      <c r="F31" s="157"/>
+      <c r="G31" s="168"/>
       <c r="H31" s="102"/>
       <c r="I31" s="102"/>
       <c r="J31"/>
@@ -11061,12 +11067,12 @@
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="107"/>
-      <c r="B32" s="150"/>
-      <c r="C32" s="150"/>
-      <c r="D32" s="150"/>
-      <c r="E32" s="150"/>
-      <c r="F32" s="150"/>
-      <c r="G32" s="151"/>
+      <c r="B32" s="158"/>
+      <c r="C32" s="158"/>
+      <c r="D32" s="158"/>
+      <c r="E32" s="158"/>
+      <c r="F32" s="158"/>
+      <c r="G32" s="169"/>
       <c r="H32" s="102"/>
       <c r="I32" s="102"/>
       <c r="K32" s="102"/>
@@ -11078,12 +11084,12 @@
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="108"/>
-      <c r="B33" s="152"/>
-      <c r="C33" s="152"/>
-      <c r="D33" s="152"/>
-      <c r="E33" s="152"/>
-      <c r="F33" s="152"/>
-      <c r="G33" s="153"/>
+      <c r="B33" s="159"/>
+      <c r="C33" s="159"/>
+      <c r="D33" s="159"/>
+      <c r="E33" s="159"/>
+      <c r="F33" s="159"/>
+      <c r="G33" s="170"/>
       <c r="H33" s="102"/>
       <c r="I33" s="102"/>
       <c r="J33" s="95"/>
@@ -11136,64 +11142,64 @@
       <c r="P36" s="49"/>
     </row>
     <row r="37" spans="1:17" ht="15">
-      <c r="A37" s="180" t="s">
+      <c r="A37" s="181" t="s">
         <v>115</v>
       </c>
-      <c r="B37" s="180" t="s">
+      <c r="B37" s="181" t="s">
         <v>116</v>
       </c>
       <c r="C37" s="51" t="s">
         <v>117</v>
       </c>
-      <c r="D37" s="180" t="s">
+      <c r="D37" s="181" t="s">
         <v>99</v>
       </c>
-      <c r="E37" s="180" t="s">
+      <c r="E37" s="181" t="s">
         <v>156</v>
       </c>
-      <c r="F37" s="180" t="s">
+      <c r="F37" s="181" t="s">
         <v>171</v>
       </c>
-      <c r="G37" s="180" t="s">
+      <c r="G37" s="181" t="s">
         <v>136</v>
       </c>
-      <c r="H37" s="180" t="s">
+      <c r="H37" s="181" t="s">
         <v>113</v>
       </c>
-      <c r="I37" s="180" t="s">
+      <c r="I37" s="181" t="s">
         <v>230</v>
       </c>
       <c r="J37" s="176" t="s">
         <v>190</v>
       </c>
-      <c r="K37" s="185" t="s">
+      <c r="K37" s="186" t="s">
         <v>119</v>
       </c>
-      <c r="L37" s="186"/>
-      <c r="M37" s="187" t="s">
+      <c r="L37" s="187"/>
+      <c r="M37" s="188" t="s">
         <v>120</v>
       </c>
-      <c r="N37" s="186"/>
+      <c r="N37" s="187"/>
       <c r="O37" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="P37" s="180" t="s">
+      <c r="P37" s="181" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="15">
-      <c r="A38" s="188"/>
-      <c r="B38" s="188"/>
+      <c r="A38" s="185"/>
+      <c r="B38" s="185"/>
       <c r="C38" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="D38" s="188"/>
-      <c r="E38" s="181"/>
-      <c r="F38" s="181"/>
-      <c r="G38" s="188"/>
-      <c r="H38" s="188"/>
-      <c r="I38" s="188"/>
-      <c r="J38" s="177"/>
+      <c r="D38" s="185"/>
+      <c r="E38" s="182"/>
+      <c r="F38" s="182"/>
+      <c r="G38" s="185"/>
+      <c r="H38" s="185"/>
+      <c r="I38" s="185"/>
+      <c r="J38" s="183"/>
       <c r="K38" s="53" t="s">
         <v>123</v>
       </c>
@@ -11209,7 +11215,7 @@
       <c r="O38" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="P38" s="188"/>
+      <c r="P38" s="185"/>
     </row>
     <row r="39" spans="1:17">
       <c r="A39" s="55">
@@ -11707,6 +11713,23 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="P37:P38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="J37:J38"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
     <mergeCell ref="B27:G27"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
@@ -11719,23 +11742,6 @@
     <mergeCell ref="B24:G24"/>
     <mergeCell ref="B25:G25"/>
     <mergeCell ref="B26:G26"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="A29:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="P37:P38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="J37:J38"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="M37:N37"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">
@@ -11783,8 +11789,8 @@
   </sheetPr>
   <dimension ref="A1:Q64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -11945,10 +11951,10 @@
         <v>168</v>
       </c>
       <c r="B15" s="111"/>
-      <c r="C15" s="133" t="s">
+      <c r="C15" s="151" t="s">
         <v>169</v>
       </c>
-      <c r="D15" s="133"/>
+      <c r="D15" s="151"/>
       <c r="E15" s="1" t="s">
         <v>170</v>
       </c>
@@ -11958,10 +11964,10 @@
         <v>171</v>
       </c>
       <c r="B16" s="111"/>
-      <c r="C16" s="133" t="s">
+      <c r="C16" s="151" t="s">
         <v>172</v>
       </c>
-      <c r="D16" s="133"/>
+      <c r="D16" s="151"/>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="112" t="s">
@@ -11987,28 +11993,28 @@
       <c r="A18" s="6"/>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="169" t="s">
+      <c r="A19" s="146" t="s">
         <v>186</v>
       </c>
-      <c r="B19" s="169"/>
-      <c r="C19" s="169"/>
-      <c r="D19" s="169"/>
-      <c r="E19" s="169"/>
-      <c r="F19" s="169"/>
-      <c r="G19" s="169"/>
+      <c r="B19" s="146"/>
+      <c r="C19" s="146"/>
+      <c r="D19" s="146"/>
+      <c r="E19" s="146"/>
+      <c r="F19" s="146"/>
+      <c r="G19" s="146"/>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B20" s="163" t="s">
+      <c r="B20" s="140" t="s">
         <v>177</v>
       </c>
-      <c r="C20" s="164"/>
-      <c r="D20" s="164"/>
-      <c r="E20" s="164"/>
-      <c r="F20" s="164"/>
-      <c r="G20" s="165"/>
+      <c r="C20" s="141"/>
+      <c r="D20" s="141"/>
+      <c r="E20" s="141"/>
+      <c r="F20" s="141"/>
+      <c r="G20" s="142"/>
       <c r="H20" s="95"/>
       <c r="I20" s="95"/>
       <c r="K20" s="95"/>
@@ -12020,12 +12026,12 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="106"/>
-      <c r="B21" s="148"/>
-      <c r="C21" s="148"/>
-      <c r="D21" s="148"/>
-      <c r="E21" s="148"/>
-      <c r="F21" s="148"/>
-      <c r="G21" s="148"/>
+      <c r="B21" s="157"/>
+      <c r="C21" s="157"/>
+      <c r="D21" s="157"/>
+      <c r="E21" s="157"/>
+      <c r="F21" s="157"/>
+      <c r="G21" s="157"/>
       <c r="H21" s="102"/>
       <c r="I21" s="102"/>
       <c r="K21" s="102"/>
@@ -12037,12 +12043,12 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="107"/>
-      <c r="B22" s="150"/>
-      <c r="C22" s="150"/>
-      <c r="D22" s="150"/>
-      <c r="E22" s="150"/>
-      <c r="F22" s="150"/>
-      <c r="G22" s="150"/>
+      <c r="B22" s="158"/>
+      <c r="C22" s="158"/>
+      <c r="D22" s="158"/>
+      <c r="E22" s="158"/>
+      <c r="F22" s="158"/>
+      <c r="G22" s="158"/>
       <c r="H22" s="102"/>
       <c r="I22" s="102"/>
       <c r="K22" s="102"/>
@@ -12054,12 +12060,12 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="108"/>
-      <c r="B23" s="152"/>
-      <c r="C23" s="152"/>
-      <c r="D23" s="152"/>
-      <c r="E23" s="152"/>
-      <c r="F23" s="152"/>
-      <c r="G23" s="152"/>
+      <c r="B23" s="159"/>
+      <c r="C23" s="159"/>
+      <c r="D23" s="159"/>
+      <c r="E23" s="159"/>
+      <c r="F23" s="159"/>
+      <c r="G23" s="159"/>
       <c r="H23" s="102"/>
       <c r="I23" s="102"/>
       <c r="J23" s="95"/>
@@ -12075,29 +12081,29 @@
       <c r="J24" s="102"/>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" s="166" t="s">
+      <c r="A25" s="143" t="s">
         <v>187</v>
       </c>
-      <c r="B25" s="167"/>
-      <c r="C25" s="167"/>
-      <c r="D25" s="167"/>
-      <c r="E25" s="167"/>
-      <c r="F25" s="167"/>
-      <c r="G25" s="168"/>
+      <c r="B25" s="144"/>
+      <c r="C25" s="144"/>
+      <c r="D25" s="144"/>
+      <c r="E25" s="144"/>
+      <c r="F25" s="144"/>
+      <c r="G25" s="145"/>
       <c r="J25" s="102"/>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="144" t="s">
+      <c r="B26" s="164" t="s">
         <v>178</v>
       </c>
-      <c r="C26" s="144"/>
-      <c r="D26" s="144"/>
-      <c r="E26" s="144"/>
-      <c r="F26" s="144"/>
-      <c r="G26" s="144"/>
+      <c r="C26" s="164"/>
+      <c r="D26" s="164"/>
+      <c r="E26" s="164"/>
+      <c r="F26" s="164"/>
+      <c r="G26" s="164"/>
       <c r="H26" s="95"/>
       <c r="I26" s="95"/>
       <c r="J26" s="102"/>
@@ -12112,14 +12118,14 @@
       <c r="A27" s="106">
         <v>1</v>
       </c>
-      <c r="B27" s="145" t="s">
+      <c r="B27" s="165" t="s">
         <v>179</v>
       </c>
-      <c r="C27" s="145"/>
-      <c r="D27" s="145"/>
-      <c r="E27" s="145"/>
-      <c r="F27" s="145"/>
-      <c r="G27" s="145"/>
+      <c r="C27" s="165"/>
+      <c r="D27" s="165"/>
+      <c r="E27" s="165"/>
+      <c r="F27" s="165"/>
+      <c r="G27" s="165"/>
       <c r="H27" s="102"/>
       <c r="I27" s="102"/>
       <c r="K27" s="102"/>
@@ -12131,12 +12137,12 @@
     </row>
     <row r="28" spans="1:17">
       <c r="A28" s="107"/>
-      <c r="B28" s="146"/>
-      <c r="C28" s="146"/>
-      <c r="D28" s="146"/>
-      <c r="E28" s="146"/>
-      <c r="F28" s="146"/>
-      <c r="G28" s="146"/>
+      <c r="B28" s="166"/>
+      <c r="C28" s="166"/>
+      <c r="D28" s="166"/>
+      <c r="E28" s="166"/>
+      <c r="F28" s="166"/>
+      <c r="G28" s="166"/>
       <c r="H28" s="102"/>
       <c r="I28" s="102"/>
       <c r="K28" s="102"/>
@@ -12148,12 +12154,12 @@
     </row>
     <row r="29" spans="1:17">
       <c r="A29" s="108"/>
-      <c r="B29" s="147"/>
-      <c r="C29" s="147"/>
-      <c r="D29" s="147"/>
-      <c r="E29" s="147"/>
-      <c r="F29" s="147"/>
-      <c r="G29" s="147"/>
+      <c r="B29" s="167"/>
+      <c r="C29" s="167"/>
+      <c r="D29" s="167"/>
+      <c r="E29" s="167"/>
+      <c r="F29" s="167"/>
+      <c r="G29" s="167"/>
       <c r="H29" s="102"/>
       <c r="I29" s="102"/>
       <c r="J29" s="95"/>
@@ -12182,29 +12188,29 @@
       <c r="O30"/>
     </row>
     <row r="31" spans="1:17">
-      <c r="A31" s="166" t="s">
+      <c r="A31" s="143" t="s">
         <v>188</v>
       </c>
-      <c r="B31" s="167"/>
-      <c r="C31" s="167"/>
-      <c r="D31" s="167"/>
-      <c r="E31" s="167"/>
-      <c r="F31" s="167"/>
-      <c r="G31" s="168"/>
+      <c r="B31" s="144"/>
+      <c r="C31" s="144"/>
+      <c r="D31" s="144"/>
+      <c r="E31" s="144"/>
+      <c r="F31" s="144"/>
+      <c r="G31" s="145"/>
       <c r="J31" s="102"/>
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="144" t="s">
+      <c r="B32" s="164" t="s">
         <v>180</v>
       </c>
-      <c r="C32" s="144"/>
-      <c r="D32" s="144"/>
-      <c r="E32" s="144"/>
-      <c r="F32" s="144"/>
-      <c r="G32" s="144"/>
+      <c r="C32" s="164"/>
+      <c r="D32" s="164"/>
+      <c r="E32" s="164"/>
+      <c r="F32" s="164"/>
+      <c r="G32" s="164"/>
       <c r="H32" s="95"/>
       <c r="I32" s="95"/>
       <c r="J32" s="102"/>
@@ -12217,12 +12223,12 @@
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="106"/>
-      <c r="B33" s="148"/>
-      <c r="C33" s="148"/>
-      <c r="D33" s="148"/>
-      <c r="E33" s="148"/>
-      <c r="F33" s="148"/>
-      <c r="G33" s="149"/>
+      <c r="B33" s="157"/>
+      <c r="C33" s="157"/>
+      <c r="D33" s="157"/>
+      <c r="E33" s="157"/>
+      <c r="F33" s="157"/>
+      <c r="G33" s="168"/>
       <c r="H33" s="102"/>
       <c r="I33" s="102"/>
       <c r="J33"/>
@@ -12235,12 +12241,12 @@
     </row>
     <row r="34" spans="1:17">
       <c r="A34" s="107"/>
-      <c r="B34" s="150"/>
-      <c r="C34" s="150"/>
-      <c r="D34" s="150"/>
-      <c r="E34" s="150"/>
-      <c r="F34" s="150"/>
-      <c r="G34" s="151"/>
+      <c r="B34" s="158"/>
+      <c r="C34" s="158"/>
+      <c r="D34" s="158"/>
+      <c r="E34" s="158"/>
+      <c r="F34" s="158"/>
+      <c r="G34" s="169"/>
       <c r="H34" s="102"/>
       <c r="I34" s="102"/>
       <c r="K34" s="102"/>
@@ -12252,12 +12258,12 @@
     </row>
     <row r="35" spans="1:17">
       <c r="A35" s="108"/>
-      <c r="B35" s="152"/>
-      <c r="C35" s="152"/>
-      <c r="D35" s="152"/>
-      <c r="E35" s="152"/>
-      <c r="F35" s="152"/>
-      <c r="G35" s="153"/>
+      <c r="B35" s="159"/>
+      <c r="C35" s="159"/>
+      <c r="D35" s="159"/>
+      <c r="E35" s="159"/>
+      <c r="F35" s="159"/>
+      <c r="G35" s="170"/>
       <c r="H35" s="102"/>
       <c r="I35" s="102"/>
       <c r="J35" s="95"/>
@@ -12310,25 +12316,25 @@
       <c r="P38" s="49"/>
     </row>
     <row r="39" spans="1:17" ht="15">
-      <c r="A39" s="180" t="s">
+      <c r="A39" s="181" t="s">
         <v>115</v>
       </c>
-      <c r="B39" s="180" t="s">
+      <c r="B39" s="181" t="s">
         <v>116</v>
       </c>
       <c r="C39" s="51" t="s">
         <v>117</v>
       </c>
-      <c r="D39" s="180" t="s">
+      <c r="D39" s="181" t="s">
         <v>99</v>
       </c>
-      <c r="E39" s="180" t="s">
+      <c r="E39" s="181" t="s">
         <v>156</v>
       </c>
-      <c r="F39" s="180" t="s">
+      <c r="F39" s="181" t="s">
         <v>171</v>
       </c>
-      <c r="G39" s="180" t="s">
+      <c r="G39" s="181" t="s">
         <v>136</v>
       </c>
       <c r="H39" s="189" t="s">
@@ -12340,34 +12346,34 @@
       <c r="J39" s="176" t="s">
         <v>190</v>
       </c>
-      <c r="K39" s="185" t="s">
+      <c r="K39" s="186" t="s">
         <v>119</v>
       </c>
-      <c r="L39" s="186"/>
-      <c r="M39" s="187" t="s">
+      <c r="L39" s="187"/>
+      <c r="M39" s="188" t="s">
         <v>120</v>
       </c>
-      <c r="N39" s="186"/>
+      <c r="N39" s="187"/>
       <c r="O39" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="P39" s="180" t="s">
+      <c r="P39" s="181" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="15">
-      <c r="A40" s="188"/>
-      <c r="B40" s="188"/>
+      <c r="A40" s="185"/>
+      <c r="B40" s="185"/>
       <c r="C40" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="D40" s="188"/>
-      <c r="E40" s="181"/>
-      <c r="F40" s="181"/>
-      <c r="G40" s="188"/>
-      <c r="H40" s="188"/>
-      <c r="I40" s="188"/>
-      <c r="J40" s="177"/>
+      <c r="D40" s="185"/>
+      <c r="E40" s="182"/>
+      <c r="F40" s="182"/>
+      <c r="G40" s="185"/>
+      <c r="H40" s="185"/>
+      <c r="I40" s="185"/>
+      <c r="J40" s="183"/>
       <c r="K40" s="53" t="s">
         <v>123</v>
       </c>
@@ -12383,7 +12389,7 @@
       <c r="O40" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="P40" s="188"/>
+      <c r="P40" s="185"/>
     </row>
     <row r="41" spans="1:17">
       <c r="A41" s="55">
@@ -12839,6 +12845,23 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="P39:P40"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="I39:I40"/>
+    <mergeCell ref="J39:J40"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
     <mergeCell ref="B29:G29"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C16:D16"/>
@@ -12851,26 +12874,9 @@
     <mergeCell ref="B26:G26"/>
     <mergeCell ref="B27:G27"/>
     <mergeCell ref="B28:G28"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="P39:P40"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="I39:I40"/>
-    <mergeCell ref="J39:J40"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="M39:N39"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
-  <dataValidations count="3">
+  <dataValidations disablePrompts="1" count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{5153E67C-3569-F04C-93A4-3601574FAD6F}">
       <formula1>Validate実装パターン</formula1>
     </dataValidation>
@@ -12889,7 +12895,7 @@
   </headerFooter>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8FD8E9D1-D5B4-D14C-A9F6-5418E672D3E4}">
           <x14:formula1>
             <xm:f>config!$B$5:$B$6</xm:f>
@@ -13250,7 +13256,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>

</xml_diff>

<commit_message>
3.1.4: Correct treating of trailed "/" of locationUrl.
</commit_message>
<xml_diff>
--- a/meta/plainApi/BlancoApiPlainSample.xlsx
+++ b/meta/plainApi/BlancoApiPlainSample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10719"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorTs/meta/plainApi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78906414-04E9-B34B-A873-74C3755B5F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE63B43-3CED-A143-93D8-0C32328514A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2440" yWindow="500" windowWidth="29440" windowHeight="20500" tabRatio="860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2440" yWindow="500" windowWidth="29440" windowHeight="20500" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="process" sheetId="19" r:id="rId1"/>
@@ -1641,10 +1641,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>/api/3.0.0</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>型</t>
   </si>
   <si>
@@ -2496,6 +2492,10 @@
   </si>
   <si>
     <t>/get_addition</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/api/3.0.0</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -4379,8 +4379,8 @@
   </sheetPr>
   <dimension ref="A1:O75"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -4409,17 +4409,17 @@
       </c>
       <c r="B1" s="18"/>
       <c r="E1" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -4438,7 +4438,7 @@
       <c r="B6" s="174"/>
       <c r="C6" s="175"/>
       <c r="D6" s="171" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E6" s="171"/>
     </row>
@@ -4449,7 +4449,7 @@
       <c r="B7" s="162"/>
       <c r="C7" s="162"/>
       <c r="D7" s="171" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E7" s="171"/>
     </row>
@@ -4460,7 +4460,7 @@
       <c r="B8" s="162"/>
       <c r="C8" s="162"/>
       <c r="D8" s="171" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E8" s="171"/>
     </row>
@@ -4471,7 +4471,7 @@
       <c r="B9" s="162"/>
       <c r="C9" s="162"/>
       <c r="D9" s="171" t="s">
-        <v>98</v>
+        <v>244</v>
       </c>
       <c r="E9" s="171"/>
     </row>
@@ -4491,73 +4491,73 @@
       <c r="B11" s="162"/>
       <c r="C11" s="162"/>
       <c r="D11" s="171" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E11" s="171"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="134" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B12" s="134"/>
       <c r="C12" s="134"/>
       <c r="D12" s="151" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E12" s="151"/>
       <c r="F12" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="134" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B13" s="134"/>
       <c r="C13" s="134"/>
       <c r="D13" s="150" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E13" s="151"/>
     </row>
     <row r="14" spans="1:6" ht="55" customHeight="1">
       <c r="A14" s="134" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B14" s="134"/>
       <c r="C14" s="134"/>
       <c r="D14" s="172" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E14" s="151"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="134" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B15" s="134"/>
       <c r="C15" s="134"/>
       <c r="D15" s="150"/>
       <c r="E15" s="151"/>
       <c r="F15" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="134" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B16" s="134"/>
       <c r="C16" s="134"/>
       <c r="D16" s="150"/>
       <c r="E16" s="151"/>
       <c r="F16" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:15">
       <c r="A17" s="152" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B17" s="153"/>
       <c r="C17" s="154"/>
@@ -4565,15 +4565,15 @@
     </row>
     <row r="18" spans="1:15">
       <c r="A18" s="135" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B18" s="136"/>
       <c r="C18" s="137"/>
       <c r="D18" s="90" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F18"/>
       <c r="G18"/>
@@ -4589,7 +4589,7 @@
     </row>
     <row r="20" spans="1:15">
       <c r="A20" s="147" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B20" s="148"/>
       <c r="C20" s="148"/>
@@ -4600,7 +4600,7 @@
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="91" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B21" s="100"/>
       <c r="C21" s="92"/>
@@ -4627,7 +4627,7 @@
     </row>
     <row r="23" spans="1:15">
       <c r="A23" s="88" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B23" s="103"/>
       <c r="C23" s="89"/>
@@ -4641,7 +4641,7 @@
     </row>
     <row r="25" spans="1:15">
       <c r="A25" s="146" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B25" s="146"/>
       <c r="C25" s="146"/>
@@ -4655,7 +4655,7 @@
         <v>68</v>
       </c>
       <c r="B26" s="140" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C26" s="141"/>
       <c r="D26" s="141"/>
@@ -4723,7 +4723,7 @@
     </row>
     <row r="31" spans="1:15">
       <c r="A31" s="143" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B31" s="144"/>
       <c r="C31" s="144"/>
@@ -4737,7 +4737,7 @@
         <v>68</v>
       </c>
       <c r="B32" s="164" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C32" s="164"/>
       <c r="D32" s="164"/>
@@ -4757,7 +4757,7 @@
         <v>1</v>
       </c>
       <c r="B33" s="165" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C33" s="165"/>
       <c r="D33" s="165"/>
@@ -4821,7 +4821,7 @@
     </row>
     <row r="37" spans="1:15">
       <c r="A37" s="143" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B37" s="144"/>
       <c r="C37" s="144"/>
@@ -4835,7 +4835,7 @@
         <v>68</v>
       </c>
       <c r="B38" s="164" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C38" s="164"/>
       <c r="D38" s="164"/>
@@ -4916,7 +4916,7 @@
     </row>
     <row r="43" spans="1:15">
       <c r="A43" s="146" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B43" s="146"/>
       <c r="C43" s="146"/>
@@ -4930,10 +4930,10 @@
         <v>68</v>
       </c>
       <c r="B44" s="105" t="s">
+        <v>195</v>
+      </c>
+      <c r="C44" s="105" t="s">
         <v>196</v>
-      </c>
-      <c r="C44" s="105" t="s">
-        <v>197</v>
       </c>
       <c r="D44" s="105"/>
       <c r="E44" s="105"/>
@@ -4952,10 +4952,10 @@
         <v>1</v>
       </c>
       <c r="B45" s="120" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C45" s="120" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D45" s="120"/>
       <c r="E45" s="120"/>
@@ -4974,10 +4974,10 @@
         <v>2</v>
       </c>
       <c r="B46" s="120" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C46" s="120" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D46" s="120"/>
       <c r="E46" s="120"/>
@@ -4996,10 +4996,10 @@
         <v>3</v>
       </c>
       <c r="B47" s="120" t="s">
+        <v>199</v>
+      </c>
+      <c r="C47" s="120" t="s">
         <v>200</v>
-      </c>
-      <c r="C47" s="120" t="s">
-        <v>201</v>
       </c>
       <c r="D47" s="120"/>
       <c r="E47" s="120"/>
@@ -5385,7 +5385,7 @@
   </sheetPr>
   <dimension ref="A1:V67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" activeCellId="1" sqref="C14 C13"/>
     </sheetView>
   </sheetViews>
@@ -5425,7 +5425,7 @@
         <v>22</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -5463,7 +5463,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="46" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D7" s="33"/>
       <c r="S7"/>
@@ -5474,23 +5474,23 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="110" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D8" s="114"/>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="110" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="47" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="110"/>
@@ -5498,7 +5498,7 @@
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="110"/>
@@ -5506,7 +5506,7 @@
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="47" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="110"/>
@@ -5514,15 +5514,15 @@
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="46" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D13" s="33"/>
       <c r="E13" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -5539,53 +5539,53 @@
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="46" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D15" s="33"/>
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="111" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B16" s="111"/>
       <c r="C16" s="151" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D16" s="151"/>
       <c r="E16" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="17" spans="1:22">
       <c r="A17" s="111" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B17" s="111"/>
       <c r="C17" s="151" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D17" s="151"/>
     </row>
     <row r="18" spans="1:22">
       <c r="A18" s="111" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B18" s="111"/>
       <c r="C18" s="150" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D18" s="151"/>
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="112" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B19" s="113"/>
       <c r="C19" s="90" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F19"/>
       <c r="G19"/>
@@ -5604,14 +5604,14 @@
     </row>
     <row r="20" spans="1:22">
       <c r="A20" s="112" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B20" s="113"/>
       <c r="C20" s="90" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F20"/>
       <c r="G20"/>
@@ -5633,7 +5633,7 @@
     </row>
     <row r="22" spans="1:22">
       <c r="A22" s="146" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B22" s="146"/>
       <c r="C22" s="146"/>
@@ -5647,7 +5647,7 @@
         <v>68</v>
       </c>
       <c r="B23" s="140" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C23" s="141"/>
       <c r="D23" s="141"/>
@@ -5743,7 +5743,7 @@
     </row>
     <row r="28" spans="1:22">
       <c r="A28" s="143" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B28" s="144"/>
       <c r="C28" s="144"/>
@@ -5757,7 +5757,7 @@
         <v>68</v>
       </c>
       <c r="B29" s="164" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C29" s="164"/>
       <c r="D29" s="164"/>
@@ -5784,7 +5784,7 @@
         <v>1</v>
       </c>
       <c r="B30" s="165" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C30" s="165"/>
       <c r="D30" s="165"/>
@@ -5876,7 +5876,7 @@
     </row>
     <row r="34" spans="1:22">
       <c r="A34" s="143" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B34" s="144"/>
       <c r="C34" s="144"/>
@@ -5890,7 +5890,7 @@
         <v>68</v>
       </c>
       <c r="B35" s="164" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C35" s="164"/>
       <c r="D35" s="164"/>
@@ -6006,7 +6006,7 @@
     <row r="40" spans="1:22">
       <c r="A40" s="6"/>
       <c r="N40" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="41" spans="1:22">
@@ -6048,37 +6048,37 @@
         <v>2</v>
       </c>
       <c r="E42" s="181" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F42" s="181" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G42" s="176" t="s">
         <v>12</v>
       </c>
       <c r="H42" s="176" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I42" s="176" t="s">
+        <v>236</v>
+      </c>
+      <c r="J42" s="181" t="s">
         <v>237</v>
       </c>
-      <c r="J42" s="181" t="s">
-        <v>238</v>
-      </c>
       <c r="K42" s="181" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L42" s="184" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="M42" s="176" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N42" s="176" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="O42" s="176" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="P42" s="179" t="s">
         <v>70</v>
@@ -6139,27 +6139,27 @@
         <v>90</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E44" s="23"/>
       <c r="F44" s="128"/>
       <c r="G44" s="75" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H44" s="23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I44" s="23"/>
       <c r="J44" s="23"/>
       <c r="K44" s="23"/>
       <c r="L44" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="M44" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N44" s="120" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O44" s="23"/>
       <c r="P44" s="23">
@@ -6185,7 +6185,7 @@
         <v>92</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E45" s="24"/>
       <c r="F45" s="24"/>
@@ -6199,10 +6199,10 @@
       <c r="L45" s="24"/>
       <c r="M45" s="24"/>
       <c r="N45" s="120" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="O45" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P45" s="20"/>
       <c r="Q45" s="29"/>
@@ -6225,7 +6225,7 @@
       </c>
       <c r="C46" s="13"/>
       <c r="D46" s="25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E46" s="25"/>
       <c r="F46" s="25"/>
@@ -6239,7 +6239,7 @@
       <c r="L46" s="25"/>
       <c r="M46" s="25"/>
       <c r="N46" s="120" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="O46" s="24"/>
       <c r="P46" s="20"/>
@@ -6259,27 +6259,27 @@
       </c>
       <c r="C47" s="13"/>
       <c r="D47" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E47" s="73" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F47" s="73"/>
       <c r="G47" s="78"/>
       <c r="H47" s="73" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I47" s="23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J47" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K47" s="73"/>
       <c r="L47" s="73"/>
       <c r="M47" s="73"/>
       <c r="N47" s="120" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="O47" s="24"/>
       <c r="P47" s="20"/>
@@ -6299,15 +6299,15 @@
       </c>
       <c r="C48" s="13"/>
       <c r="D48" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E48" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F48" s="25"/>
       <c r="G48" s="77"/>
       <c r="H48" s="25" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I48" s="25"/>
       <c r="J48" s="25"/>
@@ -6322,7 +6322,7 @@
       <c r="S48" s="30"/>
       <c r="T48" s="30"/>
       <c r="U48" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="49" spans="1:21">
@@ -6335,13 +6335,13 @@
       </c>
       <c r="C49" s="13"/>
       <c r="D49" s="25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E49" s="25"/>
       <c r="F49" s="25"/>
       <c r="G49" s="77"/>
       <c r="H49" s="25" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I49" s="25"/>
       <c r="J49" s="25"/>
@@ -6363,17 +6363,17 @@
         <v>7</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C50" s="13"/>
       <c r="D50" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E50" s="25"/>
       <c r="F50" s="25"/>
       <c r="G50" s="77"/>
       <c r="H50" s="25" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I50" s="25"/>
       <c r="J50" s="25"/>
@@ -6913,7 +6913,7 @@
         <v>22</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -6951,7 +6951,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="46" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D7" s="33"/>
       <c r="N7"/>
@@ -6968,23 +6968,23 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="74" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D9" s="85"/>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="46"/>
       <c r="D10" s="33"/>
       <c r="E10" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -7001,43 +7001,43 @@
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="46" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D12" s="33"/>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="111" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B13" s="111"/>
       <c r="C13" s="151" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D13" s="151"/>
       <c r="E13" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" s="111" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B14" s="111"/>
       <c r="C14" s="151" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D14" s="151"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="112" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B15" s="113"/>
       <c r="C15" s="90" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G15"/>
       <c r="H15"/>
@@ -7053,7 +7053,7 @@
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="146" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B17" s="146"/>
       <c r="C17" s="146"/>
@@ -7067,7 +7067,7 @@
         <v>68</v>
       </c>
       <c r="B18" s="140" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C18" s="141"/>
       <c r="D18" s="141"/>
@@ -7141,7 +7141,7 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="143" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B23" s="144"/>
       <c r="C23" s="144"/>
@@ -7156,7 +7156,7 @@
         <v>68</v>
       </c>
       <c r="B24" s="164" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C24" s="164"/>
       <c r="D24" s="164"/>
@@ -7178,7 +7178,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="165" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C25" s="165"/>
       <c r="D25" s="165"/>
@@ -7248,7 +7248,7 @@
     </row>
     <row r="29" spans="1:17">
       <c r="A29" s="143" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B29" s="144"/>
       <c r="C29" s="144"/>
@@ -7263,7 +7263,7 @@
         <v>68</v>
       </c>
       <c r="B30" s="164" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C30" s="164"/>
       <c r="D30" s="164"/>
@@ -7356,7 +7356,7 @@
     </row>
     <row r="36" spans="1:17">
       <c r="A36" s="47" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B36" s="48"/>
       <c r="C36" s="48"/>
@@ -7376,55 +7376,55 @@
     </row>
     <row r="37" spans="1:17" ht="15">
       <c r="A37" s="181" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37" s="181" t="s">
         <v>115</v>
       </c>
-      <c r="B37" s="181" t="s">
+      <c r="C37" s="51" t="s">
         <v>116</v>
       </c>
-      <c r="C37" s="51" t="s">
-        <v>117</v>
-      </c>
       <c r="D37" s="181" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E37" s="181" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F37" s="181" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G37" s="181" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H37" s="181" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I37" s="181" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J37" s="176" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K37" s="186" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L37" s="187"/>
       <c r="M37" s="188" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N37" s="187"/>
       <c r="O37" s="50" t="s">
+        <v>120</v>
+      </c>
+      <c r="P37" s="181" t="s">
         <v>121</v>
-      </c>
-      <c r="P37" s="181" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="15">
       <c r="A38" s="185"/>
       <c r="B38" s="185"/>
       <c r="C38" s="52" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D38" s="185"/>
       <c r="E38" s="182"/>
@@ -7434,19 +7434,19 @@
       <c r="I38" s="185"/>
       <c r="J38" s="183"/>
       <c r="K38" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="L38" s="53" t="s">
         <v>123</v>
       </c>
-      <c r="L38" s="53" t="s">
+      <c r="M38" s="53" t="s">
         <v>124</v>
       </c>
-      <c r="M38" s="53" t="s">
+      <c r="N38" s="53" t="s">
         <v>125</v>
       </c>
-      <c r="N38" s="53" t="s">
+      <c r="O38" s="54" t="s">
         <v>126</v>
-      </c>
-      <c r="O38" s="54" t="s">
-        <v>127</v>
       </c>
       <c r="P38" s="185"/>
     </row>
@@ -7455,13 +7455,13 @@
         <v>1</v>
       </c>
       <c r="B39" s="56" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C39" s="57" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D39" s="58" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E39" s="58"/>
       <c r="F39" s="58"/>
@@ -7469,7 +7469,7 @@
       <c r="H39" s="58"/>
       <c r="I39" s="58"/>
       <c r="J39" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K39" s="58"/>
       <c r="L39" s="58"/>
@@ -7483,13 +7483,13 @@
         <v>2</v>
       </c>
       <c r="B40" s="56" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C40" s="57" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D40" s="58" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E40" s="58"/>
       <c r="F40" s="58"/>
@@ -7497,7 +7497,7 @@
       <c r="H40" s="58"/>
       <c r="I40" s="58"/>
       <c r="J40" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K40" s="56"/>
       <c r="L40" s="56"/>
@@ -7511,11 +7511,11 @@
         <v>3</v>
       </c>
       <c r="B41" s="60" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C41" s="45"/>
       <c r="D41" s="61" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E41" s="61"/>
       <c r="F41" s="61"/>
@@ -7523,7 +7523,7 @@
       <c r="H41" s="61"/>
       <c r="I41" s="61"/>
       <c r="J41" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K41" s="56"/>
       <c r="L41" s="56"/>
@@ -7537,11 +7537,11 @@
         <v>4</v>
       </c>
       <c r="B42" s="63" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C42" s="64"/>
       <c r="D42" s="65" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E42" s="65"/>
       <c r="F42" s="65"/>
@@ -7549,7 +7549,7 @@
       <c r="H42" s="65"/>
       <c r="I42" s="65"/>
       <c r="J42" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K42" s="56"/>
       <c r="L42" s="56"/>
@@ -7563,21 +7563,21 @@
         <v>5</v>
       </c>
       <c r="B43" s="63" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C43" s="64"/>
       <c r="D43" s="65" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E43" s="65" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F43" s="65"/>
       <c r="G43" s="82"/>
       <c r="H43" s="65"/>
       <c r="I43" s="65"/>
       <c r="J43" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K43" s="58"/>
       <c r="L43" s="58"/>
@@ -7591,11 +7591,11 @@
         <v>6</v>
       </c>
       <c r="B44" s="63" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C44" s="64"/>
       <c r="D44" s="65" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E44" s="65"/>
       <c r="F44" s="65"/>
@@ -7603,7 +7603,7 @@
       <c r="H44" s="65"/>
       <c r="I44" s="65"/>
       <c r="J44" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K44" s="56"/>
       <c r="L44" s="56"/>
@@ -7617,11 +7617,11 @@
         <v>7</v>
       </c>
       <c r="B45" s="63" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C45" s="64"/>
       <c r="D45" s="65" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E45" s="65"/>
       <c r="F45" s="65"/>
@@ -7629,7 +7629,7 @@
       <c r="H45" s="65"/>
       <c r="I45" s="65"/>
       <c r="J45" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K45" s="56"/>
       <c r="L45" s="56"/>
@@ -8061,7 +8061,7 @@
         <v>22</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -8099,7 +8099,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="46" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D7" s="33"/>
       <c r="N7"/>
@@ -8110,55 +8110,55 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D8" s="34"/>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="74" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D9" s="85"/>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="127" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D10" s="33"/>
       <c r="E10" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="127" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D11" s="33"/>
       <c r="E11" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="46"/>
       <c r="D12" s="33"/>
       <c r="E12" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -8175,43 +8175,43 @@
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="46" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D14" s="33"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="111" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B15" s="111"/>
       <c r="C15" s="151" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D15" s="151"/>
       <c r="E15" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="111" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B16" s="111"/>
       <c r="C16" s="151" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D16" s="151"/>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="112" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B17" s="113"/>
       <c r="C17" s="90" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G17"/>
       <c r="H17"/>
@@ -8227,7 +8227,7 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="146" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B19" s="146"/>
       <c r="C19" s="146"/>
@@ -8241,7 +8241,7 @@
         <v>68</v>
       </c>
       <c r="B20" s="140" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C20" s="141"/>
       <c r="D20" s="141"/>
@@ -8315,7 +8315,7 @@
     </row>
     <row r="25" spans="1:17">
       <c r="A25" s="143" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B25" s="144"/>
       <c r="C25" s="144"/>
@@ -8330,7 +8330,7 @@
         <v>68</v>
       </c>
       <c r="B26" s="164" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C26" s="164"/>
       <c r="D26" s="164"/>
@@ -8352,7 +8352,7 @@
         <v>1</v>
       </c>
       <c r="B27" s="165" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C27" s="165"/>
       <c r="D27" s="165"/>
@@ -8422,7 +8422,7 @@
     </row>
     <row r="31" spans="1:17">
       <c r="A31" s="143" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B31" s="144"/>
       <c r="C31" s="144"/>
@@ -8437,7 +8437,7 @@
         <v>68</v>
       </c>
       <c r="B32" s="164" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C32" s="164"/>
       <c r="D32" s="164"/>
@@ -8530,7 +8530,7 @@
     </row>
     <row r="38" spans="1:17">
       <c r="A38" s="47" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B38" s="48"/>
       <c r="C38" s="48"/>
@@ -8550,55 +8550,55 @@
     </row>
     <row r="39" spans="1:17" ht="15">
       <c r="A39" s="181" t="s">
+        <v>114</v>
+      </c>
+      <c r="B39" s="181" t="s">
         <v>115</v>
       </c>
-      <c r="B39" s="181" t="s">
+      <c r="C39" s="51" t="s">
         <v>116</v>
       </c>
-      <c r="C39" s="51" t="s">
-        <v>117</v>
-      </c>
       <c r="D39" s="181" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E39" s="181" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F39" s="181" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G39" s="181" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H39" s="189" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I39" s="189" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J39" s="176" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K39" s="186" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L39" s="187"/>
       <c r="M39" s="188" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N39" s="187"/>
       <c r="O39" s="50" t="s">
+        <v>120</v>
+      </c>
+      <c r="P39" s="181" t="s">
         <v>121</v>
-      </c>
-      <c r="P39" s="181" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="15">
       <c r="A40" s="185"/>
       <c r="B40" s="185"/>
       <c r="C40" s="52" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D40" s="185"/>
       <c r="E40" s="182"/>
@@ -8608,19 +8608,19 @@
       <c r="I40" s="185"/>
       <c r="J40" s="183"/>
       <c r="K40" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="L40" s="53" t="s">
         <v>123</v>
       </c>
-      <c r="L40" s="53" t="s">
+      <c r="M40" s="53" t="s">
         <v>124</v>
       </c>
-      <c r="M40" s="53" t="s">
+      <c r="N40" s="53" t="s">
         <v>125</v>
       </c>
-      <c r="N40" s="53" t="s">
+      <c r="O40" s="54" t="s">
         <v>126</v>
-      </c>
-      <c r="O40" s="54" t="s">
-        <v>127</v>
       </c>
       <c r="P40" s="185"/>
     </row>
@@ -8629,13 +8629,13 @@
         <v>1</v>
       </c>
       <c r="B41" s="56" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C41" s="57" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D41" s="58" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E41" s="58"/>
       <c r="F41" s="58"/>
@@ -8643,7 +8643,7 @@
       <c r="H41" s="58"/>
       <c r="I41" s="58"/>
       <c r="J41" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K41" s="58"/>
       <c r="L41" s="58"/>
@@ -8657,13 +8657,13 @@
         <v>2</v>
       </c>
       <c r="B42" s="56" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C42" s="57" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D42" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E42" s="58"/>
       <c r="F42" s="58"/>
@@ -8671,7 +8671,7 @@
       <c r="H42" s="58"/>
       <c r="I42" s="58"/>
       <c r="J42" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K42" s="56"/>
       <c r="L42" s="56"/>
@@ -9194,7 +9194,7 @@
         <v>22</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -9232,7 +9232,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="46" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D7" s="33"/>
       <c r="S7"/>
@@ -9243,23 +9243,23 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="110" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D8" s="114"/>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="110" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="47" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="110"/>
@@ -9267,7 +9267,7 @@
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="110"/>
@@ -9275,7 +9275,7 @@
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="47" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="110"/>
@@ -9283,13 +9283,13 @@
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="46"/>
       <c r="D13" s="33"/>
       <c r="E13" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -9306,53 +9306,53 @@
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="46" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D15" s="33"/>
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="111" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B16" s="111"/>
       <c r="C16" s="151" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D16" s="151"/>
       <c r="E16" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="17" spans="1:22">
       <c r="A17" s="111" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B17" s="111"/>
       <c r="C17" s="151" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D17" s="151"/>
     </row>
     <row r="18" spans="1:22">
       <c r="A18" s="111" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B18" s="111"/>
       <c r="C18" s="150" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D18" s="151"/>
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="112" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B19" s="113"/>
       <c r="C19" s="90" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F19"/>
       <c r="G19"/>
@@ -9371,14 +9371,14 @@
     </row>
     <row r="20" spans="1:22">
       <c r="A20" s="112" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B20" s="113"/>
       <c r="C20" s="90" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F20"/>
       <c r="G20"/>
@@ -9400,7 +9400,7 @@
     </row>
     <row r="22" spans="1:22">
       <c r="A22" s="146" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B22" s="146"/>
       <c r="C22" s="146"/>
@@ -9414,7 +9414,7 @@
         <v>68</v>
       </c>
       <c r="B23" s="140" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C23" s="141"/>
       <c r="D23" s="141"/>
@@ -9510,7 +9510,7 @@
     </row>
     <row r="28" spans="1:22">
       <c r="A28" s="143" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B28" s="144"/>
       <c r="C28" s="144"/>
@@ -9524,7 +9524,7 @@
         <v>68</v>
       </c>
       <c r="B29" s="164" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C29" s="164"/>
       <c r="D29" s="164"/>
@@ -9551,7 +9551,7 @@
         <v>1</v>
       </c>
       <c r="B30" s="165" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C30" s="165"/>
       <c r="D30" s="165"/>
@@ -9643,7 +9643,7 @@
     </row>
     <row r="34" spans="1:22">
       <c r="A34" s="143" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B34" s="144"/>
       <c r="C34" s="144"/>
@@ -9657,7 +9657,7 @@
         <v>68</v>
       </c>
       <c r="B35" s="164" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C35" s="164"/>
       <c r="D35" s="164"/>
@@ -9773,7 +9773,7 @@
     <row r="40" spans="1:22">
       <c r="A40" s="6"/>
       <c r="N40" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="41" spans="1:22">
@@ -9815,37 +9815,37 @@
         <v>2</v>
       </c>
       <c r="E42" s="181" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F42" s="181" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G42" s="176" t="s">
         <v>12</v>
       </c>
       <c r="H42" s="176" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I42" s="176" t="s">
+        <v>236</v>
+      </c>
+      <c r="J42" s="181" t="s">
         <v>237</v>
       </c>
-      <c r="J42" s="181" t="s">
-        <v>238</v>
-      </c>
       <c r="K42" s="181" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L42" s="184" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="M42" s="176" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N42" s="176" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="O42" s="176" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="P42" s="179" t="s">
         <v>70</v>
@@ -9906,27 +9906,27 @@
         <v>90</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E44" s="23"/>
       <c r="F44" s="128"/>
       <c r="G44" s="75" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H44" s="23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I44" s="23"/>
       <c r="J44" s="23"/>
       <c r="K44" s="23"/>
       <c r="L44" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="M44" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N44" s="120" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O44" s="23"/>
       <c r="P44" s="23">
@@ -9952,7 +9952,7 @@
         <v>92</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E45" s="24"/>
       <c r="F45" s="24"/>
@@ -9966,10 +9966,10 @@
       <c r="L45" s="24"/>
       <c r="M45" s="24"/>
       <c r="N45" s="120" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="O45" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P45" s="20"/>
       <c r="Q45" s="29"/>
@@ -9992,15 +9992,15 @@
       </c>
       <c r="C46" s="13"/>
       <c r="D46" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E46" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F46" s="25"/>
       <c r="G46" s="77"/>
       <c r="H46" s="25" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I46" s="25"/>
       <c r="J46" s="25"/>
@@ -10008,7 +10008,7 @@
       <c r="L46" s="25"/>
       <c r="M46" s="25"/>
       <c r="N46" s="120" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="O46" s="24"/>
       <c r="P46" s="20"/>
@@ -10028,21 +10028,21 @@
       </c>
       <c r="C47" s="13"/>
       <c r="D47" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E47" s="73" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F47" s="73"/>
       <c r="G47" s="78"/>
       <c r="H47" s="73" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I47" s="23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J47" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K47" s="73"/>
       <c r="L47" s="73"/>
@@ -10066,15 +10066,15 @@
       </c>
       <c r="C48" s="13"/>
       <c r="D48" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E48" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F48" s="25"/>
       <c r="G48" s="77"/>
       <c r="H48" s="25" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I48" s="25"/>
       <c r="J48" s="25"/>
@@ -10089,7 +10089,7 @@
       <c r="S48" s="30"/>
       <c r="T48" s="30"/>
       <c r="U48" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="49" spans="1:21">
@@ -10102,13 +10102,13 @@
       </c>
       <c r="C49" s="13"/>
       <c r="D49" s="25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E49" s="25"/>
       <c r="F49" s="25"/>
       <c r="G49" s="77"/>
       <c r="H49" s="25" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I49" s="25"/>
       <c r="J49" s="25"/>
@@ -10130,17 +10130,17 @@
         <v>7</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C50" s="13"/>
       <c r="D50" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E50" s="25"/>
       <c r="F50" s="25"/>
       <c r="G50" s="77"/>
       <c r="H50" s="25" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I50" s="25"/>
       <c r="J50" s="25"/>
@@ -10680,7 +10680,7 @@
         <v>22</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -10718,7 +10718,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="46" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D7" s="33"/>
       <c r="N7"/>
@@ -10735,23 +10735,23 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="74" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D9" s="85"/>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="46"/>
       <c r="D10" s="33"/>
       <c r="E10" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -10768,43 +10768,43 @@
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="46" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D12" s="33"/>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="111" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B13" s="111"/>
       <c r="C13" s="151" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D13" s="151"/>
       <c r="E13" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" s="111" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B14" s="111"/>
       <c r="C14" s="151" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D14" s="151"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="112" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B15" s="113"/>
       <c r="C15" s="90" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G15"/>
       <c r="H15"/>
@@ -10820,7 +10820,7 @@
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="146" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B17" s="146"/>
       <c r="C17" s="146"/>
@@ -10834,7 +10834,7 @@
         <v>68</v>
       </c>
       <c r="B18" s="140" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C18" s="141"/>
       <c r="D18" s="141"/>
@@ -10908,7 +10908,7 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="143" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B23" s="144"/>
       <c r="C23" s="144"/>
@@ -10923,7 +10923,7 @@
         <v>68</v>
       </c>
       <c r="B24" s="164" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C24" s="164"/>
       <c r="D24" s="164"/>
@@ -10945,7 +10945,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="165" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C25" s="165"/>
       <c r="D25" s="165"/>
@@ -11015,7 +11015,7 @@
     </row>
     <row r="29" spans="1:17">
       <c r="A29" s="143" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B29" s="144"/>
       <c r="C29" s="144"/>
@@ -11030,7 +11030,7 @@
         <v>68</v>
       </c>
       <c r="B30" s="164" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C30" s="164"/>
       <c r="D30" s="164"/>
@@ -11123,7 +11123,7 @@
     </row>
     <row r="36" spans="1:17">
       <c r="A36" s="47" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B36" s="48"/>
       <c r="C36" s="48"/>
@@ -11143,55 +11143,55 @@
     </row>
     <row r="37" spans="1:17" ht="15">
       <c r="A37" s="181" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37" s="181" t="s">
         <v>115</v>
       </c>
-      <c r="B37" s="181" t="s">
+      <c r="C37" s="51" t="s">
         <v>116</v>
       </c>
-      <c r="C37" s="51" t="s">
-        <v>117</v>
-      </c>
       <c r="D37" s="181" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E37" s="181" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F37" s="181" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G37" s="181" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H37" s="181" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I37" s="181" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J37" s="176" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K37" s="186" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L37" s="187"/>
       <c r="M37" s="188" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N37" s="187"/>
       <c r="O37" s="50" t="s">
+        <v>120</v>
+      </c>
+      <c r="P37" s="181" t="s">
         <v>121</v>
-      </c>
-      <c r="P37" s="181" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="15">
       <c r="A38" s="185"/>
       <c r="B38" s="185"/>
       <c r="C38" s="52" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D38" s="185"/>
       <c r="E38" s="182"/>
@@ -11201,19 +11201,19 @@
       <c r="I38" s="185"/>
       <c r="J38" s="183"/>
       <c r="K38" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="L38" s="53" t="s">
         <v>123</v>
       </c>
-      <c r="L38" s="53" t="s">
+      <c r="M38" s="53" t="s">
         <v>124</v>
       </c>
-      <c r="M38" s="53" t="s">
+      <c r="N38" s="53" t="s">
         <v>125</v>
       </c>
-      <c r="N38" s="53" t="s">
+      <c r="O38" s="54" t="s">
         <v>126</v>
-      </c>
-      <c r="O38" s="54" t="s">
-        <v>127</v>
       </c>
       <c r="P38" s="185"/>
     </row>
@@ -11222,13 +11222,13 @@
         <v>1</v>
       </c>
       <c r="B39" s="56" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C39" s="57" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D39" s="58" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E39" s="58"/>
       <c r="F39" s="58"/>
@@ -11236,7 +11236,7 @@
       <c r="H39" s="58"/>
       <c r="I39" s="58"/>
       <c r="J39" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K39" s="58"/>
       <c r="L39" s="58"/>
@@ -11250,13 +11250,13 @@
         <v>2</v>
       </c>
       <c r="B40" s="56" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C40" s="57" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D40" s="58" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E40" s="58"/>
       <c r="F40" s="58"/>
@@ -11264,7 +11264,7 @@
       <c r="H40" s="58"/>
       <c r="I40" s="58"/>
       <c r="J40" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K40" s="56"/>
       <c r="L40" s="56"/>
@@ -11278,11 +11278,11 @@
         <v>3</v>
       </c>
       <c r="B41" s="60" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C41" s="45"/>
       <c r="D41" s="61" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E41" s="61"/>
       <c r="F41" s="61"/>
@@ -11290,7 +11290,7 @@
       <c r="H41" s="61"/>
       <c r="I41" s="61"/>
       <c r="J41" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K41" s="56"/>
       <c r="L41" s="56"/>
@@ -11304,11 +11304,11 @@
         <v>4</v>
       </c>
       <c r="B42" s="63" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C42" s="64"/>
       <c r="D42" s="65" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E42" s="65"/>
       <c r="F42" s="65"/>
@@ -11316,7 +11316,7 @@
       <c r="H42" s="65"/>
       <c r="I42" s="65"/>
       <c r="J42" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K42" s="56"/>
       <c r="L42" s="56"/>
@@ -11330,21 +11330,21 @@
         <v>5</v>
       </c>
       <c r="B43" s="63" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C43" s="64"/>
       <c r="D43" s="65" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E43" s="65" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F43" s="65"/>
       <c r="G43" s="82"/>
       <c r="H43" s="65"/>
       <c r="I43" s="65"/>
       <c r="J43" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K43" s="58"/>
       <c r="L43" s="58"/>
@@ -11358,11 +11358,11 @@
         <v>6</v>
       </c>
       <c r="B44" s="63" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C44" s="64"/>
       <c r="D44" s="65" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E44" s="65"/>
       <c r="F44" s="65"/>
@@ -11370,7 +11370,7 @@
       <c r="H44" s="65"/>
       <c r="I44" s="65"/>
       <c r="J44" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K44" s="56"/>
       <c r="L44" s="56"/>
@@ -11384,11 +11384,11 @@
         <v>7</v>
       </c>
       <c r="B45" s="63" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C45" s="64"/>
       <c r="D45" s="65" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E45" s="65"/>
       <c r="F45" s="65"/>
@@ -11396,7 +11396,7 @@
       <c r="H45" s="65"/>
       <c r="I45" s="65"/>
       <c r="J45" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K45" s="56"/>
       <c r="L45" s="56"/>
@@ -11828,7 +11828,7 @@
         <v>22</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -11866,7 +11866,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="46" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D7" s="33"/>
       <c r="N7"/>
@@ -11877,55 +11877,55 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D8" s="34"/>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="74" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D9" s="85"/>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="127" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D10" s="33"/>
       <c r="E10" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="127" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D11" s="33"/>
       <c r="E11" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="46"/>
       <c r="D12" s="33"/>
       <c r="E12" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -11942,43 +11942,43 @@
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="46" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D14" s="33"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="111" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B15" s="111"/>
       <c r="C15" s="151" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D15" s="151"/>
       <c r="E15" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="111" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B16" s="111"/>
       <c r="C16" s="151" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D16" s="151"/>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="112" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B17" s="113"/>
       <c r="C17" s="90" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G17"/>
       <c r="H17"/>
@@ -11994,7 +11994,7 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="146" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B19" s="146"/>
       <c r="C19" s="146"/>
@@ -12008,7 +12008,7 @@
         <v>68</v>
       </c>
       <c r="B20" s="140" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C20" s="141"/>
       <c r="D20" s="141"/>
@@ -12082,7 +12082,7 @@
     </row>
     <row r="25" spans="1:17">
       <c r="A25" s="143" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B25" s="144"/>
       <c r="C25" s="144"/>
@@ -12097,7 +12097,7 @@
         <v>68</v>
       </c>
       <c r="B26" s="164" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C26" s="164"/>
       <c r="D26" s="164"/>
@@ -12119,7 +12119,7 @@
         <v>1</v>
       </c>
       <c r="B27" s="165" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C27" s="165"/>
       <c r="D27" s="165"/>
@@ -12189,7 +12189,7 @@
     </row>
     <row r="31" spans="1:17">
       <c r="A31" s="143" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B31" s="144"/>
       <c r="C31" s="144"/>
@@ -12204,7 +12204,7 @@
         <v>68</v>
       </c>
       <c r="B32" s="164" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C32" s="164"/>
       <c r="D32" s="164"/>
@@ -12297,7 +12297,7 @@
     </row>
     <row r="38" spans="1:17">
       <c r="A38" s="47" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B38" s="48"/>
       <c r="C38" s="48"/>
@@ -12317,55 +12317,55 @@
     </row>
     <row r="39" spans="1:17" ht="15">
       <c r="A39" s="181" t="s">
+        <v>114</v>
+      </c>
+      <c r="B39" s="181" t="s">
         <v>115</v>
       </c>
-      <c r="B39" s="181" t="s">
+      <c r="C39" s="51" t="s">
         <v>116</v>
       </c>
-      <c r="C39" s="51" t="s">
-        <v>117</v>
-      </c>
       <c r="D39" s="181" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E39" s="181" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F39" s="181" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G39" s="181" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H39" s="189" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I39" s="189" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J39" s="176" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K39" s="186" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L39" s="187"/>
       <c r="M39" s="188" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N39" s="187"/>
       <c r="O39" s="50" t="s">
+        <v>120</v>
+      </c>
+      <c r="P39" s="181" t="s">
         <v>121</v>
-      </c>
-      <c r="P39" s="181" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="15">
       <c r="A40" s="185"/>
       <c r="B40" s="185"/>
       <c r="C40" s="52" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D40" s="185"/>
       <c r="E40" s="182"/>
@@ -12375,19 +12375,19 @@
       <c r="I40" s="185"/>
       <c r="J40" s="183"/>
       <c r="K40" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="L40" s="53" t="s">
         <v>123</v>
       </c>
-      <c r="L40" s="53" t="s">
+      <c r="M40" s="53" t="s">
         <v>124</v>
       </c>
-      <c r="M40" s="53" t="s">
+      <c r="N40" s="53" t="s">
         <v>125</v>
       </c>
-      <c r="N40" s="53" t="s">
+      <c r="O40" s="54" t="s">
         <v>126</v>
-      </c>
-      <c r="O40" s="54" t="s">
-        <v>127</v>
       </c>
       <c r="P40" s="185"/>
     </row>
@@ -12396,13 +12396,13 @@
         <v>1</v>
       </c>
       <c r="B41" s="56" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C41" s="57" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D41" s="58" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E41" s="58"/>
       <c r="F41" s="58"/>
@@ -12410,7 +12410,7 @@
       <c r="H41" s="58"/>
       <c r="I41" s="58"/>
       <c r="J41" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K41" s="58"/>
       <c r="L41" s="58"/>
@@ -12424,13 +12424,13 @@
         <v>2</v>
       </c>
       <c r="B42" s="56" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C42" s="57" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D42" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E42" s="58"/>
       <c r="F42" s="58"/>
@@ -12438,7 +12438,7 @@
       <c r="H42" s="58"/>
       <c r="I42" s="58"/>
       <c r="J42" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K42" s="56"/>
       <c r="L42" s="56"/>
@@ -12937,7 +12937,7 @@
         <v>22</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -13279,7 +13279,7 @@
       <c r="B1" s="36"/>
       <c r="C1" s="36"/>
       <c r="E1" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -13297,22 +13297,22 @@
         <v>12</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D4" s="38" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E4" s="38" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G4" s="124" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H4" s="38" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -13320,23 +13320,23 @@
         <v>5</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C5" s="40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G5" s="125" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H5" s="40" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -13345,42 +13345,42 @@
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="42" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D6" s="57" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E6" s="57"/>
       <c r="F6" s="57"/>
       <c r="G6" s="43" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H6" s="42" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="41" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G7" s="126"/>
       <c r="H7" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="C8" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H8" s="11"/>
     </row>

</xml_diff>

<commit_message>
3.1.6: Support aliasKt and modify getPathParams function. CAUTION: getPathParams modification may causes syntax error to your program...Sorry.
</commit_message>
<xml_diff>
--- a/meta/plainApi/BlancoApiPlainSample.xlsx
+++ b/meta/plainApi/BlancoApiPlainSample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorTs/meta/plainApi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE63B43-3CED-A143-93D8-0C32328514A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F33DE8-C373-3D42-BAD6-6B9DBAE94B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2440" yWindow="500" windowWidth="29440" windowHeight="20500" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2440" yWindow="500" windowWidth="29440" windowHeight="20500" tabRatio="860" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="process" sheetId="19" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="251">
   <si>
     <t>項目名</t>
     <rPh sb="0" eb="3">
@@ -2496,6 +2496,33 @@
   </si>
   <si>
     <t>/api/3.0.0</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>別名(ts)</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">ベツメイ </t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>getSample</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>array_string</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>SimpleSample</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>new SimpleSample()</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>simple_sample</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -3652,10 +3679,88 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="49" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3667,9 +3772,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3678,12 +3780,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3715,12 +3811,6 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3730,73 +3820,22 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3806,21 +3845,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3828,6 +3852,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4379,7 +4406,7 @@
   </sheetPr>
   <dimension ref="A1:O75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="D10" sqref="D10:E10"/>
     </sheetView>
   </sheetViews>
@@ -4423,152 +4450,152 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="162" t="s">
+      <c r="A5" s="129" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="162"/>
-      <c r="C5" s="162"/>
-      <c r="D5" s="162"/>
-      <c r="E5" s="162"/>
+      <c r="B5" s="129"/>
+      <c r="C5" s="129"/>
+      <c r="D5" s="129"/>
+      <c r="E5" s="129"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="173" t="s">
+      <c r="A6" s="135" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="174"/>
-      <c r="C6" s="175"/>
-      <c r="D6" s="171" t="s">
+      <c r="B6" s="136"/>
+      <c r="C6" s="137"/>
+      <c r="D6" s="130" t="s">
         <v>233</v>
       </c>
-      <c r="E6" s="171"/>
+      <c r="E6" s="130"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="162" t="s">
+      <c r="A7" s="129" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="162"/>
-      <c r="C7" s="162"/>
-      <c r="D7" s="171" t="s">
+      <c r="B7" s="129"/>
+      <c r="C7" s="129"/>
+      <c r="D7" s="130" t="s">
         <v>159</v>
       </c>
-      <c r="E7" s="171"/>
+      <c r="E7" s="130"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="162" t="s">
+      <c r="A8" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="162"/>
-      <c r="C8" s="162"/>
-      <c r="D8" s="171" t="s">
+      <c r="B8" s="129"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="130" t="s">
         <v>233</v>
       </c>
-      <c r="E8" s="171"/>
+      <c r="E8" s="130"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="162" t="s">
+      <c r="A9" s="129" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="162"/>
-      <c r="C9" s="162"/>
-      <c r="D9" s="171" t="s">
+      <c r="B9" s="129"/>
+      <c r="C9" s="129"/>
+      <c r="D9" s="130" t="s">
         <v>244</v>
       </c>
-      <c r="E9" s="171"/>
+      <c r="E9" s="130"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="162" t="s">
+      <c r="A10" s="129" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="162"/>
-      <c r="C10" s="162"/>
-      <c r="D10" s="171"/>
-      <c r="E10" s="171"/>
+      <c r="B10" s="129"/>
+      <c r="C10" s="129"/>
+      <c r="D10" s="130"/>
+      <c r="E10" s="130"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="162" t="s">
+      <c r="A11" s="129" t="s">
         <v>97</v>
       </c>
-      <c r="B11" s="162"/>
-      <c r="C11" s="162"/>
-      <c r="D11" s="171" t="s">
+      <c r="B11" s="129"/>
+      <c r="C11" s="129"/>
+      <c r="D11" s="130" t="s">
         <v>156</v>
       </c>
-      <c r="E11" s="171"/>
+      <c r="E11" s="130"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="134" t="s">
+      <c r="A12" s="131" t="s">
         <v>167</v>
       </c>
-      <c r="B12" s="134"/>
-      <c r="C12" s="134"/>
-      <c r="D12" s="151" t="s">
+      <c r="B12" s="131"/>
+      <c r="C12" s="131"/>
+      <c r="D12" s="133" t="s">
         <v>168</v>
       </c>
-      <c r="E12" s="151"/>
+      <c r="E12" s="133"/>
       <c r="F12" s="1" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="134" t="s">
+      <c r="A13" s="131" t="s">
         <v>170</v>
       </c>
-      <c r="B13" s="134"/>
-      <c r="C13" s="134"/>
-      <c r="D13" s="150" t="s">
+      <c r="B13" s="131"/>
+      <c r="C13" s="131"/>
+      <c r="D13" s="132" t="s">
         <v>208</v>
       </c>
-      <c r="E13" s="151"/>
+      <c r="E13" s="133"/>
     </row>
     <row r="14" spans="1:6" ht="55" customHeight="1">
-      <c r="A14" s="134" t="s">
+      <c r="A14" s="131" t="s">
         <v>207</v>
       </c>
-      <c r="B14" s="134"/>
-      <c r="C14" s="134"/>
-      <c r="D14" s="172" t="s">
+      <c r="B14" s="131"/>
+      <c r="C14" s="131"/>
+      <c r="D14" s="134" t="s">
         <v>232</v>
       </c>
-      <c r="E14" s="151"/>
+      <c r="E14" s="133"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="134" t="s">
+      <c r="A15" s="131" t="s">
         <v>191</v>
       </c>
-      <c r="B15" s="134"/>
-      <c r="C15" s="134"/>
-      <c r="D15" s="150"/>
-      <c r="E15" s="151"/>
+      <c r="B15" s="131"/>
+      <c r="C15" s="131"/>
+      <c r="D15" s="132"/>
+      <c r="E15" s="133"/>
       <c r="F15" s="1" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="134" t="s">
+      <c r="A16" s="131" t="s">
         <v>192</v>
       </c>
-      <c r="B16" s="134"/>
-      <c r="C16" s="134"/>
-      <c r="D16" s="150"/>
-      <c r="E16" s="151"/>
+      <c r="B16" s="131"/>
+      <c r="C16" s="131"/>
+      <c r="D16" s="132"/>
+      <c r="E16" s="133"/>
       <c r="F16" s="1" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="152" t="s">
+      <c r="A17" s="173" t="s">
         <v>138</v>
       </c>
-      <c r="B17" s="153"/>
-      <c r="C17" s="154"/>
+      <c r="B17" s="174"/>
+      <c r="C17" s="175"/>
       <c r="D17" s="104"/>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="135" t="s">
+      <c r="A18" s="160" t="s">
         <v>172</v>
       </c>
-      <c r="B18" s="136"/>
-      <c r="C18" s="137"/>
+      <c r="B18" s="161"/>
+      <c r="C18" s="162"/>
       <c r="D18" s="90" t="s">
         <v>136</v>
       </c>
@@ -4588,15 +4615,15 @@
       <c r="B19" s="6"/>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="147" t="s">
+      <c r="A20" s="170" t="s">
         <v>181</v>
       </c>
-      <c r="B20" s="148"/>
-      <c r="C20" s="148"/>
-      <c r="D20" s="148"/>
-      <c r="E20" s="148"/>
-      <c r="F20" s="148"/>
-      <c r="G20" s="149"/>
+      <c r="B20" s="171"/>
+      <c r="C20" s="171"/>
+      <c r="D20" s="171"/>
+      <c r="E20" s="171"/>
+      <c r="F20" s="171"/>
+      <c r="G20" s="172"/>
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="91" t="s">
@@ -4640,28 +4667,28 @@
       <c r="C24"/>
     </row>
     <row r="25" spans="1:15">
-      <c r="A25" s="146" t="s">
+      <c r="A25" s="169" t="s">
         <v>182</v>
       </c>
-      <c r="B25" s="146"/>
-      <c r="C25" s="146"/>
-      <c r="D25" s="146"/>
-      <c r="E25" s="146"/>
-      <c r="F25" s="146"/>
-      <c r="G25" s="146"/>
+      <c r="B25" s="169"/>
+      <c r="C25" s="169"/>
+      <c r="D25" s="169"/>
+      <c r="E25" s="169"/>
+      <c r="F25" s="169"/>
+      <c r="G25" s="169"/>
     </row>
     <row r="26" spans="1:15">
       <c r="A26" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="140" t="s">
+      <c r="B26" s="163" t="s">
         <v>176</v>
       </c>
-      <c r="C26" s="141"/>
-      <c r="D26" s="141"/>
-      <c r="E26" s="141"/>
-      <c r="F26" s="141"/>
-      <c r="G26" s="142"/>
+      <c r="C26" s="164"/>
+      <c r="D26" s="164"/>
+      <c r="E26" s="164"/>
+      <c r="F26" s="164"/>
+      <c r="G26" s="165"/>
       <c r="H26" s="95"/>
       <c r="I26" s="95"/>
       <c r="J26" s="95"/>
@@ -4672,12 +4699,12 @@
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="106"/>
-      <c r="B27" s="157"/>
-      <c r="C27" s="157"/>
-      <c r="D27" s="157"/>
-      <c r="E27" s="157"/>
-      <c r="F27" s="157"/>
-      <c r="G27" s="157"/>
+      <c r="B27" s="148"/>
+      <c r="C27" s="148"/>
+      <c r="D27" s="148"/>
+      <c r="E27" s="148"/>
+      <c r="F27" s="148"/>
+      <c r="G27" s="148"/>
       <c r="H27" s="102"/>
       <c r="I27" s="102"/>
       <c r="J27" s="102"/>
@@ -4688,12 +4715,12 @@
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="107"/>
-      <c r="B28" s="158"/>
-      <c r="C28" s="158"/>
-      <c r="D28" s="158"/>
-      <c r="E28" s="158"/>
-      <c r="F28" s="158"/>
-      <c r="G28" s="158"/>
+      <c r="B28" s="150"/>
+      <c r="C28" s="150"/>
+      <c r="D28" s="150"/>
+      <c r="E28" s="150"/>
+      <c r="F28" s="150"/>
+      <c r="G28" s="150"/>
       <c r="H28" s="102"/>
       <c r="I28" s="102"/>
       <c r="J28" s="102"/>
@@ -4704,12 +4731,12 @@
     </row>
     <row r="29" spans="1:15">
       <c r="A29" s="108"/>
-      <c r="B29" s="159"/>
-      <c r="C29" s="159"/>
-      <c r="D29" s="159"/>
-      <c r="E29" s="159"/>
-      <c r="F29" s="159"/>
-      <c r="G29" s="159"/>
+      <c r="B29" s="152"/>
+      <c r="C29" s="152"/>
+      <c r="D29" s="152"/>
+      <c r="E29" s="152"/>
+      <c r="F29" s="152"/>
+      <c r="G29" s="152"/>
       <c r="H29" s="102"/>
       <c r="I29" s="102"/>
       <c r="J29" s="102"/>
@@ -4722,28 +4749,28 @@
       <c r="C30"/>
     </row>
     <row r="31" spans="1:15">
-      <c r="A31" s="143" t="s">
+      <c r="A31" s="166" t="s">
         <v>183</v>
       </c>
-      <c r="B31" s="144"/>
-      <c r="C31" s="144"/>
-      <c r="D31" s="144"/>
-      <c r="E31" s="144"/>
-      <c r="F31" s="144"/>
-      <c r="G31" s="145"/>
+      <c r="B31" s="167"/>
+      <c r="C31" s="167"/>
+      <c r="D31" s="167"/>
+      <c r="E31" s="167"/>
+      <c r="F31" s="167"/>
+      <c r="G31" s="168"/>
     </row>
     <row r="32" spans="1:15">
       <c r="A32" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="164" t="s">
+      <c r="B32" s="144" t="s">
         <v>177</v>
       </c>
-      <c r="C32" s="164"/>
-      <c r="D32" s="164"/>
-      <c r="E32" s="164"/>
-      <c r="F32" s="164"/>
-      <c r="G32" s="164"/>
+      <c r="C32" s="144"/>
+      <c r="D32" s="144"/>
+      <c r="E32" s="144"/>
+      <c r="F32" s="144"/>
+      <c r="G32" s="144"/>
       <c r="H32" s="95"/>
       <c r="I32" s="95"/>
       <c r="J32" s="95"/>
@@ -4756,14 +4783,14 @@
       <c r="A33" s="106">
         <v>1</v>
       </c>
-      <c r="B33" s="165" t="s">
+      <c r="B33" s="145" t="s">
         <v>178</v>
       </c>
-      <c r="C33" s="165"/>
-      <c r="D33" s="165"/>
-      <c r="E33" s="165"/>
-      <c r="F33" s="165"/>
-      <c r="G33" s="165"/>
+      <c r="C33" s="145"/>
+      <c r="D33" s="145"/>
+      <c r="E33" s="145"/>
+      <c r="F33" s="145"/>
+      <c r="G33" s="145"/>
       <c r="H33" s="102"/>
       <c r="I33" s="102"/>
       <c r="J33" s="102"/>
@@ -4774,12 +4801,12 @@
     </row>
     <row r="34" spans="1:15">
       <c r="A34" s="107"/>
-      <c r="B34" s="166"/>
-      <c r="C34" s="166"/>
-      <c r="D34" s="166"/>
-      <c r="E34" s="166"/>
-      <c r="F34" s="166"/>
-      <c r="G34" s="166"/>
+      <c r="B34" s="146"/>
+      <c r="C34" s="146"/>
+      <c r="D34" s="146"/>
+      <c r="E34" s="146"/>
+      <c r="F34" s="146"/>
+      <c r="G34" s="146"/>
       <c r="H34" s="102"/>
       <c r="I34" s="102"/>
       <c r="J34" s="102"/>
@@ -4790,12 +4817,12 @@
     </row>
     <row r="35" spans="1:15">
       <c r="A35" s="108"/>
-      <c r="B35" s="167"/>
-      <c r="C35" s="167"/>
-      <c r="D35" s="167"/>
-      <c r="E35" s="167"/>
-      <c r="F35" s="167"/>
-      <c r="G35" s="167"/>
+      <c r="B35" s="147"/>
+      <c r="C35" s="147"/>
+      <c r="D35" s="147"/>
+      <c r="E35" s="147"/>
+      <c r="F35" s="147"/>
+      <c r="G35" s="147"/>
       <c r="H35" s="102"/>
       <c r="I35" s="102"/>
       <c r="J35" s="102"/>
@@ -4820,28 +4847,28 @@
       <c r="M36"/>
     </row>
     <row r="37" spans="1:15">
-      <c r="A37" s="143" t="s">
+      <c r="A37" s="166" t="s">
         <v>184</v>
       </c>
-      <c r="B37" s="144"/>
-      <c r="C37" s="144"/>
-      <c r="D37" s="144"/>
-      <c r="E37" s="144"/>
-      <c r="F37" s="144"/>
-      <c r="G37" s="145"/>
+      <c r="B37" s="167"/>
+      <c r="C37" s="167"/>
+      <c r="D37" s="167"/>
+      <c r="E37" s="167"/>
+      <c r="F37" s="167"/>
+      <c r="G37" s="168"/>
     </row>
     <row r="38" spans="1:15">
       <c r="A38" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B38" s="164" t="s">
+      <c r="B38" s="144" t="s">
         <v>179</v>
       </c>
-      <c r="C38" s="164"/>
-      <c r="D38" s="164"/>
-      <c r="E38" s="164"/>
-      <c r="F38" s="164"/>
-      <c r="G38" s="164"/>
+      <c r="C38" s="144"/>
+      <c r="D38" s="144"/>
+      <c r="E38" s="144"/>
+      <c r="F38" s="144"/>
+      <c r="G38" s="144"/>
       <c r="H38" s="95"/>
       <c r="I38" s="95"/>
       <c r="J38" s="95"/>
@@ -4852,12 +4879,12 @@
     </row>
     <row r="39" spans="1:15">
       <c r="A39" s="106"/>
-      <c r="B39" s="157"/>
-      <c r="C39" s="157"/>
-      <c r="D39" s="157"/>
-      <c r="E39" s="157"/>
-      <c r="F39" s="157"/>
-      <c r="G39" s="168"/>
+      <c r="B39" s="148"/>
+      <c r="C39" s="148"/>
+      <c r="D39" s="148"/>
+      <c r="E39" s="148"/>
+      <c r="F39" s="148"/>
+      <c r="G39" s="149"/>
       <c r="H39" s="102"/>
       <c r="I39" s="102"/>
       <c r="J39" s="102"/>
@@ -4868,12 +4895,12 @@
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="107"/>
-      <c r="B40" s="158"/>
-      <c r="C40" s="158"/>
-      <c r="D40" s="158"/>
-      <c r="E40" s="158"/>
-      <c r="F40" s="158"/>
-      <c r="G40" s="169"/>
+      <c r="B40" s="150"/>
+      <c r="C40" s="150"/>
+      <c r="D40" s="150"/>
+      <c r="E40" s="150"/>
+      <c r="F40" s="150"/>
+      <c r="G40" s="151"/>
       <c r="H40" s="102"/>
       <c r="I40" s="102"/>
       <c r="J40" s="102"/>
@@ -4884,12 +4911,12 @@
     </row>
     <row r="41" spans="1:15">
       <c r="A41" s="108"/>
-      <c r="B41" s="159"/>
-      <c r="C41" s="159"/>
-      <c r="D41" s="159"/>
-      <c r="E41" s="159"/>
-      <c r="F41" s="159"/>
-      <c r="G41" s="170"/>
+      <c r="B41" s="152"/>
+      <c r="C41" s="152"/>
+      <c r="D41" s="152"/>
+      <c r="E41" s="152"/>
+      <c r="F41" s="152"/>
+      <c r="G41" s="153"/>
       <c r="H41" s="102"/>
       <c r="I41" s="102"/>
       <c r="J41" s="102"/>
@@ -4915,15 +4942,15 @@
       <c r="O42"/>
     </row>
     <row r="43" spans="1:15">
-      <c r="A43" s="146" t="s">
+      <c r="A43" s="169" t="s">
         <v>204</v>
       </c>
-      <c r="B43" s="146"/>
-      <c r="C43" s="146"/>
-      <c r="D43" s="146"/>
-      <c r="E43" s="146"/>
-      <c r="F43" s="146"/>
-      <c r="G43" s="146"/>
+      <c r="B43" s="169"/>
+      <c r="C43" s="169"/>
+      <c r="D43" s="169"/>
+      <c r="E43" s="169"/>
+      <c r="F43" s="169"/>
+      <c r="G43" s="169"/>
     </row>
     <row r="44" spans="1:15">
       <c r="A44" s="105" t="s">
@@ -5039,221 +5066,299 @@
       <c r="F49" s="5"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="131" t="s">
+      <c r="A50" s="157" t="s">
         <v>64</v>
       </c>
-      <c r="B50" s="133"/>
-      <c r="C50" s="131" t="s">
+      <c r="B50" s="159"/>
+      <c r="C50" s="157" t="s">
         <v>65</v>
       </c>
-      <c r="D50" s="132"/>
-      <c r="E50" s="133"/>
+      <c r="D50" s="158"/>
+      <c r="E50" s="159"/>
       <c r="F50" s="27" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="138"/>
-      <c r="B51" s="139"/>
-      <c r="C51" s="138"/>
-      <c r="D51" s="160"/>
-      <c r="E51" s="139"/>
+      <c r="A51" s="154"/>
+      <c r="B51" s="156"/>
+      <c r="C51" s="154"/>
+      <c r="D51" s="155"/>
+      <c r="E51" s="156"/>
       <c r="F51" s="43"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="129"/>
-      <c r="B52" s="130"/>
-      <c r="C52" s="129"/>
-      <c r="D52" s="161"/>
-      <c r="E52" s="130"/>
+      <c r="A52" s="138"/>
+      <c r="B52" s="140"/>
+      <c r="C52" s="138"/>
+      <c r="D52" s="139"/>
+      <c r="E52" s="140"/>
       <c r="F52" s="43"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="129"/>
-      <c r="B53" s="130"/>
-      <c r="C53" s="129"/>
-      <c r="D53" s="161"/>
-      <c r="E53" s="130"/>
+      <c r="A53" s="138"/>
+      <c r="B53" s="140"/>
+      <c r="C53" s="138"/>
+      <c r="D53" s="139"/>
+      <c r="E53" s="140"/>
       <c r="F53" s="43"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="129"/>
-      <c r="B54" s="130"/>
-      <c r="C54" s="129"/>
-      <c r="D54" s="161"/>
-      <c r="E54" s="130"/>
+      <c r="A54" s="138"/>
+      <c r="B54" s="140"/>
+      <c r="C54" s="138"/>
+      <c r="D54" s="139"/>
+      <c r="E54" s="140"/>
       <c r="F54" s="43"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="129"/>
-      <c r="B55" s="130"/>
-      <c r="C55" s="129"/>
-      <c r="D55" s="161"/>
-      <c r="E55" s="130"/>
+      <c r="A55" s="138"/>
+      <c r="B55" s="140"/>
+      <c r="C55" s="138"/>
+      <c r="D55" s="139"/>
+      <c r="E55" s="140"/>
       <c r="F55" s="43"/>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="129"/>
-      <c r="B56" s="130"/>
-      <c r="C56" s="129"/>
-      <c r="D56" s="161"/>
-      <c r="E56" s="130"/>
+      <c r="A56" s="138"/>
+      <c r="B56" s="140"/>
+      <c r="C56" s="138"/>
+      <c r="D56" s="139"/>
+      <c r="E56" s="140"/>
       <c r="F56" s="43"/>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="129"/>
-      <c r="B57" s="130"/>
-      <c r="C57" s="129"/>
-      <c r="D57" s="161"/>
-      <c r="E57" s="130"/>
+      <c r="A57" s="138"/>
+      <c r="B57" s="140"/>
+      <c r="C57" s="138"/>
+      <c r="D57" s="139"/>
+      <c r="E57" s="140"/>
       <c r="F57" s="43"/>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="129"/>
-      <c r="B58" s="130"/>
-      <c r="C58" s="129"/>
-      <c r="D58" s="161"/>
-      <c r="E58" s="130"/>
+      <c r="A58" s="138"/>
+      <c r="B58" s="140"/>
+      <c r="C58" s="138"/>
+      <c r="D58" s="139"/>
+      <c r="E58" s="140"/>
       <c r="F58" s="43"/>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="129"/>
-      <c r="B59" s="130"/>
-      <c r="C59" s="129"/>
-      <c r="D59" s="161"/>
-      <c r="E59" s="130"/>
+      <c r="A59" s="138"/>
+      <c r="B59" s="140"/>
+      <c r="C59" s="138"/>
+      <c r="D59" s="139"/>
+      <c r="E59" s="140"/>
       <c r="F59" s="43"/>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="129"/>
-      <c r="B60" s="130"/>
-      <c r="C60" s="129"/>
-      <c r="D60" s="161"/>
-      <c r="E60" s="130"/>
+      <c r="A60" s="138"/>
+      <c r="B60" s="140"/>
+      <c r="C60" s="138"/>
+      <c r="D60" s="139"/>
+      <c r="E60" s="140"/>
       <c r="F60" s="43"/>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="129"/>
-      <c r="B61" s="130"/>
-      <c r="C61" s="129"/>
-      <c r="D61" s="161"/>
-      <c r="E61" s="130"/>
+      <c r="A61" s="138"/>
+      <c r="B61" s="140"/>
+      <c r="C61" s="138"/>
+      <c r="D61" s="139"/>
+      <c r="E61" s="140"/>
       <c r="F61" s="43"/>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="129"/>
-      <c r="B62" s="130"/>
-      <c r="C62" s="129"/>
-      <c r="D62" s="161"/>
-      <c r="E62" s="130"/>
+      <c r="A62" s="138"/>
+      <c r="B62" s="140"/>
+      <c r="C62" s="138"/>
+      <c r="D62" s="139"/>
+      <c r="E62" s="140"/>
       <c r="F62" s="43"/>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="129"/>
-      <c r="B63" s="130"/>
-      <c r="C63" s="129"/>
-      <c r="D63" s="161"/>
-      <c r="E63" s="130"/>
+      <c r="A63" s="138"/>
+      <c r="B63" s="140"/>
+      <c r="C63" s="138"/>
+      <c r="D63" s="139"/>
+      <c r="E63" s="140"/>
       <c r="F63" s="43"/>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="129"/>
-      <c r="B64" s="130"/>
-      <c r="C64" s="129"/>
-      <c r="D64" s="161"/>
-      <c r="E64" s="130"/>
+      <c r="A64" s="138"/>
+      <c r="B64" s="140"/>
+      <c r="C64" s="138"/>
+      <c r="D64" s="139"/>
+      <c r="E64" s="140"/>
       <c r="F64" s="43"/>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="129"/>
-      <c r="B65" s="130"/>
-      <c r="C65" s="129"/>
-      <c r="D65" s="161"/>
-      <c r="E65" s="130"/>
+      <c r="A65" s="138"/>
+      <c r="B65" s="140"/>
+      <c r="C65" s="138"/>
+      <c r="D65" s="139"/>
+      <c r="E65" s="140"/>
       <c r="F65" s="43"/>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="129"/>
-      <c r="B66" s="130"/>
-      <c r="C66" s="129"/>
-      <c r="D66" s="161"/>
-      <c r="E66" s="130"/>
+      <c r="A66" s="138"/>
+      <c r="B66" s="140"/>
+      <c r="C66" s="138"/>
+      <c r="D66" s="139"/>
+      <c r="E66" s="140"/>
       <c r="F66" s="43"/>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="129"/>
-      <c r="B67" s="130"/>
-      <c r="C67" s="129"/>
-      <c r="D67" s="161"/>
-      <c r="E67" s="130"/>
+      <c r="A67" s="138"/>
+      <c r="B67" s="140"/>
+      <c r="C67" s="138"/>
+      <c r="D67" s="139"/>
+      <c r="E67" s="140"/>
       <c r="F67" s="43"/>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="129"/>
-      <c r="B68" s="130"/>
-      <c r="C68" s="129"/>
-      <c r="D68" s="161"/>
-      <c r="E68" s="130"/>
+      <c r="A68" s="138"/>
+      <c r="B68" s="140"/>
+      <c r="C68" s="138"/>
+      <c r="D68" s="139"/>
+      <c r="E68" s="140"/>
       <c r="F68" s="43"/>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="129"/>
-      <c r="B69" s="130"/>
-      <c r="C69" s="129"/>
-      <c r="D69" s="161"/>
-      <c r="E69" s="130"/>
+      <c r="A69" s="138"/>
+      <c r="B69" s="140"/>
+      <c r="C69" s="138"/>
+      <c r="D69" s="139"/>
+      <c r="E69" s="140"/>
       <c r="F69" s="43"/>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="129"/>
-      <c r="B70" s="130"/>
-      <c r="C70" s="129"/>
-      <c r="D70" s="161"/>
-      <c r="E70" s="130"/>
+      <c r="A70" s="138"/>
+      <c r="B70" s="140"/>
+      <c r="C70" s="138"/>
+      <c r="D70" s="139"/>
+      <c r="E70" s="140"/>
       <c r="F70" s="43"/>
     </row>
     <row r="71" spans="1:6">
-      <c r="A71" s="129"/>
-      <c r="B71" s="130"/>
-      <c r="C71" s="129"/>
-      <c r="D71" s="161"/>
-      <c r="E71" s="130"/>
+      <c r="A71" s="138"/>
+      <c r="B71" s="140"/>
+      <c r="C71" s="138"/>
+      <c r="D71" s="139"/>
+      <c r="E71" s="140"/>
       <c r="F71" s="43"/>
     </row>
     <row r="72" spans="1:6">
-      <c r="A72" s="129"/>
-      <c r="B72" s="130"/>
-      <c r="C72" s="129"/>
-      <c r="D72" s="161"/>
-      <c r="E72" s="130"/>
+      <c r="A72" s="138"/>
+      <c r="B72" s="140"/>
+      <c r="C72" s="138"/>
+      <c r="D72" s="139"/>
+      <c r="E72" s="140"/>
       <c r="F72" s="43"/>
     </row>
     <row r="73" spans="1:6">
-      <c r="A73" s="129"/>
-      <c r="B73" s="130"/>
-      <c r="C73" s="129"/>
-      <c r="D73" s="161"/>
-      <c r="E73" s="130"/>
+      <c r="A73" s="138"/>
+      <c r="B73" s="140"/>
+      <c r="C73" s="138"/>
+      <c r="D73" s="139"/>
+      <c r="E73" s="140"/>
       <c r="F73" s="43"/>
     </row>
     <row r="74" spans="1:6">
-      <c r="A74" s="129"/>
-      <c r="B74" s="130"/>
-      <c r="C74" s="129"/>
-      <c r="D74" s="161"/>
-      <c r="E74" s="130"/>
+      <c r="A74" s="138"/>
+      <c r="B74" s="140"/>
+      <c r="C74" s="138"/>
+      <c r="D74" s="139"/>
+      <c r="E74" s="140"/>
       <c r="F74" s="43"/>
     </row>
     <row r="75" spans="1:6">
-      <c r="A75" s="155"/>
-      <c r="B75" s="156"/>
-      <c r="C75" s="155"/>
-      <c r="D75" s="163"/>
-      <c r="E75" s="156"/>
+      <c r="A75" s="141"/>
+      <c r="B75" s="143"/>
+      <c r="C75" s="141"/>
+      <c r="D75" s="142"/>
+      <c r="E75" s="143"/>
       <c r="F75" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="94">
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A43:G43"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C73:E73"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C75:E75"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="C72:E72"/>
     <mergeCell ref="A5:E5"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D7:E7"/>
@@ -5270,84 +5375,6 @@
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="C75:E75"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C73:E73"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="A37:G37"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="A20:G20"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A43:G43"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="2">
@@ -5548,10 +5575,10 @@
         <v>167</v>
       </c>
       <c r="B16" s="111"/>
-      <c r="C16" s="151" t="s">
+      <c r="C16" s="133" t="s">
         <v>168</v>
       </c>
-      <c r="D16" s="151"/>
+      <c r="D16" s="133"/>
       <c r="E16" s="1" t="s">
         <v>169</v>
       </c>
@@ -5561,20 +5588,20 @@
         <v>170</v>
       </c>
       <c r="B17" s="111"/>
-      <c r="C17" s="151" t="s">
+      <c r="C17" s="133" t="s">
         <v>171</v>
       </c>
-      <c r="D17" s="151"/>
+      <c r="D17" s="133"/>
     </row>
     <row r="18" spans="1:22">
       <c r="A18" s="111" t="s">
         <v>207</v>
       </c>
       <c r="B18" s="111"/>
-      <c r="C18" s="150" t="s">
+      <c r="C18" s="132" t="s">
         <v>209</v>
       </c>
-      <c r="D18" s="151"/>
+      <c r="D18" s="133"/>
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="112" t="s">
@@ -5632,28 +5659,28 @@
       <c r="A21" s="6"/>
     </row>
     <row r="22" spans="1:22">
-      <c r="A22" s="146" t="s">
+      <c r="A22" s="169" t="s">
         <v>185</v>
       </c>
-      <c r="B22" s="146"/>
-      <c r="C22" s="146"/>
-      <c r="D22" s="146"/>
-      <c r="E22" s="146"/>
-      <c r="F22" s="146"/>
-      <c r="G22" s="146"/>
+      <c r="B22" s="169"/>
+      <c r="C22" s="169"/>
+      <c r="D22" s="169"/>
+      <c r="E22" s="169"/>
+      <c r="F22" s="169"/>
+      <c r="G22" s="169"/>
     </row>
     <row r="23" spans="1:22">
       <c r="A23" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="140" t="s">
+      <c r="B23" s="163" t="s">
         <v>176</v>
       </c>
-      <c r="C23" s="141"/>
-      <c r="D23" s="141"/>
-      <c r="E23" s="141"/>
-      <c r="F23" s="141"/>
-      <c r="G23" s="142"/>
+      <c r="C23" s="164"/>
+      <c r="D23" s="164"/>
+      <c r="E23" s="164"/>
+      <c r="F23" s="164"/>
+      <c r="G23" s="165"/>
       <c r="H23" s="95"/>
       <c r="I23" s="95"/>
       <c r="J23" s="95"/>
@@ -5671,12 +5698,12 @@
     </row>
     <row r="24" spans="1:22">
       <c r="A24" s="106"/>
-      <c r="B24" s="157"/>
-      <c r="C24" s="157"/>
-      <c r="D24" s="157"/>
-      <c r="E24" s="157"/>
-      <c r="F24" s="157"/>
-      <c r="G24" s="157"/>
+      <c r="B24" s="148"/>
+      <c r="C24" s="148"/>
+      <c r="D24" s="148"/>
+      <c r="E24" s="148"/>
+      <c r="F24" s="148"/>
+      <c r="G24" s="148"/>
       <c r="H24" s="102"/>
       <c r="I24" s="102"/>
       <c r="J24" s="102"/>
@@ -5694,12 +5721,12 @@
     </row>
     <row r="25" spans="1:22">
       <c r="A25" s="107"/>
-      <c r="B25" s="158"/>
-      <c r="C25" s="158"/>
-      <c r="D25" s="158"/>
-      <c r="E25" s="158"/>
-      <c r="F25" s="158"/>
-      <c r="G25" s="158"/>
+      <c r="B25" s="150"/>
+      <c r="C25" s="150"/>
+      <c r="D25" s="150"/>
+      <c r="E25" s="150"/>
+      <c r="F25" s="150"/>
+      <c r="G25" s="150"/>
       <c r="H25" s="102"/>
       <c r="I25" s="102"/>
       <c r="J25" s="102"/>
@@ -5717,12 +5744,12 @@
     </row>
     <row r="26" spans="1:22">
       <c r="A26" s="108"/>
-      <c r="B26" s="159"/>
-      <c r="C26" s="159"/>
-      <c r="D26" s="159"/>
-      <c r="E26" s="159"/>
-      <c r="F26" s="159"/>
-      <c r="G26" s="159"/>
+      <c r="B26" s="152"/>
+      <c r="C26" s="152"/>
+      <c r="D26" s="152"/>
+      <c r="E26" s="152"/>
+      <c r="F26" s="152"/>
+      <c r="G26" s="152"/>
       <c r="H26" s="102"/>
       <c r="I26" s="102"/>
       <c r="J26" s="102"/>
@@ -5742,28 +5769,28 @@
       <c r="C27"/>
     </row>
     <row r="28" spans="1:22">
-      <c r="A28" s="143" t="s">
+      <c r="A28" s="166" t="s">
         <v>186</v>
       </c>
-      <c r="B28" s="144"/>
-      <c r="C28" s="144"/>
-      <c r="D28" s="144"/>
-      <c r="E28" s="144"/>
-      <c r="F28" s="144"/>
-      <c r="G28" s="145"/>
+      <c r="B28" s="167"/>
+      <c r="C28" s="167"/>
+      <c r="D28" s="167"/>
+      <c r="E28" s="167"/>
+      <c r="F28" s="167"/>
+      <c r="G28" s="168"/>
     </row>
     <row r="29" spans="1:22">
       <c r="A29" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="164" t="s">
+      <c r="B29" s="144" t="s">
         <v>177</v>
       </c>
-      <c r="C29" s="164"/>
-      <c r="D29" s="164"/>
-      <c r="E29" s="164"/>
-      <c r="F29" s="164"/>
-      <c r="G29" s="164"/>
+      <c r="C29" s="144"/>
+      <c r="D29" s="144"/>
+      <c r="E29" s="144"/>
+      <c r="F29" s="144"/>
+      <c r="G29" s="144"/>
       <c r="H29" s="95"/>
       <c r="I29" s="95"/>
       <c r="J29" s="95"/>
@@ -5783,14 +5810,14 @@
       <c r="A30" s="106">
         <v>1</v>
       </c>
-      <c r="B30" s="165" t="s">
+      <c r="B30" s="145" t="s">
         <v>178</v>
       </c>
-      <c r="C30" s="165"/>
-      <c r="D30" s="165"/>
-      <c r="E30" s="165"/>
-      <c r="F30" s="165"/>
-      <c r="G30" s="165"/>
+      <c r="C30" s="145"/>
+      <c r="D30" s="145"/>
+      <c r="E30" s="145"/>
+      <c r="F30" s="145"/>
+      <c r="G30" s="145"/>
       <c r="H30" s="102"/>
       <c r="I30" s="102"/>
       <c r="J30" s="102"/>
@@ -5808,12 +5835,12 @@
     </row>
     <row r="31" spans="1:22">
       <c r="A31" s="107"/>
-      <c r="B31" s="166"/>
-      <c r="C31" s="166"/>
-      <c r="D31" s="166"/>
-      <c r="E31" s="166"/>
-      <c r="F31" s="166"/>
-      <c r="G31" s="166"/>
+      <c r="B31" s="146"/>
+      <c r="C31" s="146"/>
+      <c r="D31" s="146"/>
+      <c r="E31" s="146"/>
+      <c r="F31" s="146"/>
+      <c r="G31" s="146"/>
       <c r="H31" s="102"/>
       <c r="I31" s="102"/>
       <c r="J31" s="102"/>
@@ -5831,12 +5858,12 @@
     </row>
     <row r="32" spans="1:22">
       <c r="A32" s="108"/>
-      <c r="B32" s="167"/>
-      <c r="C32" s="167"/>
-      <c r="D32" s="167"/>
-      <c r="E32" s="167"/>
-      <c r="F32" s="167"/>
-      <c r="G32" s="167"/>
+      <c r="B32" s="147"/>
+      <c r="C32" s="147"/>
+      <c r="D32" s="147"/>
+      <c r="E32" s="147"/>
+      <c r="F32" s="147"/>
+      <c r="G32" s="147"/>
       <c r="H32" s="102"/>
       <c r="I32" s="102"/>
       <c r="J32" s="102"/>
@@ -5875,28 +5902,28 @@
       <c r="T33"/>
     </row>
     <row r="34" spans="1:22">
-      <c r="A34" s="143" t="s">
+      <c r="A34" s="166" t="s">
         <v>187</v>
       </c>
-      <c r="B34" s="144"/>
-      <c r="C34" s="144"/>
-      <c r="D34" s="144"/>
-      <c r="E34" s="144"/>
-      <c r="F34" s="144"/>
-      <c r="G34" s="145"/>
+      <c r="B34" s="167"/>
+      <c r="C34" s="167"/>
+      <c r="D34" s="167"/>
+      <c r="E34" s="167"/>
+      <c r="F34" s="167"/>
+      <c r="G34" s="168"/>
     </row>
     <row r="35" spans="1:22">
       <c r="A35" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="164" t="s">
+      <c r="B35" s="144" t="s">
         <v>179</v>
       </c>
-      <c r="C35" s="164"/>
-      <c r="D35" s="164"/>
-      <c r="E35" s="164"/>
-      <c r="F35" s="164"/>
-      <c r="G35" s="164"/>
+      <c r="C35" s="144"/>
+      <c r="D35" s="144"/>
+      <c r="E35" s="144"/>
+      <c r="F35" s="144"/>
+      <c r="G35" s="144"/>
       <c r="H35" s="95"/>
       <c r="I35" s="95"/>
       <c r="J35" s="95"/>
@@ -5914,12 +5941,12 @@
     </row>
     <row r="36" spans="1:22">
       <c r="A36" s="106"/>
-      <c r="B36" s="157"/>
-      <c r="C36" s="157"/>
-      <c r="D36" s="157"/>
-      <c r="E36" s="157"/>
-      <c r="F36" s="157"/>
-      <c r="G36" s="168"/>
+      <c r="B36" s="148"/>
+      <c r="C36" s="148"/>
+      <c r="D36" s="148"/>
+      <c r="E36" s="148"/>
+      <c r="F36" s="148"/>
+      <c r="G36" s="149"/>
       <c r="H36" s="102"/>
       <c r="I36" s="102"/>
       <c r="J36" s="102"/>
@@ -5937,12 +5964,12 @@
     </row>
     <row r="37" spans="1:22">
       <c r="A37" s="107"/>
-      <c r="B37" s="158"/>
-      <c r="C37" s="158"/>
-      <c r="D37" s="158"/>
-      <c r="E37" s="158"/>
-      <c r="F37" s="158"/>
-      <c r="G37" s="169"/>
+      <c r="B37" s="150"/>
+      <c r="C37" s="150"/>
+      <c r="D37" s="150"/>
+      <c r="E37" s="150"/>
+      <c r="F37" s="150"/>
+      <c r="G37" s="151"/>
       <c r="H37" s="102"/>
       <c r="I37" s="102"/>
       <c r="J37" s="102"/>
@@ -5960,12 +5987,12 @@
     </row>
     <row r="38" spans="1:22">
       <c r="A38" s="108"/>
-      <c r="B38" s="159"/>
-      <c r="C38" s="159"/>
-      <c r="D38" s="159"/>
-      <c r="E38" s="159"/>
-      <c r="F38" s="159"/>
-      <c r="G38" s="170"/>
+      <c r="B38" s="152"/>
+      <c r="C38" s="152"/>
+      <c r="D38" s="152"/>
+      <c r="E38" s="152"/>
+      <c r="F38" s="152"/>
+      <c r="G38" s="153"/>
       <c r="H38" s="102"/>
       <c r="I38" s="102"/>
       <c r="J38" s="102"/>
@@ -6041,16 +6068,16 @@
       <c r="B42" s="176" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="178" t="s">
+      <c r="C42" s="182" t="s">
         <v>1</v>
       </c>
       <c r="D42" s="176" t="s">
         <v>2</v>
       </c>
-      <c r="E42" s="181" t="s">
+      <c r="E42" s="180" t="s">
         <v>155</v>
       </c>
-      <c r="F42" s="181" t="s">
+      <c r="F42" s="180" t="s">
         <v>170</v>
       </c>
       <c r="G42" s="176" t="s">
@@ -6062,13 +6089,13 @@
       <c r="I42" s="176" t="s">
         <v>236</v>
       </c>
-      <c r="J42" s="181" t="s">
+      <c r="J42" s="180" t="s">
         <v>237</v>
       </c>
-      <c r="K42" s="181" t="s">
+      <c r="K42" s="180" t="s">
         <v>207</v>
       </c>
-      <c r="L42" s="184" t="s">
+      <c r="L42" s="179" t="s">
         <v>224</v>
       </c>
       <c r="M42" s="176" t="s">
@@ -6080,14 +6107,14 @@
       <c r="O42" s="176" t="s">
         <v>189</v>
       </c>
-      <c r="P42" s="179" t="s">
+      <c r="P42" s="183" t="s">
         <v>70</v>
       </c>
-      <c r="Q42" s="180"/>
-      <c r="R42" s="179" t="s">
+      <c r="Q42" s="184"/>
+      <c r="R42" s="183" t="s">
         <v>16</v>
       </c>
-      <c r="S42" s="180"/>
+      <c r="S42" s="184"/>
       <c r="T42" s="32" t="s">
         <v>69</v>
       </c>
@@ -6096,21 +6123,21 @@
       </c>
     </row>
     <row r="43" spans="1:22">
-      <c r="A43" s="177"/>
-      <c r="B43" s="177"/>
-      <c r="C43" s="177"/>
-      <c r="D43" s="177"/>
-      <c r="E43" s="182"/>
-      <c r="F43" s="182"/>
-      <c r="G43" s="177"/>
-      <c r="H43" s="177"/>
-      <c r="I43" s="177"/>
-      <c r="J43" s="182"/>
-      <c r="K43" s="182"/>
-      <c r="L43" s="183"/>
-      <c r="M43" s="177"/>
-      <c r="N43" s="177"/>
-      <c r="O43" s="183"/>
+      <c r="A43" s="178"/>
+      <c r="B43" s="178"/>
+      <c r="C43" s="178"/>
+      <c r="D43" s="178"/>
+      <c r="E43" s="181"/>
+      <c r="F43" s="181"/>
+      <c r="G43" s="178"/>
+      <c r="H43" s="178"/>
+      <c r="I43" s="178"/>
+      <c r="J43" s="181"/>
+      <c r="K43" s="181"/>
+      <c r="L43" s="177"/>
+      <c r="M43" s="178"/>
+      <c r="N43" s="178"/>
+      <c r="O43" s="177"/>
       <c r="P43" s="27" t="s">
         <v>74</v>
       </c>
@@ -6126,7 +6153,7 @@
       <c r="T43" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="U43" s="177"/>
+      <c r="U43" s="178"/>
     </row>
     <row r="44" spans="1:22">
       <c r="A44" s="7">
@@ -6782,26 +6809,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="O42:O43"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="A34:G34"/>
-    <mergeCell ref="M42:M43"/>
-    <mergeCell ref="H42:H43"/>
-    <mergeCell ref="L42:L43"/>
-    <mergeCell ref="K42:K43"/>
-    <mergeCell ref="I42:I43"/>
-    <mergeCell ref="J42:J43"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="A22:G22"/>
@@ -6818,6 +6825,26 @@
     <mergeCell ref="F42:F43"/>
     <mergeCell ref="B23:G23"/>
     <mergeCell ref="B24:G24"/>
+    <mergeCell ref="O42:O43"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="M42:M43"/>
+    <mergeCell ref="H42:H43"/>
+    <mergeCell ref="L42:L43"/>
+    <mergeCell ref="K42:K43"/>
+    <mergeCell ref="I42:I43"/>
+    <mergeCell ref="J42:J43"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="B35:G35"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="4">
@@ -7010,10 +7037,10 @@
         <v>167</v>
       </c>
       <c r="B13" s="111"/>
-      <c r="C13" s="151" t="s">
+      <c r="C13" s="133" t="s">
         <v>168</v>
       </c>
-      <c r="D13" s="151"/>
+      <c r="D13" s="133"/>
       <c r="E13" s="1" t="s">
         <v>169</v>
       </c>
@@ -7023,10 +7050,10 @@
         <v>170</v>
       </c>
       <c r="B14" s="111"/>
-      <c r="C14" s="151" t="s">
+      <c r="C14" s="133" t="s">
         <v>171</v>
       </c>
-      <c r="D14" s="151"/>
+      <c r="D14" s="133"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="112" t="s">
@@ -7052,28 +7079,28 @@
       <c r="A16" s="6"/>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="146" t="s">
+      <c r="A17" s="169" t="s">
         <v>185</v>
       </c>
-      <c r="B17" s="146"/>
-      <c r="C17" s="146"/>
-      <c r="D17" s="146"/>
-      <c r="E17" s="146"/>
-      <c r="F17" s="146"/>
-      <c r="G17" s="146"/>
+      <c r="B17" s="169"/>
+      <c r="C17" s="169"/>
+      <c r="D17" s="169"/>
+      <c r="E17" s="169"/>
+      <c r="F17" s="169"/>
+      <c r="G17" s="169"/>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="140" t="s">
+      <c r="B18" s="163" t="s">
         <v>176</v>
       </c>
-      <c r="C18" s="141"/>
-      <c r="D18" s="141"/>
-      <c r="E18" s="141"/>
-      <c r="F18" s="141"/>
-      <c r="G18" s="142"/>
+      <c r="C18" s="164"/>
+      <c r="D18" s="164"/>
+      <c r="E18" s="164"/>
+      <c r="F18" s="164"/>
+      <c r="G18" s="165"/>
       <c r="H18" s="95"/>
       <c r="I18" s="95"/>
       <c r="K18" s="95"/>
@@ -7085,12 +7112,12 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="106"/>
-      <c r="B19" s="157"/>
-      <c r="C19" s="157"/>
-      <c r="D19" s="157"/>
-      <c r="E19" s="157"/>
-      <c r="F19" s="157"/>
-      <c r="G19" s="157"/>
+      <c r="B19" s="148"/>
+      <c r="C19" s="148"/>
+      <c r="D19" s="148"/>
+      <c r="E19" s="148"/>
+      <c r="F19" s="148"/>
+      <c r="G19" s="148"/>
       <c r="H19" s="102"/>
       <c r="I19" s="102"/>
       <c r="K19" s="102"/>
@@ -7102,12 +7129,12 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="107"/>
-      <c r="B20" s="158"/>
-      <c r="C20" s="158"/>
-      <c r="D20" s="158"/>
-      <c r="E20" s="158"/>
-      <c r="F20" s="158"/>
-      <c r="G20" s="158"/>
+      <c r="B20" s="150"/>
+      <c r="C20" s="150"/>
+      <c r="D20" s="150"/>
+      <c r="E20" s="150"/>
+      <c r="F20" s="150"/>
+      <c r="G20" s="150"/>
       <c r="H20" s="102"/>
       <c r="I20" s="102"/>
       <c r="K20" s="102"/>
@@ -7119,12 +7146,12 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="108"/>
-      <c r="B21" s="159"/>
-      <c r="C21" s="159"/>
-      <c r="D21" s="159"/>
-      <c r="E21" s="159"/>
-      <c r="F21" s="159"/>
-      <c r="G21" s="159"/>
+      <c r="B21" s="152"/>
+      <c r="C21" s="152"/>
+      <c r="D21" s="152"/>
+      <c r="E21" s="152"/>
+      <c r="F21" s="152"/>
+      <c r="G21" s="152"/>
       <c r="H21" s="102"/>
       <c r="I21" s="102"/>
       <c r="J21" s="95"/>
@@ -7140,29 +7167,29 @@
       <c r="J22" s="102"/>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="143" t="s">
+      <c r="A23" s="166" t="s">
         <v>186</v>
       </c>
-      <c r="B23" s="144"/>
-      <c r="C23" s="144"/>
-      <c r="D23" s="144"/>
-      <c r="E23" s="144"/>
-      <c r="F23" s="144"/>
-      <c r="G23" s="145"/>
+      <c r="B23" s="167"/>
+      <c r="C23" s="167"/>
+      <c r="D23" s="167"/>
+      <c r="E23" s="167"/>
+      <c r="F23" s="167"/>
+      <c r="G23" s="168"/>
       <c r="J23" s="102"/>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="164" t="s">
+      <c r="B24" s="144" t="s">
         <v>177</v>
       </c>
-      <c r="C24" s="164"/>
-      <c r="D24" s="164"/>
-      <c r="E24" s="164"/>
-      <c r="F24" s="164"/>
-      <c r="G24" s="164"/>
+      <c r="C24" s="144"/>
+      <c r="D24" s="144"/>
+      <c r="E24" s="144"/>
+      <c r="F24" s="144"/>
+      <c r="G24" s="144"/>
       <c r="H24" s="95"/>
       <c r="I24" s="95"/>
       <c r="J24" s="102"/>
@@ -7177,14 +7204,14 @@
       <c r="A25" s="106">
         <v>1</v>
       </c>
-      <c r="B25" s="165" t="s">
+      <c r="B25" s="145" t="s">
         <v>178</v>
       </c>
-      <c r="C25" s="165"/>
-      <c r="D25" s="165"/>
-      <c r="E25" s="165"/>
-      <c r="F25" s="165"/>
-      <c r="G25" s="165"/>
+      <c r="C25" s="145"/>
+      <c r="D25" s="145"/>
+      <c r="E25" s="145"/>
+      <c r="F25" s="145"/>
+      <c r="G25" s="145"/>
       <c r="H25" s="102"/>
       <c r="I25" s="102"/>
       <c r="K25" s="102"/>
@@ -7196,12 +7223,12 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="107"/>
-      <c r="B26" s="166"/>
-      <c r="C26" s="166"/>
-      <c r="D26" s="166"/>
-      <c r="E26" s="166"/>
-      <c r="F26" s="166"/>
-      <c r="G26" s="166"/>
+      <c r="B26" s="146"/>
+      <c r="C26" s="146"/>
+      <c r="D26" s="146"/>
+      <c r="E26" s="146"/>
+      <c r="F26" s="146"/>
+      <c r="G26" s="146"/>
       <c r="H26" s="102"/>
       <c r="I26" s="102"/>
       <c r="K26" s="102"/>
@@ -7213,12 +7240,12 @@
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="108"/>
-      <c r="B27" s="167"/>
-      <c r="C27" s="167"/>
-      <c r="D27" s="167"/>
-      <c r="E27" s="167"/>
-      <c r="F27" s="167"/>
-      <c r="G27" s="167"/>
+      <c r="B27" s="147"/>
+      <c r="C27" s="147"/>
+      <c r="D27" s="147"/>
+      <c r="E27" s="147"/>
+      <c r="F27" s="147"/>
+      <c r="G27" s="147"/>
       <c r="H27" s="102"/>
       <c r="I27" s="102"/>
       <c r="J27" s="95"/>
@@ -7247,29 +7274,29 @@
       <c r="O28"/>
     </row>
     <row r="29" spans="1:17">
-      <c r="A29" s="143" t="s">
+      <c r="A29" s="166" t="s">
         <v>187</v>
       </c>
-      <c r="B29" s="144"/>
-      <c r="C29" s="144"/>
-      <c r="D29" s="144"/>
-      <c r="E29" s="144"/>
-      <c r="F29" s="144"/>
-      <c r="G29" s="145"/>
+      <c r="B29" s="167"/>
+      <c r="C29" s="167"/>
+      <c r="D29" s="167"/>
+      <c r="E29" s="167"/>
+      <c r="F29" s="167"/>
+      <c r="G29" s="168"/>
       <c r="J29" s="102"/>
     </row>
     <row r="30" spans="1:17">
       <c r="A30" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B30" s="164" t="s">
+      <c r="B30" s="144" t="s">
         <v>179</v>
       </c>
-      <c r="C30" s="164"/>
-      <c r="D30" s="164"/>
-      <c r="E30" s="164"/>
-      <c r="F30" s="164"/>
-      <c r="G30" s="164"/>
+      <c r="C30" s="144"/>
+      <c r="D30" s="144"/>
+      <c r="E30" s="144"/>
+      <c r="F30" s="144"/>
+      <c r="G30" s="144"/>
       <c r="H30" s="95"/>
       <c r="I30" s="95"/>
       <c r="J30" s="102"/>
@@ -7282,12 +7309,12 @@
     </row>
     <row r="31" spans="1:17">
       <c r="A31" s="106"/>
-      <c r="B31" s="157"/>
-      <c r="C31" s="157"/>
-      <c r="D31" s="157"/>
-      <c r="E31" s="157"/>
-      <c r="F31" s="157"/>
-      <c r="G31" s="168"/>
+      <c r="B31" s="148"/>
+      <c r="C31" s="148"/>
+      <c r="D31" s="148"/>
+      <c r="E31" s="148"/>
+      <c r="F31" s="148"/>
+      <c r="G31" s="149"/>
       <c r="H31" s="102"/>
       <c r="I31" s="102"/>
       <c r="J31"/>
@@ -7300,12 +7327,12 @@
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="107"/>
-      <c r="B32" s="158"/>
-      <c r="C32" s="158"/>
-      <c r="D32" s="158"/>
-      <c r="E32" s="158"/>
-      <c r="F32" s="158"/>
-      <c r="G32" s="169"/>
+      <c r="B32" s="150"/>
+      <c r="C32" s="150"/>
+      <c r="D32" s="150"/>
+      <c r="E32" s="150"/>
+      <c r="F32" s="150"/>
+      <c r="G32" s="151"/>
       <c r="H32" s="102"/>
       <c r="I32" s="102"/>
       <c r="K32" s="102"/>
@@ -7317,12 +7344,12 @@
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="108"/>
-      <c r="B33" s="159"/>
-      <c r="C33" s="159"/>
-      <c r="D33" s="159"/>
-      <c r="E33" s="159"/>
-      <c r="F33" s="159"/>
-      <c r="G33" s="170"/>
+      <c r="B33" s="152"/>
+      <c r="C33" s="152"/>
+      <c r="D33" s="152"/>
+      <c r="E33" s="152"/>
+      <c r="F33" s="152"/>
+      <c r="G33" s="153"/>
       <c r="H33" s="102"/>
       <c r="I33" s="102"/>
       <c r="J33" s="95"/>
@@ -7375,64 +7402,64 @@
       <c r="P36" s="49"/>
     </row>
     <row r="37" spans="1:17" ht="15">
-      <c r="A37" s="181" t="s">
+      <c r="A37" s="180" t="s">
         <v>114</v>
       </c>
-      <c r="B37" s="181" t="s">
+      <c r="B37" s="180" t="s">
         <v>115</v>
       </c>
       <c r="C37" s="51" t="s">
         <v>116</v>
       </c>
-      <c r="D37" s="181" t="s">
+      <c r="D37" s="180" t="s">
         <v>98</v>
       </c>
-      <c r="E37" s="181" t="s">
+      <c r="E37" s="180" t="s">
         <v>155</v>
       </c>
-      <c r="F37" s="181" t="s">
+      <c r="F37" s="180" t="s">
         <v>170</v>
       </c>
-      <c r="G37" s="181" t="s">
+      <c r="G37" s="180" t="s">
         <v>135</v>
       </c>
-      <c r="H37" s="181" t="s">
+      <c r="H37" s="180" t="s">
         <v>112</v>
       </c>
-      <c r="I37" s="181" t="s">
+      <c r="I37" s="180" t="s">
         <v>229</v>
       </c>
       <c r="J37" s="176" t="s">
         <v>189</v>
       </c>
-      <c r="K37" s="186" t="s">
+      <c r="K37" s="185" t="s">
         <v>118</v>
       </c>
-      <c r="L37" s="187"/>
-      <c r="M37" s="188" t="s">
+      <c r="L37" s="186"/>
+      <c r="M37" s="187" t="s">
         <v>119</v>
       </c>
-      <c r="N37" s="187"/>
+      <c r="N37" s="186"/>
       <c r="O37" s="50" t="s">
         <v>120</v>
       </c>
-      <c r="P37" s="181" t="s">
+      <c r="P37" s="180" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="15">
-      <c r="A38" s="185"/>
-      <c r="B38" s="185"/>
+      <c r="A38" s="188"/>
+      <c r="B38" s="188"/>
       <c r="C38" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="D38" s="185"/>
-      <c r="E38" s="182"/>
-      <c r="F38" s="182"/>
-      <c r="G38" s="185"/>
-      <c r="H38" s="185"/>
-      <c r="I38" s="185"/>
-      <c r="J38" s="183"/>
+      <c r="D38" s="188"/>
+      <c r="E38" s="181"/>
+      <c r="F38" s="181"/>
+      <c r="G38" s="188"/>
+      <c r="H38" s="188"/>
+      <c r="I38" s="188"/>
+      <c r="J38" s="177"/>
       <c r="K38" s="53" t="s">
         <v>122</v>
       </c>
@@ -7448,7 +7475,7 @@
       <c r="O38" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="P38" s="185"/>
+      <c r="P38" s="188"/>
     </row>
     <row r="39" spans="1:17">
       <c r="A39" s="55">
@@ -7946,6 +7973,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="P37:P38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="H37:H38"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="J37:J38"/>
@@ -7962,19 +8002,6 @@
     <mergeCell ref="A17:G17"/>
     <mergeCell ref="B18:G18"/>
     <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="P37:P38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">
@@ -8184,10 +8211,10 @@
         <v>167</v>
       </c>
       <c r="B15" s="111"/>
-      <c r="C15" s="151" t="s">
+      <c r="C15" s="133" t="s">
         <v>168</v>
       </c>
-      <c r="D15" s="151"/>
+      <c r="D15" s="133"/>
       <c r="E15" s="1" t="s">
         <v>169</v>
       </c>
@@ -8197,10 +8224,10 @@
         <v>170</v>
       </c>
       <c r="B16" s="111"/>
-      <c r="C16" s="151" t="s">
+      <c r="C16" s="133" t="s">
         <v>171</v>
       </c>
-      <c r="D16" s="151"/>
+      <c r="D16" s="133"/>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="112" t="s">
@@ -8226,28 +8253,28 @@
       <c r="A18" s="6"/>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="146" t="s">
+      <c r="A19" s="169" t="s">
         <v>185</v>
       </c>
-      <c r="B19" s="146"/>
-      <c r="C19" s="146"/>
-      <c r="D19" s="146"/>
-      <c r="E19" s="146"/>
-      <c r="F19" s="146"/>
-      <c r="G19" s="146"/>
+      <c r="B19" s="169"/>
+      <c r="C19" s="169"/>
+      <c r="D19" s="169"/>
+      <c r="E19" s="169"/>
+      <c r="F19" s="169"/>
+      <c r="G19" s="169"/>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B20" s="140" t="s">
+      <c r="B20" s="163" t="s">
         <v>176</v>
       </c>
-      <c r="C20" s="141"/>
-      <c r="D20" s="141"/>
-      <c r="E20" s="141"/>
-      <c r="F20" s="141"/>
-      <c r="G20" s="142"/>
+      <c r="C20" s="164"/>
+      <c r="D20" s="164"/>
+      <c r="E20" s="164"/>
+      <c r="F20" s="164"/>
+      <c r="G20" s="165"/>
       <c r="H20" s="95"/>
       <c r="I20" s="95"/>
       <c r="K20" s="95"/>
@@ -8259,12 +8286,12 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="106"/>
-      <c r="B21" s="157"/>
-      <c r="C21" s="157"/>
-      <c r="D21" s="157"/>
-      <c r="E21" s="157"/>
-      <c r="F21" s="157"/>
-      <c r="G21" s="157"/>
+      <c r="B21" s="148"/>
+      <c r="C21" s="148"/>
+      <c r="D21" s="148"/>
+      <c r="E21" s="148"/>
+      <c r="F21" s="148"/>
+      <c r="G21" s="148"/>
       <c r="H21" s="102"/>
       <c r="I21" s="102"/>
       <c r="K21" s="102"/>
@@ -8276,12 +8303,12 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="107"/>
-      <c r="B22" s="158"/>
-      <c r="C22" s="158"/>
-      <c r="D22" s="158"/>
-      <c r="E22" s="158"/>
-      <c r="F22" s="158"/>
-      <c r="G22" s="158"/>
+      <c r="B22" s="150"/>
+      <c r="C22" s="150"/>
+      <c r="D22" s="150"/>
+      <c r="E22" s="150"/>
+      <c r="F22" s="150"/>
+      <c r="G22" s="150"/>
       <c r="H22" s="102"/>
       <c r="I22" s="102"/>
       <c r="K22" s="102"/>
@@ -8293,12 +8320,12 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="108"/>
-      <c r="B23" s="159"/>
-      <c r="C23" s="159"/>
-      <c r="D23" s="159"/>
-      <c r="E23" s="159"/>
-      <c r="F23" s="159"/>
-      <c r="G23" s="159"/>
+      <c r="B23" s="152"/>
+      <c r="C23" s="152"/>
+      <c r="D23" s="152"/>
+      <c r="E23" s="152"/>
+      <c r="F23" s="152"/>
+      <c r="G23" s="152"/>
       <c r="H23" s="102"/>
       <c r="I23" s="102"/>
       <c r="J23" s="95"/>
@@ -8314,29 +8341,29 @@
       <c r="J24" s="102"/>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" s="143" t="s">
+      <c r="A25" s="166" t="s">
         <v>186</v>
       </c>
-      <c r="B25" s="144"/>
-      <c r="C25" s="144"/>
-      <c r="D25" s="144"/>
-      <c r="E25" s="144"/>
-      <c r="F25" s="144"/>
-      <c r="G25" s="145"/>
+      <c r="B25" s="167"/>
+      <c r="C25" s="167"/>
+      <c r="D25" s="167"/>
+      <c r="E25" s="167"/>
+      <c r="F25" s="167"/>
+      <c r="G25" s="168"/>
       <c r="J25" s="102"/>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="164" t="s">
+      <c r="B26" s="144" t="s">
         <v>177</v>
       </c>
-      <c r="C26" s="164"/>
-      <c r="D26" s="164"/>
-      <c r="E26" s="164"/>
-      <c r="F26" s="164"/>
-      <c r="G26" s="164"/>
+      <c r="C26" s="144"/>
+      <c r="D26" s="144"/>
+      <c r="E26" s="144"/>
+      <c r="F26" s="144"/>
+      <c r="G26" s="144"/>
       <c r="H26" s="95"/>
       <c r="I26" s="95"/>
       <c r="J26" s="102"/>
@@ -8351,14 +8378,14 @@
       <c r="A27" s="106">
         <v>1</v>
       </c>
-      <c r="B27" s="165" t="s">
+      <c r="B27" s="145" t="s">
         <v>178</v>
       </c>
-      <c r="C27" s="165"/>
-      <c r="D27" s="165"/>
-      <c r="E27" s="165"/>
-      <c r="F27" s="165"/>
-      <c r="G27" s="165"/>
+      <c r="C27" s="145"/>
+      <c r="D27" s="145"/>
+      <c r="E27" s="145"/>
+      <c r="F27" s="145"/>
+      <c r="G27" s="145"/>
       <c r="H27" s="102"/>
       <c r="I27" s="102"/>
       <c r="K27" s="102"/>
@@ -8370,12 +8397,12 @@
     </row>
     <row r="28" spans="1:17">
       <c r="A28" s="107"/>
-      <c r="B28" s="166"/>
-      <c r="C28" s="166"/>
-      <c r="D28" s="166"/>
-      <c r="E28" s="166"/>
-      <c r="F28" s="166"/>
-      <c r="G28" s="166"/>
+      <c r="B28" s="146"/>
+      <c r="C28" s="146"/>
+      <c r="D28" s="146"/>
+      <c r="E28" s="146"/>
+      <c r="F28" s="146"/>
+      <c r="G28" s="146"/>
       <c r="H28" s="102"/>
       <c r="I28" s="102"/>
       <c r="K28" s="102"/>
@@ -8387,12 +8414,12 @@
     </row>
     <row r="29" spans="1:17">
       <c r="A29" s="108"/>
-      <c r="B29" s="167"/>
-      <c r="C29" s="167"/>
-      <c r="D29" s="167"/>
-      <c r="E29" s="167"/>
-      <c r="F29" s="167"/>
-      <c r="G29" s="167"/>
+      <c r="B29" s="147"/>
+      <c r="C29" s="147"/>
+      <c r="D29" s="147"/>
+      <c r="E29" s="147"/>
+      <c r="F29" s="147"/>
+      <c r="G29" s="147"/>
       <c r="H29" s="102"/>
       <c r="I29" s="102"/>
       <c r="J29" s="95"/>
@@ -8421,29 +8448,29 @@
       <c r="O30"/>
     </row>
     <row r="31" spans="1:17">
-      <c r="A31" s="143" t="s">
+      <c r="A31" s="166" t="s">
         <v>187</v>
       </c>
-      <c r="B31" s="144"/>
-      <c r="C31" s="144"/>
-      <c r="D31" s="144"/>
-      <c r="E31" s="144"/>
-      <c r="F31" s="144"/>
-      <c r="G31" s="145"/>
+      <c r="B31" s="167"/>
+      <c r="C31" s="167"/>
+      <c r="D31" s="167"/>
+      <c r="E31" s="167"/>
+      <c r="F31" s="167"/>
+      <c r="G31" s="168"/>
       <c r="J31" s="102"/>
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="164" t="s">
+      <c r="B32" s="144" t="s">
         <v>179</v>
       </c>
-      <c r="C32" s="164"/>
-      <c r="D32" s="164"/>
-      <c r="E32" s="164"/>
-      <c r="F32" s="164"/>
-      <c r="G32" s="164"/>
+      <c r="C32" s="144"/>
+      <c r="D32" s="144"/>
+      <c r="E32" s="144"/>
+      <c r="F32" s="144"/>
+      <c r="G32" s="144"/>
       <c r="H32" s="95"/>
       <c r="I32" s="95"/>
       <c r="J32" s="102"/>
@@ -8456,12 +8483,12 @@
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="106"/>
-      <c r="B33" s="157"/>
-      <c r="C33" s="157"/>
-      <c r="D33" s="157"/>
-      <c r="E33" s="157"/>
-      <c r="F33" s="157"/>
-      <c r="G33" s="168"/>
+      <c r="B33" s="148"/>
+      <c r="C33" s="148"/>
+      <c r="D33" s="148"/>
+      <c r="E33" s="148"/>
+      <c r="F33" s="148"/>
+      <c r="G33" s="149"/>
       <c r="H33" s="102"/>
       <c r="I33" s="102"/>
       <c r="J33"/>
@@ -8474,12 +8501,12 @@
     </row>
     <row r="34" spans="1:17">
       <c r="A34" s="107"/>
-      <c r="B34" s="158"/>
-      <c r="C34" s="158"/>
-      <c r="D34" s="158"/>
-      <c r="E34" s="158"/>
-      <c r="F34" s="158"/>
-      <c r="G34" s="169"/>
+      <c r="B34" s="150"/>
+      <c r="C34" s="150"/>
+      <c r="D34" s="150"/>
+      <c r="E34" s="150"/>
+      <c r="F34" s="150"/>
+      <c r="G34" s="151"/>
       <c r="H34" s="102"/>
       <c r="I34" s="102"/>
       <c r="K34" s="102"/>
@@ -8491,12 +8518,12 @@
     </row>
     <row r="35" spans="1:17">
       <c r="A35" s="108"/>
-      <c r="B35" s="159"/>
-      <c r="C35" s="159"/>
-      <c r="D35" s="159"/>
-      <c r="E35" s="159"/>
-      <c r="F35" s="159"/>
-      <c r="G35" s="170"/>
+      <c r="B35" s="152"/>
+      <c r="C35" s="152"/>
+      <c r="D35" s="152"/>
+      <c r="E35" s="152"/>
+      <c r="F35" s="152"/>
+      <c r="G35" s="153"/>
       <c r="H35" s="102"/>
       <c r="I35" s="102"/>
       <c r="J35" s="95"/>
@@ -8549,25 +8576,25 @@
       <c r="P38" s="49"/>
     </row>
     <row r="39" spans="1:17" ht="15">
-      <c r="A39" s="181" t="s">
+      <c r="A39" s="180" t="s">
         <v>114</v>
       </c>
-      <c r="B39" s="181" t="s">
+      <c r="B39" s="180" t="s">
         <v>115</v>
       </c>
       <c r="C39" s="51" t="s">
         <v>116</v>
       </c>
-      <c r="D39" s="181" t="s">
+      <c r="D39" s="180" t="s">
         <v>98</v>
       </c>
-      <c r="E39" s="181" t="s">
+      <c r="E39" s="180" t="s">
         <v>155</v>
       </c>
-      <c r="F39" s="181" t="s">
+      <c r="F39" s="180" t="s">
         <v>170</v>
       </c>
-      <c r="G39" s="181" t="s">
+      <c r="G39" s="180" t="s">
         <v>135</v>
       </c>
       <c r="H39" s="189" t="s">
@@ -8579,34 +8606,34 @@
       <c r="J39" s="176" t="s">
         <v>189</v>
       </c>
-      <c r="K39" s="186" t="s">
+      <c r="K39" s="185" t="s">
         <v>118</v>
       </c>
-      <c r="L39" s="187"/>
-      <c r="M39" s="188" t="s">
+      <c r="L39" s="186"/>
+      <c r="M39" s="187" t="s">
         <v>119</v>
       </c>
-      <c r="N39" s="187"/>
+      <c r="N39" s="186"/>
       <c r="O39" s="50" t="s">
         <v>120</v>
       </c>
-      <c r="P39" s="181" t="s">
+      <c r="P39" s="180" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="15">
-      <c r="A40" s="185"/>
-      <c r="B40" s="185"/>
+      <c r="A40" s="188"/>
+      <c r="B40" s="188"/>
       <c r="C40" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="D40" s="185"/>
-      <c r="E40" s="182"/>
-      <c r="F40" s="182"/>
-      <c r="G40" s="185"/>
-      <c r="H40" s="185"/>
-      <c r="I40" s="185"/>
-      <c r="J40" s="183"/>
+      <c r="D40" s="188"/>
+      <c r="E40" s="181"/>
+      <c r="F40" s="181"/>
+      <c r="G40" s="188"/>
+      <c r="H40" s="188"/>
+      <c r="I40" s="188"/>
+      <c r="J40" s="177"/>
       <c r="K40" s="53" t="s">
         <v>122</v>
       </c>
@@ -8622,7 +8649,7 @@
       <c r="O40" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="P40" s="185"/>
+      <c r="P40" s="188"/>
     </row>
     <row r="41" spans="1:17">
       <c r="A41" s="55">
@@ -9078,19 +9105,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
     <mergeCell ref="P39:P40"/>
     <mergeCell ref="A31:G31"/>
     <mergeCell ref="B32:G32"/>
@@ -9107,6 +9121,19 @@
     <mergeCell ref="J39:J40"/>
     <mergeCell ref="K39:L39"/>
     <mergeCell ref="M39:N39"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">
@@ -9154,8 +9181,8 @@
   </sheetPr>
   <dimension ref="A1:V67"/>
   <sheetViews>
-    <sheetView topLeftCell="F3" workbookViewId="0">
-      <selection activeCell="M3" sqref="M1:N1048576"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="N48" sqref="N48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -9315,10 +9342,10 @@
         <v>167</v>
       </c>
       <c r="B16" s="111"/>
-      <c r="C16" s="151" t="s">
+      <c r="C16" s="133" t="s">
         <v>168</v>
       </c>
-      <c r="D16" s="151"/>
+      <c r="D16" s="133"/>
       <c r="E16" s="1" t="s">
         <v>169</v>
       </c>
@@ -9328,20 +9355,20 @@
         <v>170</v>
       </c>
       <c r="B17" s="111"/>
-      <c r="C17" s="151" t="s">
+      <c r="C17" s="133" t="s">
         <v>171</v>
       </c>
-      <c r="D17" s="151"/>
+      <c r="D17" s="133"/>
     </row>
     <row r="18" spans="1:22">
       <c r="A18" s="111" t="s">
         <v>207</v>
       </c>
       <c r="B18" s="111"/>
-      <c r="C18" s="150" t="s">
+      <c r="C18" s="132" t="s">
         <v>209</v>
       </c>
-      <c r="D18" s="151"/>
+      <c r="D18" s="133"/>
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="112" t="s">
@@ -9399,28 +9426,28 @@
       <c r="A21" s="6"/>
     </row>
     <row r="22" spans="1:22">
-      <c r="A22" s="146" t="s">
+      <c r="A22" s="169" t="s">
         <v>185</v>
       </c>
-      <c r="B22" s="146"/>
-      <c r="C22" s="146"/>
-      <c r="D22" s="146"/>
-      <c r="E22" s="146"/>
-      <c r="F22" s="146"/>
-      <c r="G22" s="146"/>
+      <c r="B22" s="169"/>
+      <c r="C22" s="169"/>
+      <c r="D22" s="169"/>
+      <c r="E22" s="169"/>
+      <c r="F22" s="169"/>
+      <c r="G22" s="169"/>
     </row>
     <row r="23" spans="1:22">
       <c r="A23" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="140" t="s">
+      <c r="B23" s="163" t="s">
         <v>176</v>
       </c>
-      <c r="C23" s="141"/>
-      <c r="D23" s="141"/>
-      <c r="E23" s="141"/>
-      <c r="F23" s="141"/>
-      <c r="G23" s="142"/>
+      <c r="C23" s="164"/>
+      <c r="D23" s="164"/>
+      <c r="E23" s="164"/>
+      <c r="F23" s="164"/>
+      <c r="G23" s="165"/>
       <c r="H23" s="95"/>
       <c r="I23" s="95"/>
       <c r="J23" s="95"/>
@@ -9438,12 +9465,12 @@
     </row>
     <row r="24" spans="1:22">
       <c r="A24" s="106"/>
-      <c r="B24" s="157"/>
-      <c r="C24" s="157"/>
-      <c r="D24" s="157"/>
-      <c r="E24" s="157"/>
-      <c r="F24" s="157"/>
-      <c r="G24" s="157"/>
+      <c r="B24" s="148"/>
+      <c r="C24" s="148"/>
+      <c r="D24" s="148"/>
+      <c r="E24" s="148"/>
+      <c r="F24" s="148"/>
+      <c r="G24" s="148"/>
       <c r="H24" s="102"/>
       <c r="I24" s="102"/>
       <c r="J24" s="102"/>
@@ -9461,12 +9488,12 @@
     </row>
     <row r="25" spans="1:22">
       <c r="A25" s="107"/>
-      <c r="B25" s="158"/>
-      <c r="C25" s="158"/>
-      <c r="D25" s="158"/>
-      <c r="E25" s="158"/>
-      <c r="F25" s="158"/>
-      <c r="G25" s="158"/>
+      <c r="B25" s="150"/>
+      <c r="C25" s="150"/>
+      <c r="D25" s="150"/>
+      <c r="E25" s="150"/>
+      <c r="F25" s="150"/>
+      <c r="G25" s="150"/>
       <c r="H25" s="102"/>
       <c r="I25" s="102"/>
       <c r="J25" s="102"/>
@@ -9484,12 +9511,12 @@
     </row>
     <row r="26" spans="1:22">
       <c r="A26" s="108"/>
-      <c r="B26" s="159"/>
-      <c r="C26" s="159"/>
-      <c r="D26" s="159"/>
-      <c r="E26" s="159"/>
-      <c r="F26" s="159"/>
-      <c r="G26" s="159"/>
+      <c r="B26" s="152"/>
+      <c r="C26" s="152"/>
+      <c r="D26" s="152"/>
+      <c r="E26" s="152"/>
+      <c r="F26" s="152"/>
+      <c r="G26" s="152"/>
       <c r="H26" s="102"/>
       <c r="I26" s="102"/>
       <c r="J26" s="102"/>
@@ -9509,28 +9536,28 @@
       <c r="C27"/>
     </row>
     <row r="28" spans="1:22">
-      <c r="A28" s="143" t="s">
+      <c r="A28" s="166" t="s">
         <v>186</v>
       </c>
-      <c r="B28" s="144"/>
-      <c r="C28" s="144"/>
-      <c r="D28" s="144"/>
-      <c r="E28" s="144"/>
-      <c r="F28" s="144"/>
-      <c r="G28" s="145"/>
+      <c r="B28" s="167"/>
+      <c r="C28" s="167"/>
+      <c r="D28" s="167"/>
+      <c r="E28" s="167"/>
+      <c r="F28" s="167"/>
+      <c r="G28" s="168"/>
     </row>
     <row r="29" spans="1:22">
       <c r="A29" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="164" t="s">
+      <c r="B29" s="144" t="s">
         <v>177</v>
       </c>
-      <c r="C29" s="164"/>
-      <c r="D29" s="164"/>
-      <c r="E29" s="164"/>
-      <c r="F29" s="164"/>
-      <c r="G29" s="164"/>
+      <c r="C29" s="144"/>
+      <c r="D29" s="144"/>
+      <c r="E29" s="144"/>
+      <c r="F29" s="144"/>
+      <c r="G29" s="144"/>
       <c r="H29" s="95"/>
       <c r="I29" s="95"/>
       <c r="J29" s="95"/>
@@ -9550,14 +9577,14 @@
       <c r="A30" s="106">
         <v>1</v>
       </c>
-      <c r="B30" s="165" t="s">
+      <c r="B30" s="145" t="s">
         <v>178</v>
       </c>
-      <c r="C30" s="165"/>
-      <c r="D30" s="165"/>
-      <c r="E30" s="165"/>
-      <c r="F30" s="165"/>
-      <c r="G30" s="165"/>
+      <c r="C30" s="145"/>
+      <c r="D30" s="145"/>
+      <c r="E30" s="145"/>
+      <c r="F30" s="145"/>
+      <c r="G30" s="145"/>
       <c r="H30" s="102"/>
       <c r="I30" s="102"/>
       <c r="J30" s="102"/>
@@ -9575,12 +9602,12 @@
     </row>
     <row r="31" spans="1:22">
       <c r="A31" s="107"/>
-      <c r="B31" s="166"/>
-      <c r="C31" s="166"/>
-      <c r="D31" s="166"/>
-      <c r="E31" s="166"/>
-      <c r="F31" s="166"/>
-      <c r="G31" s="166"/>
+      <c r="B31" s="146"/>
+      <c r="C31" s="146"/>
+      <c r="D31" s="146"/>
+      <c r="E31" s="146"/>
+      <c r="F31" s="146"/>
+      <c r="G31" s="146"/>
       <c r="H31" s="102"/>
       <c r="I31" s="102"/>
       <c r="J31" s="102"/>
@@ -9598,12 +9625,12 @@
     </row>
     <row r="32" spans="1:22">
       <c r="A32" s="108"/>
-      <c r="B32" s="167"/>
-      <c r="C32" s="167"/>
-      <c r="D32" s="167"/>
-      <c r="E32" s="167"/>
-      <c r="F32" s="167"/>
-      <c r="G32" s="167"/>
+      <c r="B32" s="147"/>
+      <c r="C32" s="147"/>
+      <c r="D32" s="147"/>
+      <c r="E32" s="147"/>
+      <c r="F32" s="147"/>
+      <c r="G32" s="147"/>
       <c r="H32" s="102"/>
       <c r="I32" s="102"/>
       <c r="J32" s="102"/>
@@ -9642,28 +9669,28 @@
       <c r="T33"/>
     </row>
     <row r="34" spans="1:22">
-      <c r="A34" s="143" t="s">
+      <c r="A34" s="166" t="s">
         <v>187</v>
       </c>
-      <c r="B34" s="144"/>
-      <c r="C34" s="144"/>
-      <c r="D34" s="144"/>
-      <c r="E34" s="144"/>
-      <c r="F34" s="144"/>
-      <c r="G34" s="145"/>
+      <c r="B34" s="167"/>
+      <c r="C34" s="167"/>
+      <c r="D34" s="167"/>
+      <c r="E34" s="167"/>
+      <c r="F34" s="167"/>
+      <c r="G34" s="168"/>
     </row>
     <row r="35" spans="1:22">
       <c r="A35" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="164" t="s">
+      <c r="B35" s="144" t="s">
         <v>179</v>
       </c>
-      <c r="C35" s="164"/>
-      <c r="D35" s="164"/>
-      <c r="E35" s="164"/>
-      <c r="F35" s="164"/>
-      <c r="G35" s="164"/>
+      <c r="C35" s="144"/>
+      <c r="D35" s="144"/>
+      <c r="E35" s="144"/>
+      <c r="F35" s="144"/>
+      <c r="G35" s="144"/>
       <c r="H35" s="95"/>
       <c r="I35" s="95"/>
       <c r="J35" s="95"/>
@@ -9681,12 +9708,12 @@
     </row>
     <row r="36" spans="1:22">
       <c r="A36" s="106"/>
-      <c r="B36" s="157"/>
-      <c r="C36" s="157"/>
-      <c r="D36" s="157"/>
-      <c r="E36" s="157"/>
-      <c r="F36" s="157"/>
-      <c r="G36" s="168"/>
+      <c r="B36" s="148"/>
+      <c r="C36" s="148"/>
+      <c r="D36" s="148"/>
+      <c r="E36" s="148"/>
+      <c r="F36" s="148"/>
+      <c r="G36" s="149"/>
       <c r="H36" s="102"/>
       <c r="I36" s="102"/>
       <c r="J36" s="102"/>
@@ -9704,12 +9731,12 @@
     </row>
     <row r="37" spans="1:22">
       <c r="A37" s="107"/>
-      <c r="B37" s="158"/>
-      <c r="C37" s="158"/>
-      <c r="D37" s="158"/>
-      <c r="E37" s="158"/>
-      <c r="F37" s="158"/>
-      <c r="G37" s="169"/>
+      <c r="B37" s="150"/>
+      <c r="C37" s="150"/>
+      <c r="D37" s="150"/>
+      <c r="E37" s="150"/>
+      <c r="F37" s="150"/>
+      <c r="G37" s="151"/>
       <c r="H37" s="102"/>
       <c r="I37" s="102"/>
       <c r="J37" s="102"/>
@@ -9727,12 +9754,12 @@
     </row>
     <row r="38" spans="1:22">
       <c r="A38" s="108"/>
-      <c r="B38" s="159"/>
-      <c r="C38" s="159"/>
-      <c r="D38" s="159"/>
-      <c r="E38" s="159"/>
-      <c r="F38" s="159"/>
-      <c r="G38" s="170"/>
+      <c r="B38" s="152"/>
+      <c r="C38" s="152"/>
+      <c r="D38" s="152"/>
+      <c r="E38" s="152"/>
+      <c r="F38" s="152"/>
+      <c r="G38" s="153"/>
       <c r="H38" s="102"/>
       <c r="I38" s="102"/>
       <c r="J38" s="102"/>
@@ -9808,16 +9835,16 @@
       <c r="B42" s="176" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="178" t="s">
+      <c r="C42" s="182" t="s">
         <v>1</v>
       </c>
       <c r="D42" s="176" t="s">
         <v>2</v>
       </c>
-      <c r="E42" s="181" t="s">
+      <c r="E42" s="180" t="s">
         <v>155</v>
       </c>
-      <c r="F42" s="181" t="s">
+      <c r="F42" s="180" t="s">
         <v>170</v>
       </c>
       <c r="G42" s="176" t="s">
@@ -9829,17 +9856,17 @@
       <c r="I42" s="176" t="s">
         <v>236</v>
       </c>
-      <c r="J42" s="181" t="s">
+      <c r="J42" s="180" t="s">
         <v>237</v>
       </c>
-      <c r="K42" s="181" t="s">
+      <c r="K42" s="180" t="s">
         <v>207</v>
       </c>
-      <c r="L42" s="184" t="s">
+      <c r="L42" s="179" t="s">
         <v>224</v>
       </c>
       <c r="M42" s="176" t="s">
-        <v>224</v>
+        <v>245</v>
       </c>
       <c r="N42" s="176" t="s">
         <v>221</v>
@@ -9847,14 +9874,14 @@
       <c r="O42" s="176" t="s">
         <v>189</v>
       </c>
-      <c r="P42" s="179" t="s">
+      <c r="P42" s="183" t="s">
         <v>70</v>
       </c>
-      <c r="Q42" s="180"/>
-      <c r="R42" s="179" t="s">
+      <c r="Q42" s="184"/>
+      <c r="R42" s="183" t="s">
         <v>16</v>
       </c>
-      <c r="S42" s="180"/>
+      <c r="S42" s="184"/>
       <c r="T42" s="32" t="s">
         <v>69</v>
       </c>
@@ -9863,21 +9890,21 @@
       </c>
     </row>
     <row r="43" spans="1:22">
-      <c r="A43" s="177"/>
-      <c r="B43" s="177"/>
-      <c r="C43" s="177"/>
-      <c r="D43" s="177"/>
-      <c r="E43" s="182"/>
-      <c r="F43" s="182"/>
-      <c r="G43" s="177"/>
-      <c r="H43" s="177"/>
-      <c r="I43" s="177"/>
-      <c r="J43" s="182"/>
-      <c r="K43" s="182"/>
-      <c r="L43" s="183"/>
-      <c r="M43" s="177"/>
-      <c r="N43" s="177"/>
-      <c r="O43" s="183"/>
+      <c r="A43" s="178"/>
+      <c r="B43" s="178"/>
+      <c r="C43" s="178"/>
+      <c r="D43" s="178"/>
+      <c r="E43" s="181"/>
+      <c r="F43" s="181"/>
+      <c r="G43" s="178"/>
+      <c r="H43" s="178"/>
+      <c r="I43" s="178"/>
+      <c r="J43" s="181"/>
+      <c r="K43" s="181"/>
+      <c r="L43" s="177"/>
+      <c r="M43" s="178"/>
+      <c r="N43" s="178"/>
+      <c r="O43" s="177"/>
       <c r="P43" s="27" t="s">
         <v>74</v>
       </c>
@@ -9893,7 +9920,7 @@
       <c r="T43" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="U43" s="177"/>
+      <c r="U43" s="178"/>
     </row>
     <row r="44" spans="1:22">
       <c r="A44" s="7">
@@ -9920,7 +9947,7 @@
       <c r="J44" s="23"/>
       <c r="K44" s="23"/>
       <c r="L44" s="23" t="s">
-        <v>223</v>
+        <v>246</v>
       </c>
       <c r="M44" s="23" t="s">
         <v>223</v>
@@ -10046,8 +10073,12 @@
       </c>
       <c r="K47" s="73"/>
       <c r="L47" s="73"/>
-      <c r="M47" s="73"/>
-      <c r="N47" s="120"/>
+      <c r="M47" s="73" t="s">
+        <v>247</v>
+      </c>
+      <c r="N47" s="120" t="s">
+        <v>197</v>
+      </c>
       <c r="O47" s="24"/>
       <c r="P47" s="20"/>
       <c r="Q47" s="29"/>
@@ -10069,7 +10100,7 @@
         <v>107</v>
       </c>
       <c r="E48" s="25" t="s">
-        <v>161</v>
+        <v>248</v>
       </c>
       <c r="F48" s="25"/>
       <c r="G48" s="77"/>
@@ -10079,7 +10110,9 @@
       <c r="I48" s="25"/>
       <c r="J48" s="25"/>
       <c r="K48" s="25"/>
-      <c r="L48" s="25"/>
+      <c r="L48" s="25" t="s">
+        <v>250</v>
+      </c>
       <c r="M48" s="25"/>
       <c r="N48" s="120"/>
       <c r="O48" s="24"/>
@@ -10134,13 +10167,13 @@
       </c>
       <c r="C50" s="13"/>
       <c r="D50" s="25" t="s">
-        <v>161</v>
+        <v>248</v>
       </c>
       <c r="E50" s="25"/>
       <c r="F50" s="25"/>
       <c r="G50" s="77"/>
       <c r="H50" s="25" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="I50" s="25"/>
       <c r="J50" s="25"/>
@@ -10549,6 +10582,30 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
     <mergeCell ref="U42:U43"/>
     <mergeCell ref="G42:G43"/>
     <mergeCell ref="H42:H43"/>
@@ -10561,30 +10618,6 @@
     <mergeCell ref="O42:O43"/>
     <mergeCell ref="P42:Q42"/>
     <mergeCell ref="R42:S42"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="A34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:G30"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="4">
@@ -10777,10 +10810,10 @@
         <v>167</v>
       </c>
       <c r="B13" s="111"/>
-      <c r="C13" s="151" t="s">
+      <c r="C13" s="133" t="s">
         <v>168</v>
       </c>
-      <c r="D13" s="151"/>
+      <c r="D13" s="133"/>
       <c r="E13" s="1" t="s">
         <v>169</v>
       </c>
@@ -10790,10 +10823,10 @@
         <v>170</v>
       </c>
       <c r="B14" s="111"/>
-      <c r="C14" s="151" t="s">
+      <c r="C14" s="133" t="s">
         <v>171</v>
       </c>
-      <c r="D14" s="151"/>
+      <c r="D14" s="133"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="112" t="s">
@@ -10819,28 +10852,28 @@
       <c r="A16" s="6"/>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="146" t="s">
+      <c r="A17" s="169" t="s">
         <v>185</v>
       </c>
-      <c r="B17" s="146"/>
-      <c r="C17" s="146"/>
-      <c r="D17" s="146"/>
-      <c r="E17" s="146"/>
-      <c r="F17" s="146"/>
-      <c r="G17" s="146"/>
+      <c r="B17" s="169"/>
+      <c r="C17" s="169"/>
+      <c r="D17" s="169"/>
+      <c r="E17" s="169"/>
+      <c r="F17" s="169"/>
+      <c r="G17" s="169"/>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="140" t="s">
+      <c r="B18" s="163" t="s">
         <v>176</v>
       </c>
-      <c r="C18" s="141"/>
-      <c r="D18" s="141"/>
-      <c r="E18" s="141"/>
-      <c r="F18" s="141"/>
-      <c r="G18" s="142"/>
+      <c r="C18" s="164"/>
+      <c r="D18" s="164"/>
+      <c r="E18" s="164"/>
+      <c r="F18" s="164"/>
+      <c r="G18" s="165"/>
       <c r="H18" s="95"/>
       <c r="I18" s="95"/>
       <c r="K18" s="95"/>
@@ -10852,12 +10885,12 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="106"/>
-      <c r="B19" s="157"/>
-      <c r="C19" s="157"/>
-      <c r="D19" s="157"/>
-      <c r="E19" s="157"/>
-      <c r="F19" s="157"/>
-      <c r="G19" s="157"/>
+      <c r="B19" s="148"/>
+      <c r="C19" s="148"/>
+      <c r="D19" s="148"/>
+      <c r="E19" s="148"/>
+      <c r="F19" s="148"/>
+      <c r="G19" s="148"/>
       <c r="H19" s="102"/>
       <c r="I19" s="102"/>
       <c r="K19" s="102"/>
@@ -10869,12 +10902,12 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="107"/>
-      <c r="B20" s="158"/>
-      <c r="C20" s="158"/>
-      <c r="D20" s="158"/>
-      <c r="E20" s="158"/>
-      <c r="F20" s="158"/>
-      <c r="G20" s="158"/>
+      <c r="B20" s="150"/>
+      <c r="C20" s="150"/>
+      <c r="D20" s="150"/>
+      <c r="E20" s="150"/>
+      <c r="F20" s="150"/>
+      <c r="G20" s="150"/>
       <c r="H20" s="102"/>
       <c r="I20" s="102"/>
       <c r="K20" s="102"/>
@@ -10886,12 +10919,12 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="108"/>
-      <c r="B21" s="159"/>
-      <c r="C21" s="159"/>
-      <c r="D21" s="159"/>
-      <c r="E21" s="159"/>
-      <c r="F21" s="159"/>
-      <c r="G21" s="159"/>
+      <c r="B21" s="152"/>
+      <c r="C21" s="152"/>
+      <c r="D21" s="152"/>
+      <c r="E21" s="152"/>
+      <c r="F21" s="152"/>
+      <c r="G21" s="152"/>
       <c r="H21" s="102"/>
       <c r="I21" s="102"/>
       <c r="J21" s="95"/>
@@ -10907,29 +10940,29 @@
       <c r="J22" s="102"/>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="143" t="s">
+      <c r="A23" s="166" t="s">
         <v>186</v>
       </c>
-      <c r="B23" s="144"/>
-      <c r="C23" s="144"/>
-      <c r="D23" s="144"/>
-      <c r="E23" s="144"/>
-      <c r="F23" s="144"/>
-      <c r="G23" s="145"/>
+      <c r="B23" s="167"/>
+      <c r="C23" s="167"/>
+      <c r="D23" s="167"/>
+      <c r="E23" s="167"/>
+      <c r="F23" s="167"/>
+      <c r="G23" s="168"/>
       <c r="J23" s="102"/>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="164" t="s">
+      <c r="B24" s="144" t="s">
         <v>177</v>
       </c>
-      <c r="C24" s="164"/>
-      <c r="D24" s="164"/>
-      <c r="E24" s="164"/>
-      <c r="F24" s="164"/>
-      <c r="G24" s="164"/>
+      <c r="C24" s="144"/>
+      <c r="D24" s="144"/>
+      <c r="E24" s="144"/>
+      <c r="F24" s="144"/>
+      <c r="G24" s="144"/>
       <c r="H24" s="95"/>
       <c r="I24" s="95"/>
       <c r="J24" s="102"/>
@@ -10944,14 +10977,14 @@
       <c r="A25" s="106">
         <v>1</v>
       </c>
-      <c r="B25" s="165" t="s">
+      <c r="B25" s="145" t="s">
         <v>178</v>
       </c>
-      <c r="C25" s="165"/>
-      <c r="D25" s="165"/>
-      <c r="E25" s="165"/>
-      <c r="F25" s="165"/>
-      <c r="G25" s="165"/>
+      <c r="C25" s="145"/>
+      <c r="D25" s="145"/>
+      <c r="E25" s="145"/>
+      <c r="F25" s="145"/>
+      <c r="G25" s="145"/>
       <c r="H25" s="102"/>
       <c r="I25" s="102"/>
       <c r="K25" s="102"/>
@@ -10963,12 +10996,12 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="107"/>
-      <c r="B26" s="166"/>
-      <c r="C26" s="166"/>
-      <c r="D26" s="166"/>
-      <c r="E26" s="166"/>
-      <c r="F26" s="166"/>
-      <c r="G26" s="166"/>
+      <c r="B26" s="146"/>
+      <c r="C26" s="146"/>
+      <c r="D26" s="146"/>
+      <c r="E26" s="146"/>
+      <c r="F26" s="146"/>
+      <c r="G26" s="146"/>
       <c r="H26" s="102"/>
       <c r="I26" s="102"/>
       <c r="K26" s="102"/>
@@ -10980,12 +11013,12 @@
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="108"/>
-      <c r="B27" s="167"/>
-      <c r="C27" s="167"/>
-      <c r="D27" s="167"/>
-      <c r="E27" s="167"/>
-      <c r="F27" s="167"/>
-      <c r="G27" s="167"/>
+      <c r="B27" s="147"/>
+      <c r="C27" s="147"/>
+      <c r="D27" s="147"/>
+      <c r="E27" s="147"/>
+      <c r="F27" s="147"/>
+      <c r="G27" s="147"/>
       <c r="H27" s="102"/>
       <c r="I27" s="102"/>
       <c r="J27" s="95"/>
@@ -11014,29 +11047,29 @@
       <c r="O28"/>
     </row>
     <row r="29" spans="1:17">
-      <c r="A29" s="143" t="s">
+      <c r="A29" s="166" t="s">
         <v>187</v>
       </c>
-      <c r="B29" s="144"/>
-      <c r="C29" s="144"/>
-      <c r="D29" s="144"/>
-      <c r="E29" s="144"/>
-      <c r="F29" s="144"/>
-      <c r="G29" s="145"/>
+      <c r="B29" s="167"/>
+      <c r="C29" s="167"/>
+      <c r="D29" s="167"/>
+      <c r="E29" s="167"/>
+      <c r="F29" s="167"/>
+      <c r="G29" s="168"/>
       <c r="J29" s="102"/>
     </row>
     <row r="30" spans="1:17">
       <c r="A30" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B30" s="164" t="s">
+      <c r="B30" s="144" t="s">
         <v>179</v>
       </c>
-      <c r="C30" s="164"/>
-      <c r="D30" s="164"/>
-      <c r="E30" s="164"/>
-      <c r="F30" s="164"/>
-      <c r="G30" s="164"/>
+      <c r="C30" s="144"/>
+      <c r="D30" s="144"/>
+      <c r="E30" s="144"/>
+      <c r="F30" s="144"/>
+      <c r="G30" s="144"/>
       <c r="H30" s="95"/>
       <c r="I30" s="95"/>
       <c r="J30" s="102"/>
@@ -11049,12 +11082,12 @@
     </row>
     <row r="31" spans="1:17">
       <c r="A31" s="106"/>
-      <c r="B31" s="157"/>
-      <c r="C31" s="157"/>
-      <c r="D31" s="157"/>
-      <c r="E31" s="157"/>
-      <c r="F31" s="157"/>
-      <c r="G31" s="168"/>
+      <c r="B31" s="148"/>
+      <c r="C31" s="148"/>
+      <c r="D31" s="148"/>
+      <c r="E31" s="148"/>
+      <c r="F31" s="148"/>
+      <c r="G31" s="149"/>
       <c r="H31" s="102"/>
       <c r="I31" s="102"/>
       <c r="J31"/>
@@ -11067,12 +11100,12 @@
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="107"/>
-      <c r="B32" s="158"/>
-      <c r="C32" s="158"/>
-      <c r="D32" s="158"/>
-      <c r="E32" s="158"/>
-      <c r="F32" s="158"/>
-      <c r="G32" s="169"/>
+      <c r="B32" s="150"/>
+      <c r="C32" s="150"/>
+      <c r="D32" s="150"/>
+      <c r="E32" s="150"/>
+      <c r="F32" s="150"/>
+      <c r="G32" s="151"/>
       <c r="H32" s="102"/>
       <c r="I32" s="102"/>
       <c r="K32" s="102"/>
@@ -11084,12 +11117,12 @@
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="108"/>
-      <c r="B33" s="159"/>
-      <c r="C33" s="159"/>
-      <c r="D33" s="159"/>
-      <c r="E33" s="159"/>
-      <c r="F33" s="159"/>
-      <c r="G33" s="170"/>
+      <c r="B33" s="152"/>
+      <c r="C33" s="152"/>
+      <c r="D33" s="152"/>
+      <c r="E33" s="152"/>
+      <c r="F33" s="152"/>
+      <c r="G33" s="153"/>
       <c r="H33" s="102"/>
       <c r="I33" s="102"/>
       <c r="J33" s="95"/>
@@ -11142,64 +11175,64 @@
       <c r="P36" s="49"/>
     </row>
     <row r="37" spans="1:17" ht="15">
-      <c r="A37" s="181" t="s">
+      <c r="A37" s="180" t="s">
         <v>114</v>
       </c>
-      <c r="B37" s="181" t="s">
+      <c r="B37" s="180" t="s">
         <v>115</v>
       </c>
       <c r="C37" s="51" t="s">
         <v>116</v>
       </c>
-      <c r="D37" s="181" t="s">
+      <c r="D37" s="180" t="s">
         <v>98</v>
       </c>
-      <c r="E37" s="181" t="s">
+      <c r="E37" s="180" t="s">
         <v>155</v>
       </c>
-      <c r="F37" s="181" t="s">
+      <c r="F37" s="180" t="s">
         <v>170</v>
       </c>
-      <c r="G37" s="181" t="s">
+      <c r="G37" s="180" t="s">
         <v>135</v>
       </c>
-      <c r="H37" s="181" t="s">
+      <c r="H37" s="180" t="s">
         <v>112</v>
       </c>
-      <c r="I37" s="181" t="s">
+      <c r="I37" s="180" t="s">
         <v>229</v>
       </c>
       <c r="J37" s="176" t="s">
         <v>189</v>
       </c>
-      <c r="K37" s="186" t="s">
+      <c r="K37" s="185" t="s">
         <v>118</v>
       </c>
-      <c r="L37" s="187"/>
-      <c r="M37" s="188" t="s">
+      <c r="L37" s="186"/>
+      <c r="M37" s="187" t="s">
         <v>119</v>
       </c>
-      <c r="N37" s="187"/>
+      <c r="N37" s="186"/>
       <c r="O37" s="50" t="s">
         <v>120</v>
       </c>
-      <c r="P37" s="181" t="s">
+      <c r="P37" s="180" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="15">
-      <c r="A38" s="185"/>
-      <c r="B38" s="185"/>
+      <c r="A38" s="188"/>
+      <c r="B38" s="188"/>
       <c r="C38" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="D38" s="185"/>
-      <c r="E38" s="182"/>
-      <c r="F38" s="182"/>
-      <c r="G38" s="185"/>
-      <c r="H38" s="185"/>
-      <c r="I38" s="185"/>
-      <c r="J38" s="183"/>
+      <c r="D38" s="188"/>
+      <c r="E38" s="181"/>
+      <c r="F38" s="181"/>
+      <c r="G38" s="188"/>
+      <c r="H38" s="188"/>
+      <c r="I38" s="188"/>
+      <c r="J38" s="177"/>
       <c r="K38" s="53" t="s">
         <v>122</v>
       </c>
@@ -11215,7 +11248,7 @@
       <c r="O38" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="P38" s="185"/>
+      <c r="P38" s="188"/>
     </row>
     <row r="39" spans="1:17">
       <c r="A39" s="55">
@@ -11713,23 +11746,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="P37:P38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="J37:J38"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="A29:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
     <mergeCell ref="B27:G27"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
@@ -11742,6 +11758,23 @@
     <mergeCell ref="B24:G24"/>
     <mergeCell ref="B25:G25"/>
     <mergeCell ref="B26:G26"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="P37:P38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="J37:J38"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="M37:N37"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">
@@ -11951,10 +11984,10 @@
         <v>167</v>
       </c>
       <c r="B15" s="111"/>
-      <c r="C15" s="151" t="s">
+      <c r="C15" s="133" t="s">
         <v>168</v>
       </c>
-      <c r="D15" s="151"/>
+      <c r="D15" s="133"/>
       <c r="E15" s="1" t="s">
         <v>169</v>
       </c>
@@ -11964,10 +11997,10 @@
         <v>170</v>
       </c>
       <c r="B16" s="111"/>
-      <c r="C16" s="151" t="s">
+      <c r="C16" s="133" t="s">
         <v>171</v>
       </c>
-      <c r="D16" s="151"/>
+      <c r="D16" s="133"/>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="112" t="s">
@@ -11993,28 +12026,28 @@
       <c r="A18" s="6"/>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="146" t="s">
+      <c r="A19" s="169" t="s">
         <v>185</v>
       </c>
-      <c r="B19" s="146"/>
-      <c r="C19" s="146"/>
-      <c r="D19" s="146"/>
-      <c r="E19" s="146"/>
-      <c r="F19" s="146"/>
-      <c r="G19" s="146"/>
+      <c r="B19" s="169"/>
+      <c r="C19" s="169"/>
+      <c r="D19" s="169"/>
+      <c r="E19" s="169"/>
+      <c r="F19" s="169"/>
+      <c r="G19" s="169"/>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B20" s="140" t="s">
+      <c r="B20" s="163" t="s">
         <v>176</v>
       </c>
-      <c r="C20" s="141"/>
-      <c r="D20" s="141"/>
-      <c r="E20" s="141"/>
-      <c r="F20" s="141"/>
-      <c r="G20" s="142"/>
+      <c r="C20" s="164"/>
+      <c r="D20" s="164"/>
+      <c r="E20" s="164"/>
+      <c r="F20" s="164"/>
+      <c r="G20" s="165"/>
       <c r="H20" s="95"/>
       <c r="I20" s="95"/>
       <c r="K20" s="95"/>
@@ -12026,12 +12059,12 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="106"/>
-      <c r="B21" s="157"/>
-      <c r="C21" s="157"/>
-      <c r="D21" s="157"/>
-      <c r="E21" s="157"/>
-      <c r="F21" s="157"/>
-      <c r="G21" s="157"/>
+      <c r="B21" s="148"/>
+      <c r="C21" s="148"/>
+      <c r="D21" s="148"/>
+      <c r="E21" s="148"/>
+      <c r="F21" s="148"/>
+      <c r="G21" s="148"/>
       <c r="H21" s="102"/>
       <c r="I21" s="102"/>
       <c r="K21" s="102"/>
@@ -12043,12 +12076,12 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="107"/>
-      <c r="B22" s="158"/>
-      <c r="C22" s="158"/>
-      <c r="D22" s="158"/>
-      <c r="E22" s="158"/>
-      <c r="F22" s="158"/>
-      <c r="G22" s="158"/>
+      <c r="B22" s="150"/>
+      <c r="C22" s="150"/>
+      <c r="D22" s="150"/>
+      <c r="E22" s="150"/>
+      <c r="F22" s="150"/>
+      <c r="G22" s="150"/>
       <c r="H22" s="102"/>
       <c r="I22" s="102"/>
       <c r="K22" s="102"/>
@@ -12060,12 +12093,12 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="108"/>
-      <c r="B23" s="159"/>
-      <c r="C23" s="159"/>
-      <c r="D23" s="159"/>
-      <c r="E23" s="159"/>
-      <c r="F23" s="159"/>
-      <c r="G23" s="159"/>
+      <c r="B23" s="152"/>
+      <c r="C23" s="152"/>
+      <c r="D23" s="152"/>
+      <c r="E23" s="152"/>
+      <c r="F23" s="152"/>
+      <c r="G23" s="152"/>
       <c r="H23" s="102"/>
       <c r="I23" s="102"/>
       <c r="J23" s="95"/>
@@ -12081,29 +12114,29 @@
       <c r="J24" s="102"/>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" s="143" t="s">
+      <c r="A25" s="166" t="s">
         <v>186</v>
       </c>
-      <c r="B25" s="144"/>
-      <c r="C25" s="144"/>
-      <c r="D25" s="144"/>
-      <c r="E25" s="144"/>
-      <c r="F25" s="144"/>
-      <c r="G25" s="145"/>
+      <c r="B25" s="167"/>
+      <c r="C25" s="167"/>
+      <c r="D25" s="167"/>
+      <c r="E25" s="167"/>
+      <c r="F25" s="167"/>
+      <c r="G25" s="168"/>
       <c r="J25" s="102"/>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="164" t="s">
+      <c r="B26" s="144" t="s">
         <v>177</v>
       </c>
-      <c r="C26" s="164"/>
-      <c r="D26" s="164"/>
-      <c r="E26" s="164"/>
-      <c r="F26" s="164"/>
-      <c r="G26" s="164"/>
+      <c r="C26" s="144"/>
+      <c r="D26" s="144"/>
+      <c r="E26" s="144"/>
+      <c r="F26" s="144"/>
+      <c r="G26" s="144"/>
       <c r="H26" s="95"/>
       <c r="I26" s="95"/>
       <c r="J26" s="102"/>
@@ -12118,14 +12151,14 @@
       <c r="A27" s="106">
         <v>1</v>
       </c>
-      <c r="B27" s="165" t="s">
+      <c r="B27" s="145" t="s">
         <v>178</v>
       </c>
-      <c r="C27" s="165"/>
-      <c r="D27" s="165"/>
-      <c r="E27" s="165"/>
-      <c r="F27" s="165"/>
-      <c r="G27" s="165"/>
+      <c r="C27" s="145"/>
+      <c r="D27" s="145"/>
+      <c r="E27" s="145"/>
+      <c r="F27" s="145"/>
+      <c r="G27" s="145"/>
       <c r="H27" s="102"/>
       <c r="I27" s="102"/>
       <c r="K27" s="102"/>
@@ -12137,12 +12170,12 @@
     </row>
     <row r="28" spans="1:17">
       <c r="A28" s="107"/>
-      <c r="B28" s="166"/>
-      <c r="C28" s="166"/>
-      <c r="D28" s="166"/>
-      <c r="E28" s="166"/>
-      <c r="F28" s="166"/>
-      <c r="G28" s="166"/>
+      <c r="B28" s="146"/>
+      <c r="C28" s="146"/>
+      <c r="D28" s="146"/>
+      <c r="E28" s="146"/>
+      <c r="F28" s="146"/>
+      <c r="G28" s="146"/>
       <c r="H28" s="102"/>
       <c r="I28" s="102"/>
       <c r="K28" s="102"/>
@@ -12154,12 +12187,12 @@
     </row>
     <row r="29" spans="1:17">
       <c r="A29" s="108"/>
-      <c r="B29" s="167"/>
-      <c r="C29" s="167"/>
-      <c r="D29" s="167"/>
-      <c r="E29" s="167"/>
-      <c r="F29" s="167"/>
-      <c r="G29" s="167"/>
+      <c r="B29" s="147"/>
+      <c r="C29" s="147"/>
+      <c r="D29" s="147"/>
+      <c r="E29" s="147"/>
+      <c r="F29" s="147"/>
+      <c r="G29" s="147"/>
       <c r="H29" s="102"/>
       <c r="I29" s="102"/>
       <c r="J29" s="95"/>
@@ -12188,29 +12221,29 @@
       <c r="O30"/>
     </row>
     <row r="31" spans="1:17">
-      <c r="A31" s="143" t="s">
+      <c r="A31" s="166" t="s">
         <v>187</v>
       </c>
-      <c r="B31" s="144"/>
-      <c r="C31" s="144"/>
-      <c r="D31" s="144"/>
-      <c r="E31" s="144"/>
-      <c r="F31" s="144"/>
-      <c r="G31" s="145"/>
+      <c r="B31" s="167"/>
+      <c r="C31" s="167"/>
+      <c r="D31" s="167"/>
+      <c r="E31" s="167"/>
+      <c r="F31" s="167"/>
+      <c r="G31" s="168"/>
       <c r="J31" s="102"/>
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="164" t="s">
+      <c r="B32" s="144" t="s">
         <v>179</v>
       </c>
-      <c r="C32" s="164"/>
-      <c r="D32" s="164"/>
-      <c r="E32" s="164"/>
-      <c r="F32" s="164"/>
-      <c r="G32" s="164"/>
+      <c r="C32" s="144"/>
+      <c r="D32" s="144"/>
+      <c r="E32" s="144"/>
+      <c r="F32" s="144"/>
+      <c r="G32" s="144"/>
       <c r="H32" s="95"/>
       <c r="I32" s="95"/>
       <c r="J32" s="102"/>
@@ -12223,12 +12256,12 @@
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="106"/>
-      <c r="B33" s="157"/>
-      <c r="C33" s="157"/>
-      <c r="D33" s="157"/>
-      <c r="E33" s="157"/>
-      <c r="F33" s="157"/>
-      <c r="G33" s="168"/>
+      <c r="B33" s="148"/>
+      <c r="C33" s="148"/>
+      <c r="D33" s="148"/>
+      <c r="E33" s="148"/>
+      <c r="F33" s="148"/>
+      <c r="G33" s="149"/>
       <c r="H33" s="102"/>
       <c r="I33" s="102"/>
       <c r="J33"/>
@@ -12241,12 +12274,12 @@
     </row>
     <row r="34" spans="1:17">
       <c r="A34" s="107"/>
-      <c r="B34" s="158"/>
-      <c r="C34" s="158"/>
-      <c r="D34" s="158"/>
-      <c r="E34" s="158"/>
-      <c r="F34" s="158"/>
-      <c r="G34" s="169"/>
+      <c r="B34" s="150"/>
+      <c r="C34" s="150"/>
+      <c r="D34" s="150"/>
+      <c r="E34" s="150"/>
+      <c r="F34" s="150"/>
+      <c r="G34" s="151"/>
       <c r="H34" s="102"/>
       <c r="I34" s="102"/>
       <c r="K34" s="102"/>
@@ -12258,12 +12291,12 @@
     </row>
     <row r="35" spans="1:17">
       <c r="A35" s="108"/>
-      <c r="B35" s="159"/>
-      <c r="C35" s="159"/>
-      <c r="D35" s="159"/>
-      <c r="E35" s="159"/>
-      <c r="F35" s="159"/>
-      <c r="G35" s="170"/>
+      <c r="B35" s="152"/>
+      <c r="C35" s="152"/>
+      <c r="D35" s="152"/>
+      <c r="E35" s="152"/>
+      <c r="F35" s="152"/>
+      <c r="G35" s="153"/>
       <c r="H35" s="102"/>
       <c r="I35" s="102"/>
       <c r="J35" s="95"/>
@@ -12316,25 +12349,25 @@
       <c r="P38" s="49"/>
     </row>
     <row r="39" spans="1:17" ht="15">
-      <c r="A39" s="181" t="s">
+      <c r="A39" s="180" t="s">
         <v>114</v>
       </c>
-      <c r="B39" s="181" t="s">
+      <c r="B39" s="180" t="s">
         <v>115</v>
       </c>
       <c r="C39" s="51" t="s">
         <v>116</v>
       </c>
-      <c r="D39" s="181" t="s">
+      <c r="D39" s="180" t="s">
         <v>98</v>
       </c>
-      <c r="E39" s="181" t="s">
+      <c r="E39" s="180" t="s">
         <v>155</v>
       </c>
-      <c r="F39" s="181" t="s">
+      <c r="F39" s="180" t="s">
         <v>170</v>
       </c>
-      <c r="G39" s="181" t="s">
+      <c r="G39" s="180" t="s">
         <v>135</v>
       </c>
       <c r="H39" s="189" t="s">
@@ -12346,34 +12379,34 @@
       <c r="J39" s="176" t="s">
         <v>189</v>
       </c>
-      <c r="K39" s="186" t="s">
+      <c r="K39" s="185" t="s">
         <v>118</v>
       </c>
-      <c r="L39" s="187"/>
-      <c r="M39" s="188" t="s">
+      <c r="L39" s="186"/>
+      <c r="M39" s="187" t="s">
         <v>119</v>
       </c>
-      <c r="N39" s="187"/>
+      <c r="N39" s="186"/>
       <c r="O39" s="50" t="s">
         <v>120</v>
       </c>
-      <c r="P39" s="181" t="s">
+      <c r="P39" s="180" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="15">
-      <c r="A40" s="185"/>
-      <c r="B40" s="185"/>
+      <c r="A40" s="188"/>
+      <c r="B40" s="188"/>
       <c r="C40" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="D40" s="185"/>
-      <c r="E40" s="182"/>
-      <c r="F40" s="182"/>
-      <c r="G40" s="185"/>
-      <c r="H40" s="185"/>
-      <c r="I40" s="185"/>
-      <c r="J40" s="183"/>
+      <c r="D40" s="188"/>
+      <c r="E40" s="181"/>
+      <c r="F40" s="181"/>
+      <c r="G40" s="188"/>
+      <c r="H40" s="188"/>
+      <c r="I40" s="188"/>
+      <c r="J40" s="177"/>
       <c r="K40" s="53" t="s">
         <v>122</v>
       </c>
@@ -12389,7 +12422,7 @@
       <c r="O40" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="P40" s="185"/>
+      <c r="P40" s="188"/>
     </row>
     <row r="41" spans="1:17">
       <c r="A41" s="55">
@@ -12845,23 +12878,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="P39:P40"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="I39:I40"/>
-    <mergeCell ref="J39:J40"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
     <mergeCell ref="B29:G29"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C16:D16"/>
@@ -12874,6 +12890,23 @@
     <mergeCell ref="B26:G26"/>
     <mergeCell ref="B27:G27"/>
     <mergeCell ref="B28:G28"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="P39:P40"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="I39:I40"/>
+    <mergeCell ref="J39:J40"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="M39:N39"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations disablePrompts="1" count="3">

</xml_diff>

<commit_message>
3.1.7: Implement 'preferAlias' switch to input. It replaces field name to alias.
</commit_message>
<xml_diff>
--- a/meta/plainApi/BlancoApiPlainSample.xlsx
+++ b/meta/plainApi/BlancoApiPlainSample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorTs/meta/plainApi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F33DE8-C373-3D42-BAD6-6B9DBAE94B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92CAB16-A630-2E4E-AFFC-52F84E1992D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2440" yWindow="500" windowWidth="29440" windowHeight="20500" tabRatio="860" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2440" yWindow="500" windowWidth="29440" windowHeight="20500" tabRatio="860" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="process" sheetId="19" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="252">
   <si>
     <t>項目名</t>
     <rPh sb="0" eb="3">
@@ -2523,6 +2523,10 @@
   </si>
   <si>
     <t>simple_sample</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>first_field</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -3679,88 +3683,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="49" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3772,6 +3698,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3780,6 +3709,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3811,6 +3746,12 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3820,22 +3761,73 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3845,6 +3837,21 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3852,9 +3859,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4450,152 +4454,152 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="129" t="s">
+      <c r="A5" s="162" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="129"/>
-      <c r="C5" s="129"/>
-      <c r="D5" s="129"/>
-      <c r="E5" s="129"/>
+      <c r="B5" s="162"/>
+      <c r="C5" s="162"/>
+      <c r="D5" s="162"/>
+      <c r="E5" s="162"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="135" t="s">
+      <c r="A6" s="173" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="136"/>
-      <c r="C6" s="137"/>
-      <c r="D6" s="130" t="s">
+      <c r="B6" s="174"/>
+      <c r="C6" s="175"/>
+      <c r="D6" s="171" t="s">
         <v>233</v>
       </c>
-      <c r="E6" s="130"/>
+      <c r="E6" s="171"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="129" t="s">
+      <c r="A7" s="162" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="129"/>
-      <c r="C7" s="129"/>
-      <c r="D7" s="130" t="s">
+      <c r="B7" s="162"/>
+      <c r="C7" s="162"/>
+      <c r="D7" s="171" t="s">
         <v>159</v>
       </c>
-      <c r="E7" s="130"/>
+      <c r="E7" s="171"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="129" t="s">
+      <c r="A8" s="162" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="129"/>
-      <c r="C8" s="129"/>
-      <c r="D8" s="130" t="s">
+      <c r="B8" s="162"/>
+      <c r="C8" s="162"/>
+      <c r="D8" s="171" t="s">
         <v>233</v>
       </c>
-      <c r="E8" s="130"/>
+      <c r="E8" s="171"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="129" t="s">
+      <c r="A9" s="162" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="129"/>
-      <c r="C9" s="129"/>
-      <c r="D9" s="130" t="s">
+      <c r="B9" s="162"/>
+      <c r="C9" s="162"/>
+      <c r="D9" s="171" t="s">
         <v>244</v>
       </c>
-      <c r="E9" s="130"/>
+      <c r="E9" s="171"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="129" t="s">
+      <c r="A10" s="162" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="129"/>
-      <c r="C10" s="129"/>
-      <c r="D10" s="130"/>
-      <c r="E10" s="130"/>
+      <c r="B10" s="162"/>
+      <c r="C10" s="162"/>
+      <c r="D10" s="171"/>
+      <c r="E10" s="171"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="129" t="s">
+      <c r="A11" s="162" t="s">
         <v>97</v>
       </c>
-      <c r="B11" s="129"/>
-      <c r="C11" s="129"/>
-      <c r="D11" s="130" t="s">
+      <c r="B11" s="162"/>
+      <c r="C11" s="162"/>
+      <c r="D11" s="171" t="s">
         <v>156</v>
       </c>
-      <c r="E11" s="130"/>
+      <c r="E11" s="171"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="131" t="s">
+      <c r="A12" s="134" t="s">
         <v>167</v>
       </c>
-      <c r="B12" s="131"/>
-      <c r="C12" s="131"/>
-      <c r="D12" s="133" t="s">
+      <c r="B12" s="134"/>
+      <c r="C12" s="134"/>
+      <c r="D12" s="151" t="s">
         <v>168</v>
       </c>
-      <c r="E12" s="133"/>
+      <c r="E12" s="151"/>
       <c r="F12" s="1" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="131" t="s">
+      <c r="A13" s="134" t="s">
         <v>170</v>
       </c>
-      <c r="B13" s="131"/>
-      <c r="C13" s="131"/>
-      <c r="D13" s="132" t="s">
+      <c r="B13" s="134"/>
+      <c r="C13" s="134"/>
+      <c r="D13" s="150" t="s">
         <v>208</v>
       </c>
-      <c r="E13" s="133"/>
+      <c r="E13" s="151"/>
     </row>
     <row r="14" spans="1:6" ht="55" customHeight="1">
-      <c r="A14" s="131" t="s">
+      <c r="A14" s="134" t="s">
         <v>207</v>
       </c>
-      <c r="B14" s="131"/>
-      <c r="C14" s="131"/>
-      <c r="D14" s="134" t="s">
+      <c r="B14" s="134"/>
+      <c r="C14" s="134"/>
+      <c r="D14" s="172" t="s">
         <v>232</v>
       </c>
-      <c r="E14" s="133"/>
+      <c r="E14" s="151"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="131" t="s">
+      <c r="A15" s="134" t="s">
         <v>191</v>
       </c>
-      <c r="B15" s="131"/>
-      <c r="C15" s="131"/>
-      <c r="D15" s="132"/>
-      <c r="E15" s="133"/>
+      <c r="B15" s="134"/>
+      <c r="C15" s="134"/>
+      <c r="D15" s="150"/>
+      <c r="E15" s="151"/>
       <c r="F15" s="1" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="131" t="s">
+      <c r="A16" s="134" t="s">
         <v>192</v>
       </c>
-      <c r="B16" s="131"/>
-      <c r="C16" s="131"/>
-      <c r="D16" s="132"/>
-      <c r="E16" s="133"/>
+      <c r="B16" s="134"/>
+      <c r="C16" s="134"/>
+      <c r="D16" s="150"/>
+      <c r="E16" s="151"/>
       <c r="F16" s="1" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="173" t="s">
+      <c r="A17" s="152" t="s">
         <v>138</v>
       </c>
-      <c r="B17" s="174"/>
-      <c r="C17" s="175"/>
+      <c r="B17" s="153"/>
+      <c r="C17" s="154"/>
       <c r="D17" s="104"/>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="160" t="s">
+      <c r="A18" s="135" t="s">
         <v>172</v>
       </c>
-      <c r="B18" s="161"/>
-      <c r="C18" s="162"/>
+      <c r="B18" s="136"/>
+      <c r="C18" s="137"/>
       <c r="D18" s="90" t="s">
         <v>136</v>
       </c>
@@ -4615,15 +4619,15 @@
       <c r="B19" s="6"/>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="170" t="s">
+      <c r="A20" s="147" t="s">
         <v>181</v>
       </c>
-      <c r="B20" s="171"/>
-      <c r="C20" s="171"/>
-      <c r="D20" s="171"/>
-      <c r="E20" s="171"/>
-      <c r="F20" s="171"/>
-      <c r="G20" s="172"/>
+      <c r="B20" s="148"/>
+      <c r="C20" s="148"/>
+      <c r="D20" s="148"/>
+      <c r="E20" s="148"/>
+      <c r="F20" s="148"/>
+      <c r="G20" s="149"/>
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="91" t="s">
@@ -4667,28 +4671,28 @@
       <c r="C24"/>
     </row>
     <row r="25" spans="1:15">
-      <c r="A25" s="169" t="s">
+      <c r="A25" s="146" t="s">
         <v>182</v>
       </c>
-      <c r="B25" s="169"/>
-      <c r="C25" s="169"/>
-      <c r="D25" s="169"/>
-      <c r="E25" s="169"/>
-      <c r="F25" s="169"/>
-      <c r="G25" s="169"/>
+      <c r="B25" s="146"/>
+      <c r="C25" s="146"/>
+      <c r="D25" s="146"/>
+      <c r="E25" s="146"/>
+      <c r="F25" s="146"/>
+      <c r="G25" s="146"/>
     </row>
     <row r="26" spans="1:15">
       <c r="A26" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="163" t="s">
+      <c r="B26" s="140" t="s">
         <v>176</v>
       </c>
-      <c r="C26" s="164"/>
-      <c r="D26" s="164"/>
-      <c r="E26" s="164"/>
-      <c r="F26" s="164"/>
-      <c r="G26" s="165"/>
+      <c r="C26" s="141"/>
+      <c r="D26" s="141"/>
+      <c r="E26" s="141"/>
+      <c r="F26" s="141"/>
+      <c r="G26" s="142"/>
       <c r="H26" s="95"/>
       <c r="I26" s="95"/>
       <c r="J26" s="95"/>
@@ -4699,12 +4703,12 @@
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="106"/>
-      <c r="B27" s="148"/>
-      <c r="C27" s="148"/>
-      <c r="D27" s="148"/>
-      <c r="E27" s="148"/>
-      <c r="F27" s="148"/>
-      <c r="G27" s="148"/>
+      <c r="B27" s="157"/>
+      <c r="C27" s="157"/>
+      <c r="D27" s="157"/>
+      <c r="E27" s="157"/>
+      <c r="F27" s="157"/>
+      <c r="G27" s="157"/>
       <c r="H27" s="102"/>
       <c r="I27" s="102"/>
       <c r="J27" s="102"/>
@@ -4715,12 +4719,12 @@
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="107"/>
-      <c r="B28" s="150"/>
-      <c r="C28" s="150"/>
-      <c r="D28" s="150"/>
-      <c r="E28" s="150"/>
-      <c r="F28" s="150"/>
-      <c r="G28" s="150"/>
+      <c r="B28" s="158"/>
+      <c r="C28" s="158"/>
+      <c r="D28" s="158"/>
+      <c r="E28" s="158"/>
+      <c r="F28" s="158"/>
+      <c r="G28" s="158"/>
       <c r="H28" s="102"/>
       <c r="I28" s="102"/>
       <c r="J28" s="102"/>
@@ -4731,12 +4735,12 @@
     </row>
     <row r="29" spans="1:15">
       <c r="A29" s="108"/>
-      <c r="B29" s="152"/>
-      <c r="C29" s="152"/>
-      <c r="D29" s="152"/>
-      <c r="E29" s="152"/>
-      <c r="F29" s="152"/>
-      <c r="G29" s="152"/>
+      <c r="B29" s="159"/>
+      <c r="C29" s="159"/>
+      <c r="D29" s="159"/>
+      <c r="E29" s="159"/>
+      <c r="F29" s="159"/>
+      <c r="G29" s="159"/>
       <c r="H29" s="102"/>
       <c r="I29" s="102"/>
       <c r="J29" s="102"/>
@@ -4749,28 +4753,28 @@
       <c r="C30"/>
     </row>
     <row r="31" spans="1:15">
-      <c r="A31" s="166" t="s">
+      <c r="A31" s="143" t="s">
         <v>183</v>
       </c>
-      <c r="B31" s="167"/>
-      <c r="C31" s="167"/>
-      <c r="D31" s="167"/>
-      <c r="E31" s="167"/>
-      <c r="F31" s="167"/>
-      <c r="G31" s="168"/>
+      <c r="B31" s="144"/>
+      <c r="C31" s="144"/>
+      <c r="D31" s="144"/>
+      <c r="E31" s="144"/>
+      <c r="F31" s="144"/>
+      <c r="G31" s="145"/>
     </row>
     <row r="32" spans="1:15">
       <c r="A32" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="144" t="s">
+      <c r="B32" s="164" t="s">
         <v>177</v>
       </c>
-      <c r="C32" s="144"/>
-      <c r="D32" s="144"/>
-      <c r="E32" s="144"/>
-      <c r="F32" s="144"/>
-      <c r="G32" s="144"/>
+      <c r="C32" s="164"/>
+      <c r="D32" s="164"/>
+      <c r="E32" s="164"/>
+      <c r="F32" s="164"/>
+      <c r="G32" s="164"/>
       <c r="H32" s="95"/>
       <c r="I32" s="95"/>
       <c r="J32" s="95"/>
@@ -4783,14 +4787,14 @@
       <c r="A33" s="106">
         <v>1</v>
       </c>
-      <c r="B33" s="145" t="s">
+      <c r="B33" s="165" t="s">
         <v>178</v>
       </c>
-      <c r="C33" s="145"/>
-      <c r="D33" s="145"/>
-      <c r="E33" s="145"/>
-      <c r="F33" s="145"/>
-      <c r="G33" s="145"/>
+      <c r="C33" s="165"/>
+      <c r="D33" s="165"/>
+      <c r="E33" s="165"/>
+      <c r="F33" s="165"/>
+      <c r="G33" s="165"/>
       <c r="H33" s="102"/>
       <c r="I33" s="102"/>
       <c r="J33" s="102"/>
@@ -4801,12 +4805,12 @@
     </row>
     <row r="34" spans="1:15">
       <c r="A34" s="107"/>
-      <c r="B34" s="146"/>
-      <c r="C34" s="146"/>
-      <c r="D34" s="146"/>
-      <c r="E34" s="146"/>
-      <c r="F34" s="146"/>
-      <c r="G34" s="146"/>
+      <c r="B34" s="166"/>
+      <c r="C34" s="166"/>
+      <c r="D34" s="166"/>
+      <c r="E34" s="166"/>
+      <c r="F34" s="166"/>
+      <c r="G34" s="166"/>
       <c r="H34" s="102"/>
       <c r="I34" s="102"/>
       <c r="J34" s="102"/>
@@ -4817,12 +4821,12 @@
     </row>
     <row r="35" spans="1:15">
       <c r="A35" s="108"/>
-      <c r="B35" s="147"/>
-      <c r="C35" s="147"/>
-      <c r="D35" s="147"/>
-      <c r="E35" s="147"/>
-      <c r="F35" s="147"/>
-      <c r="G35" s="147"/>
+      <c r="B35" s="167"/>
+      <c r="C35" s="167"/>
+      <c r="D35" s="167"/>
+      <c r="E35" s="167"/>
+      <c r="F35" s="167"/>
+      <c r="G35" s="167"/>
       <c r="H35" s="102"/>
       <c r="I35" s="102"/>
       <c r="J35" s="102"/>
@@ -4847,28 +4851,28 @@
       <c r="M36"/>
     </row>
     <row r="37" spans="1:15">
-      <c r="A37" s="166" t="s">
+      <c r="A37" s="143" t="s">
         <v>184</v>
       </c>
-      <c r="B37" s="167"/>
-      <c r="C37" s="167"/>
-      <c r="D37" s="167"/>
-      <c r="E37" s="167"/>
-      <c r="F37" s="167"/>
-      <c r="G37" s="168"/>
+      <c r="B37" s="144"/>
+      <c r="C37" s="144"/>
+      <c r="D37" s="144"/>
+      <c r="E37" s="144"/>
+      <c r="F37" s="144"/>
+      <c r="G37" s="145"/>
     </row>
     <row r="38" spans="1:15">
       <c r="A38" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B38" s="144" t="s">
+      <c r="B38" s="164" t="s">
         <v>179</v>
       </c>
-      <c r="C38" s="144"/>
-      <c r="D38" s="144"/>
-      <c r="E38" s="144"/>
-      <c r="F38" s="144"/>
-      <c r="G38" s="144"/>
+      <c r="C38" s="164"/>
+      <c r="D38" s="164"/>
+      <c r="E38" s="164"/>
+      <c r="F38" s="164"/>
+      <c r="G38" s="164"/>
       <c r="H38" s="95"/>
       <c r="I38" s="95"/>
       <c r="J38" s="95"/>
@@ -4879,12 +4883,12 @@
     </row>
     <row r="39" spans="1:15">
       <c r="A39" s="106"/>
-      <c r="B39" s="148"/>
-      <c r="C39" s="148"/>
-      <c r="D39" s="148"/>
-      <c r="E39" s="148"/>
-      <c r="F39" s="148"/>
-      <c r="G39" s="149"/>
+      <c r="B39" s="157"/>
+      <c r="C39" s="157"/>
+      <c r="D39" s="157"/>
+      <c r="E39" s="157"/>
+      <c r="F39" s="157"/>
+      <c r="G39" s="168"/>
       <c r="H39" s="102"/>
       <c r="I39" s="102"/>
       <c r="J39" s="102"/>
@@ -4895,12 +4899,12 @@
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="107"/>
-      <c r="B40" s="150"/>
-      <c r="C40" s="150"/>
-      <c r="D40" s="150"/>
-      <c r="E40" s="150"/>
-      <c r="F40" s="150"/>
-      <c r="G40" s="151"/>
+      <c r="B40" s="158"/>
+      <c r="C40" s="158"/>
+      <c r="D40" s="158"/>
+      <c r="E40" s="158"/>
+      <c r="F40" s="158"/>
+      <c r="G40" s="169"/>
       <c r="H40" s="102"/>
       <c r="I40" s="102"/>
       <c r="J40" s="102"/>
@@ -4911,12 +4915,12 @@
     </row>
     <row r="41" spans="1:15">
       <c r="A41" s="108"/>
-      <c r="B41" s="152"/>
-      <c r="C41" s="152"/>
-      <c r="D41" s="152"/>
-      <c r="E41" s="152"/>
-      <c r="F41" s="152"/>
-      <c r="G41" s="153"/>
+      <c r="B41" s="159"/>
+      <c r="C41" s="159"/>
+      <c r="D41" s="159"/>
+      <c r="E41" s="159"/>
+      <c r="F41" s="159"/>
+      <c r="G41" s="170"/>
       <c r="H41" s="102"/>
       <c r="I41" s="102"/>
       <c r="J41" s="102"/>
@@ -4942,15 +4946,15 @@
       <c r="O42"/>
     </row>
     <row r="43" spans="1:15">
-      <c r="A43" s="169" t="s">
+      <c r="A43" s="146" t="s">
         <v>204</v>
       </c>
-      <c r="B43" s="169"/>
-      <c r="C43" s="169"/>
-      <c r="D43" s="169"/>
-      <c r="E43" s="169"/>
-      <c r="F43" s="169"/>
-      <c r="G43" s="169"/>
+      <c r="B43" s="146"/>
+      <c r="C43" s="146"/>
+      <c r="D43" s="146"/>
+      <c r="E43" s="146"/>
+      <c r="F43" s="146"/>
+      <c r="G43" s="146"/>
     </row>
     <row r="44" spans="1:15">
       <c r="A44" s="105" t="s">
@@ -5066,231 +5070,289 @@
       <c r="F49" s="5"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="157" t="s">
+      <c r="A50" s="131" t="s">
         <v>64</v>
       </c>
-      <c r="B50" s="159"/>
-      <c r="C50" s="157" t="s">
+      <c r="B50" s="133"/>
+      <c r="C50" s="131" t="s">
         <v>65</v>
       </c>
-      <c r="D50" s="158"/>
-      <c r="E50" s="159"/>
+      <c r="D50" s="132"/>
+      <c r="E50" s="133"/>
       <c r="F50" s="27" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="154"/>
-      <c r="B51" s="156"/>
-      <c r="C51" s="154"/>
-      <c r="D51" s="155"/>
-      <c r="E51" s="156"/>
+      <c r="A51" s="138"/>
+      <c r="B51" s="139"/>
+      <c r="C51" s="138"/>
+      <c r="D51" s="160"/>
+      <c r="E51" s="139"/>
       <c r="F51" s="43"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="138"/>
-      <c r="B52" s="140"/>
-      <c r="C52" s="138"/>
-      <c r="D52" s="139"/>
-      <c r="E52" s="140"/>
+      <c r="A52" s="129"/>
+      <c r="B52" s="130"/>
+      <c r="C52" s="129"/>
+      <c r="D52" s="161"/>
+      <c r="E52" s="130"/>
       <c r="F52" s="43"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="138"/>
-      <c r="B53" s="140"/>
-      <c r="C53" s="138"/>
-      <c r="D53" s="139"/>
-      <c r="E53" s="140"/>
+      <c r="A53" s="129"/>
+      <c r="B53" s="130"/>
+      <c r="C53" s="129"/>
+      <c r="D53" s="161"/>
+      <c r="E53" s="130"/>
       <c r="F53" s="43"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="138"/>
-      <c r="B54" s="140"/>
-      <c r="C54" s="138"/>
-      <c r="D54" s="139"/>
-      <c r="E54" s="140"/>
+      <c r="A54" s="129"/>
+      <c r="B54" s="130"/>
+      <c r="C54" s="129"/>
+      <c r="D54" s="161"/>
+      <c r="E54" s="130"/>
       <c r="F54" s="43"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="138"/>
-      <c r="B55" s="140"/>
-      <c r="C55" s="138"/>
-      <c r="D55" s="139"/>
-      <c r="E55" s="140"/>
+      <c r="A55" s="129"/>
+      <c r="B55" s="130"/>
+      <c r="C55" s="129"/>
+      <c r="D55" s="161"/>
+      <c r="E55" s="130"/>
       <c r="F55" s="43"/>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="138"/>
-      <c r="B56" s="140"/>
-      <c r="C56" s="138"/>
-      <c r="D56" s="139"/>
-      <c r="E56" s="140"/>
+      <c r="A56" s="129"/>
+      <c r="B56" s="130"/>
+      <c r="C56" s="129"/>
+      <c r="D56" s="161"/>
+      <c r="E56" s="130"/>
       <c r="F56" s="43"/>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="138"/>
-      <c r="B57" s="140"/>
-      <c r="C57" s="138"/>
-      <c r="D57" s="139"/>
-      <c r="E57" s="140"/>
+      <c r="A57" s="129"/>
+      <c r="B57" s="130"/>
+      <c r="C57" s="129"/>
+      <c r="D57" s="161"/>
+      <c r="E57" s="130"/>
       <c r="F57" s="43"/>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="138"/>
-      <c r="B58" s="140"/>
-      <c r="C58" s="138"/>
-      <c r="D58" s="139"/>
-      <c r="E58" s="140"/>
+      <c r="A58" s="129"/>
+      <c r="B58" s="130"/>
+      <c r="C58" s="129"/>
+      <c r="D58" s="161"/>
+      <c r="E58" s="130"/>
       <c r="F58" s="43"/>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="138"/>
-      <c r="B59" s="140"/>
-      <c r="C59" s="138"/>
-      <c r="D59" s="139"/>
-      <c r="E59" s="140"/>
+      <c r="A59" s="129"/>
+      <c r="B59" s="130"/>
+      <c r="C59" s="129"/>
+      <c r="D59" s="161"/>
+      <c r="E59" s="130"/>
       <c r="F59" s="43"/>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="138"/>
-      <c r="B60" s="140"/>
-      <c r="C60" s="138"/>
-      <c r="D60" s="139"/>
-      <c r="E60" s="140"/>
+      <c r="A60" s="129"/>
+      <c r="B60" s="130"/>
+      <c r="C60" s="129"/>
+      <c r="D60" s="161"/>
+      <c r="E60" s="130"/>
       <c r="F60" s="43"/>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="138"/>
-      <c r="B61" s="140"/>
-      <c r="C61" s="138"/>
-      <c r="D61" s="139"/>
-      <c r="E61" s="140"/>
+      <c r="A61" s="129"/>
+      <c r="B61" s="130"/>
+      <c r="C61" s="129"/>
+      <c r="D61" s="161"/>
+      <c r="E61" s="130"/>
       <c r="F61" s="43"/>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="138"/>
-      <c r="B62" s="140"/>
-      <c r="C62" s="138"/>
-      <c r="D62" s="139"/>
-      <c r="E62" s="140"/>
+      <c r="A62" s="129"/>
+      <c r="B62" s="130"/>
+      <c r="C62" s="129"/>
+      <c r="D62" s="161"/>
+      <c r="E62" s="130"/>
       <c r="F62" s="43"/>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="138"/>
-      <c r="B63" s="140"/>
-      <c r="C63" s="138"/>
-      <c r="D63" s="139"/>
-      <c r="E63" s="140"/>
+      <c r="A63" s="129"/>
+      <c r="B63" s="130"/>
+      <c r="C63" s="129"/>
+      <c r="D63" s="161"/>
+      <c r="E63" s="130"/>
       <c r="F63" s="43"/>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="138"/>
-      <c r="B64" s="140"/>
-      <c r="C64" s="138"/>
-      <c r="D64" s="139"/>
-      <c r="E64" s="140"/>
+      <c r="A64" s="129"/>
+      <c r="B64" s="130"/>
+      <c r="C64" s="129"/>
+      <c r="D64" s="161"/>
+      <c r="E64" s="130"/>
       <c r="F64" s="43"/>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="138"/>
-      <c r="B65" s="140"/>
-      <c r="C65" s="138"/>
-      <c r="D65" s="139"/>
-      <c r="E65" s="140"/>
+      <c r="A65" s="129"/>
+      <c r="B65" s="130"/>
+      <c r="C65" s="129"/>
+      <c r="D65" s="161"/>
+      <c r="E65" s="130"/>
       <c r="F65" s="43"/>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="138"/>
-      <c r="B66" s="140"/>
-      <c r="C66" s="138"/>
-      <c r="D66" s="139"/>
-      <c r="E66" s="140"/>
+      <c r="A66" s="129"/>
+      <c r="B66" s="130"/>
+      <c r="C66" s="129"/>
+      <c r="D66" s="161"/>
+      <c r="E66" s="130"/>
       <c r="F66" s="43"/>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="138"/>
-      <c r="B67" s="140"/>
-      <c r="C67" s="138"/>
-      <c r="D67" s="139"/>
-      <c r="E67" s="140"/>
+      <c r="A67" s="129"/>
+      <c r="B67" s="130"/>
+      <c r="C67" s="129"/>
+      <c r="D67" s="161"/>
+      <c r="E67" s="130"/>
       <c r="F67" s="43"/>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="138"/>
-      <c r="B68" s="140"/>
-      <c r="C68" s="138"/>
-      <c r="D68" s="139"/>
-      <c r="E68" s="140"/>
+      <c r="A68" s="129"/>
+      <c r="B68" s="130"/>
+      <c r="C68" s="129"/>
+      <c r="D68" s="161"/>
+      <c r="E68" s="130"/>
       <c r="F68" s="43"/>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="138"/>
-      <c r="B69" s="140"/>
-      <c r="C69" s="138"/>
-      <c r="D69" s="139"/>
-      <c r="E69" s="140"/>
+      <c r="A69" s="129"/>
+      <c r="B69" s="130"/>
+      <c r="C69" s="129"/>
+      <c r="D69" s="161"/>
+      <c r="E69" s="130"/>
       <c r="F69" s="43"/>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="138"/>
-      <c r="B70" s="140"/>
-      <c r="C70" s="138"/>
-      <c r="D70" s="139"/>
-      <c r="E70" s="140"/>
+      <c r="A70" s="129"/>
+      <c r="B70" s="130"/>
+      <c r="C70" s="129"/>
+      <c r="D70" s="161"/>
+      <c r="E70" s="130"/>
       <c r="F70" s="43"/>
     </row>
     <row r="71" spans="1:6">
-      <c r="A71" s="138"/>
-      <c r="B71" s="140"/>
-      <c r="C71" s="138"/>
-      <c r="D71" s="139"/>
-      <c r="E71" s="140"/>
+      <c r="A71" s="129"/>
+      <c r="B71" s="130"/>
+      <c r="C71" s="129"/>
+      <c r="D71" s="161"/>
+      <c r="E71" s="130"/>
       <c r="F71" s="43"/>
     </row>
     <row r="72" spans="1:6">
-      <c r="A72" s="138"/>
-      <c r="B72" s="140"/>
-      <c r="C72" s="138"/>
-      <c r="D72" s="139"/>
-      <c r="E72" s="140"/>
+      <c r="A72" s="129"/>
+      <c r="B72" s="130"/>
+      <c r="C72" s="129"/>
+      <c r="D72" s="161"/>
+      <c r="E72" s="130"/>
       <c r="F72" s="43"/>
     </row>
     <row r="73" spans="1:6">
-      <c r="A73" s="138"/>
-      <c r="B73" s="140"/>
-      <c r="C73" s="138"/>
-      <c r="D73" s="139"/>
-      <c r="E73" s="140"/>
+      <c r="A73" s="129"/>
+      <c r="B73" s="130"/>
+      <c r="C73" s="129"/>
+      <c r="D73" s="161"/>
+      <c r="E73" s="130"/>
       <c r="F73" s="43"/>
     </row>
     <row r="74" spans="1:6">
-      <c r="A74" s="138"/>
-      <c r="B74" s="140"/>
-      <c r="C74" s="138"/>
-      <c r="D74" s="139"/>
-      <c r="E74" s="140"/>
+      <c r="A74" s="129"/>
+      <c r="B74" s="130"/>
+      <c r="C74" s="129"/>
+      <c r="D74" s="161"/>
+      <c r="E74" s="130"/>
       <c r="F74" s="43"/>
     </row>
     <row r="75" spans="1:6">
-      <c r="A75" s="141"/>
-      <c r="B75" s="143"/>
-      <c r="C75" s="141"/>
-      <c r="D75" s="142"/>
-      <c r="E75" s="143"/>
+      <c r="A75" s="155"/>
+      <c r="B75" s="156"/>
+      <c r="C75" s="155"/>
+      <c r="D75" s="163"/>
+      <c r="E75" s="156"/>
       <c r="F75" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="94">
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C75:E75"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C73:E73"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
     <mergeCell ref="C50:E50"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A18:C18"/>
@@ -5307,74 +5369,16 @@
     <mergeCell ref="A43:G43"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="D13:E13"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C73:E73"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="C75:E75"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="2">
@@ -5575,10 +5579,10 @@
         <v>167</v>
       </c>
       <c r="B16" s="111"/>
-      <c r="C16" s="133" t="s">
+      <c r="C16" s="151" t="s">
         <v>168</v>
       </c>
-      <c r="D16" s="133"/>
+      <c r="D16" s="151"/>
       <c r="E16" s="1" t="s">
         <v>169</v>
       </c>
@@ -5588,20 +5592,20 @@
         <v>170</v>
       </c>
       <c r="B17" s="111"/>
-      <c r="C17" s="133" t="s">
+      <c r="C17" s="151" t="s">
         <v>171</v>
       </c>
-      <c r="D17" s="133"/>
+      <c r="D17" s="151"/>
     </row>
     <row r="18" spans="1:22">
       <c r="A18" s="111" t="s">
         <v>207</v>
       </c>
       <c r="B18" s="111"/>
-      <c r="C18" s="132" t="s">
+      <c r="C18" s="150" t="s">
         <v>209</v>
       </c>
-      <c r="D18" s="133"/>
+      <c r="D18" s="151"/>
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="112" t="s">
@@ -5659,28 +5663,28 @@
       <c r="A21" s="6"/>
     </row>
     <row r="22" spans="1:22">
-      <c r="A22" s="169" t="s">
+      <c r="A22" s="146" t="s">
         <v>185</v>
       </c>
-      <c r="B22" s="169"/>
-      <c r="C22" s="169"/>
-      <c r="D22" s="169"/>
-      <c r="E22" s="169"/>
-      <c r="F22" s="169"/>
-      <c r="G22" s="169"/>
+      <c r="B22" s="146"/>
+      <c r="C22" s="146"/>
+      <c r="D22" s="146"/>
+      <c r="E22" s="146"/>
+      <c r="F22" s="146"/>
+      <c r="G22" s="146"/>
     </row>
     <row r="23" spans="1:22">
       <c r="A23" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="163" t="s">
+      <c r="B23" s="140" t="s">
         <v>176</v>
       </c>
-      <c r="C23" s="164"/>
-      <c r="D23" s="164"/>
-      <c r="E23" s="164"/>
-      <c r="F23" s="164"/>
-      <c r="G23" s="165"/>
+      <c r="C23" s="141"/>
+      <c r="D23" s="141"/>
+      <c r="E23" s="141"/>
+      <c r="F23" s="141"/>
+      <c r="G23" s="142"/>
       <c r="H23" s="95"/>
       <c r="I23" s="95"/>
       <c r="J23" s="95"/>
@@ -5698,12 +5702,12 @@
     </row>
     <row r="24" spans="1:22">
       <c r="A24" s="106"/>
-      <c r="B24" s="148"/>
-      <c r="C24" s="148"/>
-      <c r="D24" s="148"/>
-      <c r="E24" s="148"/>
-      <c r="F24" s="148"/>
-      <c r="G24" s="148"/>
+      <c r="B24" s="157"/>
+      <c r="C24" s="157"/>
+      <c r="D24" s="157"/>
+      <c r="E24" s="157"/>
+      <c r="F24" s="157"/>
+      <c r="G24" s="157"/>
       <c r="H24" s="102"/>
       <c r="I24" s="102"/>
       <c r="J24" s="102"/>
@@ -5721,12 +5725,12 @@
     </row>
     <row r="25" spans="1:22">
       <c r="A25" s="107"/>
-      <c r="B25" s="150"/>
-      <c r="C25" s="150"/>
-      <c r="D25" s="150"/>
-      <c r="E25" s="150"/>
-      <c r="F25" s="150"/>
-      <c r="G25" s="150"/>
+      <c r="B25" s="158"/>
+      <c r="C25" s="158"/>
+      <c r="D25" s="158"/>
+      <c r="E25" s="158"/>
+      <c r="F25" s="158"/>
+      <c r="G25" s="158"/>
       <c r="H25" s="102"/>
       <c r="I25" s="102"/>
       <c r="J25" s="102"/>
@@ -5744,12 +5748,12 @@
     </row>
     <row r="26" spans="1:22">
       <c r="A26" s="108"/>
-      <c r="B26" s="152"/>
-      <c r="C26" s="152"/>
-      <c r="D26" s="152"/>
-      <c r="E26" s="152"/>
-      <c r="F26" s="152"/>
-      <c r="G26" s="152"/>
+      <c r="B26" s="159"/>
+      <c r="C26" s="159"/>
+      <c r="D26" s="159"/>
+      <c r="E26" s="159"/>
+      <c r="F26" s="159"/>
+      <c r="G26" s="159"/>
       <c r="H26" s="102"/>
       <c r="I26" s="102"/>
       <c r="J26" s="102"/>
@@ -5769,28 +5773,28 @@
       <c r="C27"/>
     </row>
     <row r="28" spans="1:22">
-      <c r="A28" s="166" t="s">
+      <c r="A28" s="143" t="s">
         <v>186</v>
       </c>
-      <c r="B28" s="167"/>
-      <c r="C28" s="167"/>
-      <c r="D28" s="167"/>
-      <c r="E28" s="167"/>
-      <c r="F28" s="167"/>
-      <c r="G28" s="168"/>
+      <c r="B28" s="144"/>
+      <c r="C28" s="144"/>
+      <c r="D28" s="144"/>
+      <c r="E28" s="144"/>
+      <c r="F28" s="144"/>
+      <c r="G28" s="145"/>
     </row>
     <row r="29" spans="1:22">
       <c r="A29" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="144" t="s">
+      <c r="B29" s="164" t="s">
         <v>177</v>
       </c>
-      <c r="C29" s="144"/>
-      <c r="D29" s="144"/>
-      <c r="E29" s="144"/>
-      <c r="F29" s="144"/>
-      <c r="G29" s="144"/>
+      <c r="C29" s="164"/>
+      <c r="D29" s="164"/>
+      <c r="E29" s="164"/>
+      <c r="F29" s="164"/>
+      <c r="G29" s="164"/>
       <c r="H29" s="95"/>
       <c r="I29" s="95"/>
       <c r="J29" s="95"/>
@@ -5810,14 +5814,14 @@
       <c r="A30" s="106">
         <v>1</v>
       </c>
-      <c r="B30" s="145" t="s">
+      <c r="B30" s="165" t="s">
         <v>178</v>
       </c>
-      <c r="C30" s="145"/>
-      <c r="D30" s="145"/>
-      <c r="E30" s="145"/>
-      <c r="F30" s="145"/>
-      <c r="G30" s="145"/>
+      <c r="C30" s="165"/>
+      <c r="D30" s="165"/>
+      <c r="E30" s="165"/>
+      <c r="F30" s="165"/>
+      <c r="G30" s="165"/>
       <c r="H30" s="102"/>
       <c r="I30" s="102"/>
       <c r="J30" s="102"/>
@@ -5835,12 +5839,12 @@
     </row>
     <row r="31" spans="1:22">
       <c r="A31" s="107"/>
-      <c r="B31" s="146"/>
-      <c r="C31" s="146"/>
-      <c r="D31" s="146"/>
-      <c r="E31" s="146"/>
-      <c r="F31" s="146"/>
-      <c r="G31" s="146"/>
+      <c r="B31" s="166"/>
+      <c r="C31" s="166"/>
+      <c r="D31" s="166"/>
+      <c r="E31" s="166"/>
+      <c r="F31" s="166"/>
+      <c r="G31" s="166"/>
       <c r="H31" s="102"/>
       <c r="I31" s="102"/>
       <c r="J31" s="102"/>
@@ -5858,12 +5862,12 @@
     </row>
     <row r="32" spans="1:22">
       <c r="A32" s="108"/>
-      <c r="B32" s="147"/>
-      <c r="C32" s="147"/>
-      <c r="D32" s="147"/>
-      <c r="E32" s="147"/>
-      <c r="F32" s="147"/>
-      <c r="G32" s="147"/>
+      <c r="B32" s="167"/>
+      <c r="C32" s="167"/>
+      <c r="D32" s="167"/>
+      <c r="E32" s="167"/>
+      <c r="F32" s="167"/>
+      <c r="G32" s="167"/>
       <c r="H32" s="102"/>
       <c r="I32" s="102"/>
       <c r="J32" s="102"/>
@@ -5902,28 +5906,28 @@
       <c r="T33"/>
     </row>
     <row r="34" spans="1:22">
-      <c r="A34" s="166" t="s">
+      <c r="A34" s="143" t="s">
         <v>187</v>
       </c>
-      <c r="B34" s="167"/>
-      <c r="C34" s="167"/>
-      <c r="D34" s="167"/>
-      <c r="E34" s="167"/>
-      <c r="F34" s="167"/>
-      <c r="G34" s="168"/>
+      <c r="B34" s="144"/>
+      <c r="C34" s="144"/>
+      <c r="D34" s="144"/>
+      <c r="E34" s="144"/>
+      <c r="F34" s="144"/>
+      <c r="G34" s="145"/>
     </row>
     <row r="35" spans="1:22">
       <c r="A35" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="144" t="s">
+      <c r="B35" s="164" t="s">
         <v>179</v>
       </c>
-      <c r="C35" s="144"/>
-      <c r="D35" s="144"/>
-      <c r="E35" s="144"/>
-      <c r="F35" s="144"/>
-      <c r="G35" s="144"/>
+      <c r="C35" s="164"/>
+      <c r="D35" s="164"/>
+      <c r="E35" s="164"/>
+      <c r="F35" s="164"/>
+      <c r="G35" s="164"/>
       <c r="H35" s="95"/>
       <c r="I35" s="95"/>
       <c r="J35" s="95"/>
@@ -5941,12 +5945,12 @@
     </row>
     <row r="36" spans="1:22">
       <c r="A36" s="106"/>
-      <c r="B36" s="148"/>
-      <c r="C36" s="148"/>
-      <c r="D36" s="148"/>
-      <c r="E36" s="148"/>
-      <c r="F36" s="148"/>
-      <c r="G36" s="149"/>
+      <c r="B36" s="157"/>
+      <c r="C36" s="157"/>
+      <c r="D36" s="157"/>
+      <c r="E36" s="157"/>
+      <c r="F36" s="157"/>
+      <c r="G36" s="168"/>
       <c r="H36" s="102"/>
       <c r="I36" s="102"/>
       <c r="J36" s="102"/>
@@ -5964,12 +5968,12 @@
     </row>
     <row r="37" spans="1:22">
       <c r="A37" s="107"/>
-      <c r="B37" s="150"/>
-      <c r="C37" s="150"/>
-      <c r="D37" s="150"/>
-      <c r="E37" s="150"/>
-      <c r="F37" s="150"/>
-      <c r="G37" s="151"/>
+      <c r="B37" s="158"/>
+      <c r="C37" s="158"/>
+      <c r="D37" s="158"/>
+      <c r="E37" s="158"/>
+      <c r="F37" s="158"/>
+      <c r="G37" s="169"/>
       <c r="H37" s="102"/>
       <c r="I37" s="102"/>
       <c r="J37" s="102"/>
@@ -5987,12 +5991,12 @@
     </row>
     <row r="38" spans="1:22">
       <c r="A38" s="108"/>
-      <c r="B38" s="152"/>
-      <c r="C38" s="152"/>
-      <c r="D38" s="152"/>
-      <c r="E38" s="152"/>
-      <c r="F38" s="152"/>
-      <c r="G38" s="153"/>
+      <c r="B38" s="159"/>
+      <c r="C38" s="159"/>
+      <c r="D38" s="159"/>
+      <c r="E38" s="159"/>
+      <c r="F38" s="159"/>
+      <c r="G38" s="170"/>
       <c r="H38" s="102"/>
       <c r="I38" s="102"/>
       <c r="J38" s="102"/>
@@ -6068,16 +6072,16 @@
       <c r="B42" s="176" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="182" t="s">
+      <c r="C42" s="178" t="s">
         <v>1</v>
       </c>
       <c r="D42" s="176" t="s">
         <v>2</v>
       </c>
-      <c r="E42" s="180" t="s">
+      <c r="E42" s="181" t="s">
         <v>155</v>
       </c>
-      <c r="F42" s="180" t="s">
+      <c r="F42" s="181" t="s">
         <v>170</v>
       </c>
       <c r="G42" s="176" t="s">
@@ -6089,13 +6093,13 @@
       <c r="I42" s="176" t="s">
         <v>236</v>
       </c>
-      <c r="J42" s="180" t="s">
+      <c r="J42" s="181" t="s">
         <v>237</v>
       </c>
-      <c r="K42" s="180" t="s">
+      <c r="K42" s="181" t="s">
         <v>207</v>
       </c>
-      <c r="L42" s="179" t="s">
+      <c r="L42" s="184" t="s">
         <v>224</v>
       </c>
       <c r="M42" s="176" t="s">
@@ -6107,14 +6111,14 @@
       <c r="O42" s="176" t="s">
         <v>189</v>
       </c>
-      <c r="P42" s="183" t="s">
+      <c r="P42" s="179" t="s">
         <v>70</v>
       </c>
-      <c r="Q42" s="184"/>
-      <c r="R42" s="183" t="s">
+      <c r="Q42" s="180"/>
+      <c r="R42" s="179" t="s">
         <v>16</v>
       </c>
-      <c r="S42" s="184"/>
+      <c r="S42" s="180"/>
       <c r="T42" s="32" t="s">
         <v>69</v>
       </c>
@@ -6123,21 +6127,21 @@
       </c>
     </row>
     <row r="43" spans="1:22">
-      <c r="A43" s="178"/>
-      <c r="B43" s="178"/>
-      <c r="C43" s="178"/>
-      <c r="D43" s="178"/>
-      <c r="E43" s="181"/>
-      <c r="F43" s="181"/>
-      <c r="G43" s="178"/>
-      <c r="H43" s="178"/>
-      <c r="I43" s="178"/>
-      <c r="J43" s="181"/>
-      <c r="K43" s="181"/>
-      <c r="L43" s="177"/>
-      <c r="M43" s="178"/>
-      <c r="N43" s="178"/>
-      <c r="O43" s="177"/>
+      <c r="A43" s="177"/>
+      <c r="B43" s="177"/>
+      <c r="C43" s="177"/>
+      <c r="D43" s="177"/>
+      <c r="E43" s="182"/>
+      <c r="F43" s="182"/>
+      <c r="G43" s="177"/>
+      <c r="H43" s="177"/>
+      <c r="I43" s="177"/>
+      <c r="J43" s="182"/>
+      <c r="K43" s="182"/>
+      <c r="L43" s="183"/>
+      <c r="M43" s="177"/>
+      <c r="N43" s="177"/>
+      <c r="O43" s="183"/>
       <c r="P43" s="27" t="s">
         <v>74</v>
       </c>
@@ -6153,7 +6157,7 @@
       <c r="T43" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="U43" s="178"/>
+      <c r="U43" s="177"/>
     </row>
     <row r="44" spans="1:22">
       <c r="A44" s="7">
@@ -6809,6 +6813,26 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="O42:O43"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="M42:M43"/>
+    <mergeCell ref="H42:H43"/>
+    <mergeCell ref="L42:L43"/>
+    <mergeCell ref="K42:K43"/>
+    <mergeCell ref="I42:I43"/>
+    <mergeCell ref="J42:J43"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="A22:G22"/>
@@ -6825,26 +6849,6 @@
     <mergeCell ref="F42:F43"/>
     <mergeCell ref="B23:G23"/>
     <mergeCell ref="B24:G24"/>
-    <mergeCell ref="O42:O43"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="A34:G34"/>
-    <mergeCell ref="M42:M43"/>
-    <mergeCell ref="H42:H43"/>
-    <mergeCell ref="L42:L43"/>
-    <mergeCell ref="K42:K43"/>
-    <mergeCell ref="I42:I43"/>
-    <mergeCell ref="J42:J43"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="B35:G35"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="4">
@@ -7037,10 +7041,10 @@
         <v>167</v>
       </c>
       <c r="B13" s="111"/>
-      <c r="C13" s="133" t="s">
+      <c r="C13" s="151" t="s">
         <v>168</v>
       </c>
-      <c r="D13" s="133"/>
+      <c r="D13" s="151"/>
       <c r="E13" s="1" t="s">
         <v>169</v>
       </c>
@@ -7050,10 +7054,10 @@
         <v>170</v>
       </c>
       <c r="B14" s="111"/>
-      <c r="C14" s="133" t="s">
+      <c r="C14" s="151" t="s">
         <v>171</v>
       </c>
-      <c r="D14" s="133"/>
+      <c r="D14" s="151"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="112" t="s">
@@ -7079,28 +7083,28 @@
       <c r="A16" s="6"/>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="169" t="s">
+      <c r="A17" s="146" t="s">
         <v>185</v>
       </c>
-      <c r="B17" s="169"/>
-      <c r="C17" s="169"/>
-      <c r="D17" s="169"/>
-      <c r="E17" s="169"/>
-      <c r="F17" s="169"/>
-      <c r="G17" s="169"/>
+      <c r="B17" s="146"/>
+      <c r="C17" s="146"/>
+      <c r="D17" s="146"/>
+      <c r="E17" s="146"/>
+      <c r="F17" s="146"/>
+      <c r="G17" s="146"/>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="163" t="s">
+      <c r="B18" s="140" t="s">
         <v>176</v>
       </c>
-      <c r="C18" s="164"/>
-      <c r="D18" s="164"/>
-      <c r="E18" s="164"/>
-      <c r="F18" s="164"/>
-      <c r="G18" s="165"/>
+      <c r="C18" s="141"/>
+      <c r="D18" s="141"/>
+      <c r="E18" s="141"/>
+      <c r="F18" s="141"/>
+      <c r="G18" s="142"/>
       <c r="H18" s="95"/>
       <c r="I18" s="95"/>
       <c r="K18" s="95"/>
@@ -7112,12 +7116,12 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="106"/>
-      <c r="B19" s="148"/>
-      <c r="C19" s="148"/>
-      <c r="D19" s="148"/>
-      <c r="E19" s="148"/>
-      <c r="F19" s="148"/>
-      <c r="G19" s="148"/>
+      <c r="B19" s="157"/>
+      <c r="C19" s="157"/>
+      <c r="D19" s="157"/>
+      <c r="E19" s="157"/>
+      <c r="F19" s="157"/>
+      <c r="G19" s="157"/>
       <c r="H19" s="102"/>
       <c r="I19" s="102"/>
       <c r="K19" s="102"/>
@@ -7129,12 +7133,12 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="107"/>
-      <c r="B20" s="150"/>
-      <c r="C20" s="150"/>
-      <c r="D20" s="150"/>
-      <c r="E20" s="150"/>
-      <c r="F20" s="150"/>
-      <c r="G20" s="150"/>
+      <c r="B20" s="158"/>
+      <c r="C20" s="158"/>
+      <c r="D20" s="158"/>
+      <c r="E20" s="158"/>
+      <c r="F20" s="158"/>
+      <c r="G20" s="158"/>
       <c r="H20" s="102"/>
       <c r="I20" s="102"/>
       <c r="K20" s="102"/>
@@ -7146,12 +7150,12 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="108"/>
-      <c r="B21" s="152"/>
-      <c r="C21" s="152"/>
-      <c r="D21" s="152"/>
-      <c r="E21" s="152"/>
-      <c r="F21" s="152"/>
-      <c r="G21" s="152"/>
+      <c r="B21" s="159"/>
+      <c r="C21" s="159"/>
+      <c r="D21" s="159"/>
+      <c r="E21" s="159"/>
+      <c r="F21" s="159"/>
+      <c r="G21" s="159"/>
       <c r="H21" s="102"/>
       <c r="I21" s="102"/>
       <c r="J21" s="95"/>
@@ -7167,29 +7171,29 @@
       <c r="J22" s="102"/>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="166" t="s">
+      <c r="A23" s="143" t="s">
         <v>186</v>
       </c>
-      <c r="B23" s="167"/>
-      <c r="C23" s="167"/>
-      <c r="D23" s="167"/>
-      <c r="E23" s="167"/>
-      <c r="F23" s="167"/>
-      <c r="G23" s="168"/>
+      <c r="B23" s="144"/>
+      <c r="C23" s="144"/>
+      <c r="D23" s="144"/>
+      <c r="E23" s="144"/>
+      <c r="F23" s="144"/>
+      <c r="G23" s="145"/>
       <c r="J23" s="102"/>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="144" t="s">
+      <c r="B24" s="164" t="s">
         <v>177</v>
       </c>
-      <c r="C24" s="144"/>
-      <c r="D24" s="144"/>
-      <c r="E24" s="144"/>
-      <c r="F24" s="144"/>
-      <c r="G24" s="144"/>
+      <c r="C24" s="164"/>
+      <c r="D24" s="164"/>
+      <c r="E24" s="164"/>
+      <c r="F24" s="164"/>
+      <c r="G24" s="164"/>
       <c r="H24" s="95"/>
       <c r="I24" s="95"/>
       <c r="J24" s="102"/>
@@ -7204,14 +7208,14 @@
       <c r="A25" s="106">
         <v>1</v>
       </c>
-      <c r="B25" s="145" t="s">
+      <c r="B25" s="165" t="s">
         <v>178</v>
       </c>
-      <c r="C25" s="145"/>
-      <c r="D25" s="145"/>
-      <c r="E25" s="145"/>
-      <c r="F25" s="145"/>
-      <c r="G25" s="145"/>
+      <c r="C25" s="165"/>
+      <c r="D25" s="165"/>
+      <c r="E25" s="165"/>
+      <c r="F25" s="165"/>
+      <c r="G25" s="165"/>
       <c r="H25" s="102"/>
       <c r="I25" s="102"/>
       <c r="K25" s="102"/>
@@ -7223,12 +7227,12 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="107"/>
-      <c r="B26" s="146"/>
-      <c r="C26" s="146"/>
-      <c r="D26" s="146"/>
-      <c r="E26" s="146"/>
-      <c r="F26" s="146"/>
-      <c r="G26" s="146"/>
+      <c r="B26" s="166"/>
+      <c r="C26" s="166"/>
+      <c r="D26" s="166"/>
+      <c r="E26" s="166"/>
+      <c r="F26" s="166"/>
+      <c r="G26" s="166"/>
       <c r="H26" s="102"/>
       <c r="I26" s="102"/>
       <c r="K26" s="102"/>
@@ -7240,12 +7244,12 @@
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="108"/>
-      <c r="B27" s="147"/>
-      <c r="C27" s="147"/>
-      <c r="D27" s="147"/>
-      <c r="E27" s="147"/>
-      <c r="F27" s="147"/>
-      <c r="G27" s="147"/>
+      <c r="B27" s="167"/>
+      <c r="C27" s="167"/>
+      <c r="D27" s="167"/>
+      <c r="E27" s="167"/>
+      <c r="F27" s="167"/>
+      <c r="G27" s="167"/>
       <c r="H27" s="102"/>
       <c r="I27" s="102"/>
       <c r="J27" s="95"/>
@@ -7274,29 +7278,29 @@
       <c r="O28"/>
     </row>
     <row r="29" spans="1:17">
-      <c r="A29" s="166" t="s">
+      <c r="A29" s="143" t="s">
         <v>187</v>
       </c>
-      <c r="B29" s="167"/>
-      <c r="C29" s="167"/>
-      <c r="D29" s="167"/>
-      <c r="E29" s="167"/>
-      <c r="F29" s="167"/>
-      <c r="G29" s="168"/>
+      <c r="B29" s="144"/>
+      <c r="C29" s="144"/>
+      <c r="D29" s="144"/>
+      <c r="E29" s="144"/>
+      <c r="F29" s="144"/>
+      <c r="G29" s="145"/>
       <c r="J29" s="102"/>
     </row>
     <row r="30" spans="1:17">
       <c r="A30" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B30" s="144" t="s">
+      <c r="B30" s="164" t="s">
         <v>179</v>
       </c>
-      <c r="C30" s="144"/>
-      <c r="D30" s="144"/>
-      <c r="E30" s="144"/>
-      <c r="F30" s="144"/>
-      <c r="G30" s="144"/>
+      <c r="C30" s="164"/>
+      <c r="D30" s="164"/>
+      <c r="E30" s="164"/>
+      <c r="F30" s="164"/>
+      <c r="G30" s="164"/>
       <c r="H30" s="95"/>
       <c r="I30" s="95"/>
       <c r="J30" s="102"/>
@@ -7309,12 +7313,12 @@
     </row>
     <row r="31" spans="1:17">
       <c r="A31" s="106"/>
-      <c r="B31" s="148"/>
-      <c r="C31" s="148"/>
-      <c r="D31" s="148"/>
-      <c r="E31" s="148"/>
-      <c r="F31" s="148"/>
-      <c r="G31" s="149"/>
+      <c r="B31" s="157"/>
+      <c r="C31" s="157"/>
+      <c r="D31" s="157"/>
+      <c r="E31" s="157"/>
+      <c r="F31" s="157"/>
+      <c r="G31" s="168"/>
       <c r="H31" s="102"/>
       <c r="I31" s="102"/>
       <c r="J31"/>
@@ -7327,12 +7331,12 @@
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="107"/>
-      <c r="B32" s="150"/>
-      <c r="C32" s="150"/>
-      <c r="D32" s="150"/>
-      <c r="E32" s="150"/>
-      <c r="F32" s="150"/>
-      <c r="G32" s="151"/>
+      <c r="B32" s="158"/>
+      <c r="C32" s="158"/>
+      <c r="D32" s="158"/>
+      <c r="E32" s="158"/>
+      <c r="F32" s="158"/>
+      <c r="G32" s="169"/>
       <c r="H32" s="102"/>
       <c r="I32" s="102"/>
       <c r="K32" s="102"/>
@@ -7344,12 +7348,12 @@
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="108"/>
-      <c r="B33" s="152"/>
-      <c r="C33" s="152"/>
-      <c r="D33" s="152"/>
-      <c r="E33" s="152"/>
-      <c r="F33" s="152"/>
-      <c r="G33" s="153"/>
+      <c r="B33" s="159"/>
+      <c r="C33" s="159"/>
+      <c r="D33" s="159"/>
+      <c r="E33" s="159"/>
+      <c r="F33" s="159"/>
+      <c r="G33" s="170"/>
       <c r="H33" s="102"/>
       <c r="I33" s="102"/>
       <c r="J33" s="95"/>
@@ -7402,64 +7406,64 @@
       <c r="P36" s="49"/>
     </row>
     <row r="37" spans="1:17" ht="15">
-      <c r="A37" s="180" t="s">
+      <c r="A37" s="181" t="s">
         <v>114</v>
       </c>
-      <c r="B37" s="180" t="s">
+      <c r="B37" s="181" t="s">
         <v>115</v>
       </c>
       <c r="C37" s="51" t="s">
         <v>116</v>
       </c>
-      <c r="D37" s="180" t="s">
+      <c r="D37" s="181" t="s">
         <v>98</v>
       </c>
-      <c r="E37" s="180" t="s">
+      <c r="E37" s="181" t="s">
         <v>155</v>
       </c>
-      <c r="F37" s="180" t="s">
+      <c r="F37" s="181" t="s">
         <v>170</v>
       </c>
-      <c r="G37" s="180" t="s">
+      <c r="G37" s="181" t="s">
         <v>135</v>
       </c>
-      <c r="H37" s="180" t="s">
+      <c r="H37" s="181" t="s">
         <v>112</v>
       </c>
-      <c r="I37" s="180" t="s">
+      <c r="I37" s="181" t="s">
         <v>229</v>
       </c>
       <c r="J37" s="176" t="s">
         <v>189</v>
       </c>
-      <c r="K37" s="185" t="s">
+      <c r="K37" s="186" t="s">
         <v>118</v>
       </c>
-      <c r="L37" s="186"/>
-      <c r="M37" s="187" t="s">
+      <c r="L37" s="187"/>
+      <c r="M37" s="188" t="s">
         <v>119</v>
       </c>
-      <c r="N37" s="186"/>
+      <c r="N37" s="187"/>
       <c r="O37" s="50" t="s">
         <v>120</v>
       </c>
-      <c r="P37" s="180" t="s">
+      <c r="P37" s="181" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="15">
-      <c r="A38" s="188"/>
-      <c r="B38" s="188"/>
+      <c r="A38" s="185"/>
+      <c r="B38" s="185"/>
       <c r="C38" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="D38" s="188"/>
-      <c r="E38" s="181"/>
-      <c r="F38" s="181"/>
-      <c r="G38" s="188"/>
-      <c r="H38" s="188"/>
-      <c r="I38" s="188"/>
-      <c r="J38" s="177"/>
+      <c r="D38" s="185"/>
+      <c r="E38" s="182"/>
+      <c r="F38" s="182"/>
+      <c r="G38" s="185"/>
+      <c r="H38" s="185"/>
+      <c r="I38" s="185"/>
+      <c r="J38" s="183"/>
       <c r="K38" s="53" t="s">
         <v>122</v>
       </c>
@@ -7475,7 +7479,7 @@
       <c r="O38" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="P38" s="188"/>
+      <c r="P38" s="185"/>
     </row>
     <row r="39" spans="1:17">
       <c r="A39" s="55">
@@ -7973,19 +7977,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="P37:P38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="H37:H38"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="J37:J38"/>
@@ -8002,6 +7993,19 @@
     <mergeCell ref="A17:G17"/>
     <mergeCell ref="B18:G18"/>
     <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="P37:P38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">
@@ -8211,10 +8215,10 @@
         <v>167</v>
       </c>
       <c r="B15" s="111"/>
-      <c r="C15" s="133" t="s">
+      <c r="C15" s="151" t="s">
         <v>168</v>
       </c>
-      <c r="D15" s="133"/>
+      <c r="D15" s="151"/>
       <c r="E15" s="1" t="s">
         <v>169</v>
       </c>
@@ -8224,10 +8228,10 @@
         <v>170</v>
       </c>
       <c r="B16" s="111"/>
-      <c r="C16" s="133" t="s">
+      <c r="C16" s="151" t="s">
         <v>171</v>
       </c>
-      <c r="D16" s="133"/>
+      <c r="D16" s="151"/>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="112" t="s">
@@ -8253,28 +8257,28 @@
       <c r="A18" s="6"/>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="169" t="s">
+      <c r="A19" s="146" t="s">
         <v>185</v>
       </c>
-      <c r="B19" s="169"/>
-      <c r="C19" s="169"/>
-      <c r="D19" s="169"/>
-      <c r="E19" s="169"/>
-      <c r="F19" s="169"/>
-      <c r="G19" s="169"/>
+      <c r="B19" s="146"/>
+      <c r="C19" s="146"/>
+      <c r="D19" s="146"/>
+      <c r="E19" s="146"/>
+      <c r="F19" s="146"/>
+      <c r="G19" s="146"/>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B20" s="163" t="s">
+      <c r="B20" s="140" t="s">
         <v>176</v>
       </c>
-      <c r="C20" s="164"/>
-      <c r="D20" s="164"/>
-      <c r="E20" s="164"/>
-      <c r="F20" s="164"/>
-      <c r="G20" s="165"/>
+      <c r="C20" s="141"/>
+      <c r="D20" s="141"/>
+      <c r="E20" s="141"/>
+      <c r="F20" s="141"/>
+      <c r="G20" s="142"/>
       <c r="H20" s="95"/>
       <c r="I20" s="95"/>
       <c r="K20" s="95"/>
@@ -8286,12 +8290,12 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="106"/>
-      <c r="B21" s="148"/>
-      <c r="C21" s="148"/>
-      <c r="D21" s="148"/>
-      <c r="E21" s="148"/>
-      <c r="F21" s="148"/>
-      <c r="G21" s="148"/>
+      <c r="B21" s="157"/>
+      <c r="C21" s="157"/>
+      <c r="D21" s="157"/>
+      <c r="E21" s="157"/>
+      <c r="F21" s="157"/>
+      <c r="G21" s="157"/>
       <c r="H21" s="102"/>
       <c r="I21" s="102"/>
       <c r="K21" s="102"/>
@@ -8303,12 +8307,12 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="107"/>
-      <c r="B22" s="150"/>
-      <c r="C22" s="150"/>
-      <c r="D22" s="150"/>
-      <c r="E22" s="150"/>
-      <c r="F22" s="150"/>
-      <c r="G22" s="150"/>
+      <c r="B22" s="158"/>
+      <c r="C22" s="158"/>
+      <c r="D22" s="158"/>
+      <c r="E22" s="158"/>
+      <c r="F22" s="158"/>
+      <c r="G22" s="158"/>
       <c r="H22" s="102"/>
       <c r="I22" s="102"/>
       <c r="K22" s="102"/>
@@ -8320,12 +8324,12 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="108"/>
-      <c r="B23" s="152"/>
-      <c r="C23" s="152"/>
-      <c r="D23" s="152"/>
-      <c r="E23" s="152"/>
-      <c r="F23" s="152"/>
-      <c r="G23" s="152"/>
+      <c r="B23" s="159"/>
+      <c r="C23" s="159"/>
+      <c r="D23" s="159"/>
+      <c r="E23" s="159"/>
+      <c r="F23" s="159"/>
+      <c r="G23" s="159"/>
       <c r="H23" s="102"/>
       <c r="I23" s="102"/>
       <c r="J23" s="95"/>
@@ -8341,29 +8345,29 @@
       <c r="J24" s="102"/>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" s="166" t="s">
+      <c r="A25" s="143" t="s">
         <v>186</v>
       </c>
-      <c r="B25" s="167"/>
-      <c r="C25" s="167"/>
-      <c r="D25" s="167"/>
-      <c r="E25" s="167"/>
-      <c r="F25" s="167"/>
-      <c r="G25" s="168"/>
+      <c r="B25" s="144"/>
+      <c r="C25" s="144"/>
+      <c r="D25" s="144"/>
+      <c r="E25" s="144"/>
+      <c r="F25" s="144"/>
+      <c r="G25" s="145"/>
       <c r="J25" s="102"/>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="144" t="s">
+      <c r="B26" s="164" t="s">
         <v>177</v>
       </c>
-      <c r="C26" s="144"/>
-      <c r="D26" s="144"/>
-      <c r="E26" s="144"/>
-      <c r="F26" s="144"/>
-      <c r="G26" s="144"/>
+      <c r="C26" s="164"/>
+      <c r="D26" s="164"/>
+      <c r="E26" s="164"/>
+      <c r="F26" s="164"/>
+      <c r="G26" s="164"/>
       <c r="H26" s="95"/>
       <c r="I26" s="95"/>
       <c r="J26" s="102"/>
@@ -8378,14 +8382,14 @@
       <c r="A27" s="106">
         <v>1</v>
       </c>
-      <c r="B27" s="145" t="s">
+      <c r="B27" s="165" t="s">
         <v>178</v>
       </c>
-      <c r="C27" s="145"/>
-      <c r="D27" s="145"/>
-      <c r="E27" s="145"/>
-      <c r="F27" s="145"/>
-      <c r="G27" s="145"/>
+      <c r="C27" s="165"/>
+      <c r="D27" s="165"/>
+      <c r="E27" s="165"/>
+      <c r="F27" s="165"/>
+      <c r="G27" s="165"/>
       <c r="H27" s="102"/>
       <c r="I27" s="102"/>
       <c r="K27" s="102"/>
@@ -8397,12 +8401,12 @@
     </row>
     <row r="28" spans="1:17">
       <c r="A28" s="107"/>
-      <c r="B28" s="146"/>
-      <c r="C28" s="146"/>
-      <c r="D28" s="146"/>
-      <c r="E28" s="146"/>
-      <c r="F28" s="146"/>
-      <c r="G28" s="146"/>
+      <c r="B28" s="166"/>
+      <c r="C28" s="166"/>
+      <c r="D28" s="166"/>
+      <c r="E28" s="166"/>
+      <c r="F28" s="166"/>
+      <c r="G28" s="166"/>
       <c r="H28" s="102"/>
       <c r="I28" s="102"/>
       <c r="K28" s="102"/>
@@ -8414,12 +8418,12 @@
     </row>
     <row r="29" spans="1:17">
       <c r="A29" s="108"/>
-      <c r="B29" s="147"/>
-      <c r="C29" s="147"/>
-      <c r="D29" s="147"/>
-      <c r="E29" s="147"/>
-      <c r="F29" s="147"/>
-      <c r="G29" s="147"/>
+      <c r="B29" s="167"/>
+      <c r="C29" s="167"/>
+      <c r="D29" s="167"/>
+      <c r="E29" s="167"/>
+      <c r="F29" s="167"/>
+      <c r="G29" s="167"/>
       <c r="H29" s="102"/>
       <c r="I29" s="102"/>
       <c r="J29" s="95"/>
@@ -8448,29 +8452,29 @@
       <c r="O30"/>
     </row>
     <row r="31" spans="1:17">
-      <c r="A31" s="166" t="s">
+      <c r="A31" s="143" t="s">
         <v>187</v>
       </c>
-      <c r="B31" s="167"/>
-      <c r="C31" s="167"/>
-      <c r="D31" s="167"/>
-      <c r="E31" s="167"/>
-      <c r="F31" s="167"/>
-      <c r="G31" s="168"/>
+      <c r="B31" s="144"/>
+      <c r="C31" s="144"/>
+      <c r="D31" s="144"/>
+      <c r="E31" s="144"/>
+      <c r="F31" s="144"/>
+      <c r="G31" s="145"/>
       <c r="J31" s="102"/>
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="144" t="s">
+      <c r="B32" s="164" t="s">
         <v>179</v>
       </c>
-      <c r="C32" s="144"/>
-      <c r="D32" s="144"/>
-      <c r="E32" s="144"/>
-      <c r="F32" s="144"/>
-      <c r="G32" s="144"/>
+      <c r="C32" s="164"/>
+      <c r="D32" s="164"/>
+      <c r="E32" s="164"/>
+      <c r="F32" s="164"/>
+      <c r="G32" s="164"/>
       <c r="H32" s="95"/>
       <c r="I32" s="95"/>
       <c r="J32" s="102"/>
@@ -8483,12 +8487,12 @@
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="106"/>
-      <c r="B33" s="148"/>
-      <c r="C33" s="148"/>
-      <c r="D33" s="148"/>
-      <c r="E33" s="148"/>
-      <c r="F33" s="148"/>
-      <c r="G33" s="149"/>
+      <c r="B33" s="157"/>
+      <c r="C33" s="157"/>
+      <c r="D33" s="157"/>
+      <c r="E33" s="157"/>
+      <c r="F33" s="157"/>
+      <c r="G33" s="168"/>
       <c r="H33" s="102"/>
       <c r="I33" s="102"/>
       <c r="J33"/>
@@ -8501,12 +8505,12 @@
     </row>
     <row r="34" spans="1:17">
       <c r="A34" s="107"/>
-      <c r="B34" s="150"/>
-      <c r="C34" s="150"/>
-      <c r="D34" s="150"/>
-      <c r="E34" s="150"/>
-      <c r="F34" s="150"/>
-      <c r="G34" s="151"/>
+      <c r="B34" s="158"/>
+      <c r="C34" s="158"/>
+      <c r="D34" s="158"/>
+      <c r="E34" s="158"/>
+      <c r="F34" s="158"/>
+      <c r="G34" s="169"/>
       <c r="H34" s="102"/>
       <c r="I34" s="102"/>
       <c r="K34" s="102"/>
@@ -8518,12 +8522,12 @@
     </row>
     <row r="35" spans="1:17">
       <c r="A35" s="108"/>
-      <c r="B35" s="152"/>
-      <c r="C35" s="152"/>
-      <c r="D35" s="152"/>
-      <c r="E35" s="152"/>
-      <c r="F35" s="152"/>
-      <c r="G35" s="153"/>
+      <c r="B35" s="159"/>
+      <c r="C35" s="159"/>
+      <c r="D35" s="159"/>
+      <c r="E35" s="159"/>
+      <c r="F35" s="159"/>
+      <c r="G35" s="170"/>
       <c r="H35" s="102"/>
       <c r="I35" s="102"/>
       <c r="J35" s="95"/>
@@ -8576,25 +8580,25 @@
       <c r="P38" s="49"/>
     </row>
     <row r="39" spans="1:17" ht="15">
-      <c r="A39" s="180" t="s">
+      <c r="A39" s="181" t="s">
         <v>114</v>
       </c>
-      <c r="B39" s="180" t="s">
+      <c r="B39" s="181" t="s">
         <v>115</v>
       </c>
       <c r="C39" s="51" t="s">
         <v>116</v>
       </c>
-      <c r="D39" s="180" t="s">
+      <c r="D39" s="181" t="s">
         <v>98</v>
       </c>
-      <c r="E39" s="180" t="s">
+      <c r="E39" s="181" t="s">
         <v>155</v>
       </c>
-      <c r="F39" s="180" t="s">
+      <c r="F39" s="181" t="s">
         <v>170</v>
       </c>
-      <c r="G39" s="180" t="s">
+      <c r="G39" s="181" t="s">
         <v>135</v>
       </c>
       <c r="H39" s="189" t="s">
@@ -8606,34 +8610,34 @@
       <c r="J39" s="176" t="s">
         <v>189</v>
       </c>
-      <c r="K39" s="185" t="s">
+      <c r="K39" s="186" t="s">
         <v>118</v>
       </c>
-      <c r="L39" s="186"/>
-      <c r="M39" s="187" t="s">
+      <c r="L39" s="187"/>
+      <c r="M39" s="188" t="s">
         <v>119</v>
       </c>
-      <c r="N39" s="186"/>
+      <c r="N39" s="187"/>
       <c r="O39" s="50" t="s">
         <v>120</v>
       </c>
-      <c r="P39" s="180" t="s">
+      <c r="P39" s="181" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="15">
-      <c r="A40" s="188"/>
-      <c r="B40" s="188"/>
+      <c r="A40" s="185"/>
+      <c r="B40" s="185"/>
       <c r="C40" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="D40" s="188"/>
-      <c r="E40" s="181"/>
-      <c r="F40" s="181"/>
-      <c r="G40" s="188"/>
-      <c r="H40" s="188"/>
-      <c r="I40" s="188"/>
-      <c r="J40" s="177"/>
+      <c r="D40" s="185"/>
+      <c r="E40" s="182"/>
+      <c r="F40" s="182"/>
+      <c r="G40" s="185"/>
+      <c r="H40" s="185"/>
+      <c r="I40" s="185"/>
+      <c r="J40" s="183"/>
       <c r="K40" s="53" t="s">
         <v>122</v>
       </c>
@@ -8649,7 +8653,7 @@
       <c r="O40" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="P40" s="188"/>
+      <c r="P40" s="185"/>
     </row>
     <row r="41" spans="1:17">
       <c r="A41" s="55">
@@ -9105,6 +9109,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
     <mergeCell ref="P39:P40"/>
     <mergeCell ref="A31:G31"/>
     <mergeCell ref="B32:G32"/>
@@ -9121,19 +9138,6 @@
     <mergeCell ref="J39:J40"/>
     <mergeCell ref="K39:L39"/>
     <mergeCell ref="M39:N39"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">
@@ -9181,8 +9185,8 @@
   </sheetPr>
   <dimension ref="A1:V67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="N48" sqref="N48"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -9342,10 +9346,10 @@
         <v>167</v>
       </c>
       <c r="B16" s="111"/>
-      <c r="C16" s="133" t="s">
+      <c r="C16" s="151" t="s">
         <v>168</v>
       </c>
-      <c r="D16" s="133"/>
+      <c r="D16" s="151"/>
       <c r="E16" s="1" t="s">
         <v>169</v>
       </c>
@@ -9355,20 +9359,20 @@
         <v>170</v>
       </c>
       <c r="B17" s="111"/>
-      <c r="C17" s="133" t="s">
+      <c r="C17" s="151" t="s">
         <v>171</v>
       </c>
-      <c r="D17" s="133"/>
+      <c r="D17" s="151"/>
     </row>
     <row r="18" spans="1:22">
       <c r="A18" s="111" t="s">
         <v>207</v>
       </c>
       <c r="B18" s="111"/>
-      <c r="C18" s="132" t="s">
+      <c r="C18" s="150" t="s">
         <v>209</v>
       </c>
-      <c r="D18" s="133"/>
+      <c r="D18" s="151"/>
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="112" t="s">
@@ -9426,28 +9430,28 @@
       <c r="A21" s="6"/>
     </row>
     <row r="22" spans="1:22">
-      <c r="A22" s="169" t="s">
+      <c r="A22" s="146" t="s">
         <v>185</v>
       </c>
-      <c r="B22" s="169"/>
-      <c r="C22" s="169"/>
-      <c r="D22" s="169"/>
-      <c r="E22" s="169"/>
-      <c r="F22" s="169"/>
-      <c r="G22" s="169"/>
+      <c r="B22" s="146"/>
+      <c r="C22" s="146"/>
+      <c r="D22" s="146"/>
+      <c r="E22" s="146"/>
+      <c r="F22" s="146"/>
+      <c r="G22" s="146"/>
     </row>
     <row r="23" spans="1:22">
       <c r="A23" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="163" t="s">
+      <c r="B23" s="140" t="s">
         <v>176</v>
       </c>
-      <c r="C23" s="164"/>
-      <c r="D23" s="164"/>
-      <c r="E23" s="164"/>
-      <c r="F23" s="164"/>
-      <c r="G23" s="165"/>
+      <c r="C23" s="141"/>
+      <c r="D23" s="141"/>
+      <c r="E23" s="141"/>
+      <c r="F23" s="141"/>
+      <c r="G23" s="142"/>
       <c r="H23" s="95"/>
       <c r="I23" s="95"/>
       <c r="J23" s="95"/>
@@ -9465,12 +9469,12 @@
     </row>
     <row r="24" spans="1:22">
       <c r="A24" s="106"/>
-      <c r="B24" s="148"/>
-      <c r="C24" s="148"/>
-      <c r="D24" s="148"/>
-      <c r="E24" s="148"/>
-      <c r="F24" s="148"/>
-      <c r="G24" s="148"/>
+      <c r="B24" s="157"/>
+      <c r="C24" s="157"/>
+      <c r="D24" s="157"/>
+      <c r="E24" s="157"/>
+      <c r="F24" s="157"/>
+      <c r="G24" s="157"/>
       <c r="H24" s="102"/>
       <c r="I24" s="102"/>
       <c r="J24" s="102"/>
@@ -9488,12 +9492,12 @@
     </row>
     <row r="25" spans="1:22">
       <c r="A25" s="107"/>
-      <c r="B25" s="150"/>
-      <c r="C25" s="150"/>
-      <c r="D25" s="150"/>
-      <c r="E25" s="150"/>
-      <c r="F25" s="150"/>
-      <c r="G25" s="150"/>
+      <c r="B25" s="158"/>
+      <c r="C25" s="158"/>
+      <c r="D25" s="158"/>
+      <c r="E25" s="158"/>
+      <c r="F25" s="158"/>
+      <c r="G25" s="158"/>
       <c r="H25" s="102"/>
       <c r="I25" s="102"/>
       <c r="J25" s="102"/>
@@ -9511,12 +9515,12 @@
     </row>
     <row r="26" spans="1:22">
       <c r="A26" s="108"/>
-      <c r="B26" s="152"/>
-      <c r="C26" s="152"/>
-      <c r="D26" s="152"/>
-      <c r="E26" s="152"/>
-      <c r="F26" s="152"/>
-      <c r="G26" s="152"/>
+      <c r="B26" s="159"/>
+      <c r="C26" s="159"/>
+      <c r="D26" s="159"/>
+      <c r="E26" s="159"/>
+      <c r="F26" s="159"/>
+      <c r="G26" s="159"/>
       <c r="H26" s="102"/>
       <c r="I26" s="102"/>
       <c r="J26" s="102"/>
@@ -9536,28 +9540,28 @@
       <c r="C27"/>
     </row>
     <row r="28" spans="1:22">
-      <c r="A28" s="166" t="s">
+      <c r="A28" s="143" t="s">
         <v>186</v>
       </c>
-      <c r="B28" s="167"/>
-      <c r="C28" s="167"/>
-      <c r="D28" s="167"/>
-      <c r="E28" s="167"/>
-      <c r="F28" s="167"/>
-      <c r="G28" s="168"/>
+      <c r="B28" s="144"/>
+      <c r="C28" s="144"/>
+      <c r="D28" s="144"/>
+      <c r="E28" s="144"/>
+      <c r="F28" s="144"/>
+      <c r="G28" s="145"/>
     </row>
     <row r="29" spans="1:22">
       <c r="A29" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="144" t="s">
+      <c r="B29" s="164" t="s">
         <v>177</v>
       </c>
-      <c r="C29" s="144"/>
-      <c r="D29" s="144"/>
-      <c r="E29" s="144"/>
-      <c r="F29" s="144"/>
-      <c r="G29" s="144"/>
+      <c r="C29" s="164"/>
+      <c r="D29" s="164"/>
+      <c r="E29" s="164"/>
+      <c r="F29" s="164"/>
+      <c r="G29" s="164"/>
       <c r="H29" s="95"/>
       <c r="I29" s="95"/>
       <c r="J29" s="95"/>
@@ -9577,14 +9581,14 @@
       <c r="A30" s="106">
         <v>1</v>
       </c>
-      <c r="B30" s="145" t="s">
+      <c r="B30" s="165" t="s">
         <v>178</v>
       </c>
-      <c r="C30" s="145"/>
-      <c r="D30" s="145"/>
-      <c r="E30" s="145"/>
-      <c r="F30" s="145"/>
-      <c r="G30" s="145"/>
+      <c r="C30" s="165"/>
+      <c r="D30" s="165"/>
+      <c r="E30" s="165"/>
+      <c r="F30" s="165"/>
+      <c r="G30" s="165"/>
       <c r="H30" s="102"/>
       <c r="I30" s="102"/>
       <c r="J30" s="102"/>
@@ -9602,12 +9606,12 @@
     </row>
     <row r="31" spans="1:22">
       <c r="A31" s="107"/>
-      <c r="B31" s="146"/>
-      <c r="C31" s="146"/>
-      <c r="D31" s="146"/>
-      <c r="E31" s="146"/>
-      <c r="F31" s="146"/>
-      <c r="G31" s="146"/>
+      <c r="B31" s="166"/>
+      <c r="C31" s="166"/>
+      <c r="D31" s="166"/>
+      <c r="E31" s="166"/>
+      <c r="F31" s="166"/>
+      <c r="G31" s="166"/>
       <c r="H31" s="102"/>
       <c r="I31" s="102"/>
       <c r="J31" s="102"/>
@@ -9625,12 +9629,12 @@
     </row>
     <row r="32" spans="1:22">
       <c r="A32" s="108"/>
-      <c r="B32" s="147"/>
-      <c r="C32" s="147"/>
-      <c r="D32" s="147"/>
-      <c r="E32" s="147"/>
-      <c r="F32" s="147"/>
-      <c r="G32" s="147"/>
+      <c r="B32" s="167"/>
+      <c r="C32" s="167"/>
+      <c r="D32" s="167"/>
+      <c r="E32" s="167"/>
+      <c r="F32" s="167"/>
+      <c r="G32" s="167"/>
       <c r="H32" s="102"/>
       <c r="I32" s="102"/>
       <c r="J32" s="102"/>
@@ -9669,28 +9673,28 @@
       <c r="T33"/>
     </row>
     <row r="34" spans="1:22">
-      <c r="A34" s="166" t="s">
+      <c r="A34" s="143" t="s">
         <v>187</v>
       </c>
-      <c r="B34" s="167"/>
-      <c r="C34" s="167"/>
-      <c r="D34" s="167"/>
-      <c r="E34" s="167"/>
-      <c r="F34" s="167"/>
-      <c r="G34" s="168"/>
+      <c r="B34" s="144"/>
+      <c r="C34" s="144"/>
+      <c r="D34" s="144"/>
+      <c r="E34" s="144"/>
+      <c r="F34" s="144"/>
+      <c r="G34" s="145"/>
     </row>
     <row r="35" spans="1:22">
       <c r="A35" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="144" t="s">
+      <c r="B35" s="164" t="s">
         <v>179</v>
       </c>
-      <c r="C35" s="144"/>
-      <c r="D35" s="144"/>
-      <c r="E35" s="144"/>
-      <c r="F35" s="144"/>
-      <c r="G35" s="144"/>
+      <c r="C35" s="164"/>
+      <c r="D35" s="164"/>
+      <c r="E35" s="164"/>
+      <c r="F35" s="164"/>
+      <c r="G35" s="164"/>
       <c r="H35" s="95"/>
       <c r="I35" s="95"/>
       <c r="J35" s="95"/>
@@ -9708,12 +9712,12 @@
     </row>
     <row r="36" spans="1:22">
       <c r="A36" s="106"/>
-      <c r="B36" s="148"/>
-      <c r="C36" s="148"/>
-      <c r="D36" s="148"/>
-      <c r="E36" s="148"/>
-      <c r="F36" s="148"/>
-      <c r="G36" s="149"/>
+      <c r="B36" s="157"/>
+      <c r="C36" s="157"/>
+      <c r="D36" s="157"/>
+      <c r="E36" s="157"/>
+      <c r="F36" s="157"/>
+      <c r="G36" s="168"/>
       <c r="H36" s="102"/>
       <c r="I36" s="102"/>
       <c r="J36" s="102"/>
@@ -9731,12 +9735,12 @@
     </row>
     <row r="37" spans="1:22">
       <c r="A37" s="107"/>
-      <c r="B37" s="150"/>
-      <c r="C37" s="150"/>
-      <c r="D37" s="150"/>
-      <c r="E37" s="150"/>
-      <c r="F37" s="150"/>
-      <c r="G37" s="151"/>
+      <c r="B37" s="158"/>
+      <c r="C37" s="158"/>
+      <c r="D37" s="158"/>
+      <c r="E37" s="158"/>
+      <c r="F37" s="158"/>
+      <c r="G37" s="169"/>
       <c r="H37" s="102"/>
       <c r="I37" s="102"/>
       <c r="J37" s="102"/>
@@ -9754,12 +9758,12 @@
     </row>
     <row r="38" spans="1:22">
       <c r="A38" s="108"/>
-      <c r="B38" s="152"/>
-      <c r="C38" s="152"/>
-      <c r="D38" s="152"/>
-      <c r="E38" s="152"/>
-      <c r="F38" s="152"/>
-      <c r="G38" s="153"/>
+      <c r="B38" s="159"/>
+      <c r="C38" s="159"/>
+      <c r="D38" s="159"/>
+      <c r="E38" s="159"/>
+      <c r="F38" s="159"/>
+      <c r="G38" s="170"/>
       <c r="H38" s="102"/>
       <c r="I38" s="102"/>
       <c r="J38" s="102"/>
@@ -9835,16 +9839,16 @@
       <c r="B42" s="176" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="182" t="s">
+      <c r="C42" s="178" t="s">
         <v>1</v>
       </c>
       <c r="D42" s="176" t="s">
         <v>2</v>
       </c>
-      <c r="E42" s="180" t="s">
+      <c r="E42" s="181" t="s">
         <v>155</v>
       </c>
-      <c r="F42" s="180" t="s">
+      <c r="F42" s="181" t="s">
         <v>170</v>
       </c>
       <c r="G42" s="176" t="s">
@@ -9856,13 +9860,13 @@
       <c r="I42" s="176" t="s">
         <v>236</v>
       </c>
-      <c r="J42" s="180" t="s">
+      <c r="J42" s="181" t="s">
         <v>237</v>
       </c>
-      <c r="K42" s="180" t="s">
+      <c r="K42" s="181" t="s">
         <v>207</v>
       </c>
-      <c r="L42" s="179" t="s">
+      <c r="L42" s="184" t="s">
         <v>224</v>
       </c>
       <c r="M42" s="176" t="s">
@@ -9874,14 +9878,14 @@
       <c r="O42" s="176" t="s">
         <v>189</v>
       </c>
-      <c r="P42" s="183" t="s">
+      <c r="P42" s="179" t="s">
         <v>70</v>
       </c>
-      <c r="Q42" s="184"/>
-      <c r="R42" s="183" t="s">
+      <c r="Q42" s="180"/>
+      <c r="R42" s="179" t="s">
         <v>16</v>
       </c>
-      <c r="S42" s="184"/>
+      <c r="S42" s="180"/>
       <c r="T42" s="32" t="s">
         <v>69</v>
       </c>
@@ -9890,21 +9894,21 @@
       </c>
     </row>
     <row r="43" spans="1:22">
-      <c r="A43" s="178"/>
-      <c r="B43" s="178"/>
-      <c r="C43" s="178"/>
-      <c r="D43" s="178"/>
-      <c r="E43" s="181"/>
-      <c r="F43" s="181"/>
-      <c r="G43" s="178"/>
-      <c r="H43" s="178"/>
-      <c r="I43" s="178"/>
-      <c r="J43" s="181"/>
-      <c r="K43" s="181"/>
-      <c r="L43" s="177"/>
-      <c r="M43" s="178"/>
-      <c r="N43" s="178"/>
-      <c r="O43" s="177"/>
+      <c r="A43" s="177"/>
+      <c r="B43" s="177"/>
+      <c r="C43" s="177"/>
+      <c r="D43" s="177"/>
+      <c r="E43" s="182"/>
+      <c r="F43" s="182"/>
+      <c r="G43" s="177"/>
+      <c r="H43" s="177"/>
+      <c r="I43" s="177"/>
+      <c r="J43" s="182"/>
+      <c r="K43" s="182"/>
+      <c r="L43" s="183"/>
+      <c r="M43" s="177"/>
+      <c r="N43" s="177"/>
+      <c r="O43" s="183"/>
       <c r="P43" s="27" t="s">
         <v>74</v>
       </c>
@@ -9920,7 +9924,7 @@
       <c r="T43" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="U43" s="178"/>
+      <c r="U43" s="177"/>
     </row>
     <row r="44" spans="1:22">
       <c r="A44" s="7">
@@ -10582,6 +10586,30 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="U42:U43"/>
+    <mergeCell ref="G42:G43"/>
+    <mergeCell ref="H42:H43"/>
+    <mergeCell ref="I42:I43"/>
+    <mergeCell ref="J42:J43"/>
+    <mergeCell ref="K42:K43"/>
+    <mergeCell ref="L42:L43"/>
+    <mergeCell ref="M42:M43"/>
+    <mergeCell ref="N42:N43"/>
+    <mergeCell ref="O42:O43"/>
+    <mergeCell ref="P42:Q42"/>
+    <mergeCell ref="R42:S42"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
     <mergeCell ref="B31:G31"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
@@ -10594,30 +10622,6 @@
     <mergeCell ref="A28:G28"/>
     <mergeCell ref="B29:G29"/>
     <mergeCell ref="B30:G30"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="A34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="U42:U43"/>
-    <mergeCell ref="G42:G43"/>
-    <mergeCell ref="H42:H43"/>
-    <mergeCell ref="I42:I43"/>
-    <mergeCell ref="J42:J43"/>
-    <mergeCell ref="K42:K43"/>
-    <mergeCell ref="L42:L43"/>
-    <mergeCell ref="M42:M43"/>
-    <mergeCell ref="N42:N43"/>
-    <mergeCell ref="O42:O43"/>
-    <mergeCell ref="P42:Q42"/>
-    <mergeCell ref="R42:S42"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="4">
@@ -10674,8 +10678,8 @@
   </sheetPr>
   <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -10810,10 +10814,10 @@
         <v>167</v>
       </c>
       <c r="B13" s="111"/>
-      <c r="C13" s="133" t="s">
+      <c r="C13" s="151" t="s">
         <v>168</v>
       </c>
-      <c r="D13" s="133"/>
+      <c r="D13" s="151"/>
       <c r="E13" s="1" t="s">
         <v>169</v>
       </c>
@@ -10823,10 +10827,10 @@
         <v>170</v>
       </c>
       <c r="B14" s="111"/>
-      <c r="C14" s="133" t="s">
+      <c r="C14" s="151" t="s">
         <v>171</v>
       </c>
-      <c r="D14" s="133"/>
+      <c r="D14" s="151"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="112" t="s">
@@ -10852,28 +10856,28 @@
       <c r="A16" s="6"/>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="169" t="s">
+      <c r="A17" s="146" t="s">
         <v>185</v>
       </c>
-      <c r="B17" s="169"/>
-      <c r="C17" s="169"/>
-      <c r="D17" s="169"/>
-      <c r="E17" s="169"/>
-      <c r="F17" s="169"/>
-      <c r="G17" s="169"/>
+      <c r="B17" s="146"/>
+      <c r="C17" s="146"/>
+      <c r="D17" s="146"/>
+      <c r="E17" s="146"/>
+      <c r="F17" s="146"/>
+      <c r="G17" s="146"/>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="163" t="s">
+      <c r="B18" s="140" t="s">
         <v>176</v>
       </c>
-      <c r="C18" s="164"/>
-      <c r="D18" s="164"/>
-      <c r="E18" s="164"/>
-      <c r="F18" s="164"/>
-      <c r="G18" s="165"/>
+      <c r="C18" s="141"/>
+      <c r="D18" s="141"/>
+      <c r="E18" s="141"/>
+      <c r="F18" s="141"/>
+      <c r="G18" s="142"/>
       <c r="H18" s="95"/>
       <c r="I18" s="95"/>
       <c r="K18" s="95"/>
@@ -10885,12 +10889,12 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="106"/>
-      <c r="B19" s="148"/>
-      <c r="C19" s="148"/>
-      <c r="D19" s="148"/>
-      <c r="E19" s="148"/>
-      <c r="F19" s="148"/>
-      <c r="G19" s="148"/>
+      <c r="B19" s="157"/>
+      <c r="C19" s="157"/>
+      <c r="D19" s="157"/>
+      <c r="E19" s="157"/>
+      <c r="F19" s="157"/>
+      <c r="G19" s="157"/>
       <c r="H19" s="102"/>
       <c r="I19" s="102"/>
       <c r="K19" s="102"/>
@@ -10902,12 +10906,12 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="107"/>
-      <c r="B20" s="150"/>
-      <c r="C20" s="150"/>
-      <c r="D20" s="150"/>
-      <c r="E20" s="150"/>
-      <c r="F20" s="150"/>
-      <c r="G20" s="150"/>
+      <c r="B20" s="158"/>
+      <c r="C20" s="158"/>
+      <c r="D20" s="158"/>
+      <c r="E20" s="158"/>
+      <c r="F20" s="158"/>
+      <c r="G20" s="158"/>
       <c r="H20" s="102"/>
       <c r="I20" s="102"/>
       <c r="K20" s="102"/>
@@ -10919,12 +10923,12 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="108"/>
-      <c r="B21" s="152"/>
-      <c r="C21" s="152"/>
-      <c r="D21" s="152"/>
-      <c r="E21" s="152"/>
-      <c r="F21" s="152"/>
-      <c r="G21" s="152"/>
+      <c r="B21" s="159"/>
+      <c r="C21" s="159"/>
+      <c r="D21" s="159"/>
+      <c r="E21" s="159"/>
+      <c r="F21" s="159"/>
+      <c r="G21" s="159"/>
       <c r="H21" s="102"/>
       <c r="I21" s="102"/>
       <c r="J21" s="95"/>
@@ -10940,29 +10944,29 @@
       <c r="J22" s="102"/>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="166" t="s">
+      <c r="A23" s="143" t="s">
         <v>186</v>
       </c>
-      <c r="B23" s="167"/>
-      <c r="C23" s="167"/>
-      <c r="D23" s="167"/>
-      <c r="E23" s="167"/>
-      <c r="F23" s="167"/>
-      <c r="G23" s="168"/>
+      <c r="B23" s="144"/>
+      <c r="C23" s="144"/>
+      <c r="D23" s="144"/>
+      <c r="E23" s="144"/>
+      <c r="F23" s="144"/>
+      <c r="G23" s="145"/>
       <c r="J23" s="102"/>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="144" t="s">
+      <c r="B24" s="164" t="s">
         <v>177</v>
       </c>
-      <c r="C24" s="144"/>
-      <c r="D24" s="144"/>
-      <c r="E24" s="144"/>
-      <c r="F24" s="144"/>
-      <c r="G24" s="144"/>
+      <c r="C24" s="164"/>
+      <c r="D24" s="164"/>
+      <c r="E24" s="164"/>
+      <c r="F24" s="164"/>
+      <c r="G24" s="164"/>
       <c r="H24" s="95"/>
       <c r="I24" s="95"/>
       <c r="J24" s="102"/>
@@ -10977,14 +10981,14 @@
       <c r="A25" s="106">
         <v>1</v>
       </c>
-      <c r="B25" s="145" t="s">
+      <c r="B25" s="165" t="s">
         <v>178</v>
       </c>
-      <c r="C25" s="145"/>
-      <c r="D25" s="145"/>
-      <c r="E25" s="145"/>
-      <c r="F25" s="145"/>
-      <c r="G25" s="145"/>
+      <c r="C25" s="165"/>
+      <c r="D25" s="165"/>
+      <c r="E25" s="165"/>
+      <c r="F25" s="165"/>
+      <c r="G25" s="165"/>
       <c r="H25" s="102"/>
       <c r="I25" s="102"/>
       <c r="K25" s="102"/>
@@ -10996,12 +11000,12 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="107"/>
-      <c r="B26" s="146"/>
-      <c r="C26" s="146"/>
-      <c r="D26" s="146"/>
-      <c r="E26" s="146"/>
-      <c r="F26" s="146"/>
-      <c r="G26" s="146"/>
+      <c r="B26" s="166"/>
+      <c r="C26" s="166"/>
+      <c r="D26" s="166"/>
+      <c r="E26" s="166"/>
+      <c r="F26" s="166"/>
+      <c r="G26" s="166"/>
       <c r="H26" s="102"/>
       <c r="I26" s="102"/>
       <c r="K26" s="102"/>
@@ -11013,12 +11017,12 @@
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="108"/>
-      <c r="B27" s="147"/>
-      <c r="C27" s="147"/>
-      <c r="D27" s="147"/>
-      <c r="E27" s="147"/>
-      <c r="F27" s="147"/>
-      <c r="G27" s="147"/>
+      <c r="B27" s="167"/>
+      <c r="C27" s="167"/>
+      <c r="D27" s="167"/>
+      <c r="E27" s="167"/>
+      <c r="F27" s="167"/>
+      <c r="G27" s="167"/>
       <c r="H27" s="102"/>
       <c r="I27" s="102"/>
       <c r="J27" s="95"/>
@@ -11047,29 +11051,29 @@
       <c r="O28"/>
     </row>
     <row r="29" spans="1:17">
-      <c r="A29" s="166" t="s">
+      <c r="A29" s="143" t="s">
         <v>187</v>
       </c>
-      <c r="B29" s="167"/>
-      <c r="C29" s="167"/>
-      <c r="D29" s="167"/>
-      <c r="E29" s="167"/>
-      <c r="F29" s="167"/>
-      <c r="G29" s="168"/>
+      <c r="B29" s="144"/>
+      <c r="C29" s="144"/>
+      <c r="D29" s="144"/>
+      <c r="E29" s="144"/>
+      <c r="F29" s="144"/>
+      <c r="G29" s="145"/>
       <c r="J29" s="102"/>
     </row>
     <row r="30" spans="1:17">
       <c r="A30" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B30" s="144" t="s">
+      <c r="B30" s="164" t="s">
         <v>179</v>
       </c>
-      <c r="C30" s="144"/>
-      <c r="D30" s="144"/>
-      <c r="E30" s="144"/>
-      <c r="F30" s="144"/>
-      <c r="G30" s="144"/>
+      <c r="C30" s="164"/>
+      <c r="D30" s="164"/>
+      <c r="E30" s="164"/>
+      <c r="F30" s="164"/>
+      <c r="G30" s="164"/>
       <c r="H30" s="95"/>
       <c r="I30" s="95"/>
       <c r="J30" s="102"/>
@@ -11082,12 +11086,12 @@
     </row>
     <row r="31" spans="1:17">
       <c r="A31" s="106"/>
-      <c r="B31" s="148"/>
-      <c r="C31" s="148"/>
-      <c r="D31" s="148"/>
-      <c r="E31" s="148"/>
-      <c r="F31" s="148"/>
-      <c r="G31" s="149"/>
+      <c r="B31" s="157"/>
+      <c r="C31" s="157"/>
+      <c r="D31" s="157"/>
+      <c r="E31" s="157"/>
+      <c r="F31" s="157"/>
+      <c r="G31" s="168"/>
       <c r="H31" s="102"/>
       <c r="I31" s="102"/>
       <c r="J31"/>
@@ -11100,12 +11104,12 @@
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="107"/>
-      <c r="B32" s="150"/>
-      <c r="C32" s="150"/>
-      <c r="D32" s="150"/>
-      <c r="E32" s="150"/>
-      <c r="F32" s="150"/>
-      <c r="G32" s="151"/>
+      <c r="B32" s="158"/>
+      <c r="C32" s="158"/>
+      <c r="D32" s="158"/>
+      <c r="E32" s="158"/>
+      <c r="F32" s="158"/>
+      <c r="G32" s="169"/>
       <c r="H32" s="102"/>
       <c r="I32" s="102"/>
       <c r="K32" s="102"/>
@@ -11117,12 +11121,12 @@
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="108"/>
-      <c r="B33" s="152"/>
-      <c r="C33" s="152"/>
-      <c r="D33" s="152"/>
-      <c r="E33" s="152"/>
-      <c r="F33" s="152"/>
-      <c r="G33" s="153"/>
+      <c r="B33" s="159"/>
+      <c r="C33" s="159"/>
+      <c r="D33" s="159"/>
+      <c r="E33" s="159"/>
+      <c r="F33" s="159"/>
+      <c r="G33" s="170"/>
       <c r="H33" s="102"/>
       <c r="I33" s="102"/>
       <c r="J33" s="95"/>
@@ -11175,64 +11179,64 @@
       <c r="P36" s="49"/>
     </row>
     <row r="37" spans="1:17" ht="15">
-      <c r="A37" s="180" t="s">
+      <c r="A37" s="181" t="s">
         <v>114</v>
       </c>
-      <c r="B37" s="180" t="s">
+      <c r="B37" s="181" t="s">
         <v>115</v>
       </c>
       <c r="C37" s="51" t="s">
         <v>116</v>
       </c>
-      <c r="D37" s="180" t="s">
+      <c r="D37" s="181" t="s">
         <v>98</v>
       </c>
-      <c r="E37" s="180" t="s">
+      <c r="E37" s="181" t="s">
         <v>155</v>
       </c>
-      <c r="F37" s="180" t="s">
+      <c r="F37" s="181" t="s">
         <v>170</v>
       </c>
-      <c r="G37" s="180" t="s">
+      <c r="G37" s="181" t="s">
         <v>135</v>
       </c>
-      <c r="H37" s="180" t="s">
+      <c r="H37" s="181" t="s">
         <v>112</v>
       </c>
-      <c r="I37" s="180" t="s">
+      <c r="I37" s="181" t="s">
         <v>229</v>
       </c>
       <c r="J37" s="176" t="s">
         <v>189</v>
       </c>
-      <c r="K37" s="185" t="s">
+      <c r="K37" s="186" t="s">
         <v>118</v>
       </c>
-      <c r="L37" s="186"/>
-      <c r="M37" s="187" t="s">
+      <c r="L37" s="187"/>
+      <c r="M37" s="188" t="s">
         <v>119</v>
       </c>
-      <c r="N37" s="186"/>
+      <c r="N37" s="187"/>
       <c r="O37" s="50" t="s">
         <v>120</v>
       </c>
-      <c r="P37" s="180" t="s">
+      <c r="P37" s="181" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="15">
-      <c r="A38" s="188"/>
-      <c r="B38" s="188"/>
+      <c r="A38" s="185"/>
+      <c r="B38" s="185"/>
       <c r="C38" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="D38" s="188"/>
-      <c r="E38" s="181"/>
-      <c r="F38" s="181"/>
-      <c r="G38" s="188"/>
-      <c r="H38" s="188"/>
-      <c r="I38" s="188"/>
-      <c r="J38" s="177"/>
+      <c r="D38" s="185"/>
+      <c r="E38" s="182"/>
+      <c r="F38" s="182"/>
+      <c r="G38" s="185"/>
+      <c r="H38" s="185"/>
+      <c r="I38" s="185"/>
+      <c r="J38" s="183"/>
       <c r="K38" s="53" t="s">
         <v>122</v>
       </c>
@@ -11248,7 +11252,7 @@
       <c r="O38" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="P38" s="188"/>
+      <c r="P38" s="185"/>
     </row>
     <row r="39" spans="1:17">
       <c r="A39" s="55">
@@ -11267,7 +11271,9 @@
       <c r="F39" s="58"/>
       <c r="G39" s="80"/>
       <c r="H39" s="58"/>
-      <c r="I39" s="58"/>
+      <c r="I39" s="58" t="s">
+        <v>251</v>
+      </c>
       <c r="J39" s="23" t="s">
         <v>136</v>
       </c>
@@ -11746,6 +11752,23 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="P37:P38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="J37:J38"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
     <mergeCell ref="B27:G27"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
@@ -11758,23 +11781,6 @@
     <mergeCell ref="B24:G24"/>
     <mergeCell ref="B25:G25"/>
     <mergeCell ref="B26:G26"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="A29:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="P37:P38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="J37:J38"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="M37:N37"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">
@@ -11984,10 +11990,10 @@
         <v>167</v>
       </c>
       <c r="B15" s="111"/>
-      <c r="C15" s="133" t="s">
+      <c r="C15" s="151" t="s">
         <v>168</v>
       </c>
-      <c r="D15" s="133"/>
+      <c r="D15" s="151"/>
       <c r="E15" s="1" t="s">
         <v>169</v>
       </c>
@@ -11997,10 +12003,10 @@
         <v>170</v>
       </c>
       <c r="B16" s="111"/>
-      <c r="C16" s="133" t="s">
+      <c r="C16" s="151" t="s">
         <v>171</v>
       </c>
-      <c r="D16" s="133"/>
+      <c r="D16" s="151"/>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="112" t="s">
@@ -12026,28 +12032,28 @@
       <c r="A18" s="6"/>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="169" t="s">
+      <c r="A19" s="146" t="s">
         <v>185</v>
       </c>
-      <c r="B19" s="169"/>
-      <c r="C19" s="169"/>
-      <c r="D19" s="169"/>
-      <c r="E19" s="169"/>
-      <c r="F19" s="169"/>
-      <c r="G19" s="169"/>
+      <c r="B19" s="146"/>
+      <c r="C19" s="146"/>
+      <c r="D19" s="146"/>
+      <c r="E19" s="146"/>
+      <c r="F19" s="146"/>
+      <c r="G19" s="146"/>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B20" s="163" t="s">
+      <c r="B20" s="140" t="s">
         <v>176</v>
       </c>
-      <c r="C20" s="164"/>
-      <c r="D20" s="164"/>
-      <c r="E20" s="164"/>
-      <c r="F20" s="164"/>
-      <c r="G20" s="165"/>
+      <c r="C20" s="141"/>
+      <c r="D20" s="141"/>
+      <c r="E20" s="141"/>
+      <c r="F20" s="141"/>
+      <c r="G20" s="142"/>
       <c r="H20" s="95"/>
       <c r="I20" s="95"/>
       <c r="K20" s="95"/>
@@ -12059,12 +12065,12 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="106"/>
-      <c r="B21" s="148"/>
-      <c r="C21" s="148"/>
-      <c r="D21" s="148"/>
-      <c r="E21" s="148"/>
-      <c r="F21" s="148"/>
-      <c r="G21" s="148"/>
+      <c r="B21" s="157"/>
+      <c r="C21" s="157"/>
+      <c r="D21" s="157"/>
+      <c r="E21" s="157"/>
+      <c r="F21" s="157"/>
+      <c r="G21" s="157"/>
       <c r="H21" s="102"/>
       <c r="I21" s="102"/>
       <c r="K21" s="102"/>
@@ -12076,12 +12082,12 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="107"/>
-      <c r="B22" s="150"/>
-      <c r="C22" s="150"/>
-      <c r="D22" s="150"/>
-      <c r="E22" s="150"/>
-      <c r="F22" s="150"/>
-      <c r="G22" s="150"/>
+      <c r="B22" s="158"/>
+      <c r="C22" s="158"/>
+      <c r="D22" s="158"/>
+      <c r="E22" s="158"/>
+      <c r="F22" s="158"/>
+      <c r="G22" s="158"/>
       <c r="H22" s="102"/>
       <c r="I22" s="102"/>
       <c r="K22" s="102"/>
@@ -12093,12 +12099,12 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="108"/>
-      <c r="B23" s="152"/>
-      <c r="C23" s="152"/>
-      <c r="D23" s="152"/>
-      <c r="E23" s="152"/>
-      <c r="F23" s="152"/>
-      <c r="G23" s="152"/>
+      <c r="B23" s="159"/>
+      <c r="C23" s="159"/>
+      <c r="D23" s="159"/>
+      <c r="E23" s="159"/>
+      <c r="F23" s="159"/>
+      <c r="G23" s="159"/>
       <c r="H23" s="102"/>
       <c r="I23" s="102"/>
       <c r="J23" s="95"/>
@@ -12114,29 +12120,29 @@
       <c r="J24" s="102"/>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" s="166" t="s">
+      <c r="A25" s="143" t="s">
         <v>186</v>
       </c>
-      <c r="B25" s="167"/>
-      <c r="C25" s="167"/>
-      <c r="D25" s="167"/>
-      <c r="E25" s="167"/>
-      <c r="F25" s="167"/>
-      <c r="G25" s="168"/>
+      <c r="B25" s="144"/>
+      <c r="C25" s="144"/>
+      <c r="D25" s="144"/>
+      <c r="E25" s="144"/>
+      <c r="F25" s="144"/>
+      <c r="G25" s="145"/>
       <c r="J25" s="102"/>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="144" t="s">
+      <c r="B26" s="164" t="s">
         <v>177</v>
       </c>
-      <c r="C26" s="144"/>
-      <c r="D26" s="144"/>
-      <c r="E26" s="144"/>
-      <c r="F26" s="144"/>
-      <c r="G26" s="144"/>
+      <c r="C26" s="164"/>
+      <c r="D26" s="164"/>
+      <c r="E26" s="164"/>
+      <c r="F26" s="164"/>
+      <c r="G26" s="164"/>
       <c r="H26" s="95"/>
       <c r="I26" s="95"/>
       <c r="J26" s="102"/>
@@ -12151,14 +12157,14 @@
       <c r="A27" s="106">
         <v>1</v>
       </c>
-      <c r="B27" s="145" t="s">
+      <c r="B27" s="165" t="s">
         <v>178</v>
       </c>
-      <c r="C27" s="145"/>
-      <c r="D27" s="145"/>
-      <c r="E27" s="145"/>
-      <c r="F27" s="145"/>
-      <c r="G27" s="145"/>
+      <c r="C27" s="165"/>
+      <c r="D27" s="165"/>
+      <c r="E27" s="165"/>
+      <c r="F27" s="165"/>
+      <c r="G27" s="165"/>
       <c r="H27" s="102"/>
       <c r="I27" s="102"/>
       <c r="K27" s="102"/>
@@ -12170,12 +12176,12 @@
     </row>
     <row r="28" spans="1:17">
       <c r="A28" s="107"/>
-      <c r="B28" s="146"/>
-      <c r="C28" s="146"/>
-      <c r="D28" s="146"/>
-      <c r="E28" s="146"/>
-      <c r="F28" s="146"/>
-      <c r="G28" s="146"/>
+      <c r="B28" s="166"/>
+      <c r="C28" s="166"/>
+      <c r="D28" s="166"/>
+      <c r="E28" s="166"/>
+      <c r="F28" s="166"/>
+      <c r="G28" s="166"/>
       <c r="H28" s="102"/>
       <c r="I28" s="102"/>
       <c r="K28" s="102"/>
@@ -12187,12 +12193,12 @@
     </row>
     <row r="29" spans="1:17">
       <c r="A29" s="108"/>
-      <c r="B29" s="147"/>
-      <c r="C29" s="147"/>
-      <c r="D29" s="147"/>
-      <c r="E29" s="147"/>
-      <c r="F29" s="147"/>
-      <c r="G29" s="147"/>
+      <c r="B29" s="167"/>
+      <c r="C29" s="167"/>
+      <c r="D29" s="167"/>
+      <c r="E29" s="167"/>
+      <c r="F29" s="167"/>
+      <c r="G29" s="167"/>
       <c r="H29" s="102"/>
       <c r="I29" s="102"/>
       <c r="J29" s="95"/>
@@ -12221,29 +12227,29 @@
       <c r="O30"/>
     </row>
     <row r="31" spans="1:17">
-      <c r="A31" s="166" t="s">
+      <c r="A31" s="143" t="s">
         <v>187</v>
       </c>
-      <c r="B31" s="167"/>
-      <c r="C31" s="167"/>
-      <c r="D31" s="167"/>
-      <c r="E31" s="167"/>
-      <c r="F31" s="167"/>
-      <c r="G31" s="168"/>
+      <c r="B31" s="144"/>
+      <c r="C31" s="144"/>
+      <c r="D31" s="144"/>
+      <c r="E31" s="144"/>
+      <c r="F31" s="144"/>
+      <c r="G31" s="145"/>
       <c r="J31" s="102"/>
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="144" t="s">
+      <c r="B32" s="164" t="s">
         <v>179</v>
       </c>
-      <c r="C32" s="144"/>
-      <c r="D32" s="144"/>
-      <c r="E32" s="144"/>
-      <c r="F32" s="144"/>
-      <c r="G32" s="144"/>
+      <c r="C32" s="164"/>
+      <c r="D32" s="164"/>
+      <c r="E32" s="164"/>
+      <c r="F32" s="164"/>
+      <c r="G32" s="164"/>
       <c r="H32" s="95"/>
       <c r="I32" s="95"/>
       <c r="J32" s="102"/>
@@ -12256,12 +12262,12 @@
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="106"/>
-      <c r="B33" s="148"/>
-      <c r="C33" s="148"/>
-      <c r="D33" s="148"/>
-      <c r="E33" s="148"/>
-      <c r="F33" s="148"/>
-      <c r="G33" s="149"/>
+      <c r="B33" s="157"/>
+      <c r="C33" s="157"/>
+      <c r="D33" s="157"/>
+      <c r="E33" s="157"/>
+      <c r="F33" s="157"/>
+      <c r="G33" s="168"/>
       <c r="H33" s="102"/>
       <c r="I33" s="102"/>
       <c r="J33"/>
@@ -12274,12 +12280,12 @@
     </row>
     <row r="34" spans="1:17">
       <c r="A34" s="107"/>
-      <c r="B34" s="150"/>
-      <c r="C34" s="150"/>
-      <c r="D34" s="150"/>
-      <c r="E34" s="150"/>
-      <c r="F34" s="150"/>
-      <c r="G34" s="151"/>
+      <c r="B34" s="158"/>
+      <c r="C34" s="158"/>
+      <c r="D34" s="158"/>
+      <c r="E34" s="158"/>
+      <c r="F34" s="158"/>
+      <c r="G34" s="169"/>
       <c r="H34" s="102"/>
       <c r="I34" s="102"/>
       <c r="K34" s="102"/>
@@ -12291,12 +12297,12 @@
     </row>
     <row r="35" spans="1:17">
       <c r="A35" s="108"/>
-      <c r="B35" s="152"/>
-      <c r="C35" s="152"/>
-      <c r="D35" s="152"/>
-      <c r="E35" s="152"/>
-      <c r="F35" s="152"/>
-      <c r="G35" s="153"/>
+      <c r="B35" s="159"/>
+      <c r="C35" s="159"/>
+      <c r="D35" s="159"/>
+      <c r="E35" s="159"/>
+      <c r="F35" s="159"/>
+      <c r="G35" s="170"/>
       <c r="H35" s="102"/>
       <c r="I35" s="102"/>
       <c r="J35" s="95"/>
@@ -12349,25 +12355,25 @@
       <c r="P38" s="49"/>
     </row>
     <row r="39" spans="1:17" ht="15">
-      <c r="A39" s="180" t="s">
+      <c r="A39" s="181" t="s">
         <v>114</v>
       </c>
-      <c r="B39" s="180" t="s">
+      <c r="B39" s="181" t="s">
         <v>115</v>
       </c>
       <c r="C39" s="51" t="s">
         <v>116</v>
       </c>
-      <c r="D39" s="180" t="s">
+      <c r="D39" s="181" t="s">
         <v>98</v>
       </c>
-      <c r="E39" s="180" t="s">
+      <c r="E39" s="181" t="s">
         <v>155</v>
       </c>
-      <c r="F39" s="180" t="s">
+      <c r="F39" s="181" t="s">
         <v>170</v>
       </c>
-      <c r="G39" s="180" t="s">
+      <c r="G39" s="181" t="s">
         <v>135</v>
       </c>
       <c r="H39" s="189" t="s">
@@ -12379,34 +12385,34 @@
       <c r="J39" s="176" t="s">
         <v>189</v>
       </c>
-      <c r="K39" s="185" t="s">
+      <c r="K39" s="186" t="s">
         <v>118</v>
       </c>
-      <c r="L39" s="186"/>
-      <c r="M39" s="187" t="s">
+      <c r="L39" s="187"/>
+      <c r="M39" s="188" t="s">
         <v>119</v>
       </c>
-      <c r="N39" s="186"/>
+      <c r="N39" s="187"/>
       <c r="O39" s="50" t="s">
         <v>120</v>
       </c>
-      <c r="P39" s="180" t="s">
+      <c r="P39" s="181" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="15">
-      <c r="A40" s="188"/>
-      <c r="B40" s="188"/>
+      <c r="A40" s="185"/>
+      <c r="B40" s="185"/>
       <c r="C40" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="D40" s="188"/>
-      <c r="E40" s="181"/>
-      <c r="F40" s="181"/>
-      <c r="G40" s="188"/>
-      <c r="H40" s="188"/>
-      <c r="I40" s="188"/>
-      <c r="J40" s="177"/>
+      <c r="D40" s="185"/>
+      <c r="E40" s="182"/>
+      <c r="F40" s="182"/>
+      <c r="G40" s="185"/>
+      <c r="H40" s="185"/>
+      <c r="I40" s="185"/>
+      <c r="J40" s="183"/>
       <c r="K40" s="53" t="s">
         <v>122</v>
       </c>
@@ -12422,7 +12428,7 @@
       <c r="O40" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="P40" s="188"/>
+      <c r="P40" s="185"/>
     </row>
     <row r="41" spans="1:17">
       <c r="A41" s="55">
@@ -12878,6 +12884,23 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="P39:P40"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="I39:I40"/>
+    <mergeCell ref="J39:J40"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
     <mergeCell ref="B29:G29"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C16:D16"/>
@@ -12890,23 +12913,6 @@
     <mergeCell ref="B26:G26"/>
     <mergeCell ref="B27:G27"/>
     <mergeCell ref="B28:G28"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="P39:P40"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="I39:I40"/>
-    <mergeCell ref="J39:J40"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="M39:N39"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations disablePrompts="1" count="3">

</xml_diff>